<commit_message>
Remove Transition Rule Attributes x4
Strikethroughs added to lines
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Desktop\CDISC\DDF\DDF_Phase 2\CT Work Sprint 1\Data Dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE70858E-D5A4-4055-B7E7-2D562D38FF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480ABD48-22BB-42AA-902C-56FFA933E32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="320" windowWidth="17720" windowHeight="9730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2170" yWindow="1050" windowWidth="16590" windowHeight="8590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -2648,7 +2648,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2753,6 +2753,20 @@
     <font>
       <sz val="10"/>
       <color indexed="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2875,7 +2889,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3095,6 +3109,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3391,7 +3420,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
@@ -5359,56 +5388,56 @@
       </c>
     </row>
     <row r="78" spans="1:9" ht="25" x14ac:dyDescent="0.35">
-      <c r="A78" s="48">
+      <c r="A78" s="74">
         <v>77</v>
       </c>
-      <c r="B78" s="60" t="s">
+      <c r="B78" s="75" t="s">
         <v>685</v>
       </c>
-      <c r="C78" s="62" t="s">
+      <c r="C78" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="D78" s="68" t="s">
+      <c r="D78" s="77" t="s">
         <v>577</v>
       </c>
-      <c r="E78" s="61" t="s">
+      <c r="E78" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="F78" s="61" t="s">
+      <c r="F78" s="78" t="s">
         <v>832</v>
       </c>
-      <c r="G78" s="61"/>
-      <c r="H78" s="61" t="s">
+      <c r="G78" s="78"/>
+      <c r="H78" s="78" t="s">
         <v>833</v>
       </c>
-      <c r="I78" s="62" t="s">
+      <c r="I78" s="76" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="25" x14ac:dyDescent="0.35">
-      <c r="A79" s="48">
+      <c r="A79" s="74">
         <v>78</v>
       </c>
-      <c r="B79" s="60" t="s">
+      <c r="B79" s="75" t="s">
         <v>685</v>
       </c>
-      <c r="C79" s="62" t="s">
+      <c r="C79" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="D79" s="68" t="s">
+      <c r="D79" s="77" t="s">
         <v>578</v>
       </c>
-      <c r="E79" s="61" t="s">
+      <c r="E79" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="F79" s="61" t="s">
+      <c r="F79" s="78" t="s">
         <v>834</v>
       </c>
-      <c r="G79" s="61"/>
-      <c r="H79" s="61" t="s">
+      <c r="G79" s="78"/>
+      <c r="H79" s="78" t="s">
         <v>835</v>
       </c>
-      <c r="I79" s="62" t="s">
+      <c r="I79" s="76" t="s">
         <v>95</v>
       </c>
     </row>
@@ -5532,56 +5561,56 @@
       <c r="I84" s="4"/>
     </row>
     <row r="85" spans="1:9" ht="25" x14ac:dyDescent="0.35">
-      <c r="A85" s="48">
+      <c r="A85" s="74">
         <v>84</v>
       </c>
-      <c r="B85" s="60" t="s">
+      <c r="B85" s="75" t="s">
         <v>687</v>
       </c>
-      <c r="C85" s="62" t="s">
+      <c r="C85" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="D85" s="68" t="s">
+      <c r="D85" s="77" t="s">
         <v>577</v>
       </c>
-      <c r="E85" s="61" t="s">
+      <c r="E85" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="F85" s="61" t="s">
+      <c r="F85" s="78" t="s">
         <v>832</v>
       </c>
-      <c r="G85" s="61"/>
-      <c r="H85" s="61" t="s">
+      <c r="G85" s="78"/>
+      <c r="H85" s="78" t="s">
         <v>833</v>
       </c>
-      <c r="I85" s="62" t="s">
+      <c r="I85" s="76" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="25" x14ac:dyDescent="0.35">
-      <c r="A86" s="48">
+      <c r="A86" s="74">
         <v>85</v>
       </c>
-      <c r="B86" s="60" t="s">
+      <c r="B86" s="75" t="s">
         <v>687</v>
       </c>
-      <c r="C86" s="62" t="s">
+      <c r="C86" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="D86" s="68" t="s">
+      <c r="D86" s="77" t="s">
         <v>578</v>
       </c>
-      <c r="E86" s="61" t="s">
+      <c r="E86" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="F86" s="61" t="s">
+      <c r="F86" s="78" t="s">
         <v>834</v>
       </c>
-      <c r="G86" s="61"/>
-      <c r="H86" s="61" t="s">
+      <c r="G86" s="78"/>
+      <c r="H86" s="78" t="s">
         <v>835</v>
       </c>
-      <c r="I86" s="62" t="s">
+      <c r="I86" s="76" t="s">
         <v>95</v>
       </c>
     </row>
@@ -7352,7 +7381,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="21" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A24" s="22" t="s">
         <v>160</v>
       </c>
@@ -7426,7 +7455,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="21" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A27" s="22" t="s">
         <v>160</v>
       </c>
@@ -7450,7 +7479,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="21" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" s="21" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A28" s="22" t="s">
         <v>160</v>
       </c>
@@ -9819,24 +9848,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -10058,33 +10069,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10102,4 +10105,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Sprint 2 changes updated
font colors changed and strikethrough rows removed
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDAD830-5F21-419F-8630-5BA21C376DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E9CBD2-FFE5-4B46-B626-9CD8438180FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="17790" windowHeight="8850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="440" yWindow="470" windowWidth="18430" windowHeight="9680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
     <sheet name="DDF valid value sets" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DDF Entities&amp;Attributes'!$A$1:$I$140</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DDF Entities&amp;Attributes'!$A$1:$I$136</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DDF valid value sets'!$A$6:$N$124</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1723" uniqueCount="849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1695" uniqueCount="845">
   <si>
     <t>Preferred Term</t>
   </si>
@@ -2475,18 +2475,6 @@
   </si>
   <si>
     <t>Therapeutic Area</t>
-  </si>
-  <si>
-    <t>Transition Start Rule</t>
-  </si>
-  <si>
-    <t>A criterion that establishes the beginning of a subject transition within a study workflow.</t>
-  </si>
-  <si>
-    <t>Transition End Rule</t>
-  </si>
-  <si>
-    <t>A criterion that establishes the end of a subject transition within a study workflow.</t>
   </si>
   <si>
     <r>
@@ -2595,507 +2583,65 @@
 </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>interventionDesc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>interventionDescription</t>
-    </r>
-  </si>
-  <si>
     <t>studyDesignDescription</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>indicationDesc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>indicationDescription</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>populationDesc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>populationDescription</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>objectiveDesc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>objectiveDescription</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>endpointDesc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>endpointDescription</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>endpointPurposeDesc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>endpointPurposeDescription</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>studyArmDesc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>studyArmDescription</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>studyArmDataOriginDesc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>studyArmDataOriginDescription</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>studyEpochDesc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>studyEpochDescription</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>studyElementDesc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>studyElementDescription</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>transitionRuleDesc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>transitionRuleDescription</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>encounterDesc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>encounterDescription</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>activityDesc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>activityDescription</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>studyDataDesc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>studyDataDescription</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>workflowDesc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>workflowDescription</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>workflowItemDesc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>workflowItemDescription</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>intercurrentEventDesc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>intercurrentEventDescription</t>
-    </r>
+    <t>intercurrentEventDescription</t>
+  </si>
+  <si>
+    <t>populationDescription</t>
+  </si>
+  <si>
+    <t>workflowItemDescription</t>
+  </si>
+  <si>
+    <t>workflowDescription</t>
+  </si>
+  <si>
+    <t>studyDataDescription</t>
+  </si>
+  <si>
+    <t>activityDescription</t>
+  </si>
+  <si>
+    <t>encounterDescription</t>
+  </si>
+  <si>
+    <t>transitionRuleDescription</t>
+  </si>
+  <si>
+    <t>studyElementDescription</t>
+  </si>
+  <si>
+    <t>studyEpochDescription</t>
+  </si>
+  <si>
+    <t>studyArmDataOriginDescription</t>
+  </si>
+  <si>
+    <t>studyArmDescription</t>
+  </si>
+  <si>
+    <t>endpointPurposeDescription</t>
+  </si>
+  <si>
+    <t>endpointDescription</t>
+  </si>
+  <si>
+    <t>objectiveDescription</t>
+  </si>
+  <si>
+    <t>indicationDescription</t>
+  </si>
+  <si>
+    <t>interventionDescription</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3172,23 +2718,16 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -3303,7 +2842,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3440,50 +2979,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -3499,6 +2996,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3791,7 +3294,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I140"/>
+  <dimension ref="A1:I136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4682,13 +4185,13 @@
       <c r="A36" s="33">
         <v>35</v>
       </c>
-      <c r="B36" s="51" t="s">
+      <c r="B36" s="1" t="s">
         <v>657</v>
       </c>
-      <c r="C36" s="51" t="s">
+      <c r="C36" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="D36" s="52" t="s">
+      <c r="D36" s="42" t="s">
         <v>571</v>
       </c>
       <c r="E36" s="29"/>
@@ -4701,14 +4204,14 @@
       <c r="A37" s="33">
         <v>36</v>
       </c>
-      <c r="B37" s="51" t="s">
+      <c r="B37" s="1" t="s">
         <v>657</v>
       </c>
-      <c r="C37" s="51" t="s">
+      <c r="C37" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="D37" s="52" t="s">
-        <v>818</v>
+      <c r="D37" s="42" t="s">
+        <v>814</v>
       </c>
       <c r="E37" s="29"/>
       <c r="F37" s="4"/>
@@ -4824,7 +4327,7 @@
         <v>811</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>807</v>
@@ -4834,26 +4337,26 @@
       <c r="A42" s="33">
         <v>41</v>
       </c>
-      <c r="B42" s="56" t="s">
+      <c r="B42" s="4" t="s">
         <v>657</v>
       </c>
-      <c r="C42" s="51" t="s">
+      <c r="C42" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D42" s="53" t="s">
-        <v>819</v>
-      </c>
-      <c r="E42" s="54" t="s">
+      <c r="D42" s="31" t="s">
+        <v>815</v>
+      </c>
+      <c r="E42" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F42" s="54" t="s">
-        <v>820</v>
-      </c>
-      <c r="G42" s="55"/>
-      <c r="H42" s="54" t="s">
-        <v>821</v>
-      </c>
-      <c r="I42" s="51" t="s">
+      <c r="F42" s="43" t="s">
+        <v>816</v>
+      </c>
+      <c r="G42" s="52"/>
+      <c r="H42" s="43" t="s">
+        <v>817</v>
+      </c>
+      <c r="I42" s="1" t="s">
         <v>95</v>
       </c>
     </row>
@@ -4861,26 +4364,26 @@
       <c r="A43" s="33">
         <v>42</v>
       </c>
-      <c r="B43" s="56" t="s">
+      <c r="B43" s="4" t="s">
         <v>657</v>
       </c>
-      <c r="C43" s="51" t="s">
+      <c r="C43" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D43" s="53" t="s">
-        <v>832</v>
-      </c>
-      <c r="E43" s="54" t="s">
+      <c r="D43" s="31" t="s">
+        <v>827</v>
+      </c>
+      <c r="E43" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F43" s="54" t="s">
-        <v>822</v>
-      </c>
-      <c r="G43" s="55"/>
-      <c r="H43" s="54" t="s">
-        <v>823</v>
-      </c>
-      <c r="I43" s="51" t="s">
+      <c r="F43" s="43" t="s">
+        <v>818</v>
+      </c>
+      <c r="G43" s="52"/>
+      <c r="H43" s="43" t="s">
+        <v>819</v>
+      </c>
+      <c r="I43" s="1" t="s">
         <v>95</v>
       </c>
     </row>
@@ -4949,7 +4452,7 @@
         <v>96</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>831</v>
+        <v>844</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>102</v>
@@ -5030,7 +4533,7 @@
         <v>96</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>833</v>
+        <v>843</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>34</v>
@@ -5084,7 +4587,7 @@
         <v>96</v>
       </c>
       <c r="D51" s="31" t="s">
-        <v>834</v>
+        <v>829</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>743</v>
@@ -5146,7 +4649,7 @@
       <c r="H53" s="4"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="33">
         <v>53</v>
       </c>
@@ -5157,7 +4660,7 @@
         <v>96</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>835</v>
+        <v>842</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>124</v>
@@ -5227,7 +4730,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="33">
         <v>56</v>
       </c>
@@ -5238,7 +4741,7 @@
         <v>96</v>
       </c>
       <c r="D57" s="30" t="s">
-        <v>836</v>
+        <v>841</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>744</v>
@@ -5265,7 +4768,7 @@
         <v>96</v>
       </c>
       <c r="D58" s="31" t="s">
-        <v>837</v>
+        <v>840</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>745</v>
@@ -5446,7 +4949,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="33">
         <v>65</v>
       </c>
@@ -5457,7 +4960,7 @@
         <v>96</v>
       </c>
       <c r="D66" s="31" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>139</v>
@@ -5511,7 +5014,7 @@
         <v>96</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>749</v>
@@ -5627,7 +5130,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="33">
         <v>72</v>
       </c>
@@ -5638,7 +5141,7 @@
         <v>96</v>
       </c>
       <c r="D73" s="31" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>751</v>
@@ -5838,7 +5341,7 @@
         <v>96</v>
       </c>
       <c r="D81" s="31" t="s">
-        <v>841</v>
+        <v>836</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>756</v>
@@ -5854,57 +5357,57 @@
         <v>95</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A82" s="33">
         <v>81</v>
       </c>
-      <c r="B82" s="46" t="s">
-        <v>666</v>
-      </c>
-      <c r="C82" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="D82" s="48" t="s">
-        <v>572</v>
-      </c>
-      <c r="E82" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="F82" s="49" t="s">
-        <v>812</v>
-      </c>
-      <c r="G82" s="49"/>
-      <c r="H82" s="49" t="s">
-        <v>813</v>
-      </c>
-      <c r="I82" s="47" t="s">
+      <c r="B82" s="4" t="s">
+        <v>667</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="41" t="s">
+        <v>667</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G82" s="4"/>
+      <c r="H82" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I82" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="33">
         <v>82</v>
       </c>
-      <c r="B83" s="46" t="s">
-        <v>666</v>
-      </c>
-      <c r="C83" s="47" t="s">
+      <c r="B83" s="4" t="s">
+        <v>667</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D83" s="48" t="s">
-        <v>573</v>
-      </c>
-      <c r="E83" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="F83" s="49" t="s">
-        <v>814</v>
-      </c>
-      <c r="G83" s="49"/>
-      <c r="H83" s="49" t="s">
-        <v>815</v>
-      </c>
-      <c r="I83" s="47" t="s">
+      <c r="D83" s="31" t="s">
+        <v>835</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G83" s="4"/>
+      <c r="H83" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I83" s="1" t="s">
         <v>95</v>
       </c>
     </row>
@@ -5913,56 +5416,48 @@
         <v>83</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D84" s="41" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="G84" s="4"/>
-      <c r="H84" s="4" t="s">
-        <v>81</v>
+      <c r="H84" s="3" t="s">
+        <v>709</v>
       </c>
       <c r="I84" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="33">
         <v>84</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D85" s="31" t="s">
-        <v>842</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>757</v>
-      </c>
-      <c r="F85" s="4" t="s">
-        <v>110</v>
-      </c>
+        <v>652</v>
+      </c>
+      <c r="D85" s="42" t="s">
+        <v>572</v>
+      </c>
+      <c r="E85" s="1"/>
+      <c r="F85" s="4"/>
       <c r="G85" s="4"/>
-      <c r="H85" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="I85" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="H85" s="3"/>
+      <c r="I85" s="1"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="33">
         <v>85</v>
       </c>
@@ -5970,26 +5465,18 @@
         <v>668</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D86" s="41" t="s">
-        <v>668</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F86" s="4" t="s">
-        <v>58</v>
-      </c>
+        <v>652</v>
+      </c>
+      <c r="D86" s="42" t="s">
+        <v>573</v>
+      </c>
+      <c r="E86" s="1"/>
+      <c r="F86" s="4"/>
       <c r="G86" s="4"/>
-      <c r="H86" s="3" t="s">
-        <v>709</v>
-      </c>
-      <c r="I86" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H86" s="3"/>
+      <c r="I86" s="1"/>
+    </row>
+    <row r="87" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A87" s="33">
         <v>86</v>
       </c>
@@ -5997,18 +5484,26 @@
         <v>668</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D87" s="42" t="s">
-        <v>572</v>
-      </c>
-      <c r="E87" s="1"/>
-      <c r="F87" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="D87" s="31" t="s">
+        <v>574</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="G87" s="4"/>
-      <c r="H87" s="3"/>
-      <c r="I87" s="1"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H87" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A88" s="33">
         <v>87</v>
       </c>
@@ -6016,41 +5511,49 @@
         <v>668</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D88" s="42" t="s">
-        <v>573</v>
-      </c>
-      <c r="E88" s="1"/>
-      <c r="F88" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="D88" s="31" t="s">
+        <v>834</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>758</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="G88" s="4"/>
-      <c r="H88" s="3"/>
-      <c r="I88" s="1"/>
+      <c r="H88" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I88" s="43" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="89" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A89" s="33">
         <v>88</v>
       </c>
-      <c r="B89" s="46" t="s">
+      <c r="B89" s="4" t="s">
         <v>668</v>
       </c>
-      <c r="C89" s="47" t="s">
+      <c r="C89" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D89" s="48" t="s">
-        <v>572</v>
-      </c>
-      <c r="E89" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="F89" s="49" t="s">
-        <v>812</v>
-      </c>
-      <c r="G89" s="49"/>
-      <c r="H89" s="49" t="s">
-        <v>813</v>
-      </c>
-      <c r="I89" s="47" t="s">
+      <c r="D89" s="31" t="s">
+        <v>578</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>759</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4" t="s">
+        <v>720</v>
+      </c>
+      <c r="I89" s="43" t="s">
         <v>95</v>
       </c>
     </row>
@@ -6058,30 +5561,30 @@
       <c r="A90" s="33">
         <v>89</v>
       </c>
-      <c r="B90" s="46" t="s">
+      <c r="B90" s="4" t="s">
         <v>668</v>
       </c>
-      <c r="C90" s="47" t="s">
+      <c r="C90" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D90" s="48" t="s">
-        <v>573</v>
-      </c>
-      <c r="E90" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="F90" s="49" t="s">
-        <v>814</v>
-      </c>
-      <c r="G90" s="49"/>
-      <c r="H90" s="49" t="s">
-        <v>815</v>
-      </c>
-      <c r="I90" s="47" t="s">
+      <c r="D90" s="31" t="s">
+        <v>579</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>760</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>587</v>
+      </c>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4" t="s">
+        <v>721</v>
+      </c>
+      <c r="I90" s="43" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A91" s="33">
         <v>90</v>
       </c>
@@ -6092,20 +5595,20 @@
         <v>96</v>
       </c>
       <c r="D91" s="31" t="s">
-        <v>574</v>
-      </c>
-      <c r="E91" s="4" t="s">
-        <v>120</v>
+        <v>575</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>761</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>121</v>
+        <v>69</v>
       </c>
       <c r="G91" s="4"/>
-      <c r="H91" s="4" t="s">
-        <v>514</v>
+      <c r="H91" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>95</v>
+        <v>791</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -6119,20 +5622,20 @@
         <v>96</v>
       </c>
       <c r="D92" s="31" t="s">
-        <v>843</v>
-      </c>
-      <c r="E92" s="4" t="s">
-        <v>758</v>
+        <v>576</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>762</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
       <c r="G92" s="4"/>
       <c r="H92" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="I92" s="43" t="s">
-        <v>95</v>
+        <v>73</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>707</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -6146,131 +5649,115 @@
         <v>96</v>
       </c>
       <c r="D93" s="31" t="s">
-        <v>578</v>
-      </c>
-      <c r="E93" s="4" t="s">
-        <v>759</v>
+        <v>577</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>763</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>586</v>
+        <v>74</v>
       </c>
       <c r="G93" s="4"/>
       <c r="H93" s="4" t="s">
-        <v>720</v>
-      </c>
-      <c r="I93" s="43" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A94" s="33">
         <v>93</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D94" s="31" t="s">
-        <v>579</v>
-      </c>
-      <c r="E94" s="4" t="s">
-        <v>760</v>
+        <v>4</v>
+      </c>
+      <c r="D94" s="41" t="s">
+        <v>669</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>587</v>
+        <v>60</v>
       </c>
       <c r="G94" s="4"/>
-      <c r="H94" s="4" t="s">
-        <v>721</v>
-      </c>
-      <c r="I94" s="43" t="s">
+      <c r="H94" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I94" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" s="33">
         <v>94</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D95" s="31" t="s">
-        <v>575</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>761</v>
-      </c>
-      <c r="F95" s="4" t="s">
-        <v>69</v>
-      </c>
+        <v>652</v>
+      </c>
+      <c r="D95" s="42" t="s">
+        <v>589</v>
+      </c>
+      <c r="E95" s="1"/>
+      <c r="F95" s="4"/>
       <c r="G95" s="4"/>
-      <c r="H95" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I95" s="1" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+      <c r="H95" s="3"/>
+      <c r="I95" s="1"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="33">
         <v>95</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D96" s="31" t="s">
-        <v>576</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>762</v>
-      </c>
-      <c r="F96" s="4" t="s">
-        <v>72</v>
-      </c>
+        <v>652</v>
+      </c>
+      <c r="D96" s="42" t="s">
+        <v>590</v>
+      </c>
+      <c r="E96" s="1"/>
+      <c r="F96" s="4"/>
       <c r="G96" s="4"/>
-      <c r="H96" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>707</v>
-      </c>
+      <c r="H96" s="3"/>
+      <c r="I96" s="1"/>
     </row>
     <row r="97" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A97" s="33">
         <v>96</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>96</v>
       </c>
       <c r="D97" s="31" t="s">
-        <v>577</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>763</v>
+        <v>591</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>764</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>74</v>
+        <v>597</v>
       </c>
       <c r="G97" s="4"/>
       <c r="H97" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I97" s="1" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
+        <v>700</v>
+      </c>
+      <c r="I97" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A98" s="33">
         <v>97</v>
       </c>
@@ -6278,26 +5765,26 @@
         <v>669</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D98" s="41" t="s">
-        <v>669</v>
+        <v>96</v>
+      </c>
+      <c r="D98" s="31" t="s">
+        <v>833</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>89</v>
+        <v>553</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>60</v>
+        <v>554</v>
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I98" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="I98" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A99" s="33">
         <v>98</v>
       </c>
@@ -6305,18 +5792,26 @@
         <v>669</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D99" s="42" t="s">
-        <v>589</v>
-      </c>
-      <c r="E99" s="1"/>
-      <c r="F99" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="D99" s="31" t="s">
+        <v>592</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>765</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>594</v>
+      </c>
       <c r="G99" s="4"/>
-      <c r="H99" s="3"/>
-      <c r="I99" s="1"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H99" s="4" t="s">
+        <v>722</v>
+      </c>
+      <c r="I99" s="43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A100" s="33">
         <v>99</v>
       </c>
@@ -6324,41 +5819,49 @@
         <v>669</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D100" s="42" t="s">
-        <v>590</v>
-      </c>
-      <c r="E100" s="1"/>
-      <c r="F100" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="D100" s="31" t="s">
+        <v>593</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>766</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>595</v>
+      </c>
       <c r="G100" s="4"/>
-      <c r="H100" s="3"/>
-      <c r="I100" s="1"/>
-    </row>
-    <row r="101" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+      <c r="H100" s="4" t="s">
+        <v>723</v>
+      </c>
+      <c r="I100" s="43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" s="33">
         <v>100</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D101" s="31" t="s">
-        <v>591</v>
-      </c>
-      <c r="E101" s="4" t="s">
-        <v>764</v>
+        <v>4</v>
+      </c>
+      <c r="D101" s="41" t="s">
+        <v>670</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>767</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>597</v>
+        <v>76</v>
       </c>
       <c r="G101" s="4"/>
-      <c r="H101" s="4" t="s">
-        <v>700</v>
-      </c>
-      <c r="I101" s="4" t="s">
+      <c r="H101" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I101" s="1" t="s">
         <v>95</v>
       </c>
     </row>
@@ -6367,25 +5870,25 @@
         <v>101</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>96</v>
       </c>
       <c r="D102" s="31" t="s">
-        <v>844</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>553</v>
+        <v>596</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>768</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>554</v>
+        <v>152</v>
       </c>
       <c r="G102" s="4"/>
-      <c r="H102" s="3" t="s">
-        <v>555</v>
-      </c>
-      <c r="I102" s="4" t="s">
+      <c r="H102" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="I102" s="43" t="s">
         <v>95</v>
       </c>
     </row>
@@ -6394,23 +5897,23 @@
         <v>102</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>96</v>
       </c>
       <c r="D103" s="31" t="s">
-        <v>592</v>
+        <v>832</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>594</v>
+        <v>153</v>
       </c>
       <c r="G103" s="4"/>
       <c r="H103" s="4" t="s">
-        <v>722</v>
+        <v>128</v>
       </c>
       <c r="I103" s="43" t="s">
         <v>95</v>
@@ -6421,318 +5924,302 @@
         <v>103</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>96</v>
       </c>
       <c r="D104" s="31" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>766</v>
+        <v>770</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>595</v>
+        <v>649</v>
       </c>
       <c r="G104" s="4"/>
       <c r="H104" s="4" t="s">
-        <v>723</v>
+        <v>717</v>
       </c>
       <c r="I104" s="43" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A105" s="33">
         <v>104</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>670</v>
+        <v>90</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D105" s="41" t="s">
-        <v>670</v>
+        <v>90</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>767</v>
+        <v>79</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="G105" s="4"/>
-      <c r="H105" s="3" t="s">
-        <v>77</v>
+      <c r="H105" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="I105" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" s="33">
         <v>105</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>670</v>
+        <v>90</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>96</v>
       </c>
       <c r="D106" s="31" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>768</v>
+        <v>771</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="G106" s="4"/>
       <c r="H106" s="4" t="s">
-        <v>516</v>
-      </c>
-      <c r="I106" s="43" t="s">
+        <v>698</v>
+      </c>
+      <c r="I106" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" ht="50" x14ac:dyDescent="0.35">
       <c r="A107" s="33">
         <v>106</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>670</v>
+        <v>90</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>96</v>
       </c>
       <c r="D107" s="31" t="s">
-        <v>845</v>
+        <v>600</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>769</v>
+        <v>141</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>153</v>
+        <v>112</v>
       </c>
       <c r="G107" s="4"/>
       <c r="H107" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="I107" s="43" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="50" x14ac:dyDescent="0.35">
       <c r="A108" s="33">
         <v>107</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>670</v>
+        <v>603</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D108" s="31" t="s">
-        <v>598</v>
+        <v>4</v>
+      </c>
+      <c r="D108" s="41" t="s">
+        <v>603</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>770</v>
+        <v>602</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>649</v>
+        <v>603</v>
       </c>
       <c r="G108" s="4"/>
       <c r="H108" s="4" t="s">
-        <v>717</v>
-      </c>
-      <c r="I108" s="43" t="s">
+        <v>601</v>
+      </c>
+      <c r="I108" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" s="33">
         <v>108</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>90</v>
+        <v>603</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D109" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F109" s="4" t="s">
-        <v>90</v>
-      </c>
+        <v>652</v>
+      </c>
+      <c r="D109" s="42" t="s">
+        <v>604</v>
+      </c>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4"/>
       <c r="G109" s="4"/>
-      <c r="H109" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="I109" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="H109" s="4"/>
+      <c r="I109" s="4"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" s="33">
         <v>109</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>90</v>
+        <v>603</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>96</v>
       </c>
       <c r="D110" s="31" t="s">
-        <v>599</v>
+        <v>831</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G110" s="4"/>
       <c r="H110" s="4" t="s">
-        <v>698</v>
-      </c>
-      <c r="I110" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="I110" s="43" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="50" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" s="33">
         <v>110</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D111" s="31" t="s">
-        <v>600</v>
+        <v>671</v>
+      </c>
+      <c r="C111" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D111" s="41" t="s">
+        <v>671</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>141</v>
+        <v>773</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G111" s="4"/>
       <c r="H111" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" ht="50" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" s="33">
         <v>111</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>603</v>
+        <v>671</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D112" s="41" t="s">
-        <v>603</v>
-      </c>
-      <c r="E112" s="4" t="s">
-        <v>602</v>
-      </c>
-      <c r="F112" s="4" t="s">
-        <v>603</v>
-      </c>
+        <v>652</v>
+      </c>
+      <c r="D112" s="42" t="s">
+        <v>585</v>
+      </c>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
       <c r="G112" s="4"/>
-      <c r="H112" s="4" t="s">
-        <v>601</v>
-      </c>
-      <c r="I112" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="H112" s="4"/>
+      <c r="I112" s="43"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" s="33">
         <v>112</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>603</v>
+        <v>671</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>652</v>
       </c>
       <c r="D113" s="42" t="s">
-        <v>604</v>
+        <v>588</v>
       </c>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
-      <c r="I113" s="4"/>
-    </row>
-    <row r="114" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+      <c r="I113" s="43"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" s="33">
         <v>113</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>603</v>
+        <v>671</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D114" s="31" t="s">
-        <v>846</v>
+      <c r="D114" s="30" t="s">
+        <v>830</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>772</v>
-      </c>
-      <c r="F114" s="4" t="s">
-        <v>118</v>
+        <v>773</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="G114" s="4"/>
       <c r="H114" s="4" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="I114" s="43" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A115" s="33">
         <v>114</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>671</v>
       </c>
-      <c r="C115" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D115" s="41" t="s">
-        <v>671</v>
+      <c r="C115" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D115" s="30" t="s">
+        <v>605</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>111</v>
+        <v>607</v>
       </c>
       <c r="G115" s="4"/>
       <c r="H115" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="I115" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="I115" s="43" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A116" s="33">
         <v>115</v>
       </c>
@@ -6740,118 +6227,110 @@
         <v>671</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D116" s="42" t="s">
-        <v>585</v>
-      </c>
-      <c r="E116" s="4"/>
-      <c r="F116" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="D116" s="30" t="s">
+        <v>606</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>775</v>
+      </c>
+      <c r="F116" s="4" t="s">
+        <v>608</v>
+      </c>
       <c r="G116" s="4"/>
-      <c r="H116" s="4"/>
-      <c r="I116" s="43"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H116" s="4" t="s">
+        <v>725</v>
+      </c>
+      <c r="I116" s="43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A117" s="33">
         <v>116</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>671</v>
+        <v>83</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D117" s="42" t="s">
-        <v>588</v>
-      </c>
-      <c r="E117" s="4"/>
-      <c r="F117" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="D117" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="F117" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="G117" s="4"/>
-      <c r="H117" s="4"/>
-      <c r="I117" s="43"/>
-    </row>
-    <row r="118" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+      <c r="H117" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I117" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" s="33">
         <v>117</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>671</v>
+        <v>83</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D118" s="30" t="s">
-        <v>847</v>
-      </c>
-      <c r="E118" s="4" t="s">
-        <v>773</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>111</v>
-      </c>
+        <v>652</v>
+      </c>
+      <c r="D118" s="42" t="s">
+        <v>558</v>
+      </c>
+      <c r="E118" s="1"/>
+      <c r="F118" s="4"/>
       <c r="G118" s="4"/>
-      <c r="H118" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="I118" s="43" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+      <c r="H118" s="4"/>
+      <c r="I118" s="1"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" s="33">
         <v>118</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>671</v>
+        <v>83</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D119" s="30" t="s">
-        <v>605</v>
-      </c>
-      <c r="E119" s="4" t="s">
-        <v>774</v>
-      </c>
-      <c r="F119" s="4" t="s">
-        <v>607</v>
-      </c>
+        <v>652</v>
+      </c>
+      <c r="D119" s="42" t="s">
+        <v>559</v>
+      </c>
+      <c r="E119" s="1"/>
+      <c r="F119" s="4"/>
       <c r="G119" s="4"/>
-      <c r="H119" s="4" t="s">
-        <v>724</v>
-      </c>
-      <c r="I119" s="43" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+      <c r="H119" s="4"/>
+      <c r="I119" s="1"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" s="33">
         <v>119</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>671</v>
+        <v>83</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D120" s="30" t="s">
-        <v>606</v>
-      </c>
-      <c r="E120" s="4" t="s">
-        <v>775</v>
-      </c>
-      <c r="F120" s="4" t="s">
-        <v>608</v>
-      </c>
+        <v>652</v>
+      </c>
+      <c r="D120" s="42" t="s">
+        <v>565</v>
+      </c>
+      <c r="E120" s="1"/>
+      <c r="F120" s="4"/>
       <c r="G120" s="4"/>
-      <c r="H120" s="4" t="s">
-        <v>725</v>
-      </c>
-      <c r="I120" s="43" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="H120" s="4"/>
+      <c r="I120" s="1"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" s="33">
         <v>120</v>
       </c>
@@ -6859,26 +6338,18 @@
         <v>83</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D121" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>776</v>
-      </c>
-      <c r="F121" s="4" t="s">
-        <v>83</v>
-      </c>
+        <v>652</v>
+      </c>
+      <c r="D121" s="42" t="s">
+        <v>564</v>
+      </c>
+      <c r="E121" s="1"/>
+      <c r="F121" s="4"/>
       <c r="G121" s="4"/>
-      <c r="H121" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I121" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H121" s="4"/>
+      <c r="I121" s="1"/>
+    </row>
+    <row r="122" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A122" s="33">
         <v>121</v>
       </c>
@@ -6886,125 +6357,157 @@
         <v>83</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D122" s="42" t="s">
-        <v>558</v>
-      </c>
-      <c r="E122" s="1"/>
-      <c r="F122" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="D122" s="31" t="s">
+        <v>562</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="F122" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="G122" s="4"/>
-      <c r="H122" s="4"/>
-      <c r="I122" s="1"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H122" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I122" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="75" x14ac:dyDescent="0.35">
       <c r="A123" s="33">
         <v>122</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>83</v>
+        <v>672</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D123" s="42" t="s">
-        <v>559</v>
-      </c>
-      <c r="E123" s="1"/>
-      <c r="F123" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="D123" s="41" t="s">
+        <v>672</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="F123" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="G123" s="4"/>
-      <c r="H123" s="4"/>
-      <c r="I123" s="1"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H123" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="I123" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A124" s="33">
         <v>123</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>83</v>
+        <v>672</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D124" s="42" t="s">
-        <v>565</v>
-      </c>
-      <c r="E124" s="1"/>
-      <c r="F124" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="D124" s="31" t="s">
+        <v>829</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="F124" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="G124" s="4"/>
-      <c r="H124" s="4"/>
-      <c r="I124" s="1"/>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H124" s="4" t="s">
+        <v>647</v>
+      </c>
+      <c r="I124" s="43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="50" x14ac:dyDescent="0.35">
       <c r="A125" s="33">
         <v>124</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>83</v>
+        <v>673</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D125" s="42" t="s">
-        <v>564</v>
-      </c>
-      <c r="E125" s="1"/>
-      <c r="F125" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="D125" s="41" t="s">
+        <v>673</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="F125" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="G125" s="4"/>
-      <c r="H125" s="4"/>
-      <c r="I125" s="1"/>
+      <c r="H125" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="126" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A126" s="33">
         <v>125</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>83</v>
+        <v>673</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>96</v>
       </c>
       <c r="D126" s="31" t="s">
-        <v>562</v>
-      </c>
-      <c r="E126" s="1" t="s">
-        <v>777</v>
+        <v>560</v>
+      </c>
+      <c r="E126" s="4" t="s">
+        <v>780</v>
       </c>
       <c r="F126" s="4" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="G126" s="4"/>
       <c r="H126" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="I126" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="I126" s="43" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="75" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A127" s="33">
         <v>126</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D127" s="41" t="s">
-        <v>672</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>778</v>
+        <v>96</v>
+      </c>
+      <c r="D127" s="31" t="s">
+        <v>828</v>
+      </c>
+      <c r="E127" s="4" t="s">
+        <v>781</v>
       </c>
       <c r="F127" s="4" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="G127" s="4"/>
       <c r="H127" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="I127" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I127" s="43" t="s">
         <v>95</v>
       </c>
     </row>
@@ -7013,77 +6516,77 @@
         <v>127</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D128" s="31" t="s">
-        <v>834</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>778</v>
-      </c>
-      <c r="F128" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G128" s="4"/>
+      <c r="D128" s="46" t="s">
+        <v>561</v>
+      </c>
+      <c r="E128" s="33" t="s">
+        <v>782</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="G128" s="33"/>
       <c r="H128" s="4" t="s">
-        <v>647</v>
+        <v>716</v>
       </c>
       <c r="I128" s="43" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="50" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A129" s="33">
         <v>128</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D129" s="41" t="s">
-        <v>673</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>779</v>
+        <v>676</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>682</v>
       </c>
       <c r="F129" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G129" s="4"/>
+        <v>676</v>
+      </c>
+      <c r="G129" s="35"/>
       <c r="H129" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="I129" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="I129" s="43" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" s="33">
         <v>129</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>96</v>
       </c>
       <c r="D130" s="31" t="s">
-        <v>560</v>
+        <v>677</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="F130" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G130" s="4"/>
+        <v>711</v>
+      </c>
+      <c r="G130" s="35"/>
       <c r="H130" s="4" t="s">
-        <v>515</v>
+        <v>712</v>
       </c>
       <c r="I130" s="43" t="s">
         <v>95</v>
@@ -7094,50 +6597,50 @@
         <v>130</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>96</v>
       </c>
       <c r="D131" s="31" t="s">
-        <v>848</v>
+        <v>678</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
       <c r="F131" s="4" t="s">
-        <v>115</v>
+        <v>710</v>
       </c>
       <c r="G131" s="4"/>
       <c r="H131" s="4" t="s">
-        <v>129</v>
+        <v>713</v>
       </c>
       <c r="I131" s="43" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" s="33">
         <v>131</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D132" s="50" t="s">
-        <v>561</v>
-      </c>
-      <c r="E132" s="33" t="s">
-        <v>782</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="G132" s="33"/>
+      <c r="D132" s="31" t="s">
+        <v>679</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>785</v>
+      </c>
+      <c r="F132" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="G132" s="4"/>
       <c r="H132" s="4" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="I132" s="43" t="s">
         <v>95</v>
@@ -7151,200 +6654,92 @@
         <v>676</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D133" s="41" t="s">
-        <v>676</v>
+        <v>96</v>
+      </c>
+      <c r="D133" s="31" t="s">
+        <v>680</v>
       </c>
       <c r="E133" s="4" t="s">
-        <v>682</v>
+        <v>786</v>
       </c>
       <c r="F133" s="4" t="s">
-        <v>676</v>
+        <v>699</v>
       </c>
       <c r="G133" s="35"/>
       <c r="H133" s="4" t="s">
-        <v>681</v>
+        <v>715</v>
       </c>
       <c r="I133" s="43" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A134" s="33">
         <v>133</v>
       </c>
-      <c r="B134" s="4" t="s">
-        <v>676</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D134" s="31" t="s">
-        <v>677</v>
-      </c>
-      <c r="E134" s="4" t="s">
-        <v>783</v>
-      </c>
-      <c r="F134" s="4" t="s">
-        <v>711</v>
-      </c>
-      <c r="G134" s="35"/>
-      <c r="H134" s="4" t="s">
-        <v>712</v>
-      </c>
-      <c r="I134" s="43" t="s">
+      <c r="B134" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="C134" s="33" t="s">
+        <v>821</v>
+      </c>
+      <c r="D134" s="41" t="s">
+        <v>822</v>
+      </c>
+      <c r="E134" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F134" s="33" t="s">
+        <v>823</v>
+      </c>
+      <c r="G134" s="33"/>
+      <c r="H134" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="I134" s="33" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" s="33">
         <v>134</v>
       </c>
-      <c r="B135" s="4" t="s">
-        <v>676</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D135" s="31" t="s">
-        <v>678</v>
-      </c>
-      <c r="E135" s="4" t="s">
-        <v>784</v>
-      </c>
-      <c r="F135" s="4" t="s">
-        <v>710</v>
-      </c>
-      <c r="G135" s="4"/>
-      <c r="H135" s="4" t="s">
-        <v>713</v>
-      </c>
-      <c r="I135" s="43" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B135" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="C135" s="33" t="s">
+        <v>652</v>
+      </c>
+      <c r="D135" s="53" t="s">
+        <v>825</v>
+      </c>
+      <c r="E135" s="33"/>
+      <c r="F135" s="33"/>
+      <c r="G135" s="33"/>
+      <c r="H135" s="33"/>
+      <c r="I135" s="33"/>
+    </row>
+    <row r="136" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A136" s="33">
         <v>135</v>
       </c>
-      <c r="B136" s="4" t="s">
-        <v>676</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D136" s="31" t="s">
-        <v>679</v>
-      </c>
-      <c r="E136" s="4" t="s">
-        <v>785</v>
-      </c>
-      <c r="F136" s="4" t="s">
-        <v>683</v>
-      </c>
-      <c r="G136" s="4"/>
-      <c r="H136" s="4" t="s">
-        <v>714</v>
-      </c>
-      <c r="I136" s="43" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" ht="25" x14ac:dyDescent="0.35">
-      <c r="A137" s="33">
-        <v>136</v>
-      </c>
-      <c r="B137" s="4" t="s">
-        <v>676</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D137" s="31" t="s">
-        <v>680</v>
-      </c>
-      <c r="E137" s="4" t="s">
-        <v>786</v>
-      </c>
-      <c r="F137" s="4" t="s">
-        <v>699</v>
-      </c>
-      <c r="G137" s="35"/>
-      <c r="H137" s="4" t="s">
-        <v>715</v>
-      </c>
-      <c r="I137" s="43" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" ht="25" x14ac:dyDescent="0.35">
-      <c r="A138" s="33">
-        <v>137</v>
-      </c>
-      <c r="B138" s="51" t="s">
+      <c r="B136" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="C136" s="33" t="s">
+        <v>652</v>
+      </c>
+      <c r="D136" s="53" t="s">
         <v>826</v>
       </c>
-      <c r="C138" s="57" t="s">
-        <v>825</v>
-      </c>
-      <c r="D138" s="58" t="s">
-        <v>826</v>
-      </c>
-      <c r="E138" s="57" t="s">
-        <v>16</v>
-      </c>
-      <c r="F138" s="57" t="s">
-        <v>827</v>
-      </c>
-      <c r="G138" s="57"/>
-      <c r="H138" s="51" t="s">
-        <v>828</v>
-      </c>
-      <c r="I138" s="57" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A139" s="33">
-        <v>138</v>
-      </c>
-      <c r="B139" s="51" t="s">
-        <v>826</v>
-      </c>
-      <c r="C139" s="57" t="s">
-        <v>652</v>
-      </c>
-      <c r="D139" s="60" t="s">
-        <v>829</v>
-      </c>
-      <c r="E139" s="59"/>
-      <c r="F139" s="33"/>
-      <c r="G139" s="33"/>
-      <c r="H139" s="33"/>
-      <c r="I139" s="59"/>
-    </row>
-    <row r="140" spans="1:9" ht="25" x14ac:dyDescent="0.35">
-      <c r="A140" s="33">
-        <v>139</v>
-      </c>
-      <c r="B140" s="51" t="s">
-        <v>826</v>
-      </c>
-      <c r="C140" s="57" t="s">
-        <v>652</v>
-      </c>
-      <c r="D140" s="60" t="s">
-        <v>830</v>
-      </c>
-      <c r="E140" s="59"/>
-      <c r="F140" s="33"/>
-      <c r="G140" s="33"/>
-      <c r="H140" s="33"/>
-      <c r="I140" s="59"/>
+      <c r="E136" s="33"/>
+      <c r="F136" s="33"/>
+      <c r="G136" s="33"/>
+      <c r="H136" s="33"/>
+      <c r="I136" s="33"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I140" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I136" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -7372,14 +6767,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="47" t="s">
         <v>508</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
       <c r="I1" s="6"/>
@@ -7390,16 +6785,16 @@
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="49" t="s">
         <v>507</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
@@ -7408,11 +6803,11 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:14" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="47" t="s">
         <v>509</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
       <c r="D3" s="32"/>
       <c r="E3" s="24"/>
       <c r="F3" s="20"/>
@@ -7436,10 +6831,10 @@
       <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:14" s="7" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="50" t="s">
         <v>158</v>
       </c>
-      <c r="B5" s="65"/>
+      <c r="B5" s="51"/>
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
       <c r="E5" s="25"/>
@@ -9250,7 +8645,7 @@
         <v>522</v>
       </c>
       <c r="H78" s="15" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -9276,7 +8671,7 @@
         <v>523</v>
       </c>
       <c r="H79" s="15" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
@@ -10389,6 +9784,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -10610,15 +10014,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
   <ds:schemaRefs>
@@ -10628,6 +10023,24 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10645,22 +10058,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Final changes implemented from sprint 3
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D21E3F0-FFD9-4509-B24A-8358FB7934D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C152DDEF-C658-45DA-B414-EAD2A519C74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="130" windowWidth="18430" windowHeight="7600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="660" windowWidth="13500" windowHeight="7750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -2649,127 +2649,23 @@
     <t>procedureIsOptional</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>encounterContactMode</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>encounterContactModes</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>studyIdentifier</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>studyIdentifiers</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>studyProtocolVersion</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>studyProtocolVersions</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>studyDesign</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>studyDesigns</t>
-    </r>
+    <t>studyIdentifiers</t>
+  </si>
+  <si>
+    <t>studyProtocolVersions</t>
+  </si>
+  <si>
+    <t>studyDesigns</t>
+  </si>
+  <si>
+    <t>encounterContactModes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2853,13 +2749,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2977,7 +2866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3123,21 +3012,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3152,9 +3026,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3523,7 +3394,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="33">
         <v>2</v>
       </c>
@@ -3534,7 +3405,7 @@
         <v>650</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="4"/>
@@ -3542,7 +3413,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="33">
         <v>3</v>
       </c>
@@ -3553,7 +3424,7 @@
         <v>650</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="4"/>
@@ -3561,7 +3432,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="33">
         <v>4</v>
       </c>
@@ -3572,7 +3443,7 @@
         <v>650</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="4"/>
@@ -5802,7 +5673,7 @@
         <v>96</v>
       </c>
       <c r="D93" s="31" t="s">
-        <v>849</v>
+        <v>852</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>761</v>
@@ -5995,26 +5866,26 @@
       <c r="A101" s="33">
         <v>100</v>
       </c>
-      <c r="B101" s="49" t="s">
+      <c r="B101" s="4" t="s">
         <v>667</v>
       </c>
-      <c r="C101" s="50" t="s">
+      <c r="C101" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D101" s="51" t="s">
+      <c r="D101" s="31" t="s">
         <v>843</v>
       </c>
-      <c r="E101" s="52" t="s">
+      <c r="E101" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F101" s="52" t="s">
+      <c r="F101" s="43" t="s">
         <v>844</v>
       </c>
-      <c r="G101" s="53"/>
-      <c r="H101" s="52" t="s">
+      <c r="G101" s="47"/>
+      <c r="H101" s="43" t="s">
         <v>845</v>
       </c>
-      <c r="I101" s="59" t="s">
+      <c r="I101" s="3" t="s">
         <v>95</v>
       </c>
     </row>
@@ -6211,26 +6082,26 @@
       <c r="A109" s="33">
         <v>108</v>
       </c>
-      <c r="B109" s="49" t="s">
+      <c r="B109" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C109" s="50" t="s">
+      <c r="C109" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D109" s="51" t="s">
+      <c r="D109" s="31" t="s">
         <v>848</v>
       </c>
-      <c r="E109" s="52" t="s">
+      <c r="E109" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F109" s="52" t="s">
+      <c r="F109" s="43" t="s">
         <v>846</v>
       </c>
-      <c r="G109" s="53"/>
-      <c r="H109" s="52" t="s">
+      <c r="G109" s="47"/>
+      <c r="H109" s="43" t="s">
         <v>847</v>
       </c>
-      <c r="I109" s="49" t="s">
+      <c r="I109" s="4" t="s">
         <v>95</v>
       </c>
     </row>
@@ -6958,7 +6829,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
@@ -6974,14 +6845,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="49" t="s">
         <v>508</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
       <c r="I1" s="6"/>
@@ -6992,16 +6863,16 @@
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="51" t="s">
         <v>507</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
@@ -7010,11 +6881,11 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:14" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="49" t="s">
         <v>509</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="32"/>
       <c r="E3" s="24"/>
       <c r="F3" s="20"/>
@@ -7038,10 +6909,10 @@
       <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:14" s="7" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="52" t="s">
         <v>158</v>
       </c>
-      <c r="B5" s="58"/>
+      <c r="B5" s="53"/>
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
       <c r="E5" s="25"/>
@@ -9982,24 +9853,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -10221,10 +10074,40 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10248,21 +10131,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implement sprint 6 changes
prior to sprint 7 update
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7736F939-4CF7-4C10-ADCC-CBD5A32FA39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8393429-7A46-4559-9F2C-CD999EC1CFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="330" windowWidth="18740" windowHeight="9220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="320" windowWidth="19080" windowHeight="9880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
     <sheet name="DDF valid value sets" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DDF Entities&amp;Attributes'!$A$1:$I$161</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DDF Entities&amp;Attributes'!$A$1:$I$157</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DDF valid value sets'!$A$6:$N$124</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1907" uniqueCount="956">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1879" uniqueCount="944">
   <si>
     <t>Preferred Term</t>
   </si>
@@ -2622,24 +2622,6 @@
     <t>interventionDescription</t>
   </si>
   <si>
-    <t>activityIsOptional</t>
-  </si>
-  <si>
-    <t>Study Activity is Optional</t>
-  </si>
-  <si>
-    <t>An indication as to whether the study activity is available to be performed but is not obligatory.</t>
-  </si>
-  <si>
-    <t>Study Procedure is Optional</t>
-  </si>
-  <si>
-    <t>An indication as to whether the study procedure is available to be performed but is not obligatory.</t>
-  </si>
-  <si>
-    <t>procedureIsOptional</t>
-  </si>
-  <si>
     <t>studyIdentifiers</t>
   </si>
   <si>
@@ -2652,24 +2634,6 @@
     <t>encounterContactModes</t>
   </si>
   <si>
-    <t>activityIsOptionalReason</t>
-  </si>
-  <si>
-    <t>Study Activity is Optional Reason</t>
-  </si>
-  <si>
-    <t>The explanation for why the study activity is available to be performed but is not obligatory.</t>
-  </si>
-  <si>
-    <t>procedureIsOptionalReason</t>
-  </si>
-  <si>
-    <t>Study Procedure is Optional Reason</t>
-  </si>
-  <si>
-    <t>The explanation for why the study procedure is available to be performed but is not obligatory.</t>
-  </si>
-  <si>
     <t>studyAcronym</t>
   </si>
   <si>
@@ -2859,9 +2823,6 @@
     <t>An individual, company, institution, or organization that takes responsibility for the initiation, management, and/or financing of a clinical study. [After ICH E6, WHO, 21 CFR 50.3 (e), and after IDMP]</t>
   </si>
   <si>
-    <t>Y - ISO 3166-1 Alpha-3 Country code</t>
-  </si>
-  <si>
     <t>studyDesignBlindingScheme</t>
   </si>
   <si>
@@ -2877,9 +2838,6 @@
     <t>The type of experimental design used to describe the level of awareness of the study subjects and/ or study personnel as it relates to the respective intervention(s) or assessments being observed, received or administered.</t>
   </si>
   <si>
-    <t>Y - C66735</t>
-  </si>
-  <si>
     <t>C15228</t>
   </si>
   <si>
@@ -2968,13 +2926,19 @@
   </si>
   <si>
     <t>procedureIsConditionalReason</t>
+  </si>
+  <si>
+    <t>Y (C66735)</t>
+  </si>
+  <si>
+    <t>Y (Point out to ISO 3166-1 Alpha-3 Country code)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3067,20 +3031,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -3208,7 +3158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3389,42 +3339,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3717,7 +3631,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I161"/>
+  <dimension ref="A1:I157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3804,7 +3718,7 @@
         <v>648</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>846</v>
+        <v>840</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="4"/>
@@ -3823,7 +3737,7 @@
         <v>648</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="4"/>
@@ -3842,7 +3756,7 @@
         <v>648</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>848</v>
+        <v>842</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="4"/>
@@ -4002,17 +3916,17 @@
         <v>94</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>856</v>
+        <v>844</v>
       </c>
       <c r="E11" s="54" t="s">
-        <v>858</v>
+        <v>846</v>
       </c>
       <c r="F11" s="43" t="s">
-        <v>859</v>
+        <v>847</v>
       </c>
       <c r="G11" s="43"/>
       <c r="H11" s="43" t="s">
-        <v>860</v>
+        <v>848</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>93</v>
@@ -4029,17 +3943,17 @@
         <v>94</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>857</v>
+        <v>845</v>
       </c>
       <c r="E12" s="54" t="s">
-        <v>861</v>
+        <v>849</v>
       </c>
       <c r="F12" s="43" t="s">
-        <v>862</v>
+        <v>850</v>
       </c>
       <c r="G12" s="43"/>
       <c r="H12" s="43" t="s">
-        <v>863</v>
+        <v>851</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>93</v>
@@ -4401,7 +4315,7 @@
         <v>648</v>
       </c>
       <c r="D26" s="42" t="s">
-        <v>864</v>
+        <v>852</v>
       </c>
       <c r="E26" s="49"/>
       <c r="F26" s="49"/>
@@ -4894,17 +4808,17 @@
         <v>94</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>897</v>
+        <v>885</v>
       </c>
       <c r="E47" s="54" t="s">
-        <v>894</v>
+        <v>882</v>
       </c>
       <c r="F47" s="43" t="s">
-        <v>895</v>
+        <v>883</v>
       </c>
       <c r="G47" s="43"/>
       <c r="H47" s="43" t="s">
-        <v>896</v>
+        <v>884</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>93</v>
@@ -4914,29 +4828,29 @@
       <c r="A48" s="33">
         <v>47</v>
       </c>
-      <c r="B48" s="49" t="s">
+      <c r="B48" s="4" t="s">
         <v>653</v>
       </c>
-      <c r="C48" s="50" t="s">
+      <c r="C48" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D48" s="67" t="s">
-        <v>920</v>
-      </c>
-      <c r="E48" s="68" t="s">
-        <v>921</v>
-      </c>
-      <c r="F48" s="68" t="s">
-        <v>922</v>
-      </c>
-      <c r="G48" s="68" t="s">
-        <v>923</v>
-      </c>
-      <c r="H48" s="68" t="s">
-        <v>924</v>
-      </c>
-      <c r="I48" s="68" t="s">
-        <v>925</v>
+      <c r="D48" s="31" t="s">
+        <v>907</v>
+      </c>
+      <c r="E48" s="43" t="s">
+        <v>908</v>
+      </c>
+      <c r="F48" s="43" t="s">
+        <v>909</v>
+      </c>
+      <c r="G48" s="43" t="s">
+        <v>910</v>
+      </c>
+      <c r="H48" s="43" t="s">
+        <v>911</v>
+      </c>
+      <c r="I48" s="43" t="s">
+        <v>942</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="75" x14ac:dyDescent="0.35">
@@ -4960,7 +4874,7 @@
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="43" t="s">
-        <v>916</v>
+        <v>904</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>93</v>
@@ -5166,17 +5080,17 @@
         <v>94</v>
       </c>
       <c r="D57" s="30" t="s">
-        <v>898</v>
+        <v>886</v>
       </c>
       <c r="E57" s="54" t="s">
-        <v>902</v>
+        <v>890</v>
       </c>
       <c r="F57" s="43" t="s">
-        <v>903</v>
+        <v>891</v>
       </c>
       <c r="G57" s="43"/>
       <c r="H57" s="43" t="s">
-        <v>904</v>
+        <v>892</v>
       </c>
       <c r="I57" s="43" t="s">
         <v>93</v>
@@ -5193,17 +5107,17 @@
         <v>94</v>
       </c>
       <c r="D58" s="30" t="s">
-        <v>899</v>
+        <v>887</v>
       </c>
       <c r="E58" s="54" t="s">
-        <v>905</v>
+        <v>893</v>
       </c>
       <c r="F58" s="43" t="s">
-        <v>906</v>
+        <v>894</v>
       </c>
       <c r="G58" s="43"/>
       <c r="H58" s="43" t="s">
-        <v>907</v>
+        <v>895</v>
       </c>
       <c r="I58" s="43" t="s">
         <v>93</v>
@@ -5220,17 +5134,17 @@
         <v>94</v>
       </c>
       <c r="D59" s="30" t="s">
-        <v>900</v>
+        <v>888</v>
       </c>
       <c r="E59" s="54" t="s">
-        <v>908</v>
+        <v>896</v>
       </c>
       <c r="F59" s="43" t="s">
-        <v>909</v>
+        <v>897</v>
       </c>
       <c r="G59" s="43"/>
       <c r="H59" s="43" t="s">
-        <v>910</v>
+        <v>898</v>
       </c>
       <c r="I59" s="43" t="s">
         <v>93</v>
@@ -5247,20 +5161,20 @@
         <v>94</v>
       </c>
       <c r="D60" s="30" t="s">
-        <v>901</v>
+        <v>889</v>
       </c>
       <c r="E60" s="54" t="s">
-        <v>911</v>
+        <v>899</v>
       </c>
       <c r="F60" s="43" t="s">
-        <v>912</v>
+        <v>900</v>
       </c>
       <c r="G60" s="43"/>
       <c r="H60" s="43" t="s">
-        <v>913</v>
+        <v>901</v>
       </c>
       <c r="I60" s="43" t="s">
-        <v>914</v>
+        <v>902</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
@@ -5384,7 +5298,7 @@
       </c>
       <c r="G65" s="4"/>
       <c r="H65" s="43" t="s">
-        <v>917</v>
+        <v>905</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>93</v>
@@ -6309,7 +6223,7 @@
         <v>94</v>
       </c>
       <c r="D102" s="31" t="s">
-        <v>849</v>
+        <v>843</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>758</v>
@@ -6502,26 +6416,26 @@
       <c r="A110" s="33">
         <v>109</v>
       </c>
-      <c r="B110" s="61" t="s">
+      <c r="B110" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="C110" s="62" t="s">
+      <c r="C110" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D110" s="63" t="s">
-        <v>840</v>
-      </c>
-      <c r="E110" s="64" t="s">
+      <c r="D110" s="31" t="s">
+        <v>933</v>
+      </c>
+      <c r="E110" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F110" s="64" t="s">
-        <v>841</v>
-      </c>
-      <c r="G110" s="65"/>
-      <c r="H110" s="64" t="s">
-        <v>842</v>
-      </c>
-      <c r="I110" s="66" t="s">
+      <c r="F110" s="43" t="s">
+        <v>930</v>
+      </c>
+      <c r="G110" s="47"/>
+      <c r="H110" s="43" t="s">
+        <v>931</v>
+      </c>
+      <c r="I110" s="43" t="s">
         <v>93</v>
       </c>
     </row>
@@ -6529,53 +6443,53 @@
       <c r="A111" s="33">
         <v>110</v>
       </c>
-      <c r="B111" s="61" t="s">
+      <c r="B111" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="C111" s="62" t="s">
+      <c r="C111" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D111" s="63" t="s">
-        <v>850</v>
-      </c>
-      <c r="E111" s="64" t="s">
+      <c r="D111" s="31" t="s">
+        <v>934</v>
+      </c>
+      <c r="E111" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F111" s="64" t="s">
-        <v>851</v>
-      </c>
-      <c r="G111" s="65"/>
-      <c r="H111" s="64" t="s">
-        <v>852</v>
-      </c>
-      <c r="I111" s="66" t="s">
+      <c r="F111" s="43" t="s">
+        <v>932</v>
+      </c>
+      <c r="G111" s="47"/>
+      <c r="H111" s="43" t="s">
+        <v>935</v>
+      </c>
+      <c r="I111" s="43" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" s="33">
         <v>111</v>
       </c>
-      <c r="B112" s="49" t="s">
-        <v>665</v>
-      </c>
-      <c r="C112" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="D112" s="67" t="s">
-        <v>947</v>
-      </c>
-      <c r="E112" s="68" t="s">
-        <v>16</v>
-      </c>
-      <c r="F112" s="68" t="s">
-        <v>944</v>
-      </c>
-      <c r="G112" s="72"/>
-      <c r="H112" s="68" t="s">
-        <v>945</v>
-      </c>
-      <c r="I112" s="68" t="s">
+      <c r="B112" s="4" t="s">
+        <v>666</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D112" s="41" t="s">
+        <v>666</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="F112" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G112" s="4"/>
+      <c r="H112" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I112" s="1" t="s">
         <v>93</v>
       </c>
     </row>
@@ -6583,30 +6497,30 @@
       <c r="A113" s="33">
         <v>112</v>
       </c>
-      <c r="B113" s="49" t="s">
-        <v>665</v>
-      </c>
-      <c r="C113" s="50" t="s">
+      <c r="B113" s="4" t="s">
+        <v>666</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D113" s="67" t="s">
-        <v>948</v>
-      </c>
-      <c r="E113" s="68" t="s">
-        <v>16</v>
-      </c>
-      <c r="F113" s="68" t="s">
-        <v>946</v>
-      </c>
-      <c r="G113" s="72"/>
-      <c r="H113" s="68" t="s">
-        <v>949</v>
-      </c>
-      <c r="I113" s="68" t="s">
+      <c r="D113" s="31" t="s">
+        <v>594</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>763</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G113" s="4"/>
+      <c r="H113" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="I113" s="43" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A114" s="33">
         <v>113</v>
       </c>
@@ -6614,22 +6528,22 @@
         <v>666</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D114" s="41" t="s">
-        <v>666</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>762</v>
+        <v>94</v>
+      </c>
+      <c r="D114" s="31" t="s">
+        <v>827</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>764</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>74</v>
+        <v>151</v>
       </c>
       <c r="G114" s="4"/>
-      <c r="H114" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I114" s="1" t="s">
+      <c r="H114" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="I114" s="43" t="s">
         <v>93</v>
       </c>
     </row>
@@ -6644,77 +6558,77 @@
         <v>94</v>
       </c>
       <c r="D115" s="31" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>150</v>
+        <v>645</v>
       </c>
       <c r="G115" s="4"/>
       <c r="H115" s="4" t="s">
-        <v>514</v>
+        <v>713</v>
       </c>
       <c r="I115" s="43" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A116" s="33">
         <v>115</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>666</v>
+        <v>88</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D116" s="31" t="s">
-        <v>827</v>
-      </c>
-      <c r="E116" s="4" t="s">
-        <v>764</v>
+        <v>4</v>
+      </c>
+      <c r="D116" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>151</v>
+        <v>88</v>
       </c>
       <c r="G116" s="4"/>
       <c r="H116" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="I116" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="I116" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" s="33">
         <v>116</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>666</v>
+        <v>88</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D117" s="31" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>645</v>
+        <v>117</v>
       </c>
       <c r="G117" s="4"/>
       <c r="H117" s="4" t="s">
-        <v>713</v>
-      </c>
-      <c r="I117" s="43" t="s">
+        <v>694</v>
+      </c>
+      <c r="I117" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" ht="50" x14ac:dyDescent="0.35">
       <c r="A118" s="33">
         <v>117</v>
       </c>
@@ -6722,26 +6636,26 @@
         <v>88</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D118" s="41" t="s">
-        <v>88</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>77</v>
+        <v>94</v>
+      </c>
+      <c r="D118" s="31" t="s">
+        <v>598</v>
+      </c>
+      <c r="E118" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="G118" s="4"/>
       <c r="H118" s="4" t="s">
-        <v>76</v>
+        <v>140</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A119" s="33">
         <v>118</v>
       </c>
@@ -6752,23 +6666,23 @@
         <v>94</v>
       </c>
       <c r="D119" s="31" t="s">
-        <v>597</v>
-      </c>
-      <c r="E119" s="4" t="s">
-        <v>766</v>
-      </c>
-      <c r="F119" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G119" s="4"/>
-      <c r="H119" s="4" t="s">
-        <v>694</v>
-      </c>
-      <c r="I119" s="4" t="s">
+        <v>940</v>
+      </c>
+      <c r="E119" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="F119" s="43" t="s">
+        <v>936</v>
+      </c>
+      <c r="G119" s="47"/>
+      <c r="H119" s="43" t="s">
+        <v>938</v>
+      </c>
+      <c r="I119" s="43" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="50" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A120" s="33">
         <v>119</v>
       </c>
@@ -6779,231 +6693,215 @@
         <v>94</v>
       </c>
       <c r="D120" s="31" t="s">
-        <v>598</v>
-      </c>
-      <c r="E120" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="F120" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G120" s="4"/>
-      <c r="H120" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="I120" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+        <v>941</v>
+      </c>
+      <c r="E120" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="F120" s="43" t="s">
+        <v>937</v>
+      </c>
+      <c r="G120" s="47"/>
+      <c r="H120" s="43" t="s">
+        <v>939</v>
+      </c>
+      <c r="I120" s="43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="50" x14ac:dyDescent="0.35">
       <c r="A121" s="33">
         <v>120</v>
       </c>
-      <c r="B121" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="C121" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="D121" s="63" t="s">
-        <v>845</v>
-      </c>
-      <c r="E121" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="F121" s="64" t="s">
-        <v>843</v>
-      </c>
-      <c r="G121" s="65"/>
-      <c r="H121" s="64" t="s">
-        <v>844</v>
-      </c>
-      <c r="I121" s="61" t="s">
+      <c r="B121" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D121" s="41" t="s">
+        <v>601</v>
+      </c>
+      <c r="E121" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="F121" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="G121" s="4"/>
+      <c r="H121" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="I121" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" s="33">
         <v>121</v>
       </c>
-      <c r="B122" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="C122" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="D122" s="63" t="s">
-        <v>853</v>
-      </c>
-      <c r="E122" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="F122" s="64" t="s">
-        <v>854</v>
-      </c>
-      <c r="G122" s="65"/>
-      <c r="H122" s="64" t="s">
-        <v>855</v>
-      </c>
-      <c r="I122" s="61" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+      <c r="B122" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="D122" s="42" t="s">
+        <v>602</v>
+      </c>
+      <c r="E122" s="4"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
+      <c r="H122" s="4"/>
+      <c r="I122" s="4"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" s="33">
         <v>122</v>
       </c>
-      <c r="B123" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="C123" s="50" t="s">
+      <c r="B123" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D123" s="67" t="s">
-        <v>954</v>
-      </c>
-      <c r="E123" s="68" t="s">
-        <v>16</v>
-      </c>
-      <c r="F123" s="68" t="s">
-        <v>950</v>
-      </c>
-      <c r="G123" s="72"/>
-      <c r="H123" s="68" t="s">
-        <v>952</v>
-      </c>
-      <c r="I123" s="68" t="s">
+      <c r="D123" s="31" t="s">
+        <v>826</v>
+      </c>
+      <c r="E123" s="4" t="s">
+        <v>767</v>
+      </c>
+      <c r="F123" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G123" s="4"/>
+      <c r="H123" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="I123" s="43" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" s="33">
         <v>123</v>
       </c>
-      <c r="B124" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="C124" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="D124" s="67" t="s">
-        <v>955</v>
-      </c>
-      <c r="E124" s="68" t="s">
-        <v>16</v>
-      </c>
-      <c r="F124" s="68" t="s">
-        <v>951</v>
-      </c>
-      <c r="G124" s="72"/>
-      <c r="H124" s="68" t="s">
-        <v>953</v>
-      </c>
-      <c r="I124" s="68" t="s">
+      <c r="B124" s="4" t="s">
+        <v>667</v>
+      </c>
+      <c r="C124" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D124" s="41" t="s">
+        <v>667</v>
+      </c>
+      <c r="E124" s="4" t="s">
+        <v>768</v>
+      </c>
+      <c r="F124" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G124" s="4"/>
+      <c r="H124" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="I124" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="50" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" s="33">
         <v>124</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>601</v>
+        <v>667</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D125" s="41" t="s">
-        <v>601</v>
-      </c>
-      <c r="E125" s="4" t="s">
-        <v>600</v>
-      </c>
-      <c r="F125" s="4" t="s">
-        <v>601</v>
-      </c>
+        <v>648</v>
+      </c>
+      <c r="D125" s="42" t="s">
+        <v>583</v>
+      </c>
+      <c r="E125" s="4"/>
+      <c r="F125" s="4"/>
       <c r="G125" s="4"/>
-      <c r="H125" s="4" t="s">
-        <v>599</v>
-      </c>
-      <c r="I125" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="H125" s="4"/>
+      <c r="I125" s="43"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" s="33">
         <v>125</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>601</v>
+        <v>667</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>648</v>
       </c>
       <c r="D126" s="42" t="s">
-        <v>602</v>
+        <v>586</v>
       </c>
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
       <c r="G126" s="4"/>
       <c r="H126" s="4"/>
-      <c r="I126" s="4"/>
+      <c r="I126" s="43"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" s="33">
         <v>126</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>601</v>
+        <v>667</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D127" s="31" t="s">
-        <v>826</v>
+      <c r="D127" s="30" t="s">
+        <v>825</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>767</v>
-      </c>
-      <c r="F127" s="4" t="s">
-        <v>116</v>
+        <v>768</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="G127" s="4"/>
       <c r="H127" s="4" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="I127" s="43" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A128" s="33">
         <v>127</v>
       </c>
       <c r="B128" s="4" t="s">
         <v>667</v>
       </c>
-      <c r="C128" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D128" s="41" t="s">
-        <v>667</v>
+      <c r="C128" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D128" s="30" t="s">
+        <v>603</v>
       </c>
       <c r="E128" s="4" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="F128" s="4" t="s">
-        <v>109</v>
+        <v>605</v>
       </c>
       <c r="G128" s="4"/>
       <c r="H128" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="I128" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="I128" s="43" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A129" s="33">
         <v>128</v>
       </c>
@@ -7011,118 +6909,110 @@
         <v>667</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="D129" s="42" t="s">
-        <v>583</v>
-      </c>
-      <c r="E129" s="4"/>
-      <c r="F129" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="D129" s="30" t="s">
+        <v>604</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>770</v>
+      </c>
+      <c r="F129" s="4" t="s">
+        <v>606</v>
+      </c>
       <c r="G129" s="4"/>
-      <c r="H129" s="4"/>
-      <c r="I129" s="43"/>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H129" s="4" t="s">
+        <v>721</v>
+      </c>
+      <c r="I129" s="43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A130" s="33">
         <v>129</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>667</v>
+        <v>81</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="D130" s="42" t="s">
-        <v>586</v>
-      </c>
-      <c r="E130" s="4"/>
-      <c r="F130" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="D130" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="F130" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="G130" s="4"/>
-      <c r="H130" s="4"/>
-      <c r="I130" s="43"/>
+      <c r="H130" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I130" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" s="33">
         <v>130</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>667</v>
+        <v>81</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D131" s="30" t="s">
-        <v>825</v>
-      </c>
-      <c r="E131" s="4" t="s">
-        <v>768</v>
-      </c>
-      <c r="F131" s="1" t="s">
-        <v>109</v>
-      </c>
+        <v>648</v>
+      </c>
+      <c r="D131" s="42" t="s">
+        <v>556</v>
+      </c>
+      <c r="E131" s="1"/>
+      <c r="F131" s="4"/>
       <c r="G131" s="4"/>
-      <c r="H131" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="I131" s="43" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+      <c r="H131" s="4"/>
+      <c r="I131" s="1"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" s="33">
         <v>131</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>667</v>
+        <v>81</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D132" s="30" t="s">
-        <v>603</v>
-      </c>
-      <c r="E132" s="4" t="s">
-        <v>769</v>
-      </c>
-      <c r="F132" s="4" t="s">
-        <v>605</v>
-      </c>
+        <v>648</v>
+      </c>
+      <c r="D132" s="42" t="s">
+        <v>557</v>
+      </c>
+      <c r="E132" s="1"/>
+      <c r="F132" s="4"/>
       <c r="G132" s="4"/>
-      <c r="H132" s="4" t="s">
-        <v>720</v>
-      </c>
-      <c r="I132" s="43" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+      <c r="H132" s="4"/>
+      <c r="I132" s="1"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" s="33">
         <v>132</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>667</v>
+        <v>81</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D133" s="30" t="s">
-        <v>604</v>
-      </c>
-      <c r="E133" s="4" t="s">
-        <v>770</v>
-      </c>
-      <c r="F133" s="4" t="s">
-        <v>606</v>
-      </c>
+        <v>648</v>
+      </c>
+      <c r="D133" s="42" t="s">
+        <v>563</v>
+      </c>
+      <c r="E133" s="1"/>
+      <c r="F133" s="4"/>
       <c r="G133" s="4"/>
-      <c r="H133" s="4" t="s">
-        <v>721</v>
-      </c>
-      <c r="I133" s="43" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="H133" s="4"/>
+      <c r="I133" s="1"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" s="33">
         <v>133</v>
       </c>
@@ -7130,26 +7020,18 @@
         <v>81</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D134" s="41" t="s">
-        <v>81</v>
-      </c>
-      <c r="E134" s="1" t="s">
-        <v>771</v>
-      </c>
-      <c r="F134" s="4" t="s">
-        <v>81</v>
-      </c>
+        <v>648</v>
+      </c>
+      <c r="D134" s="42" t="s">
+        <v>562</v>
+      </c>
+      <c r="E134" s="1"/>
+      <c r="F134" s="4"/>
       <c r="G134" s="4"/>
-      <c r="H134" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I134" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H134" s="4"/>
+      <c r="I134" s="1"/>
+    </row>
+    <row r="135" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A135" s="33">
         <v>134</v>
       </c>
@@ -7157,125 +7039,157 @@
         <v>81</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="D135" s="42" t="s">
-        <v>556</v>
-      </c>
-      <c r="E135" s="1"/>
-      <c r="F135" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="D135" s="31" t="s">
+        <v>560</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="F135" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="G135" s="4"/>
-      <c r="H135" s="4"/>
-      <c r="I135" s="1"/>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H135" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I135" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="75" x14ac:dyDescent="0.35">
       <c r="A136" s="33">
         <v>135</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>81</v>
+        <v>668</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="D136" s="42" t="s">
-        <v>557</v>
-      </c>
-      <c r="E136" s="1"/>
-      <c r="F136" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="D136" s="41" t="s">
+        <v>668</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="F136" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="G136" s="4"/>
-      <c r="H136" s="4"/>
-      <c r="I136" s="1"/>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H136" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="I136" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A137" s="33">
         <v>136</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>81</v>
+        <v>668</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="D137" s="42" t="s">
-        <v>563</v>
-      </c>
-      <c r="E137" s="1"/>
-      <c r="F137" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="D137" s="31" t="s">
+        <v>824</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="F137" s="4" t="s">
+        <v>146</v>
+      </c>
       <c r="G137" s="4"/>
-      <c r="H137" s="4"/>
-      <c r="I137" s="1"/>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H137" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="I137" s="43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" ht="50" x14ac:dyDescent="0.35">
       <c r="A138" s="33">
         <v>137</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>81</v>
+        <v>669</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="D138" s="42" t="s">
-        <v>562</v>
-      </c>
-      <c r="E138" s="1"/>
-      <c r="F138" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="D138" s="41" t="s">
+        <v>669</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="F138" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="G138" s="4"/>
-      <c r="H138" s="4"/>
-      <c r="I138" s="1"/>
+      <c r="H138" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I138" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="139" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A139" s="33">
         <v>138</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>81</v>
+        <v>669</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D139" s="31" t="s">
-        <v>560</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>772</v>
+        <v>558</v>
+      </c>
+      <c r="E139" s="4" t="s">
+        <v>775</v>
       </c>
       <c r="F139" s="4" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="G139" s="4"/>
       <c r="H139" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I139" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="I139" s="43" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="75" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A140" s="33">
         <v>139</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D140" s="41" t="s">
-        <v>668</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>773</v>
+        <v>94</v>
+      </c>
+      <c r="D140" s="31" t="s">
+        <v>823</v>
+      </c>
+      <c r="E140" s="4" t="s">
+        <v>776</v>
       </c>
       <c r="F140" s="4" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="G140" s="4"/>
       <c r="H140" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="I140" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I140" s="43" t="s">
         <v>93</v>
       </c>
     </row>
@@ -7284,77 +7198,77 @@
         <v>140</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D141" s="31" t="s">
-        <v>824</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>773</v>
-      </c>
-      <c r="F141" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="G141" s="4"/>
+      <c r="D141" s="46" t="s">
+        <v>559</v>
+      </c>
+      <c r="E141" s="33" t="s">
+        <v>777</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="G141" s="33"/>
       <c r="H141" s="4" t="s">
-        <v>643</v>
+        <v>712</v>
       </c>
       <c r="I141" s="43" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="50" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A142" s="33">
         <v>141</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D142" s="41" t="s">
-        <v>669</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>774</v>
+        <v>672</v>
+      </c>
+      <c r="E142" s="4" t="s">
+        <v>678</v>
       </c>
       <c r="F142" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G142" s="4"/>
+        <v>672</v>
+      </c>
+      <c r="G142" s="35"/>
       <c r="H142" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="I142" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="I142" s="43" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143" s="33">
         <v>142</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D143" s="31" t="s">
-        <v>558</v>
+        <v>673</v>
       </c>
       <c r="E143" s="4" t="s">
-        <v>775</v>
+        <v>778</v>
       </c>
       <c r="F143" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G143" s="4"/>
+        <v>707</v>
+      </c>
+      <c r="G143" s="35"/>
       <c r="H143" s="4" t="s">
-        <v>513</v>
+        <v>708</v>
       </c>
       <c r="I143" s="43" t="s">
         <v>93</v>
@@ -7365,50 +7279,50 @@
         <v>143</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D144" s="31" t="s">
-        <v>823</v>
+        <v>674</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>776</v>
+        <v>779</v>
       </c>
       <c r="F144" s="4" t="s">
-        <v>113</v>
+        <v>706</v>
       </c>
       <c r="G144" s="4"/>
       <c r="H144" s="4" t="s">
-        <v>127</v>
+        <v>709</v>
       </c>
       <c r="I144" s="43" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="145" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145" s="33">
         <v>144</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D145" s="46" t="s">
-        <v>559</v>
-      </c>
-      <c r="E145" s="33" t="s">
-        <v>777</v>
-      </c>
-      <c r="F145" s="1" t="s">
-        <v>578</v>
-      </c>
-      <c r="G145" s="33"/>
+      <c r="D145" s="31" t="s">
+        <v>675</v>
+      </c>
+      <c r="E145" s="4" t="s">
+        <v>780</v>
+      </c>
+      <c r="F145" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="G145" s="4"/>
       <c r="H145" s="4" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="I145" s="43" t="s">
         <v>93</v>
@@ -7422,271 +7336,271 @@
         <v>672</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D146" s="41" t="s">
-        <v>672</v>
+        <v>94</v>
+      </c>
+      <c r="D146" s="31" t="s">
+        <v>676</v>
       </c>
       <c r="E146" s="4" t="s">
-        <v>678</v>
+        <v>781</v>
       </c>
       <c r="F146" s="4" t="s">
-        <v>672</v>
+        <v>695</v>
       </c>
       <c r="G146" s="35"/>
       <c r="H146" s="4" t="s">
-        <v>677</v>
+        <v>711</v>
       </c>
       <c r="I146" s="43" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A147" s="33">
         <v>146</v>
       </c>
-      <c r="B147" s="4" t="s">
-        <v>672</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D147" s="31" t="s">
-        <v>673</v>
-      </c>
-      <c r="E147" s="4" t="s">
-        <v>778</v>
-      </c>
-      <c r="F147" s="4" t="s">
-        <v>707</v>
-      </c>
-      <c r="G147" s="35"/>
-      <c r="H147" s="4" t="s">
-        <v>708</v>
-      </c>
-      <c r="I147" s="43" t="s">
+      <c r="B147" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="C147" s="33" t="s">
+        <v>816</v>
+      </c>
+      <c r="D147" s="41" t="s">
+        <v>817</v>
+      </c>
+      <c r="E147" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F147" s="33" t="s">
+        <v>818</v>
+      </c>
+      <c r="G147" s="33"/>
+      <c r="H147" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="I147" s="33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="148" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A148" s="33">
         <v>147</v>
       </c>
-      <c r="B148" s="4" t="s">
-        <v>672</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D148" s="31" t="s">
-        <v>674</v>
-      </c>
-      <c r="E148" s="4" t="s">
-        <v>779</v>
-      </c>
-      <c r="F148" s="4" t="s">
-        <v>706</v>
-      </c>
-      <c r="G148" s="4"/>
-      <c r="H148" s="4" t="s">
-        <v>709</v>
-      </c>
-      <c r="I148" s="43" t="s">
+      <c r="B148" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="C148" s="33" t="s">
+        <v>648</v>
+      </c>
+      <c r="D148" s="48" t="s">
+        <v>820</v>
+      </c>
+      <c r="E148" s="33"/>
+      <c r="F148" s="33"/>
+      <c r="G148" s="33"/>
+      <c r="H148" s="33"/>
+      <c r="I148" s="33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A149" s="33">
         <v>148</v>
       </c>
-      <c r="B149" s="4" t="s">
-        <v>672</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D149" s="31" t="s">
-        <v>675</v>
-      </c>
-      <c r="E149" s="4" t="s">
-        <v>780</v>
-      </c>
-      <c r="F149" s="4" t="s">
-        <v>679</v>
-      </c>
-      <c r="G149" s="4"/>
-      <c r="H149" s="4" t="s">
-        <v>710</v>
-      </c>
-      <c r="I149" s="43" t="s">
+      <c r="B149" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="C149" s="33" t="s">
+        <v>648</v>
+      </c>
+      <c r="D149" s="48" t="s">
+        <v>821</v>
+      </c>
+      <c r="E149" s="33"/>
+      <c r="F149" s="33"/>
+      <c r="G149" s="33"/>
+      <c r="H149" s="33"/>
+      <c r="I149" s="33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:9" s="51" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A150" s="33">
         <v>149</v>
       </c>
-      <c r="B150" s="4" t="s">
-        <v>672</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D150" s="31" t="s">
-        <v>676</v>
-      </c>
-      <c r="E150" s="4" t="s">
-        <v>781</v>
-      </c>
-      <c r="F150" s="4" t="s">
-        <v>695</v>
-      </c>
-      <c r="G150" s="35"/>
-      <c r="H150" s="4" t="s">
-        <v>711</v>
-      </c>
-      <c r="I150" s="43" t="s">
+      <c r="B150" s="33" t="s">
+        <v>853</v>
+      </c>
+      <c r="C150" s="55" t="s">
+        <v>816</v>
+      </c>
+      <c r="D150" s="41" t="s">
+        <v>817</v>
+      </c>
+      <c r="E150" s="54" t="s">
+        <v>880</v>
+      </c>
+      <c r="F150" s="43" t="s">
+        <v>853</v>
+      </c>
+      <c r="G150" s="47"/>
+      <c r="H150" s="43" t="s">
+        <v>881</v>
+      </c>
+      <c r="I150" s="33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="151" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:9" s="51" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A151" s="33">
         <v>150</v>
       </c>
-      <c r="B151" s="1" t="s">
-        <v>817</v>
-      </c>
-      <c r="C151" s="33" t="s">
-        <v>816</v>
-      </c>
-      <c r="D151" s="41" t="s">
-        <v>817</v>
-      </c>
-      <c r="E151" s="33" t="s">
+      <c r="B151" s="33" t="s">
+        <v>853</v>
+      </c>
+      <c r="C151" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="D151" s="30" t="s">
+        <v>854</v>
+      </c>
+      <c r="E151" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="F151" s="33" t="s">
-        <v>818</v>
-      </c>
-      <c r="G151" s="33"/>
-      <c r="H151" s="1" t="s">
-        <v>819</v>
+      <c r="F151" s="43" t="s">
+        <v>861</v>
+      </c>
+      <c r="G151" s="47"/>
+      <c r="H151" s="43" t="s">
+        <v>862</v>
       </c>
       <c r="I151" s="33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9" s="51" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A152" s="33">
         <v>151</v>
       </c>
-      <c r="B152" s="1" t="s">
-        <v>817</v>
-      </c>
-      <c r="C152" s="33" t="s">
-        <v>648</v>
-      </c>
-      <c r="D152" s="48" t="s">
-        <v>820</v>
-      </c>
-      <c r="E152" s="33"/>
-      <c r="F152" s="33"/>
-      <c r="G152" s="33"/>
-      <c r="H152" s="33"/>
+      <c r="B152" s="33" t="s">
+        <v>853</v>
+      </c>
+      <c r="C152" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="D152" s="30" t="s">
+        <v>855</v>
+      </c>
+      <c r="E152" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="F152" s="43" t="s">
+        <v>863</v>
+      </c>
+      <c r="G152" s="47"/>
+      <c r="H152" s="43" t="s">
+        <v>864</v>
+      </c>
       <c r="I152" s="33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="153" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:9" s="51" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A153" s="33">
         <v>152</v>
       </c>
-      <c r="B153" s="1" t="s">
-        <v>817</v>
-      </c>
-      <c r="C153" s="33" t="s">
-        <v>648</v>
-      </c>
-      <c r="D153" s="48" t="s">
-        <v>821</v>
-      </c>
-      <c r="E153" s="33"/>
-      <c r="F153" s="33"/>
-      <c r="G153" s="33"/>
-      <c r="H153" s="33"/>
+      <c r="B153" s="33" t="s">
+        <v>853</v>
+      </c>
+      <c r="C153" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="D153" s="30" t="s">
+        <v>856</v>
+      </c>
+      <c r="E153" s="54" t="s">
+        <v>865</v>
+      </c>
+      <c r="F153" s="43" t="s">
+        <v>866</v>
+      </c>
+      <c r="G153" s="47"/>
+      <c r="H153" s="43" t="s">
+        <v>867</v>
+      </c>
       <c r="I153" s="33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="154" spans="1:9" s="51" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9" s="51" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A154" s="33">
         <v>153</v>
       </c>
       <c r="B154" s="33" t="s">
-        <v>865</v>
+        <v>853</v>
       </c>
       <c r="C154" s="55" t="s">
-        <v>816</v>
-      </c>
-      <c r="D154" s="41" t="s">
-        <v>817</v>
+        <v>94</v>
+      </c>
+      <c r="D154" s="30" t="s">
+        <v>857</v>
       </c>
       <c r="E154" s="54" t="s">
-        <v>892</v>
+        <v>868</v>
       </c>
       <c r="F154" s="43" t="s">
-        <v>865</v>
+        <v>869</v>
       </c>
       <c r="G154" s="47"/>
       <c r="H154" s="43" t="s">
-        <v>893</v>
+        <v>870</v>
       </c>
       <c r="I154" s="33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="155" spans="1:9" s="51" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:9" s="51" customFormat="1" ht="50" x14ac:dyDescent="0.35">
       <c r="A155" s="33">
         <v>154</v>
       </c>
       <c r="B155" s="33" t="s">
-        <v>865</v>
+        <v>853</v>
       </c>
       <c r="C155" s="55" t="s">
         <v>94</v>
       </c>
       <c r="D155" s="30" t="s">
-        <v>866</v>
+        <v>858</v>
       </c>
       <c r="E155" s="54" t="s">
-        <v>16</v>
+        <v>871</v>
       </c>
       <c r="F155" s="43" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="G155" s="47"/>
       <c r="H155" s="43" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="I155" s="33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="156" spans="1:9" s="51" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:9" s="51" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A156" s="33">
         <v>155</v>
       </c>
       <c r="B156" s="33" t="s">
-        <v>865</v>
+        <v>853</v>
       </c>
       <c r="C156" s="55" t="s">
         <v>94</v>
       </c>
       <c r="D156" s="30" t="s">
-        <v>867</v>
-      </c>
-      <c r="E156" s="43" t="s">
-        <v>16</v>
+        <v>859</v>
+      </c>
+      <c r="E156" s="54" t="s">
+        <v>874</v>
       </c>
       <c r="F156" s="43" t="s">
         <v>875</v>
@@ -7699,18 +7613,18 @@
         <v>93</v>
       </c>
     </row>
-    <row r="157" spans="1:9" s="51" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9" s="51" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A157" s="33">
         <v>156</v>
       </c>
       <c r="B157" s="33" t="s">
-        <v>865</v>
+        <v>853</v>
       </c>
       <c r="C157" s="55" t="s">
         <v>94</v>
       </c>
       <c r="D157" s="30" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="E157" s="54" t="s">
         <v>877</v>
@@ -7722,120 +7636,12 @@
       <c r="H157" s="43" t="s">
         <v>879</v>
       </c>
-      <c r="I157" s="33" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="158" spans="1:9" s="51" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="A158" s="33">
-        <v>157</v>
-      </c>
-      <c r="B158" s="33" t="s">
-        <v>865</v>
-      </c>
-      <c r="C158" s="55" t="s">
-        <v>94</v>
-      </c>
-      <c r="D158" s="30" t="s">
-        <v>869</v>
-      </c>
-      <c r="E158" s="54" t="s">
-        <v>880</v>
-      </c>
-      <c r="F158" s="43" t="s">
-        <v>881</v>
-      </c>
-      <c r="G158" s="47"/>
-      <c r="H158" s="43" t="s">
-        <v>882</v>
-      </c>
-      <c r="I158" s="33" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9" s="51" customFormat="1" ht="50" x14ac:dyDescent="0.35">
-      <c r="A159" s="33">
-        <v>158</v>
-      </c>
-      <c r="B159" s="33" t="s">
-        <v>865</v>
-      </c>
-      <c r="C159" s="55" t="s">
-        <v>94</v>
-      </c>
-      <c r="D159" s="30" t="s">
-        <v>870</v>
-      </c>
-      <c r="E159" s="54" t="s">
-        <v>883</v>
-      </c>
-      <c r="F159" s="43" t="s">
-        <v>884</v>
-      </c>
-      <c r="G159" s="47"/>
-      <c r="H159" s="43" t="s">
-        <v>885</v>
-      </c>
-      <c r="I159" s="33" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9" s="51" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A160" s="33">
-        <v>159</v>
-      </c>
-      <c r="B160" s="33" t="s">
-        <v>865</v>
-      </c>
-      <c r="C160" s="55" t="s">
-        <v>94</v>
-      </c>
-      <c r="D160" s="30" t="s">
-        <v>871</v>
-      </c>
-      <c r="E160" s="54" t="s">
-        <v>886</v>
-      </c>
-      <c r="F160" s="43" t="s">
-        <v>887</v>
-      </c>
-      <c r="G160" s="47"/>
-      <c r="H160" s="43" t="s">
-        <v>888</v>
-      </c>
-      <c r="I160" s="33" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" s="51" customFormat="1" ht="25" x14ac:dyDescent="0.35">
-      <c r="A161" s="33">
-        <v>160</v>
-      </c>
-      <c r="B161" s="33" t="s">
-        <v>865</v>
-      </c>
-      <c r="C161" s="55" t="s">
-        <v>94</v>
-      </c>
-      <c r="D161" s="30" t="s">
-        <v>872</v>
-      </c>
-      <c r="E161" s="54" t="s">
-        <v>889</v>
-      </c>
-      <c r="F161" s="43" t="s">
-        <v>890</v>
-      </c>
-      <c r="G161" s="47"/>
-      <c r="H161" s="43" t="s">
-        <v>891</v>
-      </c>
-      <c r="I161" s="50" t="s">
-        <v>919</v>
+      <c r="I157" s="1" t="s">
+        <v>943</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I161" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I157" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -7846,7 +7652,7 @@
   <dimension ref="A1:N129"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
@@ -8546,10 +8352,10 @@
         <v>722</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>915</v>
+        <v>903</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>918</v>
+        <v>906</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="14" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -10861,127 +10667,127 @@
       </c>
     </row>
     <row r="125" spans="1:8" ht="25" x14ac:dyDescent="0.35">
-      <c r="A125" s="69" t="s">
-        <v>158</v>
-      </c>
-      <c r="B125" s="70" t="s">
+      <c r="A125" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B125" s="36" t="s">
         <v>653</v>
       </c>
-      <c r="C125" s="71" t="s">
+      <c r="C125" s="19" t="s">
+        <v>907</v>
+      </c>
+      <c r="D125" s="19" t="s">
+        <v>929</v>
+      </c>
+      <c r="E125" s="43" t="s">
+        <v>912</v>
+      </c>
+      <c r="F125" s="43" t="s">
+        <v>913</v>
+      </c>
+      <c r="G125" s="43" t="s">
+        <v>914</v>
+      </c>
+      <c r="H125" s="43" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="50" x14ac:dyDescent="0.35">
+      <c r="A126" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B126" s="36" t="s">
+        <v>653</v>
+      </c>
+      <c r="C126" s="19" t="s">
+        <v>907</v>
+      </c>
+      <c r="D126" s="19" t="s">
+        <v>929</v>
+      </c>
+      <c r="E126" s="43" t="s">
+        <v>916</v>
+      </c>
+      <c r="F126" s="43" t="s">
+        <v>917</v>
+      </c>
+      <c r="G126" s="43"/>
+      <c r="H126" s="43" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A127" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B127" s="36" t="s">
+        <v>653</v>
+      </c>
+      <c r="C127" s="19" t="s">
+        <v>907</v>
+      </c>
+      <c r="D127" s="19" t="s">
+        <v>929</v>
+      </c>
+      <c r="E127" s="43" t="s">
+        <v>919</v>
+      </c>
+      <c r="F127" s="43" t="s">
         <v>920</v>
       </c>
-      <c r="D125" s="71" t="s">
-        <v>943</v>
-      </c>
-      <c r="E125" s="68" t="s">
+      <c r="G127" s="43"/>
+      <c r="H127" s="43" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="A128" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B128" s="36" t="s">
+        <v>653</v>
+      </c>
+      <c r="C128" s="19" t="s">
+        <v>907</v>
+      </c>
+      <c r="D128" s="19" t="s">
+        <v>929</v>
+      </c>
+      <c r="E128" s="43" t="s">
+        <v>922</v>
+      </c>
+      <c r="F128" s="43" t="s">
+        <v>923</v>
+      </c>
+      <c r="G128" s="43"/>
+      <c r="H128" s="43" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="A129" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B129" s="36" t="s">
+        <v>653</v>
+      </c>
+      <c r="C129" s="19" t="s">
+        <v>907</v>
+      </c>
+      <c r="D129" s="19" t="s">
+        <v>929</v>
+      </c>
+      <c r="E129" s="43" t="s">
+        <v>925</v>
+      </c>
+      <c r="F129" s="43" t="s">
         <v>926</v>
       </c>
-      <c r="F125" s="68" t="s">
+      <c r="G129" s="43" t="s">
         <v>927</v>
       </c>
-      <c r="G125" s="68" t="s">
+      <c r="H129" s="43" t="s">
         <v>928</v>
-      </c>
-      <c r="H125" s="68" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" ht="50" x14ac:dyDescent="0.35">
-      <c r="A126" s="69" t="s">
-        <v>158</v>
-      </c>
-      <c r="B126" s="70" t="s">
-        <v>653</v>
-      </c>
-      <c r="C126" s="71" t="s">
-        <v>920</v>
-      </c>
-      <c r="D126" s="71" t="s">
-        <v>943</v>
-      </c>
-      <c r="E126" s="68" t="s">
-        <v>930</v>
-      </c>
-      <c r="F126" s="68" t="s">
-        <v>931</v>
-      </c>
-      <c r="G126" s="68"/>
-      <c r="H126" s="68" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="A127" s="69" t="s">
-        <v>158</v>
-      </c>
-      <c r="B127" s="70" t="s">
-        <v>653</v>
-      </c>
-      <c r="C127" s="71" t="s">
-        <v>920</v>
-      </c>
-      <c r="D127" s="71" t="s">
-        <v>943</v>
-      </c>
-      <c r="E127" s="68" t="s">
-        <v>933</v>
-      </c>
-      <c r="F127" s="68" t="s">
-        <v>934</v>
-      </c>
-      <c r="G127" s="68"/>
-      <c r="H127" s="68" t="s">
-        <v>935</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" ht="25" x14ac:dyDescent="0.35">
-      <c r="A128" s="69" t="s">
-        <v>158</v>
-      </c>
-      <c r="B128" s="70" t="s">
-        <v>653</v>
-      </c>
-      <c r="C128" s="71" t="s">
-        <v>920</v>
-      </c>
-      <c r="D128" s="71" t="s">
-        <v>943</v>
-      </c>
-      <c r="E128" s="68" t="s">
-        <v>936</v>
-      </c>
-      <c r="F128" s="68" t="s">
-        <v>937</v>
-      </c>
-      <c r="G128" s="68"/>
-      <c r="H128" s="68" t="s">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" ht="25" x14ac:dyDescent="0.35">
-      <c r="A129" s="69" t="s">
-        <v>158</v>
-      </c>
-      <c r="B129" s="70" t="s">
-        <v>653</v>
-      </c>
-      <c r="C129" s="71" t="s">
-        <v>920</v>
-      </c>
-      <c r="D129" s="71" t="s">
-        <v>943</v>
-      </c>
-      <c r="E129" s="68" t="s">
-        <v>939</v>
-      </c>
-      <c r="F129" s="68" t="s">
-        <v>940</v>
-      </c>
-      <c r="G129" s="68" t="s">
-        <v>941</v>
-      </c>
-      <c r="H129" s="68" t="s">
-        <v>942</v>
       </c>
     </row>
   </sheetData>
@@ -10997,24 +10803,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -11236,10 +11024,40 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11263,21 +11081,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
QA checks from Dave
2023-02-07
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA531ADF-8F16-46A8-92E5-C4F3E83E5FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE20EE5C-C577-4863-A086-F0430603836B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="770" yWindow="120" windowWidth="17200" windowHeight="9880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5980" yWindow="0" windowWidth="17200" windowHeight="9880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="1024">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="1027">
   <si>
     <t>Preferred Term</t>
   </si>
@@ -3225,6 +3225,15 @@
   </si>
   <si>
     <t>nextActivityId</t>
+  </si>
+  <si>
+    <t>biomedicalConcepts</t>
+  </si>
+  <si>
+    <t>bcCategories</t>
+  </si>
+  <si>
+    <t>bcSurrogates</t>
   </si>
 </sst>
 </file>
@@ -3633,6 +3642,18 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3647,18 +3668,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3954,8 +3963,8 @@
   <dimension ref="A1:I191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
@@ -4960,7 +4969,7 @@
         <v>646</v>
       </c>
       <c r="D41" s="59" t="s">
-        <v>954</v>
+        <v>1024</v>
       </c>
       <c r="E41" s="29"/>
       <c r="F41" s="4"/>
@@ -4979,7 +4988,7 @@
         <v>646</v>
       </c>
       <c r="D42" s="59" t="s">
-        <v>955</v>
+        <v>1025</v>
       </c>
       <c r="E42" s="29"/>
       <c r="F42" s="4"/>
@@ -4998,7 +5007,7 @@
         <v>646</v>
       </c>
       <c r="D43" s="59" t="s">
-        <v>956</v>
+        <v>1026</v>
       </c>
       <c r="E43" s="29"/>
       <c r="F43" s="4"/>
@@ -6834,26 +6843,26 @@
       <c r="A116" s="33">
         <v>115</v>
       </c>
-      <c r="B116" s="68" t="s">
+      <c r="B116" s="63" t="s">
         <v>663</v>
       </c>
-      <c r="C116" s="69" t="s">
+      <c r="C116" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="D116" s="70" t="s">
+      <c r="D116" s="65" t="s">
         <v>588</v>
       </c>
-      <c r="E116" s="68" t="s">
+      <c r="E116" s="63" t="s">
         <v>758</v>
       </c>
-      <c r="F116" s="68" t="s">
+      <c r="F116" s="63" t="s">
         <v>590</v>
       </c>
-      <c r="G116" s="68"/>
-      <c r="H116" s="68" t="s">
+      <c r="G116" s="63"/>
+      <c r="H116" s="63" t="s">
         <v>716</v>
       </c>
-      <c r="I116" s="71" t="s">
+      <c r="I116" s="66" t="s">
         <v>93</v>
       </c>
     </row>
@@ -6861,26 +6870,26 @@
       <c r="A117" s="33">
         <v>116</v>
       </c>
-      <c r="B117" s="68" t="s">
+      <c r="B117" s="63" t="s">
         <v>663</v>
       </c>
-      <c r="C117" s="69" t="s">
+      <c r="C117" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="D117" s="70" t="s">
+      <c r="D117" s="65" t="s">
         <v>589</v>
       </c>
-      <c r="E117" s="68" t="s">
+      <c r="E117" s="63" t="s">
         <v>759</v>
       </c>
-      <c r="F117" s="68" t="s">
+      <c r="F117" s="63" t="s">
         <v>591</v>
       </c>
-      <c r="G117" s="68"/>
-      <c r="H117" s="68" t="s">
+      <c r="G117" s="63"/>
+      <c r="H117" s="63" t="s">
         <v>717</v>
       </c>
-      <c r="I117" s="71" t="s">
+      <c r="I117" s="66" t="s">
         <v>93</v>
       </c>
     </row>
@@ -8807,14 +8816,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="67" t="s">
         <v>506</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
       <c r="I1" s="6"/>
@@ -8825,16 +8834,16 @@
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="69" t="s">
         <v>505</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
@@ -8843,11 +8852,11 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:14" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="67" t="s">
         <v>507</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
       <c r="D3" s="32"/>
       <c r="E3" s="24"/>
       <c r="F3" s="20"/>
@@ -8871,10 +8880,10 @@
       <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:14" s="7" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="70" t="s">
         <v>156</v>
       </c>
-      <c r="B5" s="67"/>
+      <c r="B5" s="71"/>
       <c r="C5" s="26"/>
       <c r="D5" s="26"/>
       <c r="E5" s="25"/>
@@ -12017,6 +12026,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -12238,25 +12265,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12274,30 +12309,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update for sprint 10_2023-03-09
InvestigationalInterventions updated to InvestigationalIntervention
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C86D8A-70E2-44F8-B1A1-18433FBC4446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5668E2-FF5D-4CDA-ACE1-2757C2B6864F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="0" windowWidth="18290" windowHeight="9460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="910" yWindow="0" windowWidth="18290" windowHeight="9460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2341" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2341" uniqueCount="1113">
   <si>
     <t>Preferred Term</t>
   </si>
@@ -3409,6 +3409,9 @@
   </si>
   <si>
     <t>bcCategoryParentIds</t>
+  </si>
+  <si>
+    <t>InvestigationalIntervention</t>
   </si>
 </sst>
 </file>
@@ -5489,7 +5492,7 @@
         <v>4</v>
       </c>
       <c r="D52" s="41" t="s">
-        <v>647</v>
+        <v>1112</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>27</v>
@@ -13158,24 +13161,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -13397,10 +13382,40 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13424,21 +13439,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Slight fixes per Berber's e-mail 2023-07-18
The following changes do not fall under the (only Name, Id, Description rule)
•	studyArm part removed from studyArmDataOriginDescription.
•	endpointPurposeDescription changed to PurposeDescription
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E45DF8-D984-4A30-90D0-508E4ADF167E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592D0FBE-928D-4C23-999B-434D81D83208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50" yWindow="100" windowWidth="19010" windowHeight="9170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1210" yWindow="460" windowWidth="14620" windowHeight="9320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -3177,9 +3177,6 @@
     <t>encounterScheduledAtTiming</t>
   </si>
   <si>
-    <t>purposeDescription</t>
-  </si>
-  <si>
     <t>scheduledActivityInstanceEncounter</t>
   </si>
   <si>
@@ -3195,9 +3192,6 @@
     <t>scheduleTimelineEntry</t>
   </si>
   <si>
-    <t>dataOriginDescription</t>
-  </si>
-  <si>
     <t>relativeFromScheduledInstance</t>
   </si>
   <si>
@@ -3268,6 +3262,12 @@
   </si>
   <si>
     <t>Investigational Intervention Description</t>
+  </si>
+  <si>
+    <t>studyArmDataOriginDescription</t>
+  </si>
+  <si>
+    <t>endpointPurposeDescription</t>
   </si>
 </sst>
 </file>
@@ -5273,7 +5273,7 @@
       </c>
       <c r="G49" s="43"/>
       <c r="H49" s="43" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>90</v>
@@ -5406,11 +5406,11 @@
         <v>96</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>90</v>
@@ -5430,14 +5430,14 @@
         <v>596</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>90</v>
@@ -5491,7 +5491,7 @@
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="4" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>610</v>
@@ -5545,7 +5545,7 @@
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="I59" s="43" t="s">
         <v>90</v>
@@ -5728,7 +5728,7 @@
       </c>
       <c r="G66" s="4"/>
       <c r="H66" s="4" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>90</v>
@@ -5809,7 +5809,7 @@
       </c>
       <c r="G69" s="3"/>
       <c r="H69" s="4" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="I69" s="43" t="s">
         <v>90</v>
@@ -5826,7 +5826,7 @@
         <v>91</v>
       </c>
       <c r="D70" s="31" t="s">
-        <v>1045</v>
+        <v>1075</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>674</v>
@@ -6034,7 +6034,7 @@
       </c>
       <c r="G78" s="4"/>
       <c r="H78" s="4" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>90</v>
@@ -6078,7 +6078,7 @@
         <v>91</v>
       </c>
       <c r="D80" s="31" t="s">
-        <v>1051</v>
+        <v>1074</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>678</v>
@@ -6196,7 +6196,7 @@
       </c>
       <c r="G84" s="4"/>
       <c r="H84" s="4" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="I84" s="43" t="s">
         <v>90</v>
@@ -6400,7 +6400,7 @@
       </c>
       <c r="G92" s="4"/>
       <c r="H92" s="4" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>90</v>
@@ -6454,7 +6454,7 @@
       </c>
       <c r="G94" s="4"/>
       <c r="H94" s="4" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>90</v>
@@ -6598,7 +6598,7 @@
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="4" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="I100" s="43" t="s">
         <v>90</v>
@@ -6961,7 +6961,7 @@
       </c>
       <c r="G115" s="4"/>
       <c r="H115" s="3" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="I115" s="4" t="s">
         <v>90</v>
@@ -7156,7 +7156,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" s="33">
         <v>122</v>
       </c>
@@ -7204,7 +7204,7 @@
       </c>
       <c r="G124" s="61"/>
       <c r="H124" s="61" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="I124" s="43" t="s">
         <v>90</v>
@@ -7396,7 +7396,7 @@
       </c>
       <c r="G132" s="4"/>
       <c r="H132" s="4" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="I132" s="43" t="s">
         <v>90</v>
@@ -7477,7 +7477,7 @@
       </c>
       <c r="G135" s="4"/>
       <c r="H135" s="4" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="I135" s="43" t="s">
         <v>90</v>
@@ -8419,7 +8419,7 @@
       </c>
       <c r="G171" s="43"/>
       <c r="H171" s="43" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="I171" s="43" t="s">
         <v>90</v>
@@ -8569,7 +8569,7 @@
       </c>
       <c r="G177" s="43"/>
       <c r="H177" s="43" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="I177" s="43" t="s">
         <v>90</v>
@@ -8661,7 +8661,7 @@
         <v>590</v>
       </c>
       <c r="D181" s="63" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="E181" s="61"/>
       <c r="F181" s="55"/>
@@ -8790,7 +8790,7 @@
         <v>590</v>
       </c>
       <c r="D186" s="56" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="E186" s="61"/>
       <c r="F186" s="62"/>
@@ -8811,7 +8811,7 @@
         <v>590</v>
       </c>
       <c r="D187" s="56" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="E187" s="61"/>
       <c r="F187" s="62"/>
@@ -8853,7 +8853,7 @@
         <v>590</v>
       </c>
       <c r="D189" s="56" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="E189" s="61"/>
       <c r="F189" s="62"/>
@@ -8938,7 +8938,7 @@
       </c>
       <c r="G192" s="61"/>
       <c r="H192" s="61" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="I192" s="61" t="s">
         <v>90</v>
@@ -9030,7 +9030,7 @@
         <v>590</v>
       </c>
       <c r="D196" s="63" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="E196" s="61"/>
       <c r="F196" s="62"/>
@@ -9315,7 +9315,7 @@
         <v>590</v>
       </c>
       <c r="D207" s="63" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="E207" s="62"/>
       <c r="F207" s="62"/>
@@ -9336,7 +9336,7 @@
         <v>590</v>
       </c>
       <c r="D208" s="63" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="E208" s="62"/>
       <c r="F208" s="62"/>
@@ -10814,7 +10814,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="14" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" s="14" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A61" s="15" t="s">
         <v>137</v>
       </c>
@@ -12924,6 +12924,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -13145,25 +13163,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13181,30 +13207,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates to two Activity Relationships
Removal of last two 'Id' from relationship names.
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0933142-FEE0-43A8-817B-557FD05BB8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943A73EE-E7B5-4BD8-BA78-0412F6CDF66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="250" yWindow="170" windowWidth="18660" windowHeight="9820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2759,12 +2759,6 @@
     <t>Biomedical Concept Category Description</t>
   </si>
   <si>
-    <t>previousActivityId</t>
-  </si>
-  <si>
-    <t>nextActivityId</t>
-  </si>
-  <si>
     <t>biomedicalConcepts</t>
   </si>
   <si>
@@ -3265,6 +3259,12 @@
   </si>
   <si>
     <t>defaultCondition</t>
+  </si>
+  <si>
+    <t>previousActivity</t>
+  </si>
+  <si>
+    <t>nextActivity</t>
   </si>
 </sst>
 </file>
@@ -4113,7 +4113,7 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -4134,7 +4134,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -4155,7 +4155,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -4643,7 +4643,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -4718,7 +4718,7 @@
       <c r="G26" s="48"/>
       <c r="H26" s="48"/>
       <c r="I26" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -4874,7 +4874,7 @@
       <c r="G32" s="28"/>
       <c r="H32" s="28"/>
       <c r="I32" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
@@ -4895,7 +4895,7 @@
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
       <c r="I33" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
@@ -4916,7 +4916,7 @@
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
       <c r="I34" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -4937,7 +4937,7 @@
       <c r="G35" s="28"/>
       <c r="H35" s="28"/>
       <c r="I35" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
@@ -4958,7 +4958,7 @@
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
       <c r="I36" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
@@ -4979,7 +4979,7 @@
       <c r="G37" s="28"/>
       <c r="H37" s="28"/>
       <c r="I37" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
@@ -5000,7 +5000,7 @@
       <c r="G38" s="28"/>
       <c r="H38" s="28"/>
       <c r="I38" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -5021,7 +5021,7 @@
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
       <c r="I39" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -5035,14 +5035,14 @@
         <v>588</v>
       </c>
       <c r="D40" s="56" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="E40" s="57"/>
       <c r="F40" s="58"/>
       <c r="G40" s="59"/>
       <c r="H40" s="59"/>
       <c r="I40" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -5056,14 +5056,14 @@
         <v>588</v>
       </c>
       <c r="D41" s="56" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="E41" s="57"/>
       <c r="F41" s="58"/>
       <c r="G41" s="59"/>
       <c r="H41" s="59"/>
       <c r="I41" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
@@ -5077,14 +5077,14 @@
         <v>588</v>
       </c>
       <c r="D42" s="56" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="E42" s="57"/>
       <c r="F42" s="58"/>
       <c r="G42" s="59"/>
       <c r="H42" s="59"/>
       <c r="I42" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
@@ -5105,7 +5105,7 @@
       <c r="G43" s="59"/>
       <c r="H43" s="59"/>
       <c r="I43" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="45" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -5119,7 +5119,7 @@
         <v>91</v>
       </c>
       <c r="D44" s="31" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="E44" s="44" t="s">
         <v>43</v>
@@ -5216,7 +5216,7 @@
         <v>728</v>
       </c>
       <c r="H47" s="55" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>724</v>
@@ -5233,7 +5233,7 @@
         <v>91</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="E48" s="43" t="s">
         <v>16</v>
@@ -5260,7 +5260,7 @@
         <v>91</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E49" s="43" t="s">
         <v>16</v>
@@ -5270,7 +5270,7 @@
       </c>
       <c r="G49" s="43"/>
       <c r="H49" s="43" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>90</v>
@@ -5337,13 +5337,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D52" s="41" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>27</v>
@@ -5364,7 +5364,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>91</v>
@@ -5391,23 +5391,23 @@
         <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>91</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>96</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>90</v>
@@ -5427,14 +5427,14 @@
         <v>594</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>90</v>
@@ -5478,7 +5478,7 @@
         <v>91</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>31</v>
@@ -5488,7 +5488,7 @@
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="4" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>608</v>
@@ -5532,7 +5532,7 @@
         <v>91</v>
       </c>
       <c r="D59" s="31" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>670</v>
@@ -5542,7 +5542,7 @@
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="I59" s="43" t="s">
         <v>90</v>
@@ -5701,7 +5701,7 @@
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
       <c r="I65" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
@@ -5715,7 +5715,7 @@
         <v>91</v>
       </c>
       <c r="D66" s="31" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>115</v>
@@ -5725,7 +5725,7 @@
       </c>
       <c r="G66" s="4"/>
       <c r="H66" s="4" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>90</v>
@@ -5752,7 +5752,7 @@
       </c>
       <c r="G67" s="4"/>
       <c r="H67" s="4" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="I67" s="4" t="s">
         <v>706</v>
@@ -5796,7 +5796,7 @@
         <v>91</v>
       </c>
       <c r="D69" s="30" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>671</v>
@@ -5806,7 +5806,7 @@
       </c>
       <c r="G69" s="3"/>
       <c r="H69" s="4" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="I69" s="43" t="s">
         <v>90</v>
@@ -5823,7 +5823,7 @@
         <v>91</v>
       </c>
       <c r="D70" s="31" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="E70" s="4" t="s">
         <v>672</v>
@@ -5904,14 +5904,14 @@
         <v>588</v>
       </c>
       <c r="D73" s="42" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="I73" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -5925,14 +5925,14 @@
         <v>588</v>
       </c>
       <c r="D74" s="42" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
       <c r="H74" s="3"/>
       <c r="I74" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
@@ -5953,7 +5953,7 @@
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
       <c r="I75" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="50" x14ac:dyDescent="0.35">
@@ -5994,7 +5994,7 @@
         <v>91</v>
       </c>
       <c r="D77" s="31" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>119</v>
@@ -6021,7 +6021,7 @@
         <v>91</v>
       </c>
       <c r="D78" s="31" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>118</v>
@@ -6031,7 +6031,7 @@
       </c>
       <c r="G78" s="4"/>
       <c r="H78" s="4" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>90</v>
@@ -6054,14 +6054,14 @@
         <v>675</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="G79" s="4"/>
       <c r="H79" s="4" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -6075,7 +6075,7 @@
         <v>91</v>
       </c>
       <c r="D80" s="31" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>676</v>
@@ -6156,7 +6156,7 @@
         <v>91</v>
       </c>
       <c r="D83" s="31" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>63</v>
@@ -6183,7 +6183,7 @@
         <v>91</v>
       </c>
       <c r="D84" s="31" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E84" s="4" t="s">
         <v>678</v>
@@ -6193,7 +6193,7 @@
       </c>
       <c r="G84" s="4"/>
       <c r="H84" s="4" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="I84" s="43" t="s">
         <v>90</v>
@@ -6237,7 +6237,7 @@
         <v>91</v>
       </c>
       <c r="D86" s="31" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="E86" s="4" t="s">
         <v>680</v>
@@ -6264,7 +6264,7 @@
         <v>91</v>
       </c>
       <c r="D87" s="31" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>681</v>
@@ -6325,7 +6325,7 @@
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
       <c r="I89" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
@@ -6346,7 +6346,7 @@
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -6360,7 +6360,7 @@
         <v>91</v>
       </c>
       <c r="D91" s="31" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>682</v>
@@ -6387,7 +6387,7 @@
         <v>91</v>
       </c>
       <c r="D92" s="31" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>683</v>
@@ -6397,7 +6397,7 @@
       </c>
       <c r="G92" s="4"/>
       <c r="H92" s="4" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>90</v>
@@ -6441,7 +6441,7 @@
         <v>91</v>
       </c>
       <c r="D94" s="31" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>684</v>
@@ -6451,7 +6451,7 @@
       </c>
       <c r="G94" s="4"/>
       <c r="H94" s="4" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>90</v>
@@ -6502,7 +6502,7 @@
       <c r="G96" s="4"/>
       <c r="H96" s="3"/>
       <c r="I96" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
@@ -6523,7 +6523,7 @@
       <c r="G97" s="4"/>
       <c r="H97" s="3"/>
       <c r="I97" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
@@ -6537,14 +6537,14 @@
         <v>588</v>
       </c>
       <c r="D98" s="63" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="4"/>
       <c r="G98" s="4"/>
       <c r="H98" s="3"/>
       <c r="I98" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -6558,7 +6558,7 @@
         <v>91</v>
       </c>
       <c r="D99" s="31" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="E99" s="4" t="s">
         <v>112</v>
@@ -6585,7 +6585,7 @@
         <v>91</v>
       </c>
       <c r="D100" s="31" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="E100" s="4" t="s">
         <v>685</v>
@@ -6595,7 +6595,7 @@
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="4" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="I100" s="43" t="s">
         <v>90</v>
@@ -6612,7 +6612,7 @@
         <v>91</v>
       </c>
       <c r="D101" s="31" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="E101" s="4" t="s">
         <v>686</v>
@@ -6639,7 +6639,7 @@
         <v>91</v>
       </c>
       <c r="D102" s="31" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="E102" s="4" t="s">
         <v>687</v>
@@ -6781,7 +6781,7 @@
       <c r="G107" s="4"/>
       <c r="H107" s="3"/>
       <c r="I107" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
@@ -6795,14 +6795,14 @@
         <v>588</v>
       </c>
       <c r="D108" s="47" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="4"/>
       <c r="G108" s="4"/>
       <c r="H108" s="3"/>
       <c r="I108" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
@@ -6816,14 +6816,14 @@
         <v>588</v>
       </c>
       <c r="D109" s="47" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
       <c r="H109" s="3"/>
       <c r="I109" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
@@ -6837,14 +6837,14 @@
         <v>588</v>
       </c>
       <c r="D110" s="47" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="4"/>
       <c r="G110" s="4"/>
       <c r="H110" s="3"/>
       <c r="I110" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.35">
@@ -6858,14 +6858,14 @@
         <v>588</v>
       </c>
       <c r="D111" s="47" t="s">
-        <v>906</v>
+        <v>1073</v>
       </c>
       <c r="E111" s="1"/>
       <c r="F111" s="4"/>
       <c r="G111" s="4"/>
       <c r="H111" s="3"/>
       <c r="I111" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.35">
@@ -6879,14 +6879,14 @@
         <v>588</v>
       </c>
       <c r="D112" s="47" t="s">
-        <v>907</v>
+        <v>1074</v>
       </c>
       <c r="E112" s="1"/>
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
       <c r="H112" s="3"/>
       <c r="I112" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
@@ -6900,14 +6900,14 @@
         <v>588</v>
       </c>
       <c r="D113" s="56" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="E113" s="55"/>
       <c r="F113" s="58"/>
       <c r="G113" s="58"/>
       <c r="H113" s="60"/>
       <c r="I113" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -6921,7 +6921,7 @@
         <v>91</v>
       </c>
       <c r="D114" s="31" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="E114" s="4" t="s">
         <v>691</v>
@@ -6948,7 +6948,7 @@
         <v>91</v>
       </c>
       <c r="D115" s="31" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>526</v>
@@ -6958,7 +6958,7 @@
       </c>
       <c r="G115" s="4"/>
       <c r="H115" s="3" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="I115" s="4" t="s">
         <v>90</v>
@@ -7164,17 +7164,17 @@
         <v>91</v>
       </c>
       <c r="D123" s="31" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="E123" s="43" t="s">
         <v>16</v>
       </c>
       <c r="F123" s="43" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="G123" s="61"/>
       <c r="H123" s="61" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="I123" s="43" t="s">
         <v>90</v>
@@ -7191,17 +7191,17 @@
         <v>91</v>
       </c>
       <c r="D124" s="65" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E124" s="43" t="s">
         <v>16</v>
       </c>
       <c r="F124" s="61" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="G124" s="61"/>
       <c r="H124" s="61" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="I124" s="43" t="s">
         <v>90</v>
@@ -7252,7 +7252,7 @@
       <c r="G126" s="4"/>
       <c r="H126" s="4"/>
       <c r="I126" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.35">
@@ -7273,7 +7273,7 @@
       <c r="G127" s="4"/>
       <c r="H127" s="4"/>
       <c r="I127" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.35">
@@ -7294,7 +7294,7 @@
       <c r="G128" s="4"/>
       <c r="H128" s="4"/>
       <c r="I128" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.35">
@@ -7315,7 +7315,7 @@
       <c r="G129" s="4"/>
       <c r="H129" s="4"/>
       <c r="I129" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -7383,7 +7383,7 @@
         <v>91</v>
       </c>
       <c r="D132" s="31" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>695</v>
@@ -7393,7 +7393,7 @@
       </c>
       <c r="G132" s="4"/>
       <c r="H132" s="4" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="I132" s="43" t="s">
         <v>90</v>
@@ -7437,7 +7437,7 @@
         <v>91</v>
       </c>
       <c r="D134" s="31" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="E134" s="4" t="s">
         <v>697</v>
@@ -7464,7 +7464,7 @@
         <v>91</v>
       </c>
       <c r="D135" s="31" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E135" s="4" t="s">
         <v>698</v>
@@ -7474,7 +7474,7 @@
       </c>
       <c r="G135" s="4"/>
       <c r="H135" s="4" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="I135" s="43" t="s">
         <v>90</v>
@@ -7687,7 +7687,7 @@
       <c r="G143" s="33"/>
       <c r="H143" s="33"/>
       <c r="I143" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.35">
@@ -7701,14 +7701,14 @@
         <v>588</v>
       </c>
       <c r="D144" s="47" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="E144" s="33"/>
       <c r="F144" s="33"/>
       <c r="G144" s="33"/>
       <c r="H144" s="33"/>
       <c r="I144" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="145" spans="1:9" s="49" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -7972,7 +7972,7 @@
       <c r="G154" s="33"/>
       <c r="H154" s="33"/>
       <c r="I154" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -8023,7 +8023,7 @@
       </c>
       <c r="G156" s="43"/>
       <c r="H156" s="43" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="I156" s="43" t="s">
         <v>90</v>
@@ -8128,7 +8128,7 @@
       <c r="G160" s="33"/>
       <c r="H160" s="33"/>
       <c r="I160" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -8379,7 +8379,7 @@
         <v>91</v>
       </c>
       <c r="D170" s="30" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="E170" s="43" t="s">
         <v>16</v>
@@ -8406,7 +8406,7 @@
         <v>91</v>
       </c>
       <c r="D171" s="30" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="E171" s="43" t="s">
         <v>16</v>
@@ -8416,7 +8416,7 @@
       </c>
       <c r="G171" s="43"/>
       <c r="H171" s="43" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="I171" s="43" t="s">
         <v>90</v>
@@ -8487,14 +8487,14 @@
         <v>588</v>
       </c>
       <c r="D174" s="47" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="E174" s="33"/>
       <c r="F174" s="33"/>
       <c r="G174" s="33"/>
       <c r="H174" s="33"/>
       <c r="I174" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="175" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -8508,14 +8508,14 @@
         <v>588</v>
       </c>
       <c r="D175" s="47" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="E175" s="33"/>
       <c r="F175" s="33"/>
       <c r="G175" s="33"/>
       <c r="H175" s="33"/>
       <c r="I175" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="176" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -8529,7 +8529,7 @@
         <v>91</v>
       </c>
       <c r="D176" s="30" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="E176" s="43" t="s">
         <v>16</v>
@@ -8556,7 +8556,7 @@
         <v>91</v>
       </c>
       <c r="D177" s="30" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="E177" s="43" t="s">
         <v>16</v>
@@ -8566,7 +8566,7 @@
       </c>
       <c r="G177" s="43"/>
       <c r="H177" s="43" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="I177" s="43" t="s">
         <v>90</v>
@@ -8583,17 +8583,17 @@
         <v>91</v>
       </c>
       <c r="D178" s="30" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="E178" s="43" t="s">
         <v>16</v>
       </c>
       <c r="F178" s="43" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="G178" s="43"/>
       <c r="H178" s="43" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="I178" s="43" t="s">
         <v>90</v>
@@ -8604,23 +8604,23 @@
         <v>178</v>
       </c>
       <c r="B179" s="55" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C179" s="58" t="s">
         <v>4</v>
       </c>
       <c r="D179" s="54" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="E179" s="61" t="s">
         <v>16</v>
       </c>
       <c r="F179" s="55" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="G179" s="62"/>
       <c r="H179" s="61" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="I179" s="61" t="s">
         <v>90</v>
@@ -8631,7 +8631,7 @@
         <v>179</v>
       </c>
       <c r="B180" s="55" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C180" s="58" t="s">
         <v>588</v>
@@ -8644,7 +8644,7 @@
       <c r="G180" s="62"/>
       <c r="H180" s="61"/>
       <c r="I180" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="181" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -8652,20 +8652,20 @@
         <v>180</v>
       </c>
       <c r="B181" s="55" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C181" s="58" t="s">
         <v>588</v>
       </c>
       <c r="D181" s="63" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="E181" s="61"/>
       <c r="F181" s="55"/>
       <c r="G181" s="62"/>
       <c r="H181" s="61"/>
       <c r="I181" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -8673,23 +8673,23 @@
         <v>181</v>
       </c>
       <c r="B182" s="55" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C182" s="58" t="s">
         <v>4</v>
       </c>
       <c r="D182" s="54" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="E182" s="61" t="s">
         <v>16</v>
       </c>
       <c r="F182" s="55" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="G182" s="62"/>
       <c r="H182" s="61" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="I182" s="61" t="s">
         <v>90</v>
@@ -8700,23 +8700,23 @@
         <v>182</v>
       </c>
       <c r="B183" s="55" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C183" s="58" t="s">
         <v>4</v>
       </c>
       <c r="D183" s="30" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="E183" s="70" t="s">
         <v>16</v>
       </c>
       <c r="F183" s="43" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="G183" s="70"/>
       <c r="H183" s="43" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="I183" s="61" t="s">
         <v>90</v>
@@ -8727,23 +8727,23 @@
         <v>183</v>
       </c>
       <c r="B184" s="61" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C184" s="58" t="s">
         <v>4</v>
       </c>
       <c r="D184" s="64" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="E184" s="61" t="s">
         <v>16</v>
       </c>
       <c r="F184" s="55" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="G184" s="62"/>
       <c r="H184" s="61" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="I184" s="61" t="s">
         <v>90</v>
@@ -8754,23 +8754,23 @@
         <v>184</v>
       </c>
       <c r="B185" s="61" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C185" s="60" t="s">
         <v>91</v>
       </c>
       <c r="D185" s="65" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="E185" s="61" t="s">
         <v>16</v>
       </c>
       <c r="F185" s="55" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="G185" s="62"/>
       <c r="H185" s="61" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="I185" s="61" t="s">
         <v>90</v>
@@ -8781,20 +8781,20 @@
         <v>185</v>
       </c>
       <c r="B186" s="61" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C186" s="58" t="s">
         <v>588</v>
       </c>
       <c r="D186" s="56" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="E186" s="61"/>
       <c r="F186" s="62"/>
       <c r="G186" s="62"/>
       <c r="H186" s="62"/>
       <c r="I186" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="187" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
@@ -8802,20 +8802,20 @@
         <v>186</v>
       </c>
       <c r="B187" s="61" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C187" s="58" t="s">
         <v>588</v>
       </c>
       <c r="D187" s="56" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="E187" s="61"/>
       <c r="F187" s="62"/>
       <c r="G187" s="62"/>
       <c r="H187" s="62"/>
       <c r="I187" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="188" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
@@ -8823,20 +8823,20 @@
         <v>187</v>
       </c>
       <c r="B188" s="61" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C188" s="58" t="s">
         <v>588</v>
       </c>
       <c r="D188" s="56" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E188" s="61"/>
       <c r="F188" s="62"/>
       <c r="G188" s="62"/>
       <c r="H188" s="62"/>
       <c r="I188" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="189" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
@@ -8844,20 +8844,20 @@
         <v>188</v>
       </c>
       <c r="B189" s="61" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C189" s="58" t="s">
         <v>588</v>
       </c>
       <c r="D189" s="56" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="E189" s="61"/>
       <c r="F189" s="62"/>
       <c r="G189" s="62"/>
       <c r="H189" s="62"/>
       <c r="I189" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.35">
@@ -8865,23 +8865,23 @@
         <v>189</v>
       </c>
       <c r="B190" s="55" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C190" s="58" t="s">
         <v>4</v>
       </c>
       <c r="D190" s="54" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="E190" s="61" t="s">
         <v>16</v>
       </c>
       <c r="F190" s="61" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="G190" s="61"/>
       <c r="H190" s="61" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="I190" s="61" t="s">
         <v>90</v>
@@ -8892,23 +8892,23 @@
         <v>190</v>
       </c>
       <c r="B191" s="55" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C191" s="60" t="s">
         <v>91</v>
       </c>
       <c r="D191" s="66" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="E191" s="61" t="s">
         <v>16</v>
       </c>
       <c r="F191" s="55" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="G191" s="61"/>
       <c r="H191" s="61" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="I191" s="61" t="s">
         <v>90</v>
@@ -8919,23 +8919,23 @@
         <v>191</v>
       </c>
       <c r="B192" s="55" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C192" s="60" t="s">
         <v>91</v>
       </c>
       <c r="D192" s="66" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="E192" s="61" t="s">
         <v>16</v>
       </c>
       <c r="F192" s="55" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="G192" s="61"/>
       <c r="H192" s="61" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="I192" s="61" t="s">
         <v>90</v>
@@ -8946,23 +8946,23 @@
         <v>192</v>
       </c>
       <c r="B193" s="55" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C193" s="60" t="s">
         <v>91</v>
       </c>
       <c r="D193" s="66" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="E193" s="61" t="s">
         <v>16</v>
       </c>
       <c r="F193" s="55" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="G193" s="61"/>
       <c r="H193" s="61" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="I193" s="61" t="s">
         <v>90</v>
@@ -8973,23 +8973,23 @@
         <v>193</v>
       </c>
       <c r="B194" s="55" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C194" s="60" t="s">
         <v>91</v>
       </c>
       <c r="D194" s="66" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="E194" s="61" t="s">
         <v>16</v>
       </c>
       <c r="F194" s="61" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="G194" s="61"/>
       <c r="H194" s="43" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="I194" s="61" t="s">
         <v>90</v>
@@ -9000,20 +9000,20 @@
         <v>194</v>
       </c>
       <c r="B195" s="55" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C195" s="58" t="s">
         <v>588</v>
       </c>
       <c r="D195" s="63" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="E195" s="61"/>
       <c r="F195" s="55"/>
       <c r="G195" s="62"/>
       <c r="H195" s="61"/>
       <c r="I195" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="196" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
@@ -9021,20 +9021,20 @@
         <v>195</v>
       </c>
       <c r="B196" s="55" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C196" s="58" t="s">
         <v>588</v>
       </c>
       <c r="D196" s="63" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="E196" s="61"/>
       <c r="F196" s="62"/>
       <c r="G196" s="62"/>
       <c r="H196" s="62"/>
       <c r="I196" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="197" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
@@ -9042,20 +9042,20 @@
         <v>196</v>
       </c>
       <c r="B197" s="55" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C197" s="58" t="s">
         <v>588</v>
       </c>
       <c r="D197" s="63" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="E197" s="61"/>
       <c r="F197" s="62"/>
       <c r="G197" s="62"/>
       <c r="H197" s="62"/>
       <c r="I197" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="198" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
@@ -9063,23 +9063,23 @@
         <v>197</v>
       </c>
       <c r="B198" s="55" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="C198" s="58" t="s">
         <v>4</v>
       </c>
       <c r="D198" s="54" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="E198" s="61" t="s">
         <v>16</v>
       </c>
       <c r="F198" s="55" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="G198" s="62"/>
       <c r="H198" s="61" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="I198" s="61" t="s">
         <v>90</v>
@@ -9090,23 +9090,23 @@
         <v>198</v>
       </c>
       <c r="B199" s="55" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C199" s="58" t="s">
         <v>4</v>
       </c>
       <c r="D199" s="54" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="E199" s="61" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="F199" s="61" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="G199" s="62"/>
       <c r="H199" s="61" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="I199" s="61" t="s">
         <v>90</v>
@@ -9117,26 +9117,26 @@
         <v>199</v>
       </c>
       <c r="B200" s="55" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C200" s="60" t="s">
         <v>91</v>
       </c>
       <c r="D200" s="66" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="E200" s="61" t="s">
         <v>16</v>
       </c>
       <c r="F200" s="55" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="G200" s="62"/>
       <c r="H200" s="61" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="I200" s="43" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
     </row>
     <row r="201" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -9144,23 +9144,23 @@
         <v>200</v>
       </c>
       <c r="B201" s="55" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C201" s="60" t="s">
         <v>91</v>
       </c>
       <c r="D201" s="66" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="E201" s="61" t="s">
         <v>16</v>
       </c>
       <c r="F201" s="55" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="G201" s="62"/>
       <c r="H201" s="61" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="I201" s="61" t="s">
         <v>90</v>
@@ -9171,26 +9171,26 @@
         <v>201</v>
       </c>
       <c r="B202" s="55" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C202" s="60" t="s">
         <v>91</v>
       </c>
       <c r="D202" s="66" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="E202" s="61" t="s">
         <v>16</v>
       </c>
       <c r="F202" s="55" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="G202" s="62"/>
       <c r="H202" s="61" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="I202" s="43" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
     </row>
     <row r="203" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -9198,23 +9198,23 @@
         <v>202</v>
       </c>
       <c r="B203" s="55" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C203" s="60" t="s">
         <v>91</v>
       </c>
       <c r="D203" s="66" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="E203" s="61" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="F203" s="55" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="G203" s="62"/>
       <c r="H203" s="61" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="I203" s="61" t="s">
         <v>90</v>
@@ -9225,23 +9225,23 @@
         <v>203</v>
       </c>
       <c r="B204" s="55" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C204" s="60" t="s">
         <v>91</v>
       </c>
       <c r="D204" s="66" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="E204" s="61" t="s">
         <v>16</v>
       </c>
       <c r="F204" s="43" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="G204" s="61"/>
       <c r="H204" s="43" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="I204" s="61" t="s">
         <v>90</v>
@@ -9252,23 +9252,23 @@
         <v>204</v>
       </c>
       <c r="B205" s="55" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C205" s="60" t="s">
         <v>91</v>
       </c>
       <c r="D205" s="66" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="E205" s="61" t="s">
         <v>16</v>
       </c>
       <c r="F205" s="43" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="G205" s="61"/>
       <c r="H205" s="43" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="I205" s="61" t="s">
         <v>90</v>
@@ -9279,23 +9279,23 @@
         <v>205</v>
       </c>
       <c r="B206" s="55" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C206" s="60" t="s">
         <v>91</v>
       </c>
       <c r="D206" s="66" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="E206" s="61" t="s">
         <v>16</v>
       </c>
       <c r="F206" s="43" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="G206" s="61"/>
       <c r="H206" s="43" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I206" s="61" t="s">
         <v>90</v>
@@ -9306,20 +9306,20 @@
         <v>206</v>
       </c>
       <c r="B207" s="55" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C207" s="58" t="s">
         <v>588</v>
       </c>
       <c r="D207" s="63" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="E207" s="62"/>
       <c r="F207" s="62"/>
       <c r="G207" s="62"/>
       <c r="H207" s="62"/>
       <c r="I207" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="208" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
@@ -9327,20 +9327,20 @@
         <v>207</v>
       </c>
       <c r="B208" s="55" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C208" s="58" t="s">
         <v>588</v>
       </c>
       <c r="D208" s="63" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="E208" s="62"/>
       <c r="F208" s="62"/>
       <c r="G208" s="62"/>
       <c r="H208" s="62"/>
       <c r="I208" s="1" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
   </sheetData>
@@ -10115,7 +10115,7 @@
         <v>593</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>620</v>
@@ -10141,7 +10141,7 @@
         <v>593</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>620</v>
@@ -10165,7 +10165,7 @@
         <v>593</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>620</v>
@@ -10189,7 +10189,7 @@
         <v>593</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>620</v>
@@ -10213,7 +10213,7 @@
         <v>593</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D36" s="15" t="s">
         <v>620</v>
@@ -10237,7 +10237,7 @@
         <v>593</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D37" s="15" t="s">
         <v>620</v>
@@ -10261,7 +10261,7 @@
         <v>593</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>620</v>
@@ -10285,7 +10285,7 @@
         <v>593</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>620</v>
@@ -10311,7 +10311,7 @@
         <v>593</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D40" s="15" t="s">
         <v>620</v>
@@ -10335,7 +10335,7 @@
         <v>593</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>620</v>
@@ -10359,7 +10359,7 @@
         <v>593</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>620</v>
@@ -10811,7 +10811,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="14" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" s="14" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A61" s="15" t="s">
         <v>137</v>
       </c>
@@ -11248,7 +11248,7 @@
         <v>497</v>
       </c>
       <c r="H78" s="15" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -11274,7 +11274,7 @@
         <v>498</v>
       </c>
       <c r="H79" s="15" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
@@ -12570,10 +12570,10 @@
         <v>137</v>
       </c>
       <c r="B133" s="69" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C133" s="19" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="D133" s="51" t="s">
         <v>16</v>
@@ -12582,11 +12582,11 @@
         <v>16</v>
       </c>
       <c r="F133" s="55" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="G133" s="51"/>
       <c r="H133" s="55" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -12594,10 +12594,10 @@
         <v>137</v>
       </c>
       <c r="B134" s="69" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C134" s="19" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="D134" s="51" t="s">
         <v>16</v>
@@ -12606,11 +12606,11 @@
         <v>16</v>
       </c>
       <c r="F134" s="55" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="G134" s="61"/>
       <c r="H134" s="55" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -12618,10 +12618,10 @@
         <v>137</v>
       </c>
       <c r="B135" s="69" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C135" s="19" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="D135" s="51" t="s">
         <v>16</v>
@@ -12630,11 +12630,11 @@
         <v>16</v>
       </c>
       <c r="F135" s="55" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="G135" s="61"/>
       <c r="H135" s="55" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -12642,10 +12642,10 @@
         <v>137</v>
       </c>
       <c r="B136" s="69" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C136" s="19" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="D136" s="51" t="s">
         <v>16</v>
@@ -12654,11 +12654,11 @@
         <v>16</v>
       </c>
       <c r="F136" s="55" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="G136" s="61"/>
       <c r="H136" s="1" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
     <row r="137" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -12666,10 +12666,10 @@
         <v>137</v>
       </c>
       <c r="B137" s="69" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C137" s="19" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="D137" s="51" t="s">
         <v>16</v>
@@ -12678,11 +12678,11 @@
         <v>16</v>
       </c>
       <c r="F137" s="43" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="G137" s="61"/>
       <c r="H137" s="43" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -12690,10 +12690,10 @@
         <v>137</v>
       </c>
       <c r="B138" s="69" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C138" s="19" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="D138" s="51" t="s">
         <v>16</v>
@@ -12702,11 +12702,11 @@
         <v>16</v>
       </c>
       <c r="F138" s="43" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="G138" s="61"/>
       <c r="H138" s="43" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.35">
@@ -12714,10 +12714,10 @@
         <v>137</v>
       </c>
       <c r="B139" s="69" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C139" s="19" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="D139" s="51" t="s">
         <v>16</v>
@@ -12726,11 +12726,11 @@
         <v>16</v>
       </c>
       <c r="F139" s="43" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="G139" s="43"/>
       <c r="H139" s="43" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -12744,17 +12744,17 @@
         <v>580</v>
       </c>
       <c r="D140" s="71" t="s">
+        <v>978</v>
+      </c>
+      <c r="E140" s="73" t="s">
+        <v>979</v>
+      </c>
+      <c r="F140" s="73" t="s">
         <v>980</v>
-      </c>
-      <c r="E140" s="73" t="s">
-        <v>981</v>
-      </c>
-      <c r="F140" s="73" t="s">
-        <v>982</v>
       </c>
       <c r="G140" s="72"/>
       <c r="H140" s="72" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
@@ -12768,17 +12768,17 @@
         <v>580</v>
       </c>
       <c r="D141" s="71" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="E141" s="61" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="F141" s="61" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="G141" s="61"/>
       <c r="H141" s="61" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
     </row>
     <row r="142" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -12792,19 +12792,19 @@
         <v>580</v>
       </c>
       <c r="D142" s="71" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="E142" s="61" t="s">
+        <v>985</v>
+      </c>
+      <c r="F142" s="61" t="s">
+        <v>986</v>
+      </c>
+      <c r="G142" s="61" t="s">
         <v>987</v>
       </c>
-      <c r="F142" s="61" t="s">
+      <c r="H142" s="61" t="s">
         <v>988</v>
-      </c>
-      <c r="G142" s="61" t="s">
-        <v>989</v>
-      </c>
-      <c r="H142" s="61" t="s">
-        <v>990</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.35">
@@ -12818,17 +12818,17 @@
         <v>580</v>
       </c>
       <c r="D143" s="71" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="E143" s="61" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="F143" s="61" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="G143" s="61"/>
       <c r="H143" s="61" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.35">
@@ -12842,19 +12842,19 @@
         <v>580</v>
       </c>
       <c r="D144" s="71" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="E144" s="61" t="s">
+        <v>992</v>
+      </c>
+      <c r="F144" s="61" t="s">
+        <v>993</v>
+      </c>
+      <c r="G144" s="61" t="s">
         <v>994</v>
       </c>
-      <c r="F144" s="61" t="s">
+      <c r="H144" s="61" t="s">
         <v>995</v>
-      </c>
-      <c r="G144" s="61" t="s">
-        <v>996</v>
-      </c>
-      <c r="H144" s="61" t="s">
-        <v>997</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.35">
@@ -12868,19 +12868,19 @@
         <v>580</v>
       </c>
       <c r="D145" s="71" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="E145" s="61" t="s">
+        <v>996</v>
+      </c>
+      <c r="F145" s="61" t="s">
+        <v>997</v>
+      </c>
+      <c r="G145" s="61" t="s">
         <v>998</v>
       </c>
-      <c r="F145" s="61" t="s">
+      <c r="H145" s="61" t="s">
         <v>999</v>
-      </c>
-      <c r="G145" s="61" t="s">
-        <v>1000</v>
-      </c>
-      <c r="H145" s="61" t="s">
-        <v>1001</v>
       </c>
     </row>
     <row r="146" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
@@ -12894,17 +12894,17 @@
         <v>580</v>
       </c>
       <c r="D146" s="71" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="E146" s="61" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="F146" s="61" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="G146" s="61"/>
       <c r="H146" s="61" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
   </sheetData>
@@ -12921,6 +12921,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -13142,25 +13160,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13178,30 +13204,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
removal of trailing spaces
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D07C3F-1B85-4568-ACA7-5558633B4016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C754EBA-70F6-44F9-A23E-6B96C7697F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1570" yWindow="260" windowWidth="16160" windowHeight="9850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="250" windowWidth="16800" windowHeight="9850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2391" uniqueCount="1084">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2391" uniqueCount="1083">
   <si>
     <t>Preferred Term</t>
   </si>
@@ -3056,10 +3056,6 @@
     <t>The textual representation of the chronological relationship between temporal events.</t>
   </si>
   <si>
-    <t xml:space="preserve">Timing Window, Lower
-</t>
-  </si>
-  <si>
     <t>The earliest chronological value of an allowable period of time during which a temporal event takes place.</t>
   </si>
   <si>
@@ -3228,27 +3224,6 @@
     <t>sectionTitle</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
     <t>C44476</t>
   </si>
   <si>
@@ -3310,6 +3285,9 @@
   </si>
   <si>
     <t>label</t>
+  </si>
+  <si>
+    <t>Timing Window, Lower</t>
   </si>
 </sst>
 </file>
@@ -3537,7 +3515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3772,9 +3750,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4834,7 +4809,7 @@
         <v>91</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>504</v>
@@ -5104,7 +5079,7 @@
         <v>583</v>
       </c>
       <c r="D41" s="56" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="E41" s="57"/>
       <c r="F41" s="58"/>
@@ -5125,7 +5100,7 @@
         <v>583</v>
       </c>
       <c r="D42" s="56" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="E42" s="57"/>
       <c r="F42" s="58"/>
@@ -5281,7 +5256,7 @@
         <v>91</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E48" s="43" t="s">
         <v>16</v>
@@ -5308,7 +5283,7 @@
         <v>91</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E49" s="43" t="s">
         <v>16</v>
@@ -5318,7 +5293,7 @@
       </c>
       <c r="G49" s="43"/>
       <c r="H49" s="43" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>90</v>
@@ -5445,17 +5420,17 @@
         <v>91</v>
       </c>
       <c r="D54" s="31" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>96</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>90</v>
@@ -5475,14 +5450,14 @@
         <v>589</v>
       </c>
       <c r="E55" s="4" t="s">
+        <v>1041</v>
+      </c>
+      <c r="F55" s="4" t="s">
         <v>1042</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>1043</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>90</v>
@@ -5526,7 +5501,7 @@
         <v>91</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>31</v>
@@ -5536,7 +5511,7 @@
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="4" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>603</v>
@@ -5553,17 +5528,17 @@
         <v>91</v>
       </c>
       <c r="D58" s="31" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E58" s="43" t="s">
         <v>16</v>
       </c>
       <c r="F58" s="43" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="G58" s="70"/>
       <c r="H58" s="1" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="I58" s="43" t="s">
         <v>90</v>
@@ -5607,7 +5582,7 @@
         <v>91</v>
       </c>
       <c r="D60" s="31" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>661</v>
@@ -5617,7 +5592,7 @@
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="I60" s="43" t="s">
         <v>90</v>
@@ -5742,17 +5717,17 @@
         <v>91</v>
       </c>
       <c r="D65" s="30" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E65" s="43" t="s">
         <v>16</v>
       </c>
       <c r="F65" s="43" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="G65" s="70"/>
       <c r="H65" s="1" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="I65" s="43" t="s">
         <v>90</v>
@@ -5817,7 +5792,7 @@
         <v>91</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E68" s="4" t="s">
         <v>115</v>
@@ -5827,7 +5802,7 @@
       </c>
       <c r="G68" s="4"/>
       <c r="H68" s="4" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>90</v>
@@ -5871,23 +5846,23 @@
         <v>91</v>
       </c>
       <c r="D70" s="31" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E70" s="43" t="s">
         <v>16</v>
       </c>
       <c r="F70" s="43" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="G70" s="70"/>
       <c r="H70" s="1" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="I70" s="43" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" ht="100" x14ac:dyDescent="0.35">
       <c r="A71" s="33">
         <v>70</v>
       </c>
@@ -5925,7 +5900,7 @@
         <v>91</v>
       </c>
       <c r="D72" s="30" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>662</v>
@@ -5935,7 +5910,7 @@
       </c>
       <c r="G72" s="3"/>
       <c r="H72" s="4" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="I72" s="43" t="s">
         <v>90</v>
@@ -5952,7 +5927,7 @@
         <v>91</v>
       </c>
       <c r="D73" s="31" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>663</v>
@@ -6033,7 +6008,7 @@
         <v>583</v>
       </c>
       <c r="D76" s="42" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="4"/>
@@ -6054,7 +6029,7 @@
         <v>583</v>
       </c>
       <c r="D77" s="42" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="4"/>
@@ -6123,7 +6098,7 @@
         <v>91</v>
       </c>
       <c r="D80" s="31" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>119</v>
@@ -6150,7 +6125,7 @@
         <v>91</v>
       </c>
       <c r="D81" s="31" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>118</v>
@@ -6160,7 +6135,7 @@
       </c>
       <c r="G81" s="4"/>
       <c r="H81" s="4" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>90</v>
@@ -6204,7 +6179,7 @@
         <v>91</v>
       </c>
       <c r="D83" s="31" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>667</v>
@@ -6285,7 +6260,7 @@
         <v>91</v>
       </c>
       <c r="D86" s="31" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>63</v>
@@ -6312,7 +6287,7 @@
         <v>91</v>
       </c>
       <c r="D87" s="31" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>669</v>
@@ -6322,7 +6297,7 @@
       </c>
       <c r="G87" s="4"/>
       <c r="H87" s="4" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="I87" s="43" t="s">
         <v>90</v>
@@ -6366,7 +6341,7 @@
         <v>583</v>
       </c>
       <c r="D89" s="42" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
@@ -6387,7 +6362,7 @@
         <v>583</v>
       </c>
       <c r="D90" s="42" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
@@ -6477,7 +6452,7 @@
         <v>91</v>
       </c>
       <c r="D94" s="31" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>671</v>
@@ -6504,7 +6479,7 @@
         <v>91</v>
       </c>
       <c r="D95" s="31" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>672</v>
@@ -6514,7 +6489,7 @@
       </c>
       <c r="G95" s="4"/>
       <c r="H95" s="4" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="I95" s="1" t="s">
         <v>90</v>
@@ -6558,7 +6533,7 @@
         <v>91</v>
       </c>
       <c r="D97" s="31" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>673</v>
@@ -6568,7 +6543,7 @@
       </c>
       <c r="G97" s="4"/>
       <c r="H97" s="4" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="I97" s="1" t="s">
         <v>90</v>
@@ -6654,7 +6629,7 @@
         <v>583</v>
       </c>
       <c r="D101" s="63" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="4"/>
@@ -6675,7 +6650,7 @@
         <v>91</v>
       </c>
       <c r="D102" s="31" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E102" s="4" t="s">
         <v>112</v>
@@ -6702,7 +6677,7 @@
         <v>91</v>
       </c>
       <c r="D103" s="31" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>674</v>
@@ -6712,7 +6687,7 @@
       </c>
       <c r="G103" s="4"/>
       <c r="H103" s="4" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="I103" s="43" t="s">
         <v>90</v>
@@ -6729,7 +6704,7 @@
         <v>583</v>
       </c>
       <c r="D104" s="42" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
@@ -6750,7 +6725,7 @@
         <v>583</v>
       </c>
       <c r="D105" s="42" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
@@ -6963,7 +6938,7 @@
         <v>583</v>
       </c>
       <c r="D114" s="47" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E114" s="1"/>
       <c r="F114" s="4"/>
@@ -6984,7 +6959,7 @@
         <v>583</v>
       </c>
       <c r="D115" s="47" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="4"/>
@@ -7005,7 +6980,7 @@
         <v>583</v>
       </c>
       <c r="D116" s="56" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="E116" s="55"/>
       <c r="F116" s="58"/>
@@ -7026,7 +7001,7 @@
         <v>91</v>
       </c>
       <c r="D117" s="31" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E117" s="4" t="s">
         <v>678</v>
@@ -7053,7 +7028,7 @@
         <v>91</v>
       </c>
       <c r="D118" s="31" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>526</v>
@@ -7063,7 +7038,7 @@
       </c>
       <c r="G118" s="4"/>
       <c r="H118" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="I118" s="4" t="s">
         <v>90</v>
@@ -7258,7 +7233,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A126" s="33">
         <v>125</v>
       </c>
@@ -7269,7 +7244,7 @@
         <v>91</v>
       </c>
       <c r="D126" s="31" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E126" s="43" t="s">
         <v>16</v>
@@ -7296,7 +7271,7 @@
         <v>91</v>
       </c>
       <c r="D127" s="65" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E127" s="43" t="s">
         <v>16</v>
@@ -7306,7 +7281,7 @@
       </c>
       <c r="G127" s="61"/>
       <c r="H127" s="61" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="I127" s="43" t="s">
         <v>90</v>
@@ -7488,7 +7463,7 @@
         <v>91</v>
       </c>
       <c r="D135" s="31" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>682</v>
@@ -7498,7 +7473,7 @@
       </c>
       <c r="G135" s="4"/>
       <c r="H135" s="4" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="I135" s="43" t="s">
         <v>90</v>
@@ -7542,7 +7517,7 @@
         <v>91</v>
       </c>
       <c r="D137" s="31" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E137" s="4" t="s">
         <v>684</v>
@@ -7569,7 +7544,7 @@
         <v>91</v>
       </c>
       <c r="D138" s="31" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E138" s="4" t="s">
         <v>685</v>
@@ -7579,7 +7554,7 @@
       </c>
       <c r="G138" s="4"/>
       <c r="H138" s="4" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="I138" s="43" t="s">
         <v>90</v>
@@ -8091,7 +8066,7 @@
         <v>91</v>
       </c>
       <c r="D158" s="30" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E158" s="43" t="s">
         <v>16</v>
@@ -8247,7 +8222,7 @@
         <v>91</v>
       </c>
       <c r="D164" s="30" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E164" s="43" t="s">
         <v>16</v>
@@ -8484,7 +8459,7 @@
         <v>91</v>
       </c>
       <c r="D173" s="30" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E173" s="43" t="s">
         <v>16</v>
@@ -8511,7 +8486,7 @@
         <v>91</v>
       </c>
       <c r="D174" s="30" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="E174" s="43" t="s">
         <v>16</v>
@@ -8521,7 +8496,7 @@
       </c>
       <c r="G174" s="43"/>
       <c r="H174" s="43" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="I174" s="43" t="s">
         <v>90</v>
@@ -8592,7 +8567,7 @@
         <v>583</v>
       </c>
       <c r="D177" s="47" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="E177" s="33"/>
       <c r="F177" s="33"/>
@@ -8613,7 +8588,7 @@
         <v>583</v>
       </c>
       <c r="D178" s="47" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="E178" s="33"/>
       <c r="F178" s="33"/>
@@ -8634,7 +8609,7 @@
         <v>91</v>
       </c>
       <c r="D179" s="30" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E179" s="43" t="s">
         <v>16</v>
@@ -8661,7 +8636,7 @@
         <v>91</v>
       </c>
       <c r="D180" s="30" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="E180" s="43" t="s">
         <v>16</v>
@@ -8671,7 +8646,7 @@
       </c>
       <c r="G180" s="43"/>
       <c r="H180" s="43" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="I180" s="43" t="s">
         <v>90</v>
@@ -8763,7 +8738,7 @@
         <v>583</v>
       </c>
       <c r="D184" s="63" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="E184" s="61"/>
       <c r="F184" s="55"/>
@@ -8892,7 +8867,7 @@
         <v>583</v>
       </c>
       <c r="D189" s="56" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="E189" s="61"/>
       <c r="F189" s="62"/>
@@ -8913,7 +8888,7 @@
         <v>583</v>
       </c>
       <c r="D190" s="56" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="E190" s="61"/>
       <c r="F190" s="62"/>
@@ -8934,7 +8909,7 @@
         <v>583</v>
       </c>
       <c r="D191" s="56" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="E191" s="61"/>
       <c r="F191" s="62"/>
@@ -8955,7 +8930,7 @@
         <v>583</v>
       </c>
       <c r="D192" s="56" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="E192" s="61"/>
       <c r="F192" s="62"/>
@@ -9003,7 +8978,7 @@
         <v>91</v>
       </c>
       <c r="D194" s="66" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E194" s="61" t="s">
         <v>16</v>
@@ -9030,7 +9005,7 @@
         <v>91</v>
       </c>
       <c r="D195" s="66" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E195" s="61" t="s">
         <v>16</v>
@@ -9040,7 +9015,7 @@
       </c>
       <c r="G195" s="61"/>
       <c r="H195" s="61" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="I195" s="61" t="s">
         <v>90</v>
@@ -9132,7 +9107,7 @@
         <v>583</v>
       </c>
       <c r="D199" s="63" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="E199" s="61"/>
       <c r="F199" s="62"/>
@@ -9336,7 +9311,7 @@
         <v>91</v>
       </c>
       <c r="D207" s="66" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="E207" s="61" t="s">
         <v>16</v>
@@ -9369,11 +9344,11 @@
         <v>16</v>
       </c>
       <c r="F208" s="43" t="s">
-        <v>1005</v>
+        <v>1082</v>
       </c>
       <c r="G208" s="61"/>
       <c r="H208" s="43" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="I208" s="61" t="s">
         <v>90</v>
@@ -9396,11 +9371,11 @@
         <v>16</v>
       </c>
       <c r="F209" s="43" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="G209" s="61"/>
       <c r="H209" s="43" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="I209" s="61" t="s">
         <v>90</v>
@@ -9417,17 +9392,17 @@
         <v>91</v>
       </c>
       <c r="D210" s="66" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="E210" s="43" t="s">
         <v>16</v>
       </c>
       <c r="F210" s="43" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="G210" s="70"/>
       <c r="H210" s="43" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="I210" s="43" t="s">
         <v>90</v>
@@ -9444,17 +9419,17 @@
         <v>91</v>
       </c>
       <c r="D211" s="66" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="E211" s="43" t="s">
         <v>16</v>
       </c>
       <c r="F211" s="43" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="G211" s="70"/>
       <c r="H211" s="1" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="I211" s="43" t="s">
         <v>90</v>
@@ -9471,7 +9446,7 @@
         <v>583</v>
       </c>
       <c r="D212" s="63" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="E212" s="62"/>
       <c r="F212" s="62"/>
@@ -9492,7 +9467,7 @@
         <v>583</v>
       </c>
       <c r="D213" s="63" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="E213" s="62"/>
       <c r="F213" s="62"/>
@@ -9507,23 +9482,23 @@
         <v>213</v>
       </c>
       <c r="B214" s="55" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C214" s="58" t="s">
         <v>4</v>
       </c>
       <c r="D214" s="54" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="E214" s="43" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="F214" s="43" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="G214" s="70"/>
       <c r="H214" s="43" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="I214" s="43" t="s">
         <v>937</v>
@@ -9534,23 +9509,23 @@
         <v>214</v>
       </c>
       <c r="B215" s="55" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C215" s="60" t="s">
         <v>91</v>
       </c>
       <c r="D215" s="30" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="E215" s="43" t="s">
         <v>16</v>
       </c>
       <c r="F215" s="43" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="G215" s="70"/>
       <c r="H215" s="43" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="I215" s="43" t="s">
         <v>90</v>
@@ -9561,50 +9536,50 @@
         <v>215</v>
       </c>
       <c r="B216" s="55" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C216" s="60" t="s">
         <v>91</v>
       </c>
       <c r="D216" s="30" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="E216" s="43" t="s">
         <v>16</v>
       </c>
       <c r="F216" s="43" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="G216" s="43"/>
       <c r="H216" s="43" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="I216" s="43" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="217" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A217" s="33">
         <v>216</v>
       </c>
       <c r="B217" s="55" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C217" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="D217" s="79" t="s">
-        <v>1062</v>
+      <c r="D217" s="65" t="s">
+        <v>1011</v>
       </c>
       <c r="E217" s="43" t="s">
         <v>16</v>
       </c>
       <c r="F217" s="43" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="G217" s="43"/>
       <c r="H217" s="43" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="I217" s="43" t="s">
         <v>90</v>
@@ -9615,7 +9590,7 @@
         <v>217</v>
       </c>
       <c r="B218" s="55" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C218" s="60" t="s">
         <v>91</v>
@@ -9627,11 +9602,11 @@
         <v>16</v>
       </c>
       <c r="F218" s="43" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="G218" s="70"/>
       <c r="H218" s="43" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="I218" s="70" t="s">
         <v>90</v>
@@ -9642,13 +9617,13 @@
         <v>218</v>
       </c>
       <c r="B219" s="55" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C219" s="58" t="s">
         <v>583</v>
       </c>
       <c r="D219" s="63" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="E219" s="62"/>
       <c r="F219" s="62"/>
@@ -13245,15 +13220,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -13475,6 +13441,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
   <ds:schemaRefs>
@@ -13484,24 +13459,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13519,4 +13476,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
revert Description to description in 3 entities
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C754EBA-70F6-44F9-A23E-6B96C7697F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A17D03-8099-4117-B1F7-8CA1EE8D79C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="250" windowWidth="16800" windowHeight="9850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="DDF valid value sets" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DDF Entities&amp;Attributes'!$A$1:$I$213</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DDF Entities&amp;Attributes'!$A$1:$I$219</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DDF valid value sets'!$A$6:$M$124</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2391" uniqueCount="1083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2391" uniqueCount="1082">
   <si>
     <t>Preferred Term</t>
   </si>
@@ -3081,9 +3081,6 @@
   </si>
   <si>
     <t>bcCategoryChildren</t>
-  </si>
-  <si>
-    <t>Description</t>
   </si>
   <si>
     <t>encounterScheduledAtTiming</t>
@@ -5293,7 +5290,7 @@
       </c>
       <c r="G49" s="43"/>
       <c r="H49" s="43" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>90</v>
@@ -5426,11 +5423,11 @@
         <v>96</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>90</v>
@@ -5450,14 +5447,14 @@
         <v>589</v>
       </c>
       <c r="E55" s="4" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F55" s="4" t="s">
         <v>1041</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>1042</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>90</v>
@@ -5511,7 +5508,7 @@
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="4" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>603</v>
@@ -5534,11 +5531,11 @@
         <v>16</v>
       </c>
       <c r="F58" s="43" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="G58" s="70"/>
       <c r="H58" s="1" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="I58" s="43" t="s">
         <v>90</v>
@@ -5592,7 +5589,7 @@
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I60" s="43" t="s">
         <v>90</v>
@@ -5723,11 +5720,11 @@
         <v>16</v>
       </c>
       <c r="F65" s="43" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="G65" s="70"/>
       <c r="H65" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="I65" s="43" t="s">
         <v>90</v>
@@ -5802,7 +5799,7 @@
       </c>
       <c r="G68" s="4"/>
       <c r="H68" s="4" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>90</v>
@@ -5852,17 +5849,17 @@
         <v>16</v>
       </c>
       <c r="F70" s="43" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G70" s="70"/>
       <c r="H70" s="1" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="I70" s="43" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="100" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A71" s="33">
         <v>70</v>
       </c>
@@ -5910,7 +5907,7 @@
       </c>
       <c r="G72" s="3"/>
       <c r="H72" s="4" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="I72" s="43" t="s">
         <v>90</v>
@@ -5927,7 +5924,7 @@
         <v>91</v>
       </c>
       <c r="D73" s="31" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>663</v>
@@ -6008,7 +6005,7 @@
         <v>583</v>
       </c>
       <c r="D76" s="42" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="4"/>
@@ -6029,7 +6026,7 @@
         <v>583</v>
       </c>
       <c r="D77" s="42" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="4"/>
@@ -6135,7 +6132,7 @@
       </c>
       <c r="G81" s="4"/>
       <c r="H81" s="4" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>90</v>
@@ -6179,7 +6176,7 @@
         <v>91</v>
       </c>
       <c r="D83" s="31" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>667</v>
@@ -6297,7 +6294,7 @@
       </c>
       <c r="G87" s="4"/>
       <c r="H87" s="4" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="I87" s="43" t="s">
         <v>90</v>
@@ -6341,7 +6338,7 @@
         <v>583</v>
       </c>
       <c r="D89" s="42" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
@@ -6362,7 +6359,7 @@
         <v>583</v>
       </c>
       <c r="D90" s="42" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
@@ -6489,7 +6486,7 @@
       </c>
       <c r="G95" s="4"/>
       <c r="H95" s="4" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="I95" s="1" t="s">
         <v>90</v>
@@ -6543,7 +6540,7 @@
       </c>
       <c r="G97" s="4"/>
       <c r="H97" s="4" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="I97" s="1" t="s">
         <v>90</v>
@@ -6629,7 +6626,7 @@
         <v>583</v>
       </c>
       <c r="D101" s="63" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="4"/>
@@ -6677,7 +6674,7 @@
         <v>91</v>
       </c>
       <c r="D103" s="31" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>674</v>
@@ -6687,7 +6684,7 @@
       </c>
       <c r="G103" s="4"/>
       <c r="H103" s="4" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="I103" s="43" t="s">
         <v>90</v>
@@ -6704,7 +6701,7 @@
         <v>583</v>
       </c>
       <c r="D104" s="42" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="4"/>
@@ -6725,7 +6722,7 @@
         <v>583</v>
       </c>
       <c r="D105" s="42" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
@@ -6938,7 +6935,7 @@
         <v>583</v>
       </c>
       <c r="D114" s="47" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="E114" s="1"/>
       <c r="F114" s="4"/>
@@ -6959,7 +6956,7 @@
         <v>583</v>
       </c>
       <c r="D115" s="47" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="4"/>
@@ -7038,7 +7035,7 @@
       </c>
       <c r="G118" s="4"/>
       <c r="H118" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="I118" s="4" t="s">
         <v>90</v>
@@ -7233,7 +7230,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" s="33">
         <v>125</v>
       </c>
@@ -7281,7 +7278,7 @@
       </c>
       <c r="G127" s="61"/>
       <c r="H127" s="61" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="I127" s="43" t="s">
         <v>90</v>
@@ -7473,7 +7470,7 @@
       </c>
       <c r="G135" s="4"/>
       <c r="H135" s="4" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="I135" s="43" t="s">
         <v>90</v>
@@ -7554,7 +7551,7 @@
       </c>
       <c r="G138" s="4"/>
       <c r="H138" s="4" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="I138" s="43" t="s">
         <v>90</v>
@@ -8486,7 +8483,7 @@
         <v>91</v>
       </c>
       <c r="D174" s="30" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="E174" s="43" t="s">
         <v>16</v>
@@ -8496,7 +8493,7 @@
       </c>
       <c r="G174" s="43"/>
       <c r="H174" s="43" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="I174" s="43" t="s">
         <v>90</v>
@@ -8567,7 +8564,7 @@
         <v>583</v>
       </c>
       <c r="D177" s="47" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="E177" s="33"/>
       <c r="F177" s="33"/>
@@ -8636,7 +8633,7 @@
         <v>91</v>
       </c>
       <c r="D180" s="30" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="E180" s="43" t="s">
         <v>16</v>
@@ -8646,7 +8643,7 @@
       </c>
       <c r="G180" s="43"/>
       <c r="H180" s="43" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="I180" s="43" t="s">
         <v>90</v>
@@ -8738,7 +8735,7 @@
         <v>583</v>
       </c>
       <c r="D184" s="63" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="E184" s="61"/>
       <c r="F184" s="55"/>
@@ -8867,7 +8864,7 @@
         <v>583</v>
       </c>
       <c r="D189" s="56" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="E189" s="61"/>
       <c r="F189" s="62"/>
@@ -8888,7 +8885,7 @@
         <v>583</v>
       </c>
       <c r="D190" s="56" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="E190" s="61"/>
       <c r="F190" s="62"/>
@@ -8909,7 +8906,7 @@
         <v>583</v>
       </c>
       <c r="D191" s="56" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="E191" s="61"/>
       <c r="F191" s="62"/>
@@ -8930,7 +8927,7 @@
         <v>583</v>
       </c>
       <c r="D192" s="56" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="E192" s="61"/>
       <c r="F192" s="62"/>
@@ -9015,7 +9012,7 @@
       </c>
       <c r="G195" s="61"/>
       <c r="H195" s="61" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="I195" s="61" t="s">
         <v>90</v>
@@ -9107,7 +9104,7 @@
         <v>583</v>
       </c>
       <c r="D199" s="63" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="E199" s="61"/>
       <c r="F199" s="62"/>
@@ -9344,7 +9341,7 @@
         <v>16</v>
       </c>
       <c r="F208" s="43" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="G208" s="61"/>
       <c r="H208" s="43" t="s">
@@ -9392,17 +9389,17 @@
         <v>91</v>
       </c>
       <c r="D210" s="66" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="E210" s="43" t="s">
         <v>16</v>
       </c>
       <c r="F210" s="43" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="G210" s="70"/>
       <c r="H210" s="43" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="I210" s="43" t="s">
         <v>90</v>
@@ -9425,11 +9422,11 @@
         <v>16</v>
       </c>
       <c r="F211" s="43" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="G211" s="70"/>
       <c r="H211" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="I211" s="43" t="s">
         <v>90</v>
@@ -9446,7 +9443,7 @@
         <v>583</v>
       </c>
       <c r="D212" s="63" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="E212" s="62"/>
       <c r="F212" s="62"/>
@@ -9467,7 +9464,7 @@
         <v>583</v>
       </c>
       <c r="D213" s="63" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="E213" s="62"/>
       <c r="F213" s="62"/>
@@ -9482,23 +9479,23 @@
         <v>213</v>
       </c>
       <c r="B214" s="55" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C214" s="58" t="s">
         <v>4</v>
       </c>
       <c r="D214" s="54" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="E214" s="43" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="F214" s="43" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="G214" s="70"/>
       <c r="H214" s="43" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="I214" s="43" t="s">
         <v>937</v>
@@ -9509,23 +9506,23 @@
         <v>214</v>
       </c>
       <c r="B215" s="55" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C215" s="60" t="s">
         <v>91</v>
       </c>
       <c r="D215" s="30" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="E215" s="43" t="s">
         <v>16</v>
       </c>
       <c r="F215" s="43" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="G215" s="70"/>
       <c r="H215" s="43" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="I215" s="43" t="s">
         <v>90</v>
@@ -9536,23 +9533,23 @@
         <v>215</v>
       </c>
       <c r="B216" s="55" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C216" s="60" t="s">
         <v>91</v>
       </c>
       <c r="D216" s="30" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="E216" s="43" t="s">
         <v>16</v>
       </c>
       <c r="F216" s="43" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="G216" s="43"/>
       <c r="H216" s="43" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="I216" s="43" t="s">
         <v>90</v>
@@ -9563,7 +9560,7 @@
         <v>216</v>
       </c>
       <c r="B217" s="55" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C217" s="60" t="s">
         <v>91</v>
@@ -9575,11 +9572,11 @@
         <v>16</v>
       </c>
       <c r="F217" s="43" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="G217" s="43"/>
       <c r="H217" s="43" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="I217" s="43" t="s">
         <v>90</v>
@@ -9590,7 +9587,7 @@
         <v>217</v>
       </c>
       <c r="B218" s="55" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C218" s="60" t="s">
         <v>91</v>
@@ -9602,11 +9599,11 @@
         <v>16</v>
       </c>
       <c r="F218" s="43" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="G218" s="70"/>
       <c r="H218" s="43" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I218" s="70" t="s">
         <v>90</v>
@@ -9617,13 +9614,13 @@
         <v>218</v>
       </c>
       <c r="B219" s="55" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C219" s="58" t="s">
         <v>583</v>
       </c>
       <c r="D219" s="63" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="E219" s="62"/>
       <c r="F219" s="62"/>
@@ -9634,7 +9631,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I213" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I219" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -13211,12 +13208,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13442,18 +13439,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13479,19 +13486,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update definition for 'label' attributes
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E38934-B1F7-496A-AE12-CD551C4C51BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83AB76D-8C9C-46FD-A4EB-E8A5D11BD03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="0" windowWidth="18760" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="410" yWindow="120" windowWidth="16950" windowHeight="9820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
     <sheet name="DDF valid value sets" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DDF Entities&amp;Attributes'!$A$1:$I$239</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DDF Entities&amp;Attributes'!$A$1:$I$249</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DDF valid value sets'!$A$6:$M$124</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -3257,9 +3257,6 @@
     <t>Timing Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the timing.</t>
-  </si>
-  <si>
     <t>Timing Name</t>
   </si>
   <si>
@@ -3317,9 +3314,6 @@
     <t>Syntax Template Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the syntax template.</t>
-  </si>
-  <si>
     <t>templateText</t>
   </si>
   <si>
@@ -3350,9 +3344,6 @@
     <t>Syntax Template Dictionary Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the syntax template dictionary.</t>
-  </si>
-  <si>
     <t>Syntax Template Dictionary Parameter Map</t>
   </si>
   <si>
@@ -3362,109 +3353,118 @@
     <t>Organization Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the organization.</t>
-  </si>
-  <si>
     <t>Study Design Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the study design.</t>
-  </si>
-  <si>
     <t>Indication Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the indication.</t>
-  </si>
-  <si>
     <t>Study Design Population Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the study design population.</t>
-  </si>
-  <si>
     <t>Study Objective Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the study objective.</t>
-  </si>
-  <si>
     <t>Study Arm Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the study arm.</t>
-  </si>
-  <si>
     <t>Study Epoch Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the study epoch.</t>
-  </si>
-  <si>
     <t>Study Element Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the study element.</t>
-  </si>
-  <si>
     <t>Encounter Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the encounter.</t>
-  </si>
-  <si>
     <t>Activity Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the activity.</t>
-  </si>
-  <si>
     <t>Procedure Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the procedure.</t>
-  </si>
-  <si>
     <t>Intercurrent Event Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the intercurrent event.</t>
-  </si>
-  <si>
     <t>Biomedical Concept Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the biomedical concept.</t>
-  </si>
-  <si>
     <t>Biomedical Concept Property Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the biomedical concept property.</t>
-  </si>
-  <si>
     <t>Biomedical Concept Surrogate Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the biomedical concept surrogate.</t>
-  </si>
-  <si>
     <t>Biomedical Concept Category Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the biomedical concept category.</t>
-  </si>
-  <si>
     <t>Schedule Timeline Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the schedule timeline.</t>
-  </si>
-  <si>
     <t>Content Label</t>
   </si>
   <si>
-    <t>The identifying or descriptive marker that is attached to the content.</t>
+    <t>The short descriptive designation for the organization.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the study design.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the indication.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the study design population.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the study objective.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the study arm.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the study epoch.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the study element.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the encounter.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the activity.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the procedure.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the intercurrent event.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the biomedical concept.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the biomedical concept property.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the biomedical concept surrogate.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the biomedical concept category.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the schedule timeline.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the timing.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the content.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the syntax template.</t>
+  </si>
+  <si>
+    <t>The short descriptive designation for the syntax template dictionary.</t>
   </si>
 </sst>
 </file>
@@ -3847,21 +3847,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -3882,6 +3867,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4380,7 +4380,7 @@
         <v>91</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>33</v>
@@ -4968,7 +4968,7 @@
         <v>91</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>656</v>
@@ -4995,19 +4995,19 @@
         <v>91</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F31" s="58" t="s">
-        <v>1106</v>
-      </c>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58" t="s">
-        <v>1107</v>
-      </c>
-      <c r="I31" s="58" t="s">
+      <c r="F31" s="53" t="s">
+        <v>1103</v>
+      </c>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53" t="s">
+        <v>1121</v>
+      </c>
+      <c r="I31" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -5219,10 +5219,10 @@
       <c r="D41" s="49" t="s">
         <v>891</v>
       </c>
-      <c r="E41" s="59"/>
+      <c r="E41" s="54"/>
       <c r="F41" s="48"/>
-      <c r="G41" s="59"/>
-      <c r="H41" s="59"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="54"/>
       <c r="I41" s="1" t="s">
         <v>933</v>
       </c>
@@ -5240,10 +5240,10 @@
       <c r="D42" s="49" t="s">
         <v>1003</v>
       </c>
-      <c r="E42" s="59"/>
+      <c r="E42" s="54"/>
       <c r="F42" s="48"/>
-      <c r="G42" s="59"/>
-      <c r="H42" s="59"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
       <c r="I42" s="1" t="s">
         <v>933</v>
       </c>
@@ -5261,10 +5261,10 @@
       <c r="D43" s="49" t="s">
         <v>1004</v>
       </c>
-      <c r="E43" s="59"/>
+      <c r="E43" s="54"/>
       <c r="F43" s="48"/>
-      <c r="G43" s="59"/>
-      <c r="H43" s="59"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="54"/>
       <c r="I43" s="1" t="s">
         <v>933</v>
       </c>
@@ -5282,10 +5282,10 @@
       <c r="D44" s="49" t="s">
         <v>543</v>
       </c>
-      <c r="E44" s="59"/>
+      <c r="E44" s="54"/>
       <c r="F44" s="48"/>
-      <c r="G44" s="59"/>
-      <c r="H44" s="59"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="54"/>
       <c r="I44" s="1" t="s">
         <v>933</v>
       </c>
@@ -5301,12 +5301,12 @@
         <v>582</v>
       </c>
       <c r="D45" s="49" t="s">
-        <v>1077</v>
-      </c>
-      <c r="E45" s="59"/>
+        <v>1076</v>
+      </c>
+      <c r="E45" s="54"/>
       <c r="F45" s="48"/>
-      <c r="G45" s="59"/>
-      <c r="H45" s="59"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="54"/>
       <c r="I45" s="1" t="s">
         <v>933</v>
       </c>
@@ -5351,7 +5351,7 @@
         <v>91</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="E47" s="33" t="s">
         <v>37</v>
@@ -5546,19 +5546,19 @@
         <v>91</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F54" s="58" t="s">
-        <v>1108</v>
-      </c>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58" t="s">
-        <v>1109</v>
-      </c>
-      <c r="I54" s="58" t="s">
+      <c r="F54" s="53" t="s">
+        <v>1104</v>
+      </c>
+      <c r="G54" s="53"/>
+      <c r="H54" s="53" t="s">
+        <v>1122</v>
+      </c>
+      <c r="I54" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -5743,7 +5743,7 @@
       <c r="F61" s="3" t="s">
         <v>1065</v>
       </c>
-      <c r="G61" s="58"/>
+      <c r="G61" s="53"/>
       <c r="H61" s="1" t="s">
         <v>1066</v>
       </c>
@@ -5762,19 +5762,19 @@
         <v>91</v>
       </c>
       <c r="D62" s="23" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F62" s="58" t="s">
-        <v>1110</v>
-      </c>
-      <c r="G62" s="58"/>
-      <c r="H62" s="58" t="s">
-        <v>1111</v>
-      </c>
-      <c r="I62" s="58" t="s">
+      <c r="F62" s="53" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G62" s="53"/>
+      <c r="H62" s="53" t="s">
+        <v>1123</v>
+      </c>
+      <c r="I62" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -5959,7 +5959,7 @@
       <c r="F69" s="3" t="s">
         <v>1067</v>
       </c>
-      <c r="G69" s="58"/>
+      <c r="G69" s="53"/>
       <c r="H69" s="1" t="s">
         <v>1068</v>
       </c>
@@ -5978,19 +5978,19 @@
         <v>91</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F70" s="58" t="s">
-        <v>1112</v>
-      </c>
-      <c r="G70" s="58"/>
-      <c r="H70" s="58" t="s">
-        <v>1113</v>
-      </c>
-      <c r="I70" s="58" t="s">
+      <c r="F70" s="53" t="s">
+        <v>1106</v>
+      </c>
+      <c r="G70" s="53"/>
+      <c r="H70" s="53" t="s">
+        <v>1124</v>
+      </c>
+      <c r="I70" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -6115,7 +6115,7 @@
       <c r="F75" s="3" t="s">
         <v>1069</v>
       </c>
-      <c r="G75" s="58"/>
+      <c r="G75" s="53"/>
       <c r="H75" s="1" t="s">
         <v>1070</v>
       </c>
@@ -6134,19 +6134,19 @@
         <v>91</v>
       </c>
       <c r="D76" s="23" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F76" s="58" t="s">
-        <v>1114</v>
-      </c>
-      <c r="G76" s="58"/>
-      <c r="H76" s="58" t="s">
-        <v>1115</v>
-      </c>
-      <c r="I76" s="58" t="s">
+      <c r="F76" s="53" t="s">
+        <v>1107</v>
+      </c>
+      <c r="G76" s="53"/>
+      <c r="H76" s="53" t="s">
+        <v>1125</v>
+      </c>
+      <c r="I76" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -6440,7 +6440,7 @@
         <v>91</v>
       </c>
       <c r="D88" s="23" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>665</v>
@@ -6494,7 +6494,7 @@
         <v>91</v>
       </c>
       <c r="D90" s="23" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>667</v>
@@ -6521,19 +6521,19 @@
         <v>91</v>
       </c>
       <c r="D91" s="23" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F91" s="58" t="s">
-        <v>1116</v>
-      </c>
-      <c r="G91" s="58"/>
-      <c r="H91" s="58" t="s">
-        <v>1117</v>
-      </c>
-      <c r="I91" s="58" t="s">
+      <c r="F91" s="53" t="s">
+        <v>1108</v>
+      </c>
+      <c r="G91" s="53"/>
+      <c r="H91" s="53" t="s">
+        <v>1126</v>
+      </c>
+      <c r="I91" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -6629,7 +6629,7 @@
         <v>91</v>
       </c>
       <c r="D95" s="23" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>669</v>
@@ -6656,19 +6656,19 @@
         <v>91</v>
       </c>
       <c r="D96" s="23" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F96" s="58" t="s">
-        <v>1118</v>
-      </c>
-      <c r="G96" s="58"/>
-      <c r="H96" s="58" t="s">
-        <v>1119</v>
-      </c>
-      <c r="I96" s="58" t="s">
+      <c r="F96" s="53" t="s">
+        <v>1109</v>
+      </c>
+      <c r="G96" s="53"/>
+      <c r="H96" s="53" t="s">
+        <v>1127</v>
+      </c>
+      <c r="I96" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -6848,19 +6848,19 @@
         <v>91</v>
       </c>
       <c r="D104" s="23" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F104" s="58" t="s">
-        <v>1120</v>
-      </c>
-      <c r="G104" s="58"/>
-      <c r="H104" s="58" t="s">
-        <v>1121</v>
-      </c>
-      <c r="I104" s="58" t="s">
+      <c r="F104" s="53" t="s">
+        <v>1110</v>
+      </c>
+      <c r="G104" s="53"/>
+      <c r="H104" s="53" t="s">
+        <v>1128</v>
+      </c>
+      <c r="I104" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -6997,7 +6997,7 @@
       <c r="C110" s="1" t="s">
         <v>582</v>
       </c>
-      <c r="D110" s="60" t="s">
+      <c r="D110" s="55" t="s">
         <v>1009</v>
       </c>
       <c r="E110" s="1"/>
@@ -7073,19 +7073,19 @@
         <v>91</v>
       </c>
       <c r="D113" s="23" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F113" s="58" t="s">
-        <v>1122</v>
-      </c>
-      <c r="G113" s="58"/>
-      <c r="H113" s="58" t="s">
-        <v>1123</v>
-      </c>
-      <c r="I113" s="58" t="s">
+      <c r="F113" s="53" t="s">
+        <v>1111</v>
+      </c>
+      <c r="G113" s="53"/>
+      <c r="H113" s="53" t="s">
+        <v>1129</v>
+      </c>
+      <c r="I113" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -7142,7 +7142,7 @@
         <v>91</v>
       </c>
       <c r="D116" s="23" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>674</v>
@@ -7381,7 +7381,7 @@
       <c r="E126" s="48"/>
       <c r="F126" s="48"/>
       <c r="G126" s="48"/>
-      <c r="H126" s="58"/>
+      <c r="H126" s="53"/>
       <c r="I126" s="1" t="s">
         <v>933</v>
       </c>
@@ -7505,19 +7505,19 @@
         <v>91</v>
       </c>
       <c r="D131" s="23" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F131" s="58" t="s">
-        <v>1124</v>
-      </c>
-      <c r="G131" s="58"/>
-      <c r="H131" s="58" t="s">
-        <v>1125</v>
-      </c>
-      <c r="I131" s="58" t="s">
+      <c r="F131" s="53" t="s">
+        <v>1112</v>
+      </c>
+      <c r="G131" s="53"/>
+      <c r="H131" s="53" t="s">
+        <v>1130</v>
+      </c>
+      <c r="I131" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -7675,8 +7675,8 @@
       <c r="F137" s="3" t="s">
         <v>956</v>
       </c>
-      <c r="G137" s="58"/>
-      <c r="H137" s="58" t="s">
+      <c r="G137" s="53"/>
+      <c r="H137" s="53" t="s">
         <v>957</v>
       </c>
       <c r="I137" s="3" t="s">
@@ -7693,17 +7693,17 @@
       <c r="C138" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D138" s="55" t="s">
+      <c r="D138" s="50" t="s">
         <v>1007</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F138" s="58" t="s">
+      <c r="F138" s="53" t="s">
         <v>958</v>
       </c>
-      <c r="G138" s="58"/>
-      <c r="H138" s="58" t="s">
+      <c r="G138" s="53"/>
+      <c r="H138" s="53" t="s">
         <v>1028</v>
       </c>
       <c r="I138" s="3" t="s">
@@ -7720,20 +7720,20 @@
       <c r="C139" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D139" s="55" t="s">
-        <v>1075</v>
+      <c r="D139" s="50" t="s">
+        <v>1074</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F139" s="58" t="s">
-        <v>1126</v>
-      </c>
-      <c r="G139" s="58"/>
-      <c r="H139" s="58" t="s">
-        <v>1127</v>
-      </c>
-      <c r="I139" s="58" t="s">
+      <c r="F139" s="53" t="s">
+        <v>1113</v>
+      </c>
+      <c r="G139" s="53"/>
+      <c r="H139" s="53" t="s">
+        <v>1131</v>
+      </c>
+      <c r="I139" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -8048,19 +8048,19 @@
         <v>91</v>
       </c>
       <c r="D152" s="34" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F152" s="58" t="s">
-        <v>1128</v>
-      </c>
-      <c r="G152" s="58"/>
-      <c r="H152" s="58" t="s">
-        <v>1129</v>
-      </c>
-      <c r="I152" s="58" t="s">
+      <c r="F152" s="53" t="s">
+        <v>1114</v>
+      </c>
+      <c r="G152" s="53"/>
+      <c r="H152" s="53" t="s">
+        <v>1132</v>
+      </c>
+      <c r="I152" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -8278,7 +8278,7 @@
       <c r="C161" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D161" s="57" t="s">
+      <c r="D161" s="52" t="s">
         <v>736</v>
       </c>
       <c r="E161" s="39" t="s">
@@ -8651,19 +8651,19 @@
         <v>91</v>
       </c>
       <c r="D175" s="22" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F175" s="58" t="s">
-        <v>1130</v>
-      </c>
-      <c r="G175" s="58"/>
-      <c r="H175" s="58" t="s">
-        <v>1131</v>
-      </c>
-      <c r="I175" s="58" t="s">
+      <c r="F175" s="53" t="s">
+        <v>1115</v>
+      </c>
+      <c r="G175" s="53"/>
+      <c r="H175" s="53" t="s">
+        <v>1133</v>
+      </c>
+      <c r="I175" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -8861,19 +8861,19 @@
         <v>91</v>
       </c>
       <c r="D183" s="22" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E183" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F183" s="58" t="s">
-        <v>1132</v>
-      </c>
-      <c r="G183" s="58"/>
-      <c r="H183" s="58" t="s">
-        <v>1133</v>
-      </c>
-      <c r="I183" s="58" t="s">
+      <c r="F183" s="53" t="s">
+        <v>1116</v>
+      </c>
+      <c r="G183" s="53"/>
+      <c r="H183" s="53" t="s">
+        <v>1134</v>
+      </c>
+      <c r="I183" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9071,19 +9071,19 @@
         <v>91</v>
       </c>
       <c r="D191" s="22" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E191" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F191" s="58" t="s">
-        <v>1134</v>
-      </c>
-      <c r="G191" s="58"/>
-      <c r="H191" s="58" t="s">
+      <c r="F191" s="53" t="s">
+        <v>1117</v>
+      </c>
+      <c r="G191" s="53"/>
+      <c r="H191" s="53" t="s">
         <v>1135</v>
       </c>
-      <c r="I191" s="58" t="s">
+      <c r="I191" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9248,19 +9248,19 @@
         <v>91</v>
       </c>
       <c r="D198" s="22" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E198" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F198" s="58" t="s">
+      <c r="F198" s="53" t="s">
+        <v>1118</v>
+      </c>
+      <c r="G198" s="53"/>
+      <c r="H198" s="53" t="s">
         <v>1136</v>
       </c>
-      <c r="G198" s="58"/>
-      <c r="H198" s="58" t="s">
-        <v>1137</v>
-      </c>
-      <c r="I198" s="58" t="s">
+      <c r="I198" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9274,20 +9274,20 @@
       <c r="C199" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D199" s="57" t="s">
+      <c r="D199" s="52" t="s">
         <v>892</v>
       </c>
-      <c r="E199" s="58" t="s">
+      <c r="E199" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F199" s="48" t="s">
         <v>905</v>
       </c>
-      <c r="G199" s="58"/>
-      <c r="H199" s="58" t="s">
+      <c r="G199" s="53"/>
+      <c r="H199" s="53" t="s">
         <v>906</v>
       </c>
-      <c r="I199" s="58" t="s">
+      <c r="I199" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9301,13 +9301,13 @@
       <c r="C200" s="48" t="s">
         <v>582</v>
       </c>
-      <c r="D200" s="60" t="s">
+      <c r="D200" s="55" t="s">
         <v>715</v>
       </c>
-      <c r="E200" s="58"/>
+      <c r="E200" s="53"/>
       <c r="F200" s="48"/>
-      <c r="G200" s="58"/>
-      <c r="H200" s="58"/>
+      <c r="G200" s="53"/>
+      <c r="H200" s="53"/>
       <c r="I200" s="1" t="s">
         <v>933</v>
       </c>
@@ -9322,13 +9322,13 @@
       <c r="C201" s="48" t="s">
         <v>582</v>
       </c>
-      <c r="D201" s="60" t="s">
+      <c r="D201" s="55" t="s">
         <v>1010</v>
       </c>
-      <c r="E201" s="58"/>
+      <c r="E201" s="53"/>
       <c r="F201" s="48"/>
-      <c r="G201" s="58"/>
-      <c r="H201" s="58"/>
+      <c r="G201" s="53"/>
+      <c r="H201" s="53"/>
       <c r="I201" s="1" t="s">
         <v>933</v>
       </c>
@@ -9343,20 +9343,20 @@
       <c r="C202" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D202" s="57" t="s">
+      <c r="D202" s="52" t="s">
         <v>893</v>
       </c>
-      <c r="E202" s="58" t="s">
+      <c r="E202" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F202" s="48" t="s">
         <v>907</v>
       </c>
-      <c r="G202" s="58"/>
-      <c r="H202" s="58" t="s">
+      <c r="G202" s="53"/>
+      <c r="H202" s="53" t="s">
         <v>908</v>
       </c>
-      <c r="I202" s="58" t="s">
+      <c r="I202" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9373,17 +9373,17 @@
       <c r="D203" s="22" t="s">
         <v>939</v>
       </c>
-      <c r="E203" s="58" t="s">
+      <c r="E203" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F203" s="3" t="s">
         <v>940</v>
       </c>
-      <c r="G203" s="58"/>
+      <c r="G203" s="53"/>
       <c r="H203" s="3" t="s">
         <v>941</v>
       </c>
-      <c r="I203" s="58" t="s">
+      <c r="I203" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9391,26 +9391,26 @@
       <c r="A204" s="25">
         <v>203</v>
       </c>
-      <c r="B204" s="58" t="s">
+      <c r="B204" s="53" t="s">
         <v>894</v>
       </c>
       <c r="C204" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D204" s="61" t="s">
+      <c r="D204" s="56" t="s">
         <v>894</v>
       </c>
-      <c r="E204" s="58" t="s">
+      <c r="E204" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F204" s="48" t="s">
         <v>909</v>
       </c>
-      <c r="G204" s="58"/>
-      <c r="H204" s="58" t="s">
+      <c r="G204" s="53"/>
+      <c r="H204" s="53" t="s">
         <v>910</v>
       </c>
-      <c r="I204" s="58" t="s">
+      <c r="I204" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9418,26 +9418,26 @@
       <c r="A205" s="25">
         <v>204</v>
       </c>
-      <c r="B205" s="58" t="s">
+      <c r="B205" s="53" t="s">
         <v>894</v>
       </c>
-      <c r="C205" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D205" s="55" t="s">
-        <v>1079</v>
-      </c>
-      <c r="E205" s="58" t="s">
+      <c r="C205" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D205" s="50" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E205" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F205" s="48" t="s">
         <v>911</v>
       </c>
-      <c r="G205" s="58"/>
-      <c r="H205" s="58" t="s">
+      <c r="G205" s="53"/>
+      <c r="H205" s="53" t="s">
         <v>912</v>
       </c>
-      <c r="I205" s="58" t="s">
+      <c r="I205" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9445,7 +9445,7 @@
       <c r="A206" s="25">
         <v>205</v>
       </c>
-      <c r="B206" s="58" t="s">
+      <c r="B206" s="53" t="s">
         <v>894</v>
       </c>
       <c r="C206" s="48" t="s">
@@ -9454,10 +9454,10 @@
       <c r="D206" s="49" t="s">
         <v>1013</v>
       </c>
-      <c r="E206" s="58"/>
-      <c r="F206" s="58"/>
-      <c r="G206" s="58"/>
-      <c r="H206" s="58"/>
+      <c r="E206" s="53"/>
+      <c r="F206" s="53"/>
+      <c r="G206" s="53"/>
+      <c r="H206" s="53"/>
       <c r="I206" s="1" t="s">
         <v>933</v>
       </c>
@@ -9466,7 +9466,7 @@
       <c r="A207" s="25">
         <v>206</v>
       </c>
-      <c r="B207" s="58" t="s">
+      <c r="B207" s="53" t="s">
         <v>894</v>
       </c>
       <c r="C207" s="48" t="s">
@@ -9475,10 +9475,10 @@
       <c r="D207" s="49" t="s">
         <v>1012</v>
       </c>
-      <c r="E207" s="58"/>
-      <c r="F207" s="58"/>
-      <c r="G207" s="58"/>
-      <c r="H207" s="58"/>
+      <c r="E207" s="53"/>
+      <c r="F207" s="53"/>
+      <c r="G207" s="53"/>
+      <c r="H207" s="53"/>
       <c r="I207" s="1" t="s">
         <v>933</v>
       </c>
@@ -9487,7 +9487,7 @@
       <c r="A208" s="25">
         <v>207</v>
       </c>
-      <c r="B208" s="58" t="s">
+      <c r="B208" s="53" t="s">
         <v>894</v>
       </c>
       <c r="C208" s="48" t="s">
@@ -9496,10 +9496,10 @@
       <c r="D208" s="49" t="s">
         <v>1047</v>
       </c>
-      <c r="E208" s="58"/>
-      <c r="F208" s="58"/>
-      <c r="G208" s="58"/>
-      <c r="H208" s="58"/>
+      <c r="E208" s="53"/>
+      <c r="F208" s="53"/>
+      <c r="G208" s="53"/>
+      <c r="H208" s="53"/>
       <c r="I208" s="1" t="s">
         <v>933</v>
       </c>
@@ -9508,7 +9508,7 @@
       <c r="A209" s="25">
         <v>208</v>
       </c>
-      <c r="B209" s="58" t="s">
+      <c r="B209" s="53" t="s">
         <v>894</v>
       </c>
       <c r="C209" s="48" t="s">
@@ -9517,10 +9517,10 @@
       <c r="D209" s="49" t="s">
         <v>1011</v>
       </c>
-      <c r="E209" s="58"/>
-      <c r="F209" s="58"/>
-      <c r="G209" s="58"/>
-      <c r="H209" s="58"/>
+      <c r="E209" s="53"/>
+      <c r="F209" s="53"/>
+      <c r="G209" s="53"/>
+      <c r="H209" s="53"/>
       <c r="I209" s="1" t="s">
         <v>933</v>
       </c>
@@ -9529,19 +9529,19 @@
       <c r="A210" s="25">
         <v>209</v>
       </c>
-      <c r="B210" s="58" t="s">
+      <c r="B210" s="53" t="s">
         <v>894</v>
       </c>
       <c r="C210" s="48" t="s">
         <v>582</v>
       </c>
       <c r="D210" s="49" t="s">
-        <v>1078</v>
-      </c>
-      <c r="E210" s="58"/>
-      <c r="F210" s="58"/>
-      <c r="G210" s="58"/>
-      <c r="H210" s="58"/>
+        <v>1077</v>
+      </c>
+      <c r="E210" s="53"/>
+      <c r="F210" s="53"/>
+      <c r="G210" s="53"/>
+      <c r="H210" s="53"/>
       <c r="I210" s="1" t="s">
         <v>933</v>
       </c>
@@ -9556,20 +9556,20 @@
       <c r="C211" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D211" s="57" t="s">
+      <c r="D211" s="52" t="s">
         <v>895</v>
       </c>
-      <c r="E211" s="58" t="s">
+      <c r="E211" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="F211" s="58" t="s">
+      <c r="F211" s="53" t="s">
         <v>913</v>
       </c>
-      <c r="G211" s="58"/>
-      <c r="H211" s="58" t="s">
+      <c r="G211" s="53"/>
+      <c r="H211" s="53" t="s">
         <v>914</v>
       </c>
-      <c r="I211" s="58" t="s">
+      <c r="I211" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9580,23 +9580,23 @@
       <c r="B212" s="48" t="s">
         <v>895</v>
       </c>
-      <c r="C212" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D212" s="56" t="s">
+      <c r="C212" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D212" s="51" t="s">
         <v>1006</v>
       </c>
-      <c r="E212" s="58" t="s">
+      <c r="E212" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F212" s="48" t="s">
         <v>915</v>
       </c>
-      <c r="G212" s="58"/>
-      <c r="H212" s="58" t="s">
+      <c r="G212" s="53"/>
+      <c r="H212" s="53" t="s">
         <v>916</v>
       </c>
-      <c r="I212" s="58" t="s">
+      <c r="I212" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9607,23 +9607,23 @@
       <c r="B213" s="48" t="s">
         <v>895</v>
       </c>
-      <c r="C213" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D213" s="56" t="s">
+      <c r="C213" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D213" s="51" t="s">
         <v>1007</v>
       </c>
-      <c r="E213" s="58" t="s">
+      <c r="E213" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F213" s="48" t="s">
         <v>917</v>
       </c>
-      <c r="G213" s="58"/>
-      <c r="H213" s="58" t="s">
+      <c r="G213" s="53"/>
+      <c r="H213" s="53" t="s">
         <v>1033</v>
       </c>
-      <c r="I213" s="58" t="s">
+      <c r="I213" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9634,23 +9634,23 @@
       <c r="B214" s="48" t="s">
         <v>895</v>
       </c>
-      <c r="C214" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D214" s="56" t="s">
+      <c r="C214" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D214" s="51" t="s">
         <v>898</v>
       </c>
-      <c r="E214" s="58" t="s">
+      <c r="E214" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F214" s="48" t="s">
         <v>918</v>
       </c>
-      <c r="G214" s="58"/>
-      <c r="H214" s="58" t="s">
+      <c r="G214" s="53"/>
+      <c r="H214" s="53" t="s">
         <v>919</v>
       </c>
-      <c r="I214" s="58" t="s">
+      <c r="I214" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9661,23 +9661,23 @@
       <c r="B215" s="48" t="s">
         <v>895</v>
       </c>
-      <c r="C215" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D215" s="56" t="s">
+      <c r="C215" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D215" s="51" t="s">
         <v>993</v>
       </c>
-      <c r="E215" s="58" t="s">
+      <c r="E215" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="F215" s="58" t="s">
+      <c r="F215" s="53" t="s">
         <v>994</v>
       </c>
-      <c r="G215" s="58"/>
+      <c r="G215" s="53"/>
       <c r="H215" s="3" t="s">
         <v>995</v>
       </c>
-      <c r="I215" s="58" t="s">
+      <c r="I215" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9688,23 +9688,23 @@
       <c r="B216" s="48" t="s">
         <v>895</v>
       </c>
-      <c r="C216" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D216" s="56" t="s">
-        <v>1075</v>
+      <c r="C216" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D216" s="51" t="s">
+        <v>1074</v>
       </c>
       <c r="E216" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F216" s="58" t="s">
-        <v>1138</v>
-      </c>
-      <c r="G216" s="58"/>
-      <c r="H216" s="58" t="s">
-        <v>1139</v>
-      </c>
-      <c r="I216" s="58" t="s">
+      <c r="F216" s="53" t="s">
+        <v>1119</v>
+      </c>
+      <c r="G216" s="53"/>
+      <c r="H216" s="53" t="s">
+        <v>1137</v>
+      </c>
+      <c r="I216" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9718,13 +9718,13 @@
       <c r="C217" s="48" t="s">
         <v>582</v>
       </c>
-      <c r="D217" s="60" t="s">
+      <c r="D217" s="55" t="s">
         <v>899</v>
       </c>
-      <c r="E217" s="58"/>
+      <c r="E217" s="53"/>
       <c r="F217" s="48"/>
-      <c r="G217" s="58"/>
-      <c r="H217" s="58"/>
+      <c r="G217" s="53"/>
+      <c r="H217" s="53"/>
       <c r="I217" s="1" t="s">
         <v>933</v>
       </c>
@@ -9739,13 +9739,13 @@
       <c r="C218" s="48" t="s">
         <v>582</v>
       </c>
-      <c r="D218" s="60" t="s">
+      <c r="D218" s="55" t="s">
         <v>1014</v>
       </c>
-      <c r="E218" s="58"/>
-      <c r="F218" s="58"/>
-      <c r="G218" s="58"/>
-      <c r="H218" s="58"/>
+      <c r="E218" s="53"/>
+      <c r="F218" s="53"/>
+      <c r="G218" s="53"/>
+      <c r="H218" s="53"/>
       <c r="I218" s="1" t="s">
         <v>933</v>
       </c>
@@ -9760,13 +9760,13 @@
       <c r="C219" s="48" t="s">
         <v>582</v>
       </c>
-      <c r="D219" s="60" t="s">
+      <c r="D219" s="55" t="s">
         <v>900</v>
       </c>
-      <c r="E219" s="58"/>
-      <c r="F219" s="58"/>
-      <c r="G219" s="58"/>
-      <c r="H219" s="58"/>
+      <c r="E219" s="53"/>
+      <c r="F219" s="53"/>
+      <c r="G219" s="53"/>
+      <c r="H219" s="53"/>
       <c r="I219" s="1" t="s">
         <v>933</v>
       </c>
@@ -9781,20 +9781,20 @@
       <c r="C220" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D220" s="57" t="s">
+      <c r="D220" s="52" t="s">
         <v>896</v>
       </c>
-      <c r="E220" s="58" t="s">
+      <c r="E220" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F220" s="48" t="s">
         <v>920</v>
       </c>
-      <c r="G220" s="58"/>
-      <c r="H220" s="58" t="s">
+      <c r="G220" s="53"/>
+      <c r="H220" s="53" t="s">
         <v>937</v>
       </c>
-      <c r="I220" s="58" t="s">
+      <c r="I220" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9808,20 +9808,20 @@
       <c r="C221" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D221" s="57" t="s">
+      <c r="D221" s="52" t="s">
         <v>897</v>
       </c>
-      <c r="E221" s="58" t="s">
+      <c r="E221" s="53" t="s">
         <v>921</v>
       </c>
-      <c r="F221" s="58" t="s">
+      <c r="F221" s="53" t="s">
         <v>897</v>
       </c>
-      <c r="G221" s="58"/>
-      <c r="H221" s="58" t="s">
+      <c r="G221" s="53"/>
+      <c r="H221" s="53" t="s">
         <v>922</v>
       </c>
-      <c r="I221" s="58" t="s">
+      <c r="I221" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9832,20 +9832,20 @@
       <c r="B222" s="48" t="s">
         <v>897</v>
       </c>
-      <c r="C222" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D222" s="56" t="s">
-        <v>1079</v>
-      </c>
-      <c r="E222" s="58" t="s">
+      <c r="C222" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D222" s="51" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E222" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F222" s="48" t="s">
         <v>923</v>
       </c>
-      <c r="G222" s="58"/>
-      <c r="H222" s="58" t="s">
+      <c r="G222" s="53"/>
+      <c r="H222" s="53" t="s">
         <v>924</v>
       </c>
       <c r="I222" s="3" t="s">
@@ -9859,23 +9859,23 @@
       <c r="B223" s="48" t="s">
         <v>897</v>
       </c>
-      <c r="C223" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D223" s="56" t="s">
+      <c r="C223" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D223" s="51" t="s">
         <v>902</v>
       </c>
-      <c r="E223" s="58" t="s">
+      <c r="E223" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F223" s="48" t="s">
         <v>925</v>
       </c>
-      <c r="G223" s="58"/>
-      <c r="H223" s="58" t="s">
+      <c r="G223" s="53"/>
+      <c r="H223" s="53" t="s">
         <v>926</v>
       </c>
-      <c r="I223" s="58" t="s">
+      <c r="I223" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9886,20 +9886,20 @@
       <c r="B224" s="48" t="s">
         <v>897</v>
       </c>
-      <c r="C224" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D224" s="56" t="s">
+      <c r="C224" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D224" s="51" t="s">
         <v>903</v>
       </c>
-      <c r="E224" s="58" t="s">
+      <c r="E224" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F224" s="48" t="s">
         <v>927</v>
       </c>
-      <c r="G224" s="58"/>
-      <c r="H224" s="58" t="s">
+      <c r="G224" s="53"/>
+      <c r="H224" s="53" t="s">
         <v>928</v>
       </c>
       <c r="I224" s="3" t="s">
@@ -9913,23 +9913,23 @@
       <c r="B225" s="48" t="s">
         <v>897</v>
       </c>
-      <c r="C225" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D225" s="56" t="s">
+      <c r="C225" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D225" s="51" t="s">
         <v>904</v>
       </c>
-      <c r="E225" s="58" t="s">
+      <c r="E225" s="53" t="s">
         <v>929</v>
       </c>
       <c r="F225" s="48" t="s">
         <v>930</v>
       </c>
-      <c r="G225" s="58"/>
-      <c r="H225" s="58" t="s">
+      <c r="G225" s="53"/>
+      <c r="H225" s="53" t="s">
         <v>931</v>
       </c>
-      <c r="I225" s="58" t="s">
+      <c r="I225" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9940,23 +9940,23 @@
       <c r="B226" s="48" t="s">
         <v>897</v>
       </c>
-      <c r="C226" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D226" s="56" t="s">
+      <c r="C226" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D226" s="51" t="s">
         <v>1007</v>
       </c>
-      <c r="E226" s="58" t="s">
+      <c r="E226" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F226" s="3" t="s">
         <v>998</v>
       </c>
-      <c r="G226" s="58"/>
+      <c r="G226" s="53"/>
       <c r="H226" s="3" t="s">
         <v>999</v>
       </c>
-      <c r="I226" s="58" t="s">
+      <c r="I226" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9967,23 +9967,23 @@
       <c r="B227" s="48" t="s">
         <v>897</v>
       </c>
-      <c r="C227" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D227" s="56" t="s">
+      <c r="C227" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D227" s="51" t="s">
         <v>996</v>
       </c>
-      <c r="E227" s="58" t="s">
+      <c r="E227" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F227" s="3" t="s">
-        <v>1076</v>
-      </c>
-      <c r="G227" s="58"/>
+        <v>1075</v>
+      </c>
+      <c r="G227" s="53"/>
       <c r="H227" s="3" t="s">
         <v>1000</v>
       </c>
-      <c r="I227" s="58" t="s">
+      <c r="I227" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -9994,23 +9994,23 @@
       <c r="B228" s="48" t="s">
         <v>897</v>
       </c>
-      <c r="C228" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D228" s="56" t="s">
+      <c r="C228" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D228" s="51" t="s">
         <v>997</v>
       </c>
-      <c r="E228" s="58" t="s">
+      <c r="E228" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F228" s="3" t="s">
         <v>1001</v>
       </c>
-      <c r="G228" s="58"/>
+      <c r="G228" s="53"/>
       <c r="H228" s="3" t="s">
         <v>1002</v>
       </c>
-      <c r="I228" s="58" t="s">
+      <c r="I228" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -10021,11 +10021,11 @@
       <c r="B229" s="48" t="s">
         <v>897</v>
       </c>
-      <c r="C229" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D229" s="56" t="s">
-        <v>1075</v>
+      <c r="C229" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D229" s="51" t="s">
+        <v>1074</v>
       </c>
       <c r="E229" s="3" t="s">
         <v>16</v>
@@ -10033,9 +10033,9 @@
       <c r="F229" s="3" t="s">
         <v>1071</v>
       </c>
-      <c r="G229" s="58"/>
+      <c r="G229" s="53"/>
       <c r="H229" s="3" t="s">
-        <v>1072</v>
+        <v>1138</v>
       </c>
       <c r="I229" s="3" t="s">
         <v>90</v>
@@ -10048,21 +10048,21 @@
       <c r="B230" s="48" t="s">
         <v>897</v>
       </c>
-      <c r="C230" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D230" s="56" t="s">
+      <c r="C230" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D230" s="51" t="s">
         <v>1006</v>
       </c>
       <c r="E230" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F230" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="G230" s="53"/>
+      <c r="H230" s="1" t="s">
         <v>1073</v>
-      </c>
-      <c r="G230" s="58"/>
-      <c r="H230" s="1" t="s">
-        <v>1074</v>
       </c>
       <c r="I230" s="3" t="s">
         <v>90</v>
@@ -10078,13 +10078,13 @@
       <c r="C231" s="48" t="s">
         <v>582</v>
       </c>
-      <c r="D231" s="60" t="s">
+      <c r="D231" s="55" t="s">
         <v>1015</v>
       </c>
-      <c r="E231" s="58"/>
-      <c r="F231" s="58"/>
-      <c r="G231" s="58"/>
-      <c r="H231" s="58"/>
+      <c r="E231" s="53"/>
+      <c r="F231" s="53"/>
+      <c r="G231" s="53"/>
+      <c r="H231" s="53"/>
       <c r="I231" s="1" t="s">
         <v>933</v>
       </c>
@@ -10099,13 +10099,13 @@
       <c r="C232" s="48" t="s">
         <v>582</v>
       </c>
-      <c r="D232" s="60" t="s">
+      <c r="D232" s="55" t="s">
         <v>1016</v>
       </c>
-      <c r="E232" s="58"/>
-      <c r="F232" s="58"/>
-      <c r="G232" s="58"/>
-      <c r="H232" s="58"/>
+      <c r="E232" s="53"/>
+      <c r="F232" s="53"/>
+      <c r="G232" s="53"/>
+      <c r="H232" s="53"/>
       <c r="I232" s="1" t="s">
         <v>933</v>
       </c>
@@ -10120,7 +10120,7 @@
       <c r="C233" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D233" s="57" t="s">
+      <c r="D233" s="52" t="s">
         <v>1051</v>
       </c>
       <c r="E233" s="3" t="s">
@@ -10129,7 +10129,7 @@
       <c r="F233" s="3" t="s">
         <v>1051</v>
       </c>
-      <c r="G233" s="58"/>
+      <c r="G233" s="53"/>
       <c r="H233" s="3" t="s">
         <v>1056</v>
       </c>
@@ -10144,7 +10144,7 @@
       <c r="B234" s="48" t="s">
         <v>1051</v>
       </c>
-      <c r="C234" s="58" t="s">
+      <c r="C234" s="53" t="s">
         <v>91</v>
       </c>
       <c r="D234" s="22" t="s">
@@ -10156,7 +10156,7 @@
       <c r="F234" s="3" t="s">
         <v>1057</v>
       </c>
-      <c r="G234" s="58"/>
+      <c r="G234" s="53"/>
       <c r="H234" s="3" t="s">
         <v>1058</v>
       </c>
@@ -10171,7 +10171,7 @@
       <c r="B235" s="48" t="s">
         <v>1051</v>
       </c>
-      <c r="C235" s="58" t="s">
+      <c r="C235" s="53" t="s">
         <v>91</v>
       </c>
       <c r="D235" s="22" t="s">
@@ -10198,10 +10198,10 @@
       <c r="B236" s="48" t="s">
         <v>1051</v>
       </c>
-      <c r="C236" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D236" s="55" t="s">
+      <c r="C236" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D236" s="50" t="s">
         <v>1006</v>
       </c>
       <c r="E236" s="3" t="s">
@@ -10225,7 +10225,7 @@
       <c r="B237" s="48" t="s">
         <v>1051</v>
       </c>
-      <c r="C237" s="58" t="s">
+      <c r="C237" s="53" t="s">
         <v>91</v>
       </c>
       <c r="D237" s="22" t="s">
@@ -10237,11 +10237,11 @@
       <c r="F237" s="3" t="s">
         <v>1063</v>
       </c>
-      <c r="G237" s="58"/>
+      <c r="G237" s="53"/>
       <c r="H237" s="3" t="s">
         <v>1064</v>
       </c>
-      <c r="I237" s="58" t="s">
+      <c r="I237" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -10252,23 +10252,23 @@
       <c r="B238" s="48" t="s">
         <v>1051</v>
       </c>
-      <c r="C238" s="58" t="s">
+      <c r="C238" s="53" t="s">
         <v>91</v>
       </c>
       <c r="D238" s="22" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E238" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F238" s="58" t="s">
-        <v>1140</v>
-      </c>
-      <c r="G238" s="58"/>
-      <c r="H238" s="58" t="s">
-        <v>1141</v>
-      </c>
-      <c r="I238" s="58" t="s">
+      <c r="F238" s="53" t="s">
+        <v>1120</v>
+      </c>
+      <c r="G238" s="53"/>
+      <c r="H238" s="53" t="s">
+        <v>1139</v>
+      </c>
+      <c r="I238" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -10282,13 +10282,13 @@
       <c r="C239" s="48" t="s">
         <v>582</v>
       </c>
-      <c r="D239" s="60" t="s">
+      <c r="D239" s="55" t="s">
         <v>1052</v>
       </c>
-      <c r="E239" s="58"/>
-      <c r="F239" s="58"/>
-      <c r="G239" s="58"/>
-      <c r="H239" s="58"/>
+      <c r="E239" s="53"/>
+      <c r="F239" s="53"/>
+      <c r="G239" s="53"/>
+      <c r="H239" s="53"/>
       <c r="I239" s="1" t="s">
         <v>933</v>
       </c>
@@ -10298,23 +10298,23 @@
         <v>239</v>
       </c>
       <c r="B240" s="48" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="C240" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D240" s="57" t="s">
-        <v>1082</v>
+      <c r="D240" s="52" t="s">
+        <v>1081</v>
       </c>
       <c r="E240" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F240" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G240" s="53"/>
+      <c r="H240" s="3" t="s">
         <v>1083</v>
-      </c>
-      <c r="G240" s="58"/>
-      <c r="H240" s="3" t="s">
-        <v>1084</v>
       </c>
       <c r="I240" s="3" t="s">
         <v>90</v>
@@ -10325,23 +10325,23 @@
         <v>240</v>
       </c>
       <c r="B241" s="48" t="s">
-        <v>1082</v>
-      </c>
-      <c r="C241" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D241" s="55" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C241" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D241" s="50" t="s">
         <v>1006</v>
       </c>
       <c r="E241" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F241" s="3" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G241" s="53"/>
+      <c r="H241" s="3" t="s">
         <v>1085</v>
-      </c>
-      <c r="G241" s="58"/>
-      <c r="H241" s="3" t="s">
-        <v>1086</v>
       </c>
       <c r="I241" s="3" t="s">
         <v>90</v>
@@ -10352,23 +10352,23 @@
         <v>241</v>
       </c>
       <c r="B242" s="48" t="s">
-        <v>1082</v>
-      </c>
-      <c r="C242" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D242" s="55" t="s">
-        <v>1093</v>
+        <v>1081</v>
+      </c>
+      <c r="C242" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D242" s="50" t="s">
+        <v>1091</v>
       </c>
       <c r="E242" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F242" s="3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="G242" s="53"/>
+      <c r="H242" s="3" t="s">
         <v>1087</v>
-      </c>
-      <c r="G242" s="58"/>
-      <c r="H242" s="3" t="s">
-        <v>1088</v>
       </c>
       <c r="I242" s="3" t="s">
         <v>90</v>
@@ -10379,9 +10379,9 @@
         <v>242</v>
       </c>
       <c r="B243" s="48" t="s">
-        <v>1082</v>
-      </c>
-      <c r="C243" s="58" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C243" s="53" t="s">
         <v>91</v>
       </c>
       <c r="D243" s="22" t="s">
@@ -10390,12 +10390,12 @@
       <c r="E243" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F243" s="58" t="s">
+      <c r="F243" s="53" t="s">
+        <v>1088</v>
+      </c>
+      <c r="G243" s="53"/>
+      <c r="H243" s="53" t="s">
         <v>1089</v>
-      </c>
-      <c r="G243" s="58"/>
-      <c r="H243" s="58" t="s">
-        <v>1090</v>
       </c>
       <c r="I243" s="3" t="s">
         <v>90</v>
@@ -10406,23 +10406,23 @@
         <v>243</v>
       </c>
       <c r="B244" s="48" t="s">
-        <v>1082</v>
-      </c>
-      <c r="C244" s="58" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C244" s="53" t="s">
         <v>91</v>
       </c>
       <c r="D244" s="22" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E244" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F244" s="58" t="s">
-        <v>1091</v>
-      </c>
-      <c r="G244" s="58"/>
-      <c r="H244" s="58" t="s">
-        <v>1092</v>
+      <c r="F244" s="53" t="s">
+        <v>1090</v>
+      </c>
+      <c r="G244" s="53"/>
+      <c r="H244" s="53" t="s">
+        <v>1140</v>
       </c>
       <c r="I244" s="3" t="s">
         <v>90</v>
@@ -10433,23 +10433,23 @@
         <v>244</v>
       </c>
       <c r="B245" s="48" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="C245" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D245" s="57" t="s">
-        <v>1094</v>
+      <c r="D245" s="52" t="s">
+        <v>1092</v>
       </c>
       <c r="E245" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F245" s="3" t="s">
-        <v>1095</v>
-      </c>
-      <c r="G245" s="58"/>
+        <v>1093</v>
+      </c>
+      <c r="G245" s="53"/>
       <c r="H245" s="3" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="I245" s="3" t="s">
         <v>90</v>
@@ -10460,23 +10460,23 @@
         <v>245</v>
       </c>
       <c r="B246" s="48" t="s">
-        <v>1094</v>
-      </c>
-      <c r="C246" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D246" s="55" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C246" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D246" s="50" t="s">
         <v>1006</v>
       </c>
       <c r="E246" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F246" s="3" t="s">
-        <v>1098</v>
-      </c>
-      <c r="G246" s="58"/>
+        <v>1096</v>
+      </c>
+      <c r="G246" s="53"/>
       <c r="H246" s="3" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="I246" s="3" t="s">
         <v>90</v>
@@ -10487,23 +10487,23 @@
         <v>246</v>
       </c>
       <c r="B247" s="48" t="s">
-        <v>1094</v>
-      </c>
-      <c r="C247" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D247" s="55" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C247" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D247" s="50" t="s">
         <v>1007</v>
       </c>
       <c r="E247" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F247" s="3" t="s">
-        <v>1100</v>
-      </c>
-      <c r="G247" s="58"/>
+        <v>1098</v>
+      </c>
+      <c r="G247" s="53"/>
       <c r="H247" s="3" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="I247" s="3" t="s">
         <v>90</v>
@@ -10514,23 +10514,23 @@
         <v>247</v>
       </c>
       <c r="B248" s="48" t="s">
-        <v>1094</v>
-      </c>
-      <c r="C248" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D248" s="55" t="s">
-        <v>1075</v>
+        <v>1092</v>
+      </c>
+      <c r="C248" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D248" s="50" t="s">
+        <v>1074</v>
       </c>
       <c r="E248" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F248" s="3" t="s">
-        <v>1102</v>
-      </c>
-      <c r="G248" s="58"/>
-      <c r="H248" s="58" t="s">
-        <v>1103</v>
+        <v>1100</v>
+      </c>
+      <c r="G248" s="53"/>
+      <c r="H248" s="53" t="s">
+        <v>1141</v>
       </c>
       <c r="I248" s="3" t="s">
         <v>90</v>
@@ -10541,30 +10541,30 @@
         <v>248</v>
       </c>
       <c r="B249" s="48" t="s">
-        <v>1094</v>
-      </c>
-      <c r="C249" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D249" s="55" t="s">
-        <v>1097</v>
+        <v>1092</v>
+      </c>
+      <c r="C249" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D249" s="50" t="s">
+        <v>1095</v>
       </c>
       <c r="E249" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F249" s="3" t="s">
-        <v>1104</v>
-      </c>
-      <c r="G249" s="58"/>
-      <c r="H249" s="58" t="s">
-        <v>1105</v>
+        <v>1101</v>
+      </c>
+      <c r="G249" s="53"/>
+      <c r="H249" s="53" t="s">
+        <v>1102</v>
       </c>
       <c r="I249" s="3" t="s">
         <v>90</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I239" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I249" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -10592,14 +10592,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>485</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
       <c r="G1" s="16"/>
       <c r="H1" s="16"/>
       <c r="I1" s="5"/>
@@ -10609,16 +10609,16 @@
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="59" t="s">
         <v>484</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -10626,11 +10626,11 @@
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="57" t="s">
         <v>486</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
       <c r="D3" s="24"/>
       <c r="E3" s="18"/>
       <c r="F3" s="17"/>
@@ -10653,10 +10653,10 @@
       <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:13" s="6" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="B5" s="54"/>
+      <c r="B5" s="61"/>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="18"/>
@@ -14141,24 +14141,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -14380,10 +14362,40 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14407,21 +14419,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update to CT deliverables based on DDF meeting 2023-08-28
Remove 'label' from Content class
Update templateText to text
Add relationship to SyntaxTemplate class
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83AB76D-8C9C-46FD-A4EB-E8A5D11BD03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22080A98-E045-4FD7-B684-565D1411C3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="410" yWindow="120" windowWidth="16950" windowHeight="9820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="90" yWindow="150" windowWidth="16950" windowHeight="9820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2595" uniqueCount="1142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2592" uniqueCount="1140">
   <si>
     <t>Preferred Term</t>
   </si>
@@ -3314,9 +3314,6 @@
     <t>Syntax Template Label</t>
   </si>
   <si>
-    <t>templateText</t>
-  </si>
-  <si>
     <t>SyntaxTemplateDictionary</t>
   </si>
   <si>
@@ -3401,9 +3398,6 @@
     <t>Schedule Timeline Label</t>
   </si>
   <si>
-    <t>Content Label</t>
-  </si>
-  <si>
     <t>The short descriptive designation for the organization.</t>
   </si>
   <si>
@@ -3458,13 +3452,13 @@
     <t>The short descriptive designation for the timing.</t>
   </si>
   <si>
-    <t>The short descriptive designation for the content.</t>
-  </si>
-  <si>
     <t>The short descriptive designation for the syntax template.</t>
   </si>
   <si>
     <t>The short descriptive designation for the syntax template dictionary.</t>
+  </si>
+  <si>
+    <t>dictionary</t>
   </si>
 </sst>
 </file>
@@ -4984,7 +4978,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="25">
         <v>30</v>
       </c>
@@ -5001,11 +4995,11 @@
         <v>16</v>
       </c>
       <c r="F31" s="53" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="G31" s="53"/>
       <c r="H31" s="53" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="I31" s="53" t="s">
         <v>90</v>
@@ -5535,7 +5529,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="37" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="25">
         <v>53</v>
       </c>
@@ -5552,11 +5546,11 @@
         <v>16</v>
       </c>
       <c r="F54" s="53" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="G54" s="53"/>
       <c r="H54" s="53" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="I54" s="53" t="s">
         <v>90</v>
@@ -5751,7 +5745,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="25">
         <v>61</v>
       </c>
@@ -5768,11 +5762,11 @@
         <v>16</v>
       </c>
       <c r="F62" s="53" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="G62" s="53"/>
       <c r="H62" s="53" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="I62" s="53" t="s">
         <v>90</v>
@@ -5984,11 +5978,11 @@
         <v>16</v>
       </c>
       <c r="F70" s="53" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="G70" s="53"/>
       <c r="H70" s="53" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="I70" s="53" t="s">
         <v>90</v>
@@ -6123,7 +6117,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="25">
         <v>75</v>
       </c>
@@ -6140,11 +6134,11 @@
         <v>16</v>
       </c>
       <c r="F76" s="53" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="G76" s="53"/>
       <c r="H76" s="53" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="I76" s="53" t="s">
         <v>90</v>
@@ -6510,7 +6504,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="25">
         <v>90</v>
       </c>
@@ -6527,11 +6521,11 @@
         <v>16</v>
       </c>
       <c r="F91" s="53" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="G91" s="53"/>
       <c r="H91" s="53" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="I91" s="53" t="s">
         <v>90</v>
@@ -6645,7 +6639,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="25">
         <v>95</v>
       </c>
@@ -6662,11 +6656,11 @@
         <v>16</v>
       </c>
       <c r="F96" s="53" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="G96" s="53"/>
       <c r="H96" s="53" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="I96" s="53" t="s">
         <v>90</v>
@@ -6837,7 +6831,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" s="25">
         <v>103</v>
       </c>
@@ -6854,11 +6848,11 @@
         <v>16</v>
       </c>
       <c r="F104" s="53" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="G104" s="53"/>
       <c r="H104" s="53" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="I104" s="53" t="s">
         <v>90</v>
@@ -7062,7 +7056,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" s="25">
         <v>112</v>
       </c>
@@ -7079,11 +7073,11 @@
         <v>16</v>
       </c>
       <c r="F113" s="53" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="G113" s="53"/>
       <c r="H113" s="53" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="I113" s="53" t="s">
         <v>90</v>
@@ -7494,7 +7488,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" s="25">
         <v>130</v>
       </c>
@@ -7511,11 +7505,11 @@
         <v>16</v>
       </c>
       <c r="F131" s="53" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="G131" s="53"/>
       <c r="H131" s="53" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="I131" s="53" t="s">
         <v>90</v>
@@ -7710,7 +7704,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" s="25">
         <v>138</v>
       </c>
@@ -7727,11 +7721,11 @@
         <v>16</v>
       </c>
       <c r="F139" s="53" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="G139" s="53"/>
       <c r="H139" s="53" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="I139" s="53" t="s">
         <v>90</v>
@@ -8037,7 +8031,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="152" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152" s="25">
         <v>151</v>
       </c>
@@ -8054,11 +8048,11 @@
         <v>16</v>
       </c>
       <c r="F152" s="53" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="G152" s="53"/>
       <c r="H152" s="53" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="I152" s="53" t="s">
         <v>90</v>
@@ -8640,7 +8634,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A175" s="25">
         <v>174</v>
       </c>
@@ -8657,11 +8651,11 @@
         <v>16</v>
       </c>
       <c r="F175" s="53" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="G175" s="53"/>
       <c r="H175" s="53" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="I175" s="53" t="s">
         <v>90</v>
@@ -8867,11 +8861,11 @@
         <v>16</v>
       </c>
       <c r="F183" s="53" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="G183" s="53"/>
       <c r="H183" s="53" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="I183" s="53" t="s">
         <v>90</v>
@@ -9077,11 +9071,11 @@
         <v>16</v>
       </c>
       <c r="F191" s="53" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="G191" s="53"/>
       <c r="H191" s="53" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="I191" s="53" t="s">
         <v>90</v>
@@ -9254,11 +9248,11 @@
         <v>16</v>
       </c>
       <c r="F198" s="53" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="G198" s="53"/>
       <c r="H198" s="53" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="I198" s="53" t="s">
         <v>90</v>
@@ -9681,7 +9675,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="216" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A216" s="25">
         <v>215</v>
       </c>
@@ -9698,11 +9692,11 @@
         <v>16</v>
       </c>
       <c r="F216" s="53" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="G216" s="53"/>
       <c r="H216" s="53" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="I216" s="53" t="s">
         <v>90</v>
@@ -10014,7 +10008,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A229" s="25">
         <v>228</v>
       </c>
@@ -10035,7 +10029,7 @@
       </c>
       <c r="G229" s="53"/>
       <c r="H229" s="3" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="I229" s="3" t="s">
         <v>90</v>
@@ -10245,52 +10239,52 @@
         <v>90</v>
       </c>
     </row>
-    <row r="238" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A238" s="25">
         <v>237</v>
       </c>
       <c r="B238" s="48" t="s">
         <v>1051</v>
       </c>
-      <c r="C238" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="D238" s="22" t="s">
-        <v>1074</v>
-      </c>
-      <c r="E238" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F238" s="53" t="s">
-        <v>1120</v>
-      </c>
+      <c r="C238" s="48" t="s">
+        <v>582</v>
+      </c>
+      <c r="D238" s="55" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E238" s="53"/>
+      <c r="F238" s="53"/>
       <c r="G238" s="53"/>
-      <c r="H238" s="53" t="s">
-        <v>1139</v>
-      </c>
-      <c r="I238" s="53" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H238" s="53"/>
+      <c r="I238" s="1" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A239" s="25">
         <v>238</v>
       </c>
       <c r="B239" s="48" t="s">
-        <v>1051</v>
+        <v>1081</v>
       </c>
       <c r="C239" s="48" t="s">
-        <v>582</v>
-      </c>
-      <c r="D239" s="55" t="s">
-        <v>1052</v>
-      </c>
-      <c r="E239" s="53"/>
-      <c r="F239" s="53"/>
+        <v>4</v>
+      </c>
+      <c r="D239" s="52" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E239" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F239" s="3" t="s">
+        <v>1082</v>
+      </c>
       <c r="G239" s="53"/>
-      <c r="H239" s="53"/>
-      <c r="I239" s="1" t="s">
-        <v>933</v>
+      <c r="H239" s="3" t="s">
+        <v>1083</v>
+      </c>
+      <c r="I239" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="240" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -10300,21 +10294,21 @@
       <c r="B240" s="48" t="s">
         <v>1081</v>
       </c>
-      <c r="C240" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="D240" s="52" t="s">
-        <v>1081</v>
+      <c r="C240" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D240" s="50" t="s">
+        <v>1006</v>
       </c>
       <c r="E240" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F240" s="3" t="s">
-        <v>1082</v>
+        <v>1084</v>
       </c>
       <c r="G240" s="53"/>
       <c r="H240" s="3" t="s">
-        <v>1083</v>
+        <v>1085</v>
       </c>
       <c r="I240" s="3" t="s">
         <v>90</v>
@@ -10331,23 +10325,23 @@
         <v>91</v>
       </c>
       <c r="D241" s="50" t="s">
-        <v>1006</v>
+        <v>737</v>
       </c>
       <c r="E241" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F241" s="3" t="s">
-        <v>1084</v>
+        <v>1086</v>
       </c>
       <c r="G241" s="53"/>
       <c r="H241" s="3" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="I241" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="242" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A242" s="25">
         <v>241</v>
       </c>
@@ -10357,24 +10351,24 @@
       <c r="C242" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="D242" s="50" t="s">
-        <v>1091</v>
+      <c r="D242" s="22" t="s">
+        <v>1007</v>
       </c>
       <c r="E242" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F242" s="3" t="s">
-        <v>1086</v>
+      <c r="F242" s="53" t="s">
+        <v>1088</v>
       </c>
       <c r="G242" s="53"/>
-      <c r="H242" s="3" t="s">
-        <v>1087</v>
+      <c r="H242" s="53" t="s">
+        <v>1089</v>
       </c>
       <c r="I242" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A243" s="25">
         <v>242</v>
       </c>
@@ -10385,17 +10379,17 @@
         <v>91</v>
       </c>
       <c r="D243" s="22" t="s">
-        <v>1007</v>
+        <v>1074</v>
       </c>
       <c r="E243" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F243" s="53" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
       <c r="G243" s="53"/>
       <c r="H243" s="53" t="s">
-        <v>1089</v>
+        <v>1137</v>
       </c>
       <c r="I243" s="3" t="s">
         <v>90</v>
@@ -10406,26 +10400,20 @@
         <v>243</v>
       </c>
       <c r="B244" s="48" t="s">
-        <v>1081</v>
+        <v>1091</v>
       </c>
       <c r="C244" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="D244" s="22" t="s">
-        <v>1074</v>
-      </c>
-      <c r="E244" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F244" s="53" t="s">
-        <v>1090</v>
-      </c>
+        <v>582</v>
+      </c>
+      <c r="D244" s="55" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E244" s="3"/>
+      <c r="F244" s="3"/>
       <c r="G244" s="53"/>
-      <c r="H244" s="53" t="s">
-        <v>1140</v>
-      </c>
+      <c r="H244" s="53"/>
       <c r="I244" s="3" t="s">
-        <v>90</v>
+        <v>933</v>
       </c>
     </row>
     <row r="245" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -10433,23 +10421,23 @@
         <v>244</v>
       </c>
       <c r="B245" s="48" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C245" s="48" t="s">
         <v>4</v>
       </c>
       <c r="D245" s="52" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E245" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F245" s="3" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="G245" s="53"/>
       <c r="H245" s="3" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="I245" s="3" t="s">
         <v>90</v>
@@ -10460,7 +10448,7 @@
         <v>245</v>
       </c>
       <c r="B246" s="48" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C246" s="53" t="s">
         <v>91</v>
@@ -10472,11 +10460,11 @@
         <v>16</v>
       </c>
       <c r="F246" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="G246" s="53"/>
       <c r="H246" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="I246" s="3" t="s">
         <v>90</v>
@@ -10487,7 +10475,7 @@
         <v>246</v>
       </c>
       <c r="B247" s="48" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C247" s="53" t="s">
         <v>91</v>
@@ -10499,11 +10487,11 @@
         <v>16</v>
       </c>
       <c r="F247" s="3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="G247" s="53"/>
       <c r="H247" s="3" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="I247" s="3" t="s">
         <v>90</v>
@@ -10514,7 +10502,7 @@
         <v>247</v>
       </c>
       <c r="B248" s="48" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C248" s="53" t="s">
         <v>91</v>
@@ -10526,11 +10514,11 @@
         <v>16</v>
       </c>
       <c r="F248" s="3" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="G248" s="53"/>
       <c r="H248" s="53" t="s">
-        <v>1141</v>
+        <v>1138</v>
       </c>
       <c r="I248" s="3" t="s">
         <v>90</v>
@@ -10541,23 +10529,23 @@
         <v>248</v>
       </c>
       <c r="B249" s="48" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C249" s="53" t="s">
         <v>91</v>
       </c>
       <c r="D249" s="50" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E249" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F249" s="3" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="G249" s="53"/>
       <c r="H249" s="53" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="I249" s="3" t="s">
         <v>90</v>
@@ -14141,6 +14129,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -14362,40 +14368,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14419,9 +14395,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
3 Fixes in 2-3 release
3 Fixes in 2-3 release
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22080A98-E045-4FD7-B684-565D1411C3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC15FDE-D31B-49E3-B1BC-46278009C928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="150" windowWidth="16950" windowHeight="9820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="380" windowWidth="18960" windowHeight="9210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
     <sheet name="DDF valid value sets" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DDF Entities&amp;Attributes'!$A$1:$I$249</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DDF Entities&amp;Attributes'!$A$1:$I$248</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DDF valid value sets'!$A$6:$M$124</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2592" uniqueCount="1140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2585" uniqueCount="1138">
   <si>
     <t>Preferred Term</t>
   </si>
@@ -2774,12 +2774,6 @@
     <t>A scheduled occurrence of a temporal event.</t>
   </si>
   <si>
-    <t>Scheduled Instance Type</t>
-  </si>
-  <si>
-    <t>A characterization or classification of the scheduled instance.</t>
-  </si>
-  <si>
     <t>Schedule Timeline</t>
   </si>
   <si>
@@ -3269,9 +3263,6 @@
     <t>Timing Window, Lower</t>
   </si>
   <si>
-    <t>content</t>
-  </si>
-  <si>
     <t>scheduledInstanceTimings</t>
   </si>
   <si>
@@ -3459,6 +3450,9 @@
   </si>
   <si>
     <t>dictionary</t>
+  </si>
+  <si>
+    <t>contents</t>
   </si>
 </sst>
 </file>
@@ -4168,7 +4162,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I249"/>
+  <dimension ref="A1:I248"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4262,7 +4256,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -4283,7 +4277,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -4304,7 +4298,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -4374,7 +4368,7 @@
         <v>91</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>33</v>
@@ -4792,7 +4786,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -4867,7 +4861,7 @@
       <c r="G26" s="36"/>
       <c r="H26" s="36"/>
       <c r="I26" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -4935,7 +4929,7 @@
         <v>91</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>504</v>
@@ -4962,7 +4956,7 @@
         <v>91</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>656</v>
@@ -4989,17 +4983,17 @@
         <v>91</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F31" s="53" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="G31" s="53"/>
       <c r="H31" s="53" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
       <c r="I31" s="53" t="s">
         <v>90</v>
@@ -5050,7 +5044,7 @@
       <c r="G33" s="21"/>
       <c r="H33" s="21"/>
       <c r="I33" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
@@ -5071,7 +5065,7 @@
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
       <c r="I34" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -5092,7 +5086,7 @@
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
       <c r="I35" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
@@ -5113,7 +5107,7 @@
       <c r="G36" s="21"/>
       <c r="H36" s="21"/>
       <c r="I36" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
@@ -5134,7 +5128,7 @@
       <c r="G37" s="21"/>
       <c r="H37" s="21"/>
       <c r="I37" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
@@ -5155,7 +5149,7 @@
       <c r="G38" s="21"/>
       <c r="H38" s="21"/>
       <c r="I38" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -5176,7 +5170,7 @@
       <c r="G39" s="21"/>
       <c r="H39" s="21"/>
       <c r="I39" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -5197,7 +5191,7 @@
       <c r="G40" s="21"/>
       <c r="H40" s="21"/>
       <c r="I40" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -5218,7 +5212,7 @@
       <c r="G41" s="54"/>
       <c r="H41" s="54"/>
       <c r="I41" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
@@ -5232,14 +5226,14 @@
         <v>582</v>
       </c>
       <c r="D42" s="49" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="E42" s="54"/>
       <c r="F42" s="48"/>
       <c r="G42" s="54"/>
       <c r="H42" s="54"/>
       <c r="I42" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
@@ -5253,14 +5247,14 @@
         <v>582</v>
       </c>
       <c r="D43" s="49" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="E43" s="54"/>
       <c r="F43" s="48"/>
       <c r="G43" s="54"/>
       <c r="H43" s="54"/>
       <c r="I43" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -5281,7 +5275,7 @@
       <c r="G44" s="54"/>
       <c r="H44" s="54"/>
       <c r="I44" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -5295,14 +5289,14 @@
         <v>582</v>
       </c>
       <c r="D45" s="49" t="s">
-        <v>1076</v>
+        <v>1137</v>
       </c>
       <c r="E45" s="54"/>
       <c r="F45" s="48"/>
       <c r="G45" s="54"/>
       <c r="H45" s="54"/>
       <c r="I45" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -5316,7 +5310,7 @@
         <v>91</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="E46" s="33" t="s">
         <v>43</v>
@@ -5345,7 +5339,7 @@
         <v>91</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="E47" s="33" t="s">
         <v>37</v>
@@ -5413,7 +5407,7 @@
         <v>714</v>
       </c>
       <c r="H49" s="48" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>710</v>
@@ -5430,7 +5424,7 @@
         <v>91</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>16</v>
@@ -5457,7 +5451,7 @@
         <v>91</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>16</v>
@@ -5467,7 +5461,7 @@
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>90</v>
@@ -5540,17 +5534,17 @@
         <v>91</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F54" s="53" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="G54" s="53"/>
       <c r="H54" s="53" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="I54" s="53" t="s">
         <v>90</v>
@@ -5561,13 +5555,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D55" s="31" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>27</v>
@@ -5588,7 +5582,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>91</v>
@@ -5615,23 +5609,23 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>91</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>96</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>90</v>
@@ -5651,14 +5645,14 @@
         <v>588</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="1" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>90</v>
@@ -5702,7 +5696,7 @@
         <v>91</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>31</v>
@@ -5712,7 +5706,7 @@
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>602</v>
@@ -5729,17 +5723,17 @@
         <v>91</v>
       </c>
       <c r="D61" s="23" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="G61" s="53"/>
       <c r="H61" s="1" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="I61" s="3" t="s">
         <v>90</v>
@@ -5756,17 +5750,17 @@
         <v>91</v>
       </c>
       <c r="D62" s="23" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F62" s="53" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="G62" s="53"/>
       <c r="H62" s="53" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="I62" s="53" t="s">
         <v>90</v>
@@ -5810,7 +5804,7 @@
         <v>91</v>
       </c>
       <c r="D64" s="23" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>660</v>
@@ -5820,7 +5814,7 @@
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="1" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="I64" s="3" t="s">
         <v>90</v>
@@ -5945,17 +5939,17 @@
         <v>91</v>
       </c>
       <c r="D69" s="22" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="G69" s="53"/>
       <c r="H69" s="1" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="I69" s="3" t="s">
         <v>90</v>
@@ -5972,17 +5966,17 @@
         <v>91</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F70" s="53" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="G70" s="53"/>
       <c r="H70" s="53" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="I70" s="53" t="s">
         <v>90</v>
@@ -6033,7 +6027,7 @@
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
@@ -6047,7 +6041,7 @@
         <v>91</v>
       </c>
       <c r="D73" s="23" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>115</v>
@@ -6057,7 +6051,7 @@
       </c>
       <c r="G73" s="1"/>
       <c r="H73" s="1" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>90</v>
@@ -6084,7 +6078,7 @@
       </c>
       <c r="G74" s="1"/>
       <c r="H74" s="1" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>692</v>
@@ -6101,17 +6095,17 @@
         <v>91</v>
       </c>
       <c r="D75" s="23" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="G75" s="53"/>
       <c r="H75" s="1" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="I75" s="3" t="s">
         <v>90</v>
@@ -6128,17 +6122,17 @@
         <v>91</v>
       </c>
       <c r="D76" s="23" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F76" s="53" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="G76" s="53"/>
       <c r="H76" s="53" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="I76" s="53" t="s">
         <v>90</v>
@@ -6182,7 +6176,7 @@
         <v>91</v>
       </c>
       <c r="D78" s="22" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>661</v>
@@ -6192,7 +6186,7 @@
       </c>
       <c r="G78" s="3"/>
       <c r="H78" s="1" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="I78" s="3" t="s">
         <v>90</v>
@@ -6209,7 +6203,7 @@
         <v>91</v>
       </c>
       <c r="D79" s="23" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>662</v>
@@ -6290,14 +6284,14 @@
         <v>582</v>
       </c>
       <c r="D82" s="32" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
@@ -6311,14 +6305,14 @@
         <v>582</v>
       </c>
       <c r="D83" s="32" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="3"/>
       <c r="I83" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
@@ -6339,7 +6333,7 @@
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
       <c r="I84" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="50" x14ac:dyDescent="0.35">
@@ -6380,7 +6374,7 @@
         <v>91</v>
       </c>
       <c r="D86" s="23" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>119</v>
@@ -6407,7 +6401,7 @@
         <v>91</v>
       </c>
       <c r="D87" s="23" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>118</v>
@@ -6417,7 +6411,7 @@
       </c>
       <c r="G87" s="1"/>
       <c r="H87" s="1" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="I87" s="1" t="s">
         <v>90</v>
@@ -6434,20 +6428,20 @@
         <v>91</v>
       </c>
       <c r="D88" s="23" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>665</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="G88" s="1"/>
       <c r="H88" s="1" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -6461,7 +6455,7 @@
         <v>91</v>
       </c>
       <c r="D89" s="23" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>666</v>
@@ -6488,7 +6482,7 @@
         <v>91</v>
       </c>
       <c r="D90" s="23" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>667</v>
@@ -6515,17 +6509,17 @@
         <v>91</v>
       </c>
       <c r="D91" s="23" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F91" s="53" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="G91" s="53"/>
       <c r="H91" s="53" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="I91" s="53" t="s">
         <v>90</v>
@@ -6569,7 +6563,7 @@
         <v>91</v>
       </c>
       <c r="D93" s="23" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>63</v>
@@ -6596,7 +6590,7 @@
         <v>91</v>
       </c>
       <c r="D94" s="23" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>668</v>
@@ -6606,7 +6600,7 @@
       </c>
       <c r="G94" s="1"/>
       <c r="H94" s="1" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="I94" s="3" t="s">
         <v>90</v>
@@ -6623,7 +6617,7 @@
         <v>91</v>
       </c>
       <c r="D95" s="23" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>669</v>
@@ -6650,17 +6644,17 @@
         <v>91</v>
       </c>
       <c r="D96" s="23" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F96" s="53" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="G96" s="53"/>
       <c r="H96" s="53" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="I96" s="53" t="s">
         <v>90</v>
@@ -6677,14 +6671,14 @@
         <v>582</v>
       </c>
       <c r="D97" s="32" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
       <c r="I97" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
@@ -6698,14 +6692,14 @@
         <v>582</v>
       </c>
       <c r="D98" s="32" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
       <c r="I98" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="50" x14ac:dyDescent="0.35">
@@ -6753,7 +6747,7 @@
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
       <c r="I100" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
@@ -6774,7 +6768,7 @@
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
       <c r="I101" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -6788,7 +6782,7 @@
         <v>91</v>
       </c>
       <c r="D102" s="23" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>670</v>
@@ -6815,7 +6809,7 @@
         <v>91</v>
       </c>
       <c r="D103" s="23" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>671</v>
@@ -6825,7 +6819,7 @@
       </c>
       <c r="G103" s="1"/>
       <c r="H103" s="1" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>90</v>
@@ -6842,17 +6836,17 @@
         <v>91</v>
       </c>
       <c r="D104" s="23" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F104" s="53" t="s">
-        <v>1109</v>
+        <v>1106</v>
       </c>
       <c r="G104" s="53"/>
       <c r="H104" s="53" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="I104" s="53" t="s">
         <v>90</v>
@@ -6896,7 +6890,7 @@
         <v>91</v>
       </c>
       <c r="D106" s="23" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>672</v>
@@ -6906,7 +6900,7 @@
       </c>
       <c r="G106" s="1"/>
       <c r="H106" s="1" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="I106" s="1" t="s">
         <v>90</v>
@@ -6957,7 +6951,7 @@
       <c r="G108" s="1"/>
       <c r="H108" s="3"/>
       <c r="I108" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
@@ -6978,7 +6972,7 @@
       <c r="G109" s="1"/>
       <c r="H109" s="3"/>
       <c r="I109" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
@@ -6992,14 +6986,14 @@
         <v>582</v>
       </c>
       <c r="D110" s="55" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
       <c r="H110" s="3"/>
       <c r="I110" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -7013,7 +7007,7 @@
         <v>91</v>
       </c>
       <c r="D111" s="23" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>112</v>
@@ -7040,7 +7034,7 @@
         <v>91</v>
       </c>
       <c r="D112" s="23" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>673</v>
@@ -7050,7 +7044,7 @@
       </c>
       <c r="G112" s="1"/>
       <c r="H112" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="I112" s="3" t="s">
         <v>90</v>
@@ -7067,17 +7061,17 @@
         <v>91</v>
       </c>
       <c r="D113" s="23" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E113" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F113" s="53" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="G113" s="53"/>
       <c r="H113" s="53" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
       <c r="I113" s="53" t="s">
         <v>90</v>
@@ -7094,14 +7088,14 @@
         <v>582</v>
       </c>
       <c r="D114" s="32" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
       <c r="I114" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
@@ -7115,14 +7109,14 @@
         <v>582</v>
       </c>
       <c r="D115" s="32" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
       <c r="I115" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
@@ -7136,7 +7130,7 @@
         <v>91</v>
       </c>
       <c r="D116" s="23" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>674</v>
@@ -7251,7 +7245,7 @@
       <c r="G120" s="1"/>
       <c r="H120" s="3"/>
       <c r="I120" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.35">
@@ -7272,7 +7266,7 @@
       <c r="G121" s="1"/>
       <c r="H121" s="3"/>
       <c r="I121" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.35">
@@ -7293,7 +7287,7 @@
       <c r="G122" s="1"/>
       <c r="H122" s="3"/>
       <c r="I122" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.35">
@@ -7314,7 +7308,7 @@
       <c r="G123" s="1"/>
       <c r="H123" s="3"/>
       <c r="I123" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.35">
@@ -7328,14 +7322,14 @@
         <v>582</v>
       </c>
       <c r="D124" s="35" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
       <c r="H124" s="3"/>
       <c r="I124" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.35">
@@ -7349,14 +7343,14 @@
         <v>582</v>
       </c>
       <c r="D125" s="35" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
       <c r="H125" s="3"/>
       <c r="I125" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.35">
@@ -7370,14 +7364,14 @@
         <v>582</v>
       </c>
       <c r="D126" s="49" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="E126" s="48"/>
       <c r="F126" s="48"/>
       <c r="G126" s="48"/>
       <c r="H126" s="53"/>
       <c r="I126" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -7391,7 +7385,7 @@
         <v>91</v>
       </c>
       <c r="D127" s="23" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>677</v>
@@ -7418,7 +7412,7 @@
         <v>91</v>
       </c>
       <c r="D128" s="23" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>526</v>
@@ -7428,7 +7422,7 @@
       </c>
       <c r="G128" s="1"/>
       <c r="H128" s="3" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="I128" s="1" t="s">
         <v>90</v>
@@ -7499,17 +7493,17 @@
         <v>91</v>
       </c>
       <c r="D131" s="23" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F131" s="53" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="G131" s="53"/>
       <c r="H131" s="53" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="I131" s="53" t="s">
         <v>90</v>
@@ -7661,17 +7655,17 @@
         <v>91</v>
       </c>
       <c r="D137" s="23" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="G137" s="53"/>
       <c r="H137" s="53" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="I137" s="3" t="s">
         <v>90</v>
@@ -7688,17 +7682,17 @@
         <v>91</v>
       </c>
       <c r="D138" s="50" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F138" s="53" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="G138" s="53"/>
       <c r="H138" s="53" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="I138" s="3" t="s">
         <v>90</v>
@@ -7715,17 +7709,17 @@
         <v>91</v>
       </c>
       <c r="D139" s="50" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F139" s="53" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="G139" s="53"/>
       <c r="H139" s="53" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="I139" s="53" t="s">
         <v>90</v>
@@ -7776,7 +7770,7 @@
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
       <c r="I141" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.35">
@@ -7797,7 +7791,7 @@
       <c r="G142" s="1"/>
       <c r="H142" s="1"/>
       <c r="I142" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.35">
@@ -7818,7 +7812,7 @@
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
       <c r="I143" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.35">
@@ -7839,7 +7833,7 @@
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
       <c r="I144" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -7907,7 +7901,7 @@
         <v>91</v>
       </c>
       <c r="D147" s="23" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>681</v>
@@ -7917,7 +7911,7 @@
       </c>
       <c r="G147" s="1"/>
       <c r="H147" s="1" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="I147" s="3" t="s">
         <v>90</v>
@@ -7961,7 +7955,7 @@
         <v>91</v>
       </c>
       <c r="D149" s="23" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>683</v>
@@ -7988,7 +7982,7 @@
         <v>91</v>
       </c>
       <c r="D150" s="23" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>684</v>
@@ -7998,7 +7992,7 @@
       </c>
       <c r="G150" s="1"/>
       <c r="H150" s="1" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="I150" s="3" t="s">
         <v>90</v>
@@ -8042,17 +8036,17 @@
         <v>91</v>
       </c>
       <c r="D152" s="34" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F152" s="53" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
       <c r="G152" s="53"/>
       <c r="H152" s="53" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
       <c r="I152" s="53" t="s">
         <v>90</v>
@@ -8238,7 +8232,7 @@
       <c r="G159" s="25"/>
       <c r="H159" s="25"/>
       <c r="I159" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.35">
@@ -8252,14 +8246,14 @@
         <v>582</v>
       </c>
       <c r="D160" s="35" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="E160" s="25"/>
       <c r="F160" s="25"/>
       <c r="G160" s="25"/>
       <c r="H160" s="25"/>
       <c r="I160" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="161" spans="1:9" s="37" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -8523,7 +8517,7 @@
       <c r="G170" s="25"/>
       <c r="H170" s="25"/>
       <c r="I170" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -8537,7 +8531,7 @@
         <v>91</v>
       </c>
       <c r="D171" s="22" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E171" s="3" t="s">
         <v>16</v>
@@ -8574,7 +8568,7 @@
       </c>
       <c r="G172" s="3"/>
       <c r="H172" s="3" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="I172" s="3" t="s">
         <v>90</v>
@@ -8645,17 +8639,17 @@
         <v>91</v>
       </c>
       <c r="D175" s="22" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F175" s="53" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="G175" s="53"/>
       <c r="H175" s="53" t="s">
-        <v>1131</v>
+        <v>1128</v>
       </c>
       <c r="I175" s="53" t="s">
         <v>90</v>
@@ -8706,7 +8700,7 @@
       <c r="G177" s="25"/>
       <c r="H177" s="25"/>
       <c r="I177" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="178" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -8720,7 +8714,7 @@
         <v>91</v>
       </c>
       <c r="D178" s="22" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>16</v>
@@ -8855,17 +8849,17 @@
         <v>91</v>
       </c>
       <c r="D183" s="22" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E183" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F183" s="53" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="G183" s="53"/>
       <c r="H183" s="53" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
       <c r="I183" s="53" t="s">
         <v>90</v>
@@ -8984,7 +8978,7 @@
         <v>91</v>
       </c>
       <c r="D188" s="22" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E188" s="3" t="s">
         <v>16</v>
@@ -9011,7 +9005,7 @@
         <v>91</v>
       </c>
       <c r="D189" s="22" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E189" s="3" t="s">
         <v>16</v>
@@ -9021,7 +9015,7 @@
       </c>
       <c r="G189" s="3"/>
       <c r="H189" s="3" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="I189" s="3" t="s">
         <v>90</v>
@@ -9065,17 +9059,17 @@
         <v>91</v>
       </c>
       <c r="D191" s="22" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E191" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F191" s="53" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
       <c r="G191" s="53"/>
       <c r="H191" s="53" t="s">
-        <v>1133</v>
+        <v>1130</v>
       </c>
       <c r="I191" s="53" t="s">
         <v>90</v>
@@ -9119,14 +9113,14 @@
         <v>582</v>
       </c>
       <c r="D193" s="35" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="E193" s="25"/>
       <c r="F193" s="25"/>
       <c r="G193" s="25"/>
       <c r="H193" s="25"/>
       <c r="I193" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="194" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -9140,14 +9134,14 @@
         <v>582</v>
       </c>
       <c r="D194" s="35" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="E194" s="25"/>
       <c r="F194" s="25"/>
       <c r="G194" s="25"/>
       <c r="H194" s="25"/>
       <c r="I194" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="195" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -9161,7 +9155,7 @@
         <v>91</v>
       </c>
       <c r="D195" s="22" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E195" s="3" t="s">
         <v>16</v>
@@ -9188,7 +9182,7 @@
         <v>91</v>
       </c>
       <c r="D196" s="22" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E196" s="3" t="s">
         <v>16</v>
@@ -9198,7 +9192,7 @@
       </c>
       <c r="G196" s="3"/>
       <c r="H196" s="3" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="I196" s="3" t="s">
         <v>90</v>
@@ -9221,11 +9215,11 @@
         <v>16</v>
       </c>
       <c r="F197" s="3" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="G197" s="3"/>
       <c r="H197" s="3" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="I197" s="3" t="s">
         <v>90</v>
@@ -9242,17 +9236,17 @@
         <v>91</v>
       </c>
       <c r="D198" s="22" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="E198" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F198" s="53" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="G198" s="53"/>
       <c r="H198" s="53" t="s">
-        <v>1134</v>
+        <v>1131</v>
       </c>
       <c r="I198" s="53" t="s">
         <v>90</v>
@@ -9303,7 +9297,7 @@
       <c r="G200" s="53"/>
       <c r="H200" s="53"/>
       <c r="I200" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="201" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -9317,14 +9311,14 @@
         <v>582</v>
       </c>
       <c r="D201" s="55" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="E201" s="53"/>
       <c r="F201" s="48"/>
       <c r="G201" s="53"/>
       <c r="H201" s="53"/>
       <c r="I201" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="202" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -9365,17 +9359,17 @@
         <v>4</v>
       </c>
       <c r="D203" s="22" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="E203" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F203" s="3" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="G203" s="53"/>
       <c r="H203" s="3" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="I203" s="53" t="s">
         <v>90</v>
@@ -9415,24 +9409,18 @@
       <c r="B205" s="53" t="s">
         <v>894</v>
       </c>
-      <c r="C205" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="D205" s="50" t="s">
-        <v>1078</v>
-      </c>
-      <c r="E205" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="F205" s="48" t="s">
-        <v>911</v>
-      </c>
+      <c r="C205" s="48" t="s">
+        <v>582</v>
+      </c>
+      <c r="D205" s="49" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E205" s="53"/>
+      <c r="F205" s="53"/>
       <c r="G205" s="53"/>
-      <c r="H205" s="53" t="s">
-        <v>912</v>
-      </c>
-      <c r="I205" s="53" t="s">
-        <v>90</v>
+      <c r="H205" s="53"/>
+      <c r="I205" s="1" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.35">
@@ -9446,14 +9434,14 @@
         <v>582</v>
       </c>
       <c r="D206" s="49" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="E206" s="53"/>
       <c r="F206" s="53"/>
       <c r="G206" s="53"/>
       <c r="H206" s="53"/>
       <c r="I206" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.35">
@@ -9467,14 +9455,14 @@
         <v>582</v>
       </c>
       <c r="D207" s="49" t="s">
-        <v>1012</v>
+        <v>1045</v>
       </c>
       <c r="E207" s="53"/>
       <c r="F207" s="53"/>
       <c r="G207" s="53"/>
       <c r="H207" s="53"/>
       <c r="I207" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.35">
@@ -9488,14 +9476,14 @@
         <v>582</v>
       </c>
       <c r="D208" s="49" t="s">
-        <v>1047</v>
+        <v>1009</v>
       </c>
       <c r="E208" s="53"/>
       <c r="F208" s="53"/>
       <c r="G208" s="53"/>
       <c r="H208" s="53"/>
       <c r="I208" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.35">
@@ -9509,54 +9497,60 @@
         <v>582</v>
       </c>
       <c r="D209" s="49" t="s">
-        <v>1011</v>
+        <v>1074</v>
       </c>
       <c r="E209" s="53"/>
       <c r="F209" s="53"/>
       <c r="G209" s="53"/>
       <c r="H209" s="53"/>
       <c r="I209" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A210" s="25">
         <v>209</v>
       </c>
-      <c r="B210" s="53" t="s">
-        <v>894</v>
+      <c r="B210" s="48" t="s">
+        <v>895</v>
       </c>
       <c r="C210" s="48" t="s">
-        <v>582</v>
-      </c>
-      <c r="D210" s="49" t="s">
-        <v>1077</v>
-      </c>
-      <c r="E210" s="53"/>
-      <c r="F210" s="53"/>
+        <v>4</v>
+      </c>
+      <c r="D210" s="52" t="s">
+        <v>895</v>
+      </c>
+      <c r="E210" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="F210" s="53" t="s">
+        <v>911</v>
+      </c>
       <c r="G210" s="53"/>
-      <c r="H210" s="53"/>
-      <c r="I210" s="1" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H210" s="53" t="s">
+        <v>912</v>
+      </c>
+      <c r="I210" s="53" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A211" s="25">
         <v>210</v>
       </c>
       <c r="B211" s="48" t="s">
         <v>895</v>
       </c>
-      <c r="C211" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="D211" s="52" t="s">
-        <v>895</v>
+      <c r="C211" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D211" s="51" t="s">
+        <v>1004</v>
       </c>
       <c r="E211" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="F211" s="53" t="s">
+      <c r="F211" s="48" t="s">
         <v>913</v>
       </c>
       <c r="G211" s="53"/>
@@ -9578,7 +9572,7 @@
         <v>91</v>
       </c>
       <c r="D212" s="51" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="E212" s="53" t="s">
         <v>16</v>
@@ -9588,7 +9582,7 @@
       </c>
       <c r="G212" s="53"/>
       <c r="H212" s="53" t="s">
-        <v>916</v>
+        <v>1031</v>
       </c>
       <c r="I212" s="53" t="s">
         <v>90</v>
@@ -9605,17 +9599,17 @@
         <v>91</v>
       </c>
       <c r="D213" s="51" t="s">
-        <v>1007</v>
+        <v>898</v>
       </c>
       <c r="E213" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F213" s="48" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="G213" s="53"/>
       <c r="H213" s="53" t="s">
-        <v>1033</v>
+        <v>917</v>
       </c>
       <c r="I213" s="53" t="s">
         <v>90</v>
@@ -9632,23 +9626,23 @@
         <v>91</v>
       </c>
       <c r="D214" s="51" t="s">
-        <v>898</v>
+        <v>991</v>
       </c>
       <c r="E214" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="F214" s="48" t="s">
-        <v>918</v>
+      <c r="F214" s="53" t="s">
+        <v>992</v>
       </c>
       <c r="G214" s="53"/>
-      <c r="H214" s="53" t="s">
-        <v>919</v>
+      <c r="H214" s="3" t="s">
+        <v>993</v>
       </c>
       <c r="I214" s="53" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="215" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A215" s="25">
         <v>214</v>
       </c>
@@ -9659,17 +9653,17 @@
         <v>91</v>
       </c>
       <c r="D215" s="51" t="s">
-        <v>993</v>
-      </c>
-      <c r="E215" s="53" t="s">
+        <v>1072</v>
+      </c>
+      <c r="E215" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F215" s="53" t="s">
-        <v>994</v>
+        <v>1115</v>
       </c>
       <c r="G215" s="53"/>
-      <c r="H215" s="3" t="s">
-        <v>995</v>
+      <c r="H215" s="53" t="s">
+        <v>1132</v>
       </c>
       <c r="I215" s="53" t="s">
         <v>90</v>
@@ -9682,24 +9676,18 @@
       <c r="B216" s="48" t="s">
         <v>895</v>
       </c>
-      <c r="C216" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="D216" s="51" t="s">
-        <v>1074</v>
-      </c>
-      <c r="E216" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F216" s="53" t="s">
-        <v>1118</v>
-      </c>
+      <c r="C216" s="48" t="s">
+        <v>582</v>
+      </c>
+      <c r="D216" s="55" t="s">
+        <v>899</v>
+      </c>
+      <c r="E216" s="53"/>
+      <c r="F216" s="48"/>
       <c r="G216" s="53"/>
-      <c r="H216" s="53" t="s">
-        <v>1135</v>
-      </c>
-      <c r="I216" s="53" t="s">
-        <v>90</v>
+      <c r="H216" s="53"/>
+      <c r="I216" s="1" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.35">
@@ -9713,14 +9701,14 @@
         <v>582</v>
       </c>
       <c r="D217" s="55" t="s">
-        <v>899</v>
+        <v>1012</v>
       </c>
       <c r="E217" s="53"/>
-      <c r="F217" s="48"/>
+      <c r="F217" s="53"/>
       <c r="G217" s="53"/>
       <c r="H217" s="53"/>
       <c r="I217" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.35">
@@ -9734,14 +9722,14 @@
         <v>582</v>
       </c>
       <c r="D218" s="55" t="s">
-        <v>1014</v>
+        <v>900</v>
       </c>
       <c r="E218" s="53"/>
       <c r="F218" s="53"/>
       <c r="G218" s="53"/>
       <c r="H218" s="53"/>
       <c r="I218" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.35">
@@ -9749,20 +9737,26 @@
         <v>218</v>
       </c>
       <c r="B219" s="48" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="C219" s="48" t="s">
-        <v>582</v>
-      </c>
-      <c r="D219" s="55" t="s">
-        <v>900</v>
-      </c>
-      <c r="E219" s="53"/>
-      <c r="F219" s="53"/>
+        <v>4</v>
+      </c>
+      <c r="D219" s="52" t="s">
+        <v>896</v>
+      </c>
+      <c r="E219" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="F219" s="48" t="s">
+        <v>918</v>
+      </c>
       <c r="G219" s="53"/>
-      <c r="H219" s="53"/>
-      <c r="I219" s="1" t="s">
-        <v>933</v>
+      <c r="H219" s="53" t="s">
+        <v>935</v>
+      </c>
+      <c r="I219" s="53" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.35">
@@ -9770,53 +9764,53 @@
         <v>219</v>
       </c>
       <c r="B220" s="48" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="C220" s="48" t="s">
         <v>4</v>
       </c>
       <c r="D220" s="52" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="E220" s="53" t="s">
-        <v>16</v>
-      </c>
-      <c r="F220" s="48" t="s">
-        <v>920</v>
+        <v>919</v>
+      </c>
+      <c r="F220" s="53" t="s">
+        <v>897</v>
       </c>
       <c r="G220" s="53"/>
       <c r="H220" s="53" t="s">
-        <v>937</v>
+        <v>920</v>
       </c>
       <c r="I220" s="53" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A221" s="25">
         <v>220</v>
       </c>
       <c r="B221" s="48" t="s">
         <v>897</v>
       </c>
-      <c r="C221" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="D221" s="52" t="s">
-        <v>897</v>
+      <c r="C221" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D221" s="51" t="s">
+        <v>1075</v>
       </c>
       <c r="E221" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="F221" s="48" t="s">
         <v>921</v>
-      </c>
-      <c r="F221" s="53" t="s">
-        <v>897</v>
       </c>
       <c r="G221" s="53"/>
       <c r="H221" s="53" t="s">
         <v>922</v>
       </c>
-      <c r="I221" s="53" t="s">
-        <v>90</v>
+      <c r="I221" s="3" t="s">
+        <v>930</v>
       </c>
     </row>
     <row r="222" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -9830,7 +9824,7 @@
         <v>91</v>
       </c>
       <c r="D222" s="51" t="s">
-        <v>1078</v>
+        <v>902</v>
       </c>
       <c r="E222" s="53" t="s">
         <v>16</v>
@@ -9842,8 +9836,8 @@
       <c r="H222" s="53" t="s">
         <v>924</v>
       </c>
-      <c r="I222" s="3" t="s">
-        <v>932</v>
+      <c r="I222" s="53" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="223" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -9857,7 +9851,7 @@
         <v>91</v>
       </c>
       <c r="D223" s="51" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="E223" s="53" t="s">
         <v>16</v>
@@ -9869,8 +9863,8 @@
       <c r="H223" s="53" t="s">
         <v>926</v>
       </c>
-      <c r="I223" s="53" t="s">
-        <v>90</v>
+      <c r="I223" s="3" t="s">
+        <v>930</v>
       </c>
     </row>
     <row r="224" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -9884,20 +9878,20 @@
         <v>91</v>
       </c>
       <c r="D224" s="51" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="E224" s="53" t="s">
-        <v>16</v>
+        <v>927</v>
       </c>
       <c r="F224" s="48" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="G224" s="53"/>
       <c r="H224" s="53" t="s">
-        <v>928</v>
-      </c>
-      <c r="I224" s="3" t="s">
-        <v>932</v>
+        <v>929</v>
+      </c>
+      <c r="I224" s="53" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="225" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -9911,17 +9905,17 @@
         <v>91</v>
       </c>
       <c r="D225" s="51" t="s">
-        <v>904</v>
+        <v>1005</v>
       </c>
       <c r="E225" s="53" t="s">
-        <v>929</v>
-      </c>
-      <c r="F225" s="48" t="s">
-        <v>930</v>
+        <v>16</v>
+      </c>
+      <c r="F225" s="3" t="s">
+        <v>996</v>
       </c>
       <c r="G225" s="53"/>
-      <c r="H225" s="53" t="s">
-        <v>931</v>
+      <c r="H225" s="3" t="s">
+        <v>997</v>
       </c>
       <c r="I225" s="53" t="s">
         <v>90</v>
@@ -9938,17 +9932,17 @@
         <v>91</v>
       </c>
       <c r="D226" s="51" t="s">
-        <v>1007</v>
+        <v>994</v>
       </c>
       <c r="E226" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F226" s="3" t="s">
-        <v>998</v>
+        <v>1073</v>
       </c>
       <c r="G226" s="53"/>
       <c r="H226" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="I226" s="53" t="s">
         <v>90</v>
@@ -9965,13 +9959,13 @@
         <v>91</v>
       </c>
       <c r="D227" s="51" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="E227" s="53" t="s">
         <v>16</v>
       </c>
       <c r="F227" s="3" t="s">
-        <v>1075</v>
+        <v>999</v>
       </c>
       <c r="G227" s="53"/>
       <c r="H227" s="3" t="s">
@@ -9981,7 +9975,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="228" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A228" s="25">
         <v>227</v>
       </c>
@@ -9992,19 +9986,19 @@
         <v>91</v>
       </c>
       <c r="D228" s="51" t="s">
-        <v>997</v>
-      </c>
-      <c r="E228" s="53" t="s">
+        <v>1072</v>
+      </c>
+      <c r="E228" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F228" s="3" t="s">
-        <v>1001</v>
+        <v>1069</v>
       </c>
       <c r="G228" s="53"/>
       <c r="H228" s="3" t="s">
-        <v>1002</v>
-      </c>
-      <c r="I228" s="53" t="s">
+        <v>1133</v>
+      </c>
+      <c r="I228" s="3" t="s">
         <v>90</v>
       </c>
     </row>
@@ -10019,17 +10013,17 @@
         <v>91</v>
       </c>
       <c r="D229" s="51" t="s">
-        <v>1074</v>
+        <v>1004</v>
       </c>
       <c r="E229" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F229" s="3" t="s">
+        <v>1070</v>
+      </c>
+      <c r="G229" s="53"/>
+      <c r="H229" s="1" t="s">
         <v>1071</v>
-      </c>
-      <c r="G229" s="53"/>
-      <c r="H229" s="3" t="s">
-        <v>1136</v>
       </c>
       <c r="I229" s="3" t="s">
         <v>90</v>
@@ -10042,24 +10036,18 @@
       <c r="B230" s="48" t="s">
         <v>897</v>
       </c>
-      <c r="C230" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="D230" s="51" t="s">
-        <v>1006</v>
-      </c>
-      <c r="E230" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F230" s="3" t="s">
-        <v>1072</v>
-      </c>
+      <c r="C230" s="48" t="s">
+        <v>582</v>
+      </c>
+      <c r="D230" s="55" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E230" s="53"/>
+      <c r="F230" s="53"/>
       <c r="G230" s="53"/>
-      <c r="H230" s="1" t="s">
-        <v>1073</v>
-      </c>
-      <c r="I230" s="3" t="s">
-        <v>90</v>
+      <c r="H230" s="53"/>
+      <c r="I230" s="1" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.35">
@@ -10073,62 +10061,68 @@
         <v>582</v>
       </c>
       <c r="D231" s="55" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="E231" s="53"/>
       <c r="F231" s="53"/>
       <c r="G231" s="53"/>
       <c r="H231" s="53"/>
       <c r="I231" s="1" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A232" s="25">
         <v>231</v>
       </c>
       <c r="B232" s="48" t="s">
-        <v>897</v>
+        <v>1049</v>
       </c>
       <c r="C232" s="48" t="s">
-        <v>582</v>
-      </c>
-      <c r="D232" s="55" t="s">
-        <v>1016</v>
-      </c>
-      <c r="E232" s="53"/>
-      <c r="F232" s="53"/>
+        <v>4</v>
+      </c>
+      <c r="D232" s="52" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E232" s="3" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F232" s="3" t="s">
+        <v>1049</v>
+      </c>
       <c r="G232" s="53"/>
-      <c r="H232" s="53"/>
-      <c r="I232" s="1" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="233" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+      <c r="H232" s="3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="I232" s="3" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A233" s="25">
         <v>232</v>
       </c>
       <c r="B233" s="48" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C233" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D233" s="22" t="s">
         <v>1051</v>
       </c>
-      <c r="C233" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="D233" s="52" t="s">
-        <v>1051</v>
-      </c>
       <c r="E233" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F233" s="3" t="s">
         <v>1055</v>
-      </c>
-      <c r="F233" s="3" t="s">
-        <v>1051</v>
       </c>
       <c r="G233" s="53"/>
       <c r="H233" s="3" t="s">
         <v>1056</v>
       </c>
       <c r="I233" s="3" t="s">
-        <v>933</v>
+        <v>90</v>
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.35">
@@ -10136,13 +10130,13 @@
         <v>233</v>
       </c>
       <c r="B234" s="48" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="C234" s="53" t="s">
         <v>91</v>
       </c>
       <c r="D234" s="22" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="E234" s="3" t="s">
         <v>16</v>
@@ -10150,7 +10144,7 @@
       <c r="F234" s="3" t="s">
         <v>1057</v>
       </c>
-      <c r="G234" s="53"/>
+      <c r="G234" s="3"/>
       <c r="H234" s="3" t="s">
         <v>1058</v>
       </c>
@@ -10163,13 +10157,13 @@
         <v>234</v>
       </c>
       <c r="B235" s="48" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="C235" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="D235" s="22" t="s">
-        <v>1054</v>
+      <c r="D235" s="50" t="s">
+        <v>1004</v>
       </c>
       <c r="E235" s="3" t="s">
         <v>16</v>
@@ -10190,13 +10184,13 @@
         <v>235</v>
       </c>
       <c r="B236" s="48" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="C236" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="D236" s="50" t="s">
-        <v>1006</v>
+      <c r="D236" s="22" t="s">
+        <v>737</v>
       </c>
       <c r="E236" s="3" t="s">
         <v>16</v>
@@ -10204,11 +10198,11 @@
       <c r="F236" s="3" t="s">
         <v>1061</v>
       </c>
-      <c r="G236" s="3"/>
+      <c r="G236" s="53"/>
       <c r="H236" s="3" t="s">
         <v>1062</v>
       </c>
-      <c r="I236" s="3" t="s">
+      <c r="I236" s="53" t="s">
         <v>90</v>
       </c>
     </row>
@@ -10217,47 +10211,47 @@
         <v>236</v>
       </c>
       <c r="B237" s="48" t="s">
-        <v>1051</v>
-      </c>
-      <c r="C237" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="D237" s="22" t="s">
-        <v>737</v>
-      </c>
-      <c r="E237" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F237" s="3" t="s">
-        <v>1063</v>
-      </c>
+        <v>1049</v>
+      </c>
+      <c r="C237" s="48" t="s">
+        <v>582</v>
+      </c>
+      <c r="D237" s="55" t="s">
+        <v>1050</v>
+      </c>
+      <c r="E237" s="53"/>
+      <c r="F237" s="53"/>
       <c r="G237" s="53"/>
-      <c r="H237" s="3" t="s">
-        <v>1064</v>
-      </c>
-      <c r="I237" s="53" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H237" s="53"/>
+      <c r="I237" s="1" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A238" s="25">
         <v>237</v>
       </c>
       <c r="B238" s="48" t="s">
-        <v>1051</v>
+        <v>1078</v>
       </c>
       <c r="C238" s="48" t="s">
-        <v>582</v>
-      </c>
-      <c r="D238" s="55" t="s">
-        <v>1052</v>
-      </c>
-      <c r="E238" s="53"/>
-      <c r="F238" s="53"/>
+        <v>4</v>
+      </c>
+      <c r="D238" s="52" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E238" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F238" s="3" t="s">
+        <v>1079</v>
+      </c>
       <c r="G238" s="53"/>
-      <c r="H238" s="53"/>
-      <c r="I238" s="1" t="s">
-        <v>933</v>
+      <c r="H238" s="3" t="s">
+        <v>1080</v>
+      </c>
+      <c r="I238" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="239" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -10265,23 +10259,23 @@
         <v>238</v>
       </c>
       <c r="B239" s="48" t="s">
-        <v>1081</v>
-      </c>
-      <c r="C239" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="D239" s="52" t="s">
-        <v>1081</v>
+        <v>1078</v>
+      </c>
+      <c r="C239" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D239" s="50" t="s">
+        <v>1004</v>
       </c>
       <c r="E239" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F239" s="3" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="G239" s="53"/>
       <c r="H239" s="3" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="I239" s="3" t="s">
         <v>90</v>
@@ -10292,107 +10286,101 @@
         <v>239</v>
       </c>
       <c r="B240" s="48" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="C240" s="53" t="s">
         <v>91</v>
       </c>
       <c r="D240" s="50" t="s">
-        <v>1006</v>
+        <v>737</v>
       </c>
       <c r="E240" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F240" s="3" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="G240" s="53"/>
       <c r="H240" s="3" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="I240" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="241" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A241" s="25">
         <v>240</v>
       </c>
       <c r="B241" s="48" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="C241" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="D241" s="50" t="s">
-        <v>737</v>
+      <c r="D241" s="22" t="s">
+        <v>1005</v>
       </c>
       <c r="E241" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F241" s="3" t="s">
+      <c r="F241" s="53" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G241" s="53"/>
+      <c r="H241" s="53" t="s">
         <v>1086</v>
       </c>
-      <c r="G241" s="53"/>
-      <c r="H241" s="3" t="s">
-        <v>1087</v>
-      </c>
       <c r="I241" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A242" s="25">
         <v>241</v>
       </c>
       <c r="B242" s="48" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="C242" s="53" t="s">
         <v>91</v>
       </c>
       <c r="D242" s="22" t="s">
-        <v>1007</v>
+        <v>1072</v>
       </c>
       <c r="E242" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F242" s="53" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="G242" s="53"/>
       <c r="H242" s="53" t="s">
-        <v>1089</v>
+        <v>1134</v>
       </c>
       <c r="I242" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="243" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A243" s="25">
         <v>242</v>
       </c>
       <c r="B243" s="48" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="C243" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="D243" s="22" t="s">
-        <v>1074</v>
-      </c>
-      <c r="E243" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F243" s="53" t="s">
-        <v>1090</v>
-      </c>
+        <v>582</v>
+      </c>
+      <c r="D243" s="55" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E243" s="3"/>
+      <c r="F243" s="3"/>
       <c r="G243" s="53"/>
-      <c r="H243" s="53" t="s">
-        <v>1137</v>
-      </c>
+      <c r="H243" s="53"/>
       <c r="I243" s="3" t="s">
-        <v>90</v>
+        <v>931</v>
       </c>
     </row>
     <row r="244" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -10400,20 +10388,26 @@
         <v>243</v>
       </c>
       <c r="B244" s="48" t="s">
-        <v>1091</v>
-      </c>
-      <c r="C244" s="53" t="s">
-        <v>582</v>
-      </c>
-      <c r="D244" s="55" t="s">
-        <v>1139</v>
-      </c>
-      <c r="E244" s="3"/>
-      <c r="F244" s="3"/>
+        <v>1088</v>
+      </c>
+      <c r="C244" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D244" s="52" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E244" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F244" s="3" t="s">
+        <v>1089</v>
+      </c>
       <c r="G244" s="53"/>
-      <c r="H244" s="53"/>
+      <c r="H244" s="3" t="s">
+        <v>1090</v>
+      </c>
       <c r="I244" s="3" t="s">
-        <v>933</v>
+        <v>90</v>
       </c>
     </row>
     <row r="245" spans="1:9" ht="25" x14ac:dyDescent="0.35">
@@ -10421,13 +10415,13 @@
         <v>244</v>
       </c>
       <c r="B245" s="48" t="s">
-        <v>1091</v>
-      </c>
-      <c r="C245" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="D245" s="52" t="s">
-        <v>1091</v>
+        <v>1088</v>
+      </c>
+      <c r="C245" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D245" s="50" t="s">
+        <v>1004</v>
       </c>
       <c r="E245" s="3" t="s">
         <v>16</v>
@@ -10448,23 +10442,23 @@
         <v>245</v>
       </c>
       <c r="B246" s="48" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="C246" s="53" t="s">
         <v>91</v>
       </c>
       <c r="D246" s="50" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="E246" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F246" s="3" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="G246" s="53"/>
       <c r="H246" s="3" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="I246" s="3" t="s">
         <v>90</v>
@@ -10475,23 +10469,23 @@
         <v>246</v>
       </c>
       <c r="B247" s="48" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="C247" s="53" t="s">
         <v>91</v>
       </c>
       <c r="D247" s="50" t="s">
-        <v>1007</v>
+        <v>1072</v>
       </c>
       <c r="E247" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F247" s="3" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="G247" s="53"/>
-      <c r="H247" s="3" t="s">
-        <v>1098</v>
+      <c r="H247" s="53" t="s">
+        <v>1135</v>
       </c>
       <c r="I247" s="3" t="s">
         <v>90</v>
@@ -10502,57 +10496,30 @@
         <v>247</v>
       </c>
       <c r="B248" s="48" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C248" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D248" s="50" t="s">
         <v>1091</v>
-      </c>
-      <c r="C248" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="D248" s="50" t="s">
-        <v>1074</v>
       </c>
       <c r="E248" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F248" s="3" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="G248" s="53"/>
       <c r="H248" s="53" t="s">
-        <v>1138</v>
+        <v>1098</v>
       </c>
       <c r="I248" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="249" spans="1:9" ht="25" x14ac:dyDescent="0.35">
-      <c r="A249" s="25">
-        <v>248</v>
-      </c>
-      <c r="B249" s="48" t="s">
-        <v>1091</v>
-      </c>
-      <c r="C249" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="D249" s="50" t="s">
-        <v>1094</v>
-      </c>
-      <c r="E249" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F249" s="3" t="s">
-        <v>1100</v>
-      </c>
-      <c r="G249" s="53"/>
-      <c r="H249" s="53" t="s">
-        <v>1101</v>
-      </c>
-      <c r="I249" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:I249" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I248" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -11323,7 +11290,7 @@
         <v>587</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>614</v>
@@ -11349,7 +11316,7 @@
         <v>587</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>614</v>
@@ -11373,7 +11340,7 @@
         <v>587</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D34" s="13" t="s">
         <v>614</v>
@@ -11397,7 +11364,7 @@
         <v>587</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D35" s="13" t="s">
         <v>614</v>
@@ -11421,7 +11388,7 @@
         <v>587</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D36" s="13" t="s">
         <v>614</v>
@@ -11445,7 +11412,7 @@
         <v>587</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D37" s="13" t="s">
         <v>614</v>
@@ -11469,7 +11436,7 @@
         <v>587</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D38" s="13" t="s">
         <v>614</v>
@@ -11493,7 +11460,7 @@
         <v>587</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D39" s="13" t="s">
         <v>614</v>
@@ -11519,7 +11486,7 @@
         <v>587</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D40" s="13" t="s">
         <v>614</v>
@@ -11543,7 +11510,7 @@
         <v>587</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D41" s="13" t="s">
         <v>614</v>
@@ -11567,7 +11534,7 @@
         <v>587</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D42" s="13" t="s">
         <v>614</v>
@@ -12456,7 +12423,7 @@
         <v>497</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -12482,7 +12449,7 @@
         <v>498</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
@@ -13790,11 +13757,11 @@
         <v>16</v>
       </c>
       <c r="F133" s="41" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="G133" s="38"/>
       <c r="H133" s="41" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -13814,11 +13781,11 @@
         <v>16</v>
       </c>
       <c r="F134" s="41" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="G134" s="42"/>
       <c r="H134" s="41" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -13838,11 +13805,11 @@
         <v>16</v>
       </c>
       <c r="F135" s="41" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="G135" s="42"/>
       <c r="H135" s="41" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -13862,11 +13829,11 @@
         <v>16</v>
       </c>
       <c r="F136" s="41" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="G136" s="42"/>
       <c r="H136" s="1" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
     </row>
     <row r="137" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -13886,11 +13853,11 @@
         <v>16</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="G137" s="42"/>
       <c r="H137" s="3" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -13910,11 +13877,11 @@
         <v>16</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="G138" s="42"/>
       <c r="H138" s="3" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.35">
@@ -13934,11 +13901,11 @@
         <v>16</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="G139" s="3"/>
       <c r="H139" s="3" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -13952,17 +13919,17 @@
         <v>574</v>
       </c>
       <c r="D140" s="45" t="s">
+        <v>957</v>
+      </c>
+      <c r="E140" s="47" t="s">
+        <v>958</v>
+      </c>
+      <c r="F140" s="47" t="s">
         <v>959</v>
-      </c>
-      <c r="E140" s="47" t="s">
-        <v>960</v>
-      </c>
-      <c r="F140" s="47" t="s">
-        <v>961</v>
       </c>
       <c r="G140" s="46"/>
       <c r="H140" s="46" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
@@ -13976,17 +13943,17 @@
         <v>574</v>
       </c>
       <c r="D141" s="45" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="E141" s="42" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="F141" s="42" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="G141" s="42"/>
       <c r="H141" s="42" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="142" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -14000,19 +13967,19 @@
         <v>574</v>
       </c>
       <c r="D142" s="45" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="E142" s="42" t="s">
+        <v>964</v>
+      </c>
+      <c r="F142" s="42" t="s">
+        <v>965</v>
+      </c>
+      <c r="G142" s="42" t="s">
         <v>966</v>
       </c>
-      <c r="F142" s="42" t="s">
+      <c r="H142" s="42" t="s">
         <v>967</v>
-      </c>
-      <c r="G142" s="42" t="s">
-        <v>968</v>
-      </c>
-      <c r="H142" s="42" t="s">
-        <v>969</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.35">
@@ -14026,17 +13993,17 @@
         <v>574</v>
       </c>
       <c r="D143" s="45" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="E143" s="42" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="F143" s="42" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="G143" s="42"/>
       <c r="H143" s="42" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.35">
@@ -14050,19 +14017,19 @@
         <v>574</v>
       </c>
       <c r="D144" s="45" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="E144" s="42" t="s">
+        <v>971</v>
+      </c>
+      <c r="F144" s="42" t="s">
+        <v>972</v>
+      </c>
+      <c r="G144" s="42" t="s">
         <v>973</v>
       </c>
-      <c r="F144" s="42" t="s">
+      <c r="H144" s="42" t="s">
         <v>974</v>
-      </c>
-      <c r="G144" s="42" t="s">
-        <v>975</v>
-      </c>
-      <c r="H144" s="42" t="s">
-        <v>976</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.35">
@@ -14076,19 +14043,19 @@
         <v>574</v>
       </c>
       <c r="D145" s="45" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="E145" s="42" t="s">
+        <v>975</v>
+      </c>
+      <c r="F145" s="42" t="s">
+        <v>976</v>
+      </c>
+      <c r="G145" s="42" t="s">
         <v>977</v>
       </c>
-      <c r="F145" s="42" t="s">
+      <c r="H145" s="42" t="s">
         <v>978</v>
-      </c>
-      <c r="G145" s="42" t="s">
-        <v>979</v>
-      </c>
-      <c r="H145" s="42" t="s">
-        <v>980</v>
       </c>
     </row>
     <row r="146" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
@@ -14102,17 +14069,17 @@
         <v>574</v>
       </c>
       <c r="D146" s="45" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="E146" s="42" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="F146" s="42" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="G146" s="42"/>
       <c r="H146" s="42" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
   </sheetData>
@@ -14138,15 +14105,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -14368,6 +14326,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
   <ds:schemaRefs>
@@ -14377,24 +14344,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14412,4 +14361,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update 163 - add to objective level valid value set
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA56745-A1AE-4168-A25D-DB4D87AB5945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D281F9-55F3-472F-99E8-360367CF7BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="15530" windowHeight="9700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="730" yWindow="240" windowWidth="16650" windowHeight="10010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DDF Entities&amp;Attributes'!$A$1:$I$256</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DDF valid value sets'!$A$6:$M$124</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DDF valid value sets'!$A$6:$M$125</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2708" uniqueCount="1183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2715" uniqueCount="1186">
   <si>
     <t>Preferred Term</t>
   </si>
@@ -3640,6 +3640,15 @@
   </si>
   <si>
     <t>A narrative representation of the investigational intervention.</t>
+  </si>
+  <si>
+    <t>C163559</t>
+  </si>
+  <si>
+    <t>Exploratory Objective</t>
+  </si>
+  <si>
+    <t>The exploratory reason for performing a study in terms of the scientific questions to be answered by the analysis of data collected during the study.</t>
   </si>
 </sst>
 </file>
@@ -4077,7 +4086,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -4366,7 +4396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I264"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -11151,9 +11181,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M148"/>
+  <dimension ref="A1:M149"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:F1"/>
     </sheetView>
@@ -13076,28 +13106,28 @@
         <v>983</v>
       </c>
     </row>
-    <row r="80" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A80" s="13" t="s">
         <v>137</v>
       </c>
       <c r="B80" s="27" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>699</v>
-      </c>
-      <c r="E80" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="F80" s="13" t="s">
-        <v>233</v>
+        <v>698</v>
+      </c>
+      <c r="E80" s="52" t="s">
+        <v>1183</v>
+      </c>
+      <c r="F80" s="52" t="s">
+        <v>1184</v>
       </c>
       <c r="G80" s="13"/>
       <c r="H80" s="13" t="s">
-        <v>234</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="81" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
@@ -13114,17 +13144,17 @@
         <v>699</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F81" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G81" s="13"/>
       <c r="H81" s="13" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" s="20" customFormat="1" ht="50" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A82" s="13" t="s">
         <v>137</v>
       </c>
@@ -13138,41 +13168,41 @@
         <v>699</v>
       </c>
       <c r="E82" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F82" s="13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G82" s="13"/>
       <c r="H82" s="13" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" s="20" customFormat="1" ht="50" x14ac:dyDescent="0.35">
       <c r="A83" s="13" t="s">
         <v>137</v>
       </c>
       <c r="B83" s="27" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E83" s="13" t="s">
-        <v>704</v>
+        <v>241</v>
       </c>
       <c r="F83" s="13" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G83" s="13"/>
       <c r="H83" s="13" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" s="20" customFormat="1" ht="100" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A84" s="13" t="s">
         <v>137</v>
       </c>
@@ -13186,17 +13216,17 @@
         <v>700</v>
       </c>
       <c r="E84" s="13" t="s">
-        <v>251</v>
+        <v>704</v>
       </c>
       <c r="F84" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G84" s="13"/>
       <c r="H84" s="13" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" s="20" customFormat="1" ht="62.5" x14ac:dyDescent="0.35">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" s="20" customFormat="1" ht="100" x14ac:dyDescent="0.35">
       <c r="A85" s="13" t="s">
         <v>137</v>
       </c>
@@ -13210,17 +13240,17 @@
         <v>700</v>
       </c>
       <c r="E85" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F85" s="13" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G85" s="13"/>
       <c r="H85" s="13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" s="20" customFormat="1" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A86" s="13" t="s">
         <v>137</v>
       </c>
@@ -13234,17 +13264,17 @@
         <v>700</v>
       </c>
       <c r="E86" s="13" t="s">
-        <v>705</v>
+        <v>252</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G86" s="13"/>
       <c r="H86" s="13" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A87" s="13" t="s">
         <v>137</v>
       </c>
@@ -13258,38 +13288,38 @@
         <v>700</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G87" s="13"/>
       <c r="H87" s="13" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="13" t="s">
         <v>137</v>
       </c>
       <c r="B88" s="27" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>536</v>
+        <v>575</v>
       </c>
       <c r="D88" s="13" t="s">
-        <v>617</v>
+        <v>700</v>
       </c>
       <c r="E88" s="13" t="s">
-        <v>277</v>
+        <v>706</v>
       </c>
       <c r="F88" s="13" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="G88" s="13"/>
       <c r="H88" s="13" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
     </row>
     <row r="89" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -13306,14 +13336,14 @@
         <v>617</v>
       </c>
       <c r="E89" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G89" s="13"/>
       <c r="H89" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="90" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -13330,16 +13360,14 @@
         <v>617</v>
       </c>
       <c r="E90" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F90" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="G90" s="13" t="s">
-        <v>267</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="G90" s="13"/>
       <c r="H90" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="91" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -13356,14 +13384,16 @@
         <v>617</v>
       </c>
       <c r="E91" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="G91" s="13"/>
+        <v>255</v>
+      </c>
+      <c r="G91" s="13" t="s">
+        <v>267</v>
+      </c>
       <c r="H91" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="92" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -13380,16 +13410,14 @@
         <v>617</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="G92" s="13" t="s">
-        <v>270</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="G92" s="13"/>
       <c r="H92" s="13" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="93" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -13406,14 +13434,16 @@
         <v>617</v>
       </c>
       <c r="E93" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="G93" s="13"/>
+        <v>257</v>
+      </c>
+      <c r="G93" s="13" t="s">
+        <v>270</v>
+      </c>
       <c r="H93" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="94" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -13430,14 +13460,14 @@
         <v>617</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G94" s="13"/>
       <c r="H94" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="95" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -13454,17 +13484,17 @@
         <v>617</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F95" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G95" s="13"/>
       <c r="H95" s="13" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" s="20" customFormat="1" ht="50" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A96" s="13" t="s">
         <v>137</v>
       </c>
@@ -13478,17 +13508,17 @@
         <v>617</v>
       </c>
       <c r="E96" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F96" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G96" s="13"/>
       <c r="H96" s="13" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" s="20" customFormat="1" ht="50" x14ac:dyDescent="0.35">
       <c r="A97" s="13" t="s">
         <v>137</v>
       </c>
@@ -13502,14 +13532,14 @@
         <v>617</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F97" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G97" s="13"/>
       <c r="H97" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="98" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -13526,17 +13556,17 @@
         <v>617</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F98" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G98" s="13"/>
       <c r="H98" s="13" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A99" s="13" t="s">
         <v>137</v>
       </c>
@@ -13550,41 +13580,41 @@
         <v>617</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F99" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G99" s="13"/>
       <c r="H99" s="13" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A100" s="13" t="s">
         <v>137</v>
       </c>
       <c r="B100" s="27" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="C100" s="13" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>701</v>
+        <v>617</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>363</v>
+        <v>288</v>
       </c>
       <c r="F100" s="13" t="s">
-        <v>68</v>
+        <v>264</v>
       </c>
       <c r="G100" s="13"/>
       <c r="H100" s="13" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A101" s="13" t="s">
         <v>137</v>
       </c>
@@ -13592,23 +13622,23 @@
         <v>597</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D101" s="13" t="s">
-        <v>620</v>
+        <v>701</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>345</v>
+        <v>363</v>
       </c>
       <c r="F101" s="13" t="s">
-        <v>309</v>
+        <v>68</v>
       </c>
       <c r="G101" s="13"/>
       <c r="H101" s="13" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="13" t="s">
         <v>137</v>
       </c>
@@ -13622,17 +13652,17 @@
         <v>620</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F102" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G102" s="13"/>
       <c r="H102" s="13" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A103" s="13" t="s">
         <v>137</v>
       </c>
@@ -13646,17 +13676,17 @@
         <v>620</v>
       </c>
       <c r="E103" s="13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F103" s="13" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G103" s="13"/>
       <c r="H103" s="13" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A104" s="13" t="s">
         <v>137</v>
       </c>
@@ -13670,17 +13700,17 @@
         <v>620</v>
       </c>
       <c r="E104" s="13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F104" s="13" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G104" s="13"/>
       <c r="H104" s="13" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A105" s="13" t="s">
         <v>137</v>
       </c>
@@ -13694,14 +13724,14 @@
         <v>620</v>
       </c>
       <c r="E105" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F105" s="13" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G105" s="13"/>
       <c r="H105" s="13" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="106" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
@@ -13718,17 +13748,17 @@
         <v>620</v>
       </c>
       <c r="E106" s="13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F106" s="13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G106" s="13"/>
       <c r="H106" s="13" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="13" t="s">
         <v>137</v>
       </c>
@@ -13742,14 +13772,14 @@
         <v>620</v>
       </c>
       <c r="E107" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F107" s="13" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G107" s="13"/>
       <c r="H107" s="13" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="108" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -13766,17 +13796,17 @@
         <v>620</v>
       </c>
       <c r="E108" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F108" s="13" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G108" s="13"/>
       <c r="H108" s="13" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A109" s="13" t="s">
         <v>137</v>
       </c>
@@ -13790,17 +13820,17 @@
         <v>620</v>
       </c>
       <c r="E109" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F109" s="13" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G109" s="13"/>
       <c r="H109" s="13" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A110" s="13" t="s">
         <v>137</v>
       </c>
@@ -13814,17 +13844,17 @@
         <v>620</v>
       </c>
       <c r="E110" s="13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F110" s="13" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G110" s="13"/>
       <c r="H110" s="13" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A111" s="13" t="s">
         <v>137</v>
       </c>
@@ -13838,17 +13868,17 @@
         <v>620</v>
       </c>
       <c r="E111" s="13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F111" s="13" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G111" s="13"/>
       <c r="H111" s="13" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A112" s="13" t="s">
         <v>137</v>
       </c>
@@ -13862,14 +13892,14 @@
         <v>620</v>
       </c>
       <c r="E112" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F112" s="13" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G112" s="13"/>
       <c r="H112" s="13" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="113" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
@@ -13886,17 +13916,17 @@
         <v>620</v>
       </c>
       <c r="E113" s="13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F113" s="13" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G113" s="13"/>
       <c r="H113" s="13" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A114" s="13" t="s">
         <v>137</v>
       </c>
@@ -13910,17 +13940,17 @@
         <v>620</v>
       </c>
       <c r="E114" s="13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F114" s="13" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G114" s="13"/>
       <c r="H114" s="13" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A115" s="13" t="s">
         <v>137</v>
       </c>
@@ -13934,14 +13964,14 @@
         <v>620</v>
       </c>
       <c r="E115" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F115" s="13" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G115" s="13"/>
       <c r="H115" s="13" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="116" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
@@ -13958,14 +13988,14 @@
         <v>620</v>
       </c>
       <c r="E116" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F116" s="13" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G116" s="13"/>
       <c r="H116" s="13" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="117" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
@@ -13982,14 +14012,14 @@
         <v>620</v>
       </c>
       <c r="E117" s="13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F117" s="13" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G117" s="13"/>
       <c r="H117" s="13" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="118" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
@@ -14006,14 +14036,14 @@
         <v>620</v>
       </c>
       <c r="E118" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F118" s="13" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G118" s="13"/>
       <c r="H118" s="13" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="119" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
@@ -14024,25 +14054,23 @@
         <v>597</v>
       </c>
       <c r="C119" s="13" t="s">
-        <v>726</v>
+        <v>541</v>
       </c>
       <c r="D119" s="13" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E119" s="13" t="s">
-        <v>303</v>
+        <v>362</v>
       </c>
       <c r="F119" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="G119" s="13" t="s">
-        <v>290</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="G119" s="13"/>
       <c r="H119" s="13" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A120" s="13" t="s">
         <v>137</v>
       </c>
@@ -14056,19 +14084,19 @@
         <v>621</v>
       </c>
       <c r="E120" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F120" s="13" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G120" s="13" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="H120" s="13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A121" s="13" t="s">
         <v>137</v>
       </c>
@@ -14082,14 +14110,16 @@
         <v>621</v>
       </c>
       <c r="E121" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F121" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="G121" s="13"/>
+        <v>292</v>
+      </c>
+      <c r="G121" s="13" t="s">
+        <v>293</v>
+      </c>
       <c r="H121" s="13" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="122" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
@@ -14106,17 +14136,17 @@
         <v>621</v>
       </c>
       <c r="E122" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F122" s="13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G122" s="13"/>
       <c r="H122" s="13" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A123" s="13" t="s">
         <v>137</v>
       </c>
@@ -14130,17 +14160,17 @@
         <v>621</v>
       </c>
       <c r="E123" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F123" s="13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G123" s="13"/>
       <c r="H123" s="13" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A124" s="13" t="s">
         <v>137</v>
       </c>
@@ -14154,43 +14184,41 @@
         <v>621</v>
       </c>
       <c r="E124" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F124" s="13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G124" s="13"/>
       <c r="H124" s="13" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A125" s="13" t="s">
         <v>137</v>
       </c>
       <c r="B125" s="27" t="s">
-        <v>587</v>
+        <v>597</v>
       </c>
       <c r="C125" s="13" t="s">
-        <v>790</v>
+        <v>726</v>
       </c>
       <c r="D125" s="13" t="s">
-        <v>812</v>
+        <v>621</v>
       </c>
       <c r="E125" s="13" t="s">
-        <v>795</v>
+        <v>308</v>
       </c>
       <c r="F125" s="13" t="s">
-        <v>796</v>
-      </c>
-      <c r="G125" s="13" t="s">
-        <v>797</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="G125" s="13"/>
       <c r="H125" s="13" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" s="20" customFormat="1" ht="50" x14ac:dyDescent="0.35">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A126" s="13" t="s">
         <v>137</v>
       </c>
@@ -14204,17 +14232,19 @@
         <v>812</v>
       </c>
       <c r="E126" s="13" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
       <c r="F126" s="13" t="s">
-        <v>800</v>
-      </c>
-      <c r="G126" s="13"/>
+        <v>796</v>
+      </c>
+      <c r="G126" s="13" t="s">
+        <v>797</v>
+      </c>
       <c r="H126" s="13" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" s="20" customFormat="1" ht="50" x14ac:dyDescent="0.35">
       <c r="A127" s="13" t="s">
         <v>137</v>
       </c>
@@ -14228,17 +14258,17 @@
         <v>812</v>
       </c>
       <c r="E127" s="13" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="F127" s="13" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="G127" s="13"/>
       <c r="H127" s="13" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A128" s="13" t="s">
         <v>137</v>
       </c>
@@ -14252,14 +14282,14 @@
         <v>812</v>
       </c>
       <c r="E128" s="13" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="F128" s="13" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="G128" s="13"/>
       <c r="H128" s="13" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
     </row>
     <row r="129" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -14276,43 +14306,43 @@
         <v>812</v>
       </c>
       <c r="E129" s="13" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="F129" s="13" t="s">
-        <v>809</v>
-      </c>
-      <c r="G129" s="13" t="s">
-        <v>810</v>
-      </c>
+        <v>806</v>
+      </c>
+      <c r="G129" s="13"/>
       <c r="H129" s="13" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A130" s="13" t="s">
         <v>137</v>
       </c>
       <c r="B130" s="27" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C130" s="13" t="s">
-        <v>772</v>
+        <v>790</v>
       </c>
       <c r="D130" s="13" t="s">
-        <v>827</v>
+        <v>812</v>
       </c>
       <c r="E130" s="13" t="s">
-        <v>828</v>
+        <v>808</v>
       </c>
       <c r="F130" s="13" t="s">
-        <v>829</v>
-      </c>
-      <c r="G130" s="13"/>
+        <v>809</v>
+      </c>
+      <c r="G130" s="13" t="s">
+        <v>810</v>
+      </c>
       <c r="H130" s="13" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A131" s="13" t="s">
         <v>137</v>
       </c>
@@ -14326,16 +14356,14 @@
         <v>827</v>
       </c>
       <c r="E131" s="13" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="F131" s="13" t="s">
-        <v>832</v>
-      </c>
-      <c r="G131" s="13" t="s">
-        <v>833</v>
-      </c>
+        <v>829</v>
+      </c>
+      <c r="G131" s="13"/>
       <c r="H131" s="13" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
     </row>
     <row r="132" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
@@ -14352,40 +14380,42 @@
         <v>827</v>
       </c>
       <c r="E132" s="13" t="s">
+        <v>831</v>
+      </c>
+      <c r="F132" s="13" t="s">
+        <v>832</v>
+      </c>
+      <c r="G132" s="13" t="s">
+        <v>833</v>
+      </c>
+      <c r="H132" s="13" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A133" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B133" s="27" t="s">
+        <v>589</v>
+      </c>
+      <c r="C133" s="13" t="s">
+        <v>772</v>
+      </c>
+      <c r="D133" s="13" t="s">
+        <v>827</v>
+      </c>
+      <c r="E133" s="13" t="s">
         <v>835</v>
       </c>
-      <c r="F132" s="13" t="s">
+      <c r="F133" s="13" t="s">
         <v>836</v>
       </c>
-      <c r="G132" s="13" t="s">
+      <c r="G133" s="13" t="s">
         <v>837</v>
       </c>
-      <c r="H132" s="13" t="s">
+      <c r="H133" s="13" t="s">
         <v>838</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
-      <c r="A133" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="B133" s="41" t="s">
-        <v>897</v>
-      </c>
-      <c r="C133" s="13" t="s">
-        <v>903</v>
-      </c>
-      <c r="D133" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E133" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="F133" s="38" t="s">
-        <v>940</v>
-      </c>
-      <c r="G133" s="38"/>
-      <c r="H133" s="38" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="134" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -14405,11 +14435,11 @@
         <v>16</v>
       </c>
       <c r="F134" s="38" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="G134" s="38"/>
       <c r="H134" s="38" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="135" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -14429,11 +14459,11 @@
         <v>16</v>
       </c>
       <c r="F135" s="38" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="G135" s="38"/>
       <c r="H135" s="38" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="136" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -14453,11 +14483,11 @@
         <v>16</v>
       </c>
       <c r="F136" s="38" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="G136" s="38"/>
-      <c r="H136" s="13" t="s">
-        <v>947</v>
+      <c r="H136" s="38" t="s">
+        <v>945</v>
       </c>
     </row>
     <row r="137" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -14468,7 +14498,7 @@
         <v>897</v>
       </c>
       <c r="C137" s="13" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="D137" s="38" t="s">
         <v>16</v>
@@ -14476,12 +14506,12 @@
       <c r="E137" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="F137" s="13" t="s">
-        <v>948</v>
+      <c r="F137" s="38" t="s">
+        <v>946</v>
       </c>
       <c r="G137" s="38"/>
       <c r="H137" s="13" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
     </row>
     <row r="138" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
@@ -14501,14 +14531,14 @@
         <v>16</v>
       </c>
       <c r="F138" s="13" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="G138" s="38"/>
       <c r="H138" s="13" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A139" s="38" t="s">
         <v>137</v>
       </c>
@@ -14525,38 +14555,38 @@
         <v>16</v>
       </c>
       <c r="F139" s="13" t="s">
-        <v>952</v>
-      </c>
-      <c r="G139" s="13"/>
+        <v>950</v>
+      </c>
+      <c r="G139" s="38"/>
       <c r="H139" s="13" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" s="20" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A140" s="38" t="s">
         <v>137</v>
       </c>
       <c r="B140" s="41" t="s">
-        <v>593</v>
+        <v>897</v>
       </c>
       <c r="C140" s="13" t="s">
-        <v>574</v>
-      </c>
-      <c r="D140" s="42" t="s">
-        <v>957</v>
-      </c>
-      <c r="E140" s="54" t="s">
-        <v>958</v>
-      </c>
-      <c r="F140" s="54" t="s">
-        <v>959</v>
-      </c>
-      <c r="G140" s="55"/>
-      <c r="H140" s="55" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+        <v>901</v>
+      </c>
+      <c r="D140" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E140" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="F140" s="13" t="s">
+        <v>952</v>
+      </c>
+      <c r="G140" s="13"/>
+      <c r="H140" s="13" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" s="20" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A141" s="38" t="s">
         <v>137</v>
       </c>
@@ -14569,18 +14599,18 @@
       <c r="D141" s="42" t="s">
         <v>957</v>
       </c>
-      <c r="E141" s="38" t="s">
-        <v>961</v>
-      </c>
-      <c r="F141" s="38" t="s">
-        <v>962</v>
-      </c>
-      <c r="G141" s="38"/>
-      <c r="H141" s="38" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
+      <c r="E141" s="54" t="s">
+        <v>958</v>
+      </c>
+      <c r="F141" s="54" t="s">
+        <v>959</v>
+      </c>
+      <c r="G141" s="55"/>
+      <c r="H141" s="55" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A142" s="38" t="s">
         <v>137</v>
       </c>
@@ -14594,19 +14624,17 @@
         <v>957</v>
       </c>
       <c r="E142" s="38" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="F142" s="38" t="s">
-        <v>965</v>
-      </c>
-      <c r="G142" s="38" t="s">
-        <v>966</v>
-      </c>
+        <v>962</v>
+      </c>
+      <c r="G142" s="38"/>
       <c r="H142" s="38" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" s="20" customFormat="1" ht="25" x14ac:dyDescent="0.35">
       <c r="A143" s="38" t="s">
         <v>137</v>
       </c>
@@ -14620,14 +14648,16 @@
         <v>957</v>
       </c>
       <c r="E143" s="38" t="s">
-        <v>968</v>
+        <v>964</v>
       </c>
       <c r="F143" s="38" t="s">
-        <v>969</v>
-      </c>
-      <c r="G143" s="38"/>
+        <v>965</v>
+      </c>
+      <c r="G143" s="38" t="s">
+        <v>966</v>
+      </c>
       <c r="H143" s="38" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
     </row>
     <row r="144" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.35">
@@ -14644,16 +14674,14 @@
         <v>957</v>
       </c>
       <c r="E144" s="38" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="F144" s="38" t="s">
-        <v>972</v>
-      </c>
-      <c r="G144" s="38" t="s">
-        <v>973</v>
-      </c>
+        <v>969</v>
+      </c>
+      <c r="G144" s="38"/>
       <c r="H144" s="38" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
     </row>
     <row r="145" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
@@ -14670,19 +14698,19 @@
         <v>957</v>
       </c>
       <c r="E145" s="38" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="F145" s="38" t="s">
-        <v>976</v>
+        <v>972</v>
       </c>
       <c r="G145" s="38" t="s">
-        <v>977</v>
+        <v>973</v>
       </c>
       <c r="H145" s="38" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A146" s="38" t="s">
         <v>137</v>
       </c>
@@ -14696,44 +14724,43 @@
         <v>957</v>
       </c>
       <c r="E146" s="38" t="s">
+        <v>975</v>
+      </c>
+      <c r="F146" s="38" t="s">
+        <v>976</v>
+      </c>
+      <c r="G146" s="38" t="s">
+        <v>977</v>
+      </c>
+      <c r="H146" s="38" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" s="20" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A147" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="B147" s="41" t="s">
+        <v>593</v>
+      </c>
+      <c r="C147" s="13" t="s">
+        <v>574</v>
+      </c>
+      <c r="D147" s="42" t="s">
+        <v>957</v>
+      </c>
+      <c r="E147" s="38" t="s">
         <v>979</v>
       </c>
-      <c r="F146" s="38" t="s">
+      <c r="F147" s="38" t="s">
         <v>980</v>
       </c>
-      <c r="G146" s="38"/>
-      <c r="H146" s="38" t="s">
+      <c r="G147" s="38"/>
+      <c r="H147" s="38" t="s">
         <v>981</v>
       </c>
     </row>
-    <row r="147" spans="1:9" s="20" customFormat="1" ht="50" x14ac:dyDescent="0.35">
-      <c r="A147" s="52" t="s">
-        <v>137</v>
-      </c>
-      <c r="B147" s="53" t="s">
-        <v>1142</v>
-      </c>
-      <c r="C147" s="13" t="s">
-        <v>1143</v>
-      </c>
-      <c r="D147" s="42" t="s">
-        <v>1144</v>
-      </c>
-      <c r="E147" s="13" t="s">
-        <v>1145</v>
-      </c>
-      <c r="F147" s="52" t="s">
-        <v>1146</v>
-      </c>
-      <c r="G147" s="52"/>
-      <c r="H147" s="13" t="s">
-        <v>1147</v>
-      </c>
-      <c r="I147" s="13" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9" s="20" customFormat="1" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9" s="20" customFormat="1" ht="50" x14ac:dyDescent="0.35">
       <c r="A148" s="52" t="s">
         <v>137</v>
       </c>
@@ -14747,42 +14774,63 @@
         <v>1144</v>
       </c>
       <c r="E148" s="13" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
       <c r="F148" s="52" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="G148" s="52"/>
       <c r="H148" s="13" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
       <c r="I148" s="13" t="s">
         <v>931</v>
       </c>
     </row>
+    <row r="149" spans="1:9" s="20" customFormat="1" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="A149" s="52" t="s">
+        <v>137</v>
+      </c>
+      <c r="B149" s="53" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C149" s="13" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D149" s="42" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E149" s="13" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F149" s="52" t="s">
+        <v>1149</v>
+      </c>
+      <c r="G149" s="52"/>
+      <c r="H149" s="13" t="s">
+        <v>1150</v>
+      </c>
+      <c r="I149" s="13" t="s">
+        <v>931</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A6:M124" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A6:M125" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <mergeCells count="4">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A5:B5"/>
   </mergeCells>
+  <conditionalFormatting sqref="F80">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15004,6 +15052,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -15014,14 +15071,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15037,6 +15086,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
203 changes and ct deliverable
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E2A31D-965B-4B38-A540-BB9635C3089B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47799E7-191F-4B4B-87F2-E765F8A1D75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1930" yWindow="110" windowWidth="13420" windowHeight="9380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3450" yWindow="900" windowWidth="15770" windowHeight="9380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3277" uniqueCount="1425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3275" uniqueCount="1425">
   <si>
     <t>Preferred Term</t>
   </si>
@@ -14007,27 +14007,19 @@
         <v>332</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>1288</v>
-      </c>
-      <c r="C333" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D333" s="57" t="s">
-        <v>1288</v>
-      </c>
-      <c r="E333" s="1" t="s">
-        <v>1289</v>
-      </c>
-      <c r="F333" s="3" t="s">
-        <v>1290</v>
-      </c>
-      <c r="G333" s="59"/>
-      <c r="H333" s="3" t="s">
-        <v>1291</v>
-      </c>
-      <c r="I333" s="3" t="s">
-        <v>85</v>
-      </c>
+        <v>1276</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="D333" s="32" t="s">
+        <v>1306</v>
+      </c>
+      <c r="E333" s="25"/>
+      <c r="F333" s="25"/>
+      <c r="G333" s="25"/>
+      <c r="H333" s="25"/>
+      <c r="I333" s="59"/>
       <c r="J333" s="25"/>
     </row>
     <row r="334" spans="1:10" ht="25" x14ac:dyDescent="0.35">
@@ -14035,27 +14027,19 @@
         <v>333</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>1288</v>
-      </c>
-      <c r="C334" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D334" s="22" t="s">
-        <v>914</v>
-      </c>
-      <c r="E334" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F334" s="3" t="s">
-        <v>1292</v>
-      </c>
-      <c r="G334" s="59"/>
-      <c r="H334" s="3" t="s">
-        <v>1293</v>
-      </c>
-      <c r="I334" s="3" t="s">
-        <v>85</v>
-      </c>
+        <v>1276</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="D334" s="32" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E334" s="25"/>
+      <c r="F334" s="25"/>
+      <c r="G334" s="25"/>
+      <c r="H334" s="25"/>
+      <c r="I334" s="59"/>
       <c r="J334" s="25"/>
     </row>
     <row r="335" spans="1:10" ht="25" x14ac:dyDescent="0.35">
@@ -14066,27 +14050,27 @@
         <v>1288</v>
       </c>
       <c r="C335" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D335" s="22" t="s">
-        <v>915</v>
+        <v>4</v>
+      </c>
+      <c r="D335" s="57" t="s">
+        <v>1288</v>
       </c>
       <c r="E335" s="1" t="s">
-        <v>13</v>
+        <v>1289</v>
       </c>
       <c r="F335" s="3" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
       <c r="G335" s="59"/>
       <c r="H335" s="3" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="I335" s="3" t="s">
         <v>85</v>
       </c>
       <c r="J335" s="25"/>
     </row>
-    <row r="336" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:10" ht="25" x14ac:dyDescent="0.35">
       <c r="A336" s="25">
         <v>335</v>
       </c>
@@ -14097,24 +14081,24 @@
         <v>86</v>
       </c>
       <c r="D336" s="22" t="s">
-        <v>952</v>
+        <v>914</v>
       </c>
       <c r="E336" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F336" s="3" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
       <c r="G336" s="59"/>
       <c r="H336" s="3" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
       <c r="I336" s="3" t="s">
         <v>85</v>
       </c>
       <c r="J336" s="25"/>
     </row>
-    <row r="337" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:10" ht="25" x14ac:dyDescent="0.35">
       <c r="A337" s="25">
         <v>336</v>
       </c>
@@ -14125,28 +14109,24 @@
         <v>86</v>
       </c>
       <c r="D337" s="22" t="s">
-        <v>1304</v>
+        <v>915</v>
       </c>
       <c r="E337" s="1" t="s">
-        <v>1298</v>
+        <v>13</v>
       </c>
       <c r="F337" s="3" t="s">
-        <v>1299</v>
-      </c>
-      <c r="G337" s="3" t="s">
-        <v>1299</v>
-      </c>
-      <c r="H337" s="59" t="s">
-        <v>1300</v>
+        <v>1294</v>
+      </c>
+      <c r="G337" s="59"/>
+      <c r="H337" s="3" t="s">
+        <v>1295</v>
       </c>
       <c r="I337" s="3" t="s">
-        <v>1416</v>
-      </c>
-      <c r="J337" s="67" t="s">
-        <v>1417</v>
-      </c>
-    </row>
-    <row r="338" spans="1:10" ht="50" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+      <c r="J337" s="25"/>
+    </row>
+    <row r="338" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A338" s="25">
         <v>337</v>
       </c>
@@ -14157,70 +14137,86 @@
         <v>86</v>
       </c>
       <c r="D338" s="22" t="s">
-        <v>1305</v>
+        <v>952</v>
       </c>
       <c r="E338" s="1" t="s">
-        <v>1301</v>
+        <v>13</v>
       </c>
       <c r="F338" s="3" t="s">
-        <v>1302</v>
-      </c>
-      <c r="G338" s="3" t="s">
-        <v>1302</v>
-      </c>
-      <c r="H338" s="59" t="s">
-        <v>1303</v>
+        <v>1296</v>
+      </c>
+      <c r="G338" s="59"/>
+      <c r="H338" s="3" t="s">
+        <v>1297</v>
       </c>
       <c r="I338" s="3" t="s">
-        <v>1418</v>
-      </c>
-      <c r="J338" s="3" t="s">
-        <v>1419</v>
-      </c>
-    </row>
-    <row r="339" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+      <c r="J338" s="25"/>
+    </row>
+    <row r="339" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A339" s="25">
         <v>338</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>1276</v>
-      </c>
-      <c r="C339" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="D339" s="32" t="s">
-        <v>1306</v>
-      </c>
-      <c r="E339" s="1"/>
-      <c r="F339" s="3"/>
-      <c r="G339" s="59"/>
-      <c r="H339" s="59"/>
+        <v>1288</v>
+      </c>
+      <c r="C339" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D339" s="22" t="s">
+        <v>1304</v>
+      </c>
+      <c r="E339" s="1" t="s">
+        <v>1298</v>
+      </c>
+      <c r="F339" s="3" t="s">
+        <v>1299</v>
+      </c>
+      <c r="G339" s="3" t="s">
+        <v>1299</v>
+      </c>
+      <c r="H339" s="59" t="s">
+        <v>1300</v>
+      </c>
       <c r="I339" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="J339" s="25"/>
-    </row>
-    <row r="340" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+        <v>1416</v>
+      </c>
+      <c r="J339" s="67" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="340" spans="1:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A340" s="25">
         <v>339</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>1276</v>
-      </c>
-      <c r="C340" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="D340" s="32" t="s">
-        <v>1307</v>
-      </c>
-      <c r="E340" s="1"/>
-      <c r="F340" s="3"/>
-      <c r="G340" s="59"/>
-      <c r="H340" s="59"/>
+        <v>1288</v>
+      </c>
+      <c r="C340" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D340" s="22" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E340" s="1" t="s">
+        <v>1301</v>
+      </c>
+      <c r="F340" s="3" t="s">
+        <v>1302</v>
+      </c>
+      <c r="G340" s="3" t="s">
+        <v>1302</v>
+      </c>
+      <c r="H340" s="59" t="s">
+        <v>1303</v>
+      </c>
       <c r="I340" s="3" t="s">
-        <v>848</v>
-      </c>
-      <c r="J340" s="25"/>
+        <v>1418</v>
+      </c>
+      <c r="J340" s="3" t="s">
+        <v>1419</v>
+      </c>
     </row>
     <row r="341" spans="1:10" ht="25" x14ac:dyDescent="0.35">
       <c r="A341" s="25">
@@ -14328,7 +14324,7 @@
     <hyperlink ref="J302" r:id="rId12" xr:uid="{5A4ED305-DAB1-4AB2-9821-67E85648C298}"/>
     <hyperlink ref="J304" r:id="rId13" xr:uid="{4C709FBD-08C2-4341-A1B8-9E6314E092CD}"/>
     <hyperlink ref="J323" r:id="rId14" xr:uid="{A5546FE9-D80B-4535-B6AC-978D1E0D7964}"/>
-    <hyperlink ref="J337" r:id="rId15" xr:uid="{9390E52B-52E6-4CB8-8ADF-0E1102C02629}"/>
+    <hyperlink ref="J339" r:id="rId15" xr:uid="{9390E52B-52E6-4CB8-8ADF-0E1102C02629}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId16"/>
@@ -18213,6 +18209,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -18434,25 +18448,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18470,30 +18492,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
QC fix for 2-7
Unit to unit on row 377
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D5F406-0063-4A30-B38C-0C8BF3568876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F748CAAA-E47D-4F3C-91DF-9CE9B0B733F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="370" yWindow="120" windowWidth="16730" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3466" uniqueCount="1477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3466" uniqueCount="1476">
   <si>
     <t>Preferred Term</t>
   </si>
@@ -4487,9 +4487,6 @@
   </si>
   <si>
     <t>maxValue</t>
-  </si>
-  <si>
-    <t>Unit</t>
   </si>
   <si>
     <t>C38013</t>
@@ -15235,14 +15232,14 @@
         <v>1462</v>
       </c>
       <c r="E375" s="3" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="F375" s="3" t="s">
         <v>1462</v>
       </c>
       <c r="G375" s="59"/>
       <c r="H375" s="3" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="I375" s="3" t="s">
         <v>841</v>
@@ -15263,14 +15260,14 @@
         <v>1463</v>
       </c>
       <c r="E376" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="F376" s="3" t="s">
         <v>1468</v>
-      </c>
-      <c r="F376" s="3" t="s">
-        <v>1469</v>
       </c>
       <c r="G376" s="59"/>
       <c r="H376" s="3" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="I376" s="3" t="s">
         <v>85</v>
@@ -15291,14 +15288,14 @@
         <v>1464</v>
       </c>
       <c r="E377" s="3" t="s">
+        <v>1470</v>
+      </c>
+      <c r="F377" s="3" t="s">
         <v>1471</v>
-      </c>
-      <c r="F377" s="3" t="s">
-        <v>1472</v>
       </c>
       <c r="G377" s="59"/>
       <c r="H377" s="3" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="I377" s="3" t="s">
         <v>85</v>
@@ -15316,17 +15313,17 @@
         <v>86</v>
       </c>
       <c r="D378" s="44" t="s">
-        <v>1465</v>
+        <v>1352</v>
       </c>
       <c r="E378" s="3" t="s">
+        <v>1473</v>
+      </c>
+      <c r="F378" s="3" t="s">
         <v>1474</v>
-      </c>
-      <c r="F378" s="3" t="s">
-        <v>1475</v>
       </c>
       <c r="G378" s="59"/>
       <c r="H378" s="3" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="I378" s="3" t="s">
         <v>85</v>
@@ -19238,6 +19235,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -19459,25 +19474,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19495,30 +19518,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Additional attribute addition to Range class
As discussed on team meeting 2023-11-16
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F748CAAA-E47D-4F3C-91DF-9CE9B0B733F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E497307-3694-4A8C-AE9B-CBC4613890AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="370" yWindow="120" windowWidth="16730" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2220" yWindow="510" windowWidth="15450" windowHeight="9020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3466" uniqueCount="1476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3473" uniqueCount="1479">
   <si>
     <t>Preferred Term</t>
   </si>
@@ -4520,6 +4520,15 @@
   </si>
   <si>
     <t>A named quantity in terms of which other quantities are measured or specified, used as a standard measurement of like kinds.</t>
+  </si>
+  <si>
+    <t>isApproximate</t>
+  </si>
+  <si>
+    <t>Value Range is Approximate Indicator</t>
+  </si>
+  <si>
+    <t>An indication as to whether the value range is almost, but not quite, exact.</t>
   </si>
 </sst>
 </file>
@@ -5325,7 +5334,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J378"/>
+  <dimension ref="A1:J379"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -15329,6 +15338,33 @@
         <v>85</v>
       </c>
       <c r="J378" s="1"/>
+    </row>
+    <row r="379" spans="1:10" ht="25" x14ac:dyDescent="0.35">
+      <c r="A379" s="25">
+        <v>379</v>
+      </c>
+      <c r="B379" s="1" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C379" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D379" s="45" t="s">
+        <v>1476</v>
+      </c>
+      <c r="E379" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F379" s="47" t="s">
+        <v>1477</v>
+      </c>
+      <c r="G379" s="47"/>
+      <c r="H379" s="47" t="s">
+        <v>1478</v>
+      </c>
+      <c r="I379" s="47" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J347" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
@@ -19244,15 +19280,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -19474,6 +19501,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
   <ds:schemaRefs>
@@ -19493,14 +19529,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19518,4 +19546,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Sprint 12 QC items from Berber
sent over email 2023-12-13
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD49971-33EF-4CC1-8090-322A183B52F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71056B6E-326F-42C3-9CCA-CA0895090752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="490" windowWidth="15320" windowHeight="8480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5950" yWindow="850" windowWidth="12490" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -15095,7 +15095,9 @@
       <c r="C388" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="D388" s="24"/>
+      <c r="D388" s="3" t="s">
+        <v>550</v>
+      </c>
       <c r="E388" s="34" t="s">
         <v>606</v>
       </c>
@@ -15174,7 +15176,7 @@
         <v>1101</v>
       </c>
       <c r="C391" s="3" t="s">
-        <v>86</v>
+        <v>1049</v>
       </c>
       <c r="D391" s="24"/>
       <c r="E391" s="21" t="s">
@@ -15327,7 +15329,7 @@
         <v>1112</v>
       </c>
       <c r="C396" s="3" t="s">
-        <v>86</v>
+        <v>1049</v>
       </c>
       <c r="D396" s="24" t="s">
         <v>192</v>
@@ -15408,61 +15410,53 @@
       </c>
       <c r="K398" s="1"/>
     </row>
-    <row r="399" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A399" s="24">
         <v>398</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>1140</v>
-      </c>
-      <c r="C399" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D399" s="1"/>
-      <c r="E399" s="30" t="s">
-        <v>1140</v>
-      </c>
-      <c r="F399" s="3" t="s">
-        <v>1150</v>
-      </c>
-      <c r="G399" s="3" t="s">
-        <v>1151</v>
-      </c>
-      <c r="H399" s="55"/>
-      <c r="I399" s="3" t="s">
-        <v>1152</v>
-      </c>
-      <c r="J399" s="3" t="s">
-        <v>466</v>
-      </c>
+        <v>1112</v>
+      </c>
+      <c r="C399" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="D399" s="24"/>
+      <c r="E399" s="64" t="s">
+        <v>1143</v>
+      </c>
+      <c r="F399" s="24"/>
+      <c r="G399" s="24"/>
+      <c r="H399" s="24"/>
+      <c r="I399" s="24"/>
+      <c r="J399" s="24"/>
       <c r="K399" s="1"/>
     </row>
-    <row r="400" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A400" s="24">
         <v>399</v>
       </c>
-      <c r="B400" s="1" t="s">
+      <c r="B400" s="3" t="s">
         <v>1140</v>
       </c>
-      <c r="C400" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D400" s="24"/>
-      <c r="E400" s="21" t="s">
-        <v>507</v>
+      <c r="C400" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D400" s="1"/>
+      <c r="E400" s="30" t="s">
+        <v>1140</v>
       </c>
       <c r="F400" s="3" t="s">
-        <v>13</v>
+        <v>1150</v>
       </c>
       <c r="G400" s="3" t="s">
-        <v>1144</v>
+        <v>1151</v>
       </c>
       <c r="H400" s="55"/>
       <c r="I400" s="3" t="s">
-        <v>1145</v>
+        <v>1152</v>
       </c>
       <c r="J400" s="3" t="s">
-        <v>85</v>
+        <v>466</v>
       </c>
       <c r="K400" s="1"/>
     </row>
@@ -15478,17 +15472,17 @@
       </c>
       <c r="D401" s="24"/>
       <c r="E401" s="21" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F401" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G401" s="3" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="H401" s="55"/>
       <c r="I401" s="3" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="J401" s="3" t="s">
         <v>85</v>
@@ -15507,17 +15501,17 @@
       </c>
       <c r="D402" s="24"/>
       <c r="E402" s="21" t="s">
-        <v>545</v>
+        <v>508</v>
       </c>
       <c r="F402" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G402" s="3" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="H402" s="55"/>
       <c r="I402" s="3" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="J402" s="3" t="s">
         <v>85</v>
@@ -15532,18 +15526,24 @@
         <v>1140</v>
       </c>
       <c r="C403" s="3" t="s">
-        <v>224</v>
+        <v>86</v>
       </c>
       <c r="D403" s="24"/>
-      <c r="E403" s="64" t="s">
-        <v>1141</v>
-      </c>
-      <c r="F403" s="55"/>
-      <c r="G403" s="55"/>
+      <c r="E403" s="21" t="s">
+        <v>545</v>
+      </c>
+      <c r="F403" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G403" s="3" t="s">
+        <v>1148</v>
+      </c>
       <c r="H403" s="55"/>
-      <c r="I403" s="55"/>
+      <c r="I403" s="3" t="s">
+        <v>1149</v>
+      </c>
       <c r="J403" s="3" t="s">
-        <v>466</v>
+        <v>85</v>
       </c>
       <c r="K403" s="1"/>
     </row>
@@ -15559,7 +15559,7 @@
       </c>
       <c r="D404" s="24"/>
       <c r="E404" s="64" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="F404" s="55"/>
       <c r="G404" s="55"/>
@@ -15582,7 +15582,7 @@
       </c>
       <c r="D405" s="24"/>
       <c r="E405" s="64" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="F405" s="55"/>
       <c r="G405" s="55"/>
@@ -16741,21 +16741,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16981,14 +16981,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
@@ -17002,6 +16994,14 @@
     <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
#254 - addition of x4 M11 codelists
Creation of four new DDF codelists that mimic M11 codelists.
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71056B6E-326F-42C3-9CCA-CA0895090752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693EADCC-B56D-4710-9F78-6632B152DE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5950" yWindow="850" windowWidth="12490" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="15440" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2905" uniqueCount="1153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3095" uniqueCount="1217">
   <si>
     <t>Preferred Term</t>
   </si>
@@ -2702,9 +2702,6 @@
     <t>The intended use of the trial intervention within the context of the study design.</t>
   </si>
   <si>
-    <t>Y (Point to ICH M11 Intervention Use Response)</t>
-  </si>
-  <si>
     <t>C98747</t>
   </si>
   <si>
@@ -2723,9 +2720,6 @@
     <t>An indication as to whether the investigational intervention is an investigational medicinal product or an auxiliary medicinal product.</t>
   </si>
   <si>
-    <t>Y (Point to ICH M11 Investigational Medicinal Product Indicator Response)</t>
-  </si>
-  <si>
     <t>C98768</t>
   </si>
   <si>
@@ -2832,9 +2826,6 @@
   </si>
   <si>
     <t>Codelist URL</t>
-  </si>
-  <si>
-    <t>Y (Point to ICH M11 Reason for Amendment Response codelist)</t>
   </si>
   <si>
     <t>Y (Point out to external dictionaries)</t>
@@ -3369,9 +3360,6 @@
     <t>An identifying designation assigned to a masked individual within a study that corresponds with their function.</t>
   </si>
   <si>
-    <t>Y (Point to ICH M11 Trial Blinding Role Terminology)</t>
-  </si>
-  <si>
     <t>Population Definition Includes Healthy Subjects Indicator</t>
   </si>
   <si>
@@ -3499,6 +3487,210 @@
   </si>
   <si>
     <t>The location at which a study investigator conducts study activities.</t>
+  </si>
+  <si>
+    <t>Y (CNEW - Study Amendment Reason Response)</t>
+  </si>
+  <si>
+    <t>Y (CNEW - Study Intervention Role Response)</t>
+  </si>
+  <si>
+    <t>Y (CNEW - Study Intervention Product Designation Response)</t>
+  </si>
+  <si>
+    <t>Y (CNEW - Masking Role Response)</t>
+  </si>
+  <si>
+    <t>Regulatory Agency Request To Amend</t>
+  </si>
+  <si>
+    <t>A regulatory agency has expressed a need for a change(s) to, or formal clarification of, the protocol.</t>
+  </si>
+  <si>
+    <t>New Regulatory Guidance</t>
+  </si>
+  <si>
+    <t>A regulatory agency has published a guidance document that necessitates a change(s) to, or formal clarification of, the protocol.</t>
+  </si>
+  <si>
+    <t>IRB/IEC Feedback</t>
+  </si>
+  <si>
+    <t>Feedback from the institutional review board or independent ethics committee necessitates a change(s) to, or formal clarification of, the protocol.</t>
+  </si>
+  <si>
+    <t>New Safety Information Available</t>
+  </si>
+  <si>
+    <t>Previously unavailable safety data becomes available, which necessitates a change(s) to, or formal clarification of, the protocol.</t>
+  </si>
+  <si>
+    <t>Manufacturing Change</t>
+  </si>
+  <si>
+    <t>A change to manufacturing processes of the study agents necessitates a change(s) to, or formal clarification of, the protocol.</t>
+  </si>
+  <si>
+    <t>IMP Addition</t>
+  </si>
+  <si>
+    <t>The addition of an investigational medicinal product to a clinical trial design necessitates a change(s) to, or formal clarification of, the protocol.</t>
+  </si>
+  <si>
+    <t>Change In Strategy</t>
+  </si>
+  <si>
+    <t>A change in the study purpose or intent of the scientific plan necessitates a change(s) to, or formal clarification of, the protocol.</t>
+  </si>
+  <si>
+    <t>Change In Standard Of Care</t>
+  </si>
+  <si>
+    <t>A change in the standard of care necessitates a change(s) to, or formal clarification of, the protocol.</t>
+  </si>
+  <si>
+    <t>New Data Available (Other Than Safety Data)</t>
+  </si>
+  <si>
+    <t>Previously unavailable data (other than safety data) becomes available, which necessitates a change(s) to, or formal clarification of, the protocol.</t>
+  </si>
+  <si>
+    <t>Investigator/Site Feedback</t>
+  </si>
+  <si>
+    <t>Feedback from the investigator or study site necessitates a change(s) to, or formal clarification of, the protocol.</t>
+  </si>
+  <si>
+    <t>Recruitment Difficulty</t>
+  </si>
+  <si>
+    <t>Challenges with participant recruitment necessitates a change(s) to, or formal clarification of, the protocol.</t>
+  </si>
+  <si>
+    <t>Inconsistency And/Or Error In The Protocol</t>
+  </si>
+  <si>
+    <t>An error or inconsistency in the protocol necessitates a change(s) to, or formal clarification of, the protocol.</t>
+  </si>
+  <si>
+    <t>Protocol Design Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A protocol design error necessitates a change(s) to, or formal clarification of, a document. </t>
+  </si>
+  <si>
+    <t>C41161</t>
+  </si>
+  <si>
+    <t>Experimental Intervention</t>
+  </si>
+  <si>
+    <t>The drug, device, therapy, procedure, or process under investigation in a clinical study that is believed to have an effect on outcomes of interest in a study (e.g., health-related quality of life, efficacy, safety, pharmacoeconomics). [After https://grants.nih.gov/grants/policy/faq_clinical_trial_definition.htm#5224; https://grants.nih.gov/policy/clinical-trials/protocol-template.htm] See also test articles, devices, drug product, combination product, treatment, diagnosis. Contrast with investigational medicinal product.</t>
+  </si>
+  <si>
+    <t>C753</t>
+  </si>
+  <si>
+    <t>Placebo</t>
+  </si>
+  <si>
+    <t>A pharmaceutical preparation that does not contain the investigational agent and is generally prepared to be physically indistinguishable from the preparation containing the investigational product.</t>
+  </si>
+  <si>
+    <t>C165835</t>
+  </si>
+  <si>
+    <t>Rescue Medicine</t>
+  </si>
+  <si>
+    <t>Medicinal products identified in the protocol as those that may be administered to subjects when the efficacy of the investigational medicinal product (IMP) is not satisfactory, the effect of the IMP is too great and is likely to cause a hazard to the patient, or to manage an emergency situation. [After EU-CTR Recommendations from the expert group on clinical trials for the implementation of Regulation (EU) No 536/2014' dd 28 June 2017]</t>
+  </si>
+  <si>
+    <t>C165822</t>
+  </si>
+  <si>
+    <t>Background Treatment</t>
+  </si>
+  <si>
+    <t>Medicinal products that are administered to each clinical trial subject, regardless of randomization group, a) to treat the indication which is the object of the study, or b) required in the protocol as part of standard care for a condition that is not the indication under investigation, and is relevant for the clinical trial design. [After Recommendations from the expert group on clinical trials for the implementation of Regulation (EU) No 536/2014' dd 28 June 2017]</t>
+  </si>
+  <si>
+    <t>C158128</t>
+  </si>
+  <si>
+    <t>Challenge Agent</t>
+  </si>
+  <si>
+    <t>A non-investigational medicinal product (NIMP) given to trial subjects to produce a physiological response that is necessary before the pharmacological action of the investigational medicinal product can be assessed. [After Recommendations from the expert group on clinical trials for the implementation of Regulation (EU) No 536/2014' dd 28 June 2017]</t>
+  </si>
+  <si>
+    <t>C18020</t>
+  </si>
+  <si>
+    <t>Diagnostic</t>
+  </si>
+  <si>
+    <t>Any procedure or test to diagnose a disease or disorder.</t>
+  </si>
+  <si>
+    <t>Additional Required Treatment</t>
+  </si>
+  <si>
+    <t>A medicinal product that must be administered along with the experimental treatment (e.g., drug studies wherein opioid blockers are administered to prevent overdose).</t>
+  </si>
+  <si>
+    <t>IMP</t>
+  </si>
+  <si>
+    <t>A medicinal product which is being tested or used as a reference, including as a placebo, in a clinical trial. (Regulation (EU) No 536/2014 Article 2 (5))</t>
+  </si>
+  <si>
+    <t>C156473</t>
+  </si>
+  <si>
+    <t>NIMP (AxMP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A medicinal product that is related to the specific needs of the clinical trial as described in the protocol, but not as an investigational medicinal product. NOTE: Auxiliary medicinal products may be authorised for marketing in a country or region or non-authorised. [after EU-CTR]</t>
+  </si>
+  <si>
+    <t>C142710</t>
+  </si>
+  <si>
+    <t>Participant</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> A member of the clinical study population from whom data are being collected. NOTE: This new term is used with growing frequency in some clinical documents and patient-facing ones like the informed consent form, Plain Language Summaries of study results, and publications. Subject or patient are terms used in regulatory guidelines, databases, other clinical research documents, or systems to refer to study participants. (CDISC Glossary)</t>
+  </si>
+  <si>
+    <t>C17445</t>
+  </si>
+  <si>
+    <t>Care Provider</t>
+  </si>
+  <si>
+    <t>Carer</t>
+  </si>
+  <si>
+    <t>The primary person in charge of the care of a patient, usually a family member or a designated health care professional. (NCI)</t>
+  </si>
+  <si>
+    <t>C25936</t>
+  </si>
+  <si>
+    <t>Investigator</t>
+  </si>
+  <si>
+    <t>A person responsible for the conduct of the clinical trial at a trial site. If a trial is conducted by a team of individuals at the trial site, the investigator is the responsible leader of the team and may be called the principal investigator. [ICH E6]</t>
+  </si>
+  <si>
+    <t>Outcomes Assessor</t>
+  </si>
+  <si>
+    <t>The individual who evaluates the outcome(s) of interest. (Clinicaltrials.gov)</t>
+  </si>
+  <si>
+    <t>Sponsor</t>
   </si>
 </sst>
 </file>
@@ -3756,7 +3948,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3979,6 +4171,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4325,7 +4520,7 @@
         <v>83</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>219</v>
@@ -4346,7 +4541,7 @@
         <v>84</v>
       </c>
       <c r="K1" s="58" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
@@ -4577,7 +4772,7 @@
         <v>686</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="22" t="s">
@@ -4597,7 +4792,7 @@
         <v>307</v>
       </c>
       <c r="K10" s="46" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="25" x14ac:dyDescent="0.35">
@@ -4874,7 +5069,7 @@
         <v>192</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="22" t="s">
@@ -4894,7 +5089,7 @@
         <v>308</v>
       </c>
       <c r="K21" s="46" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
@@ -5105,7 +5300,7 @@
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="31" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="F30" s="20"/>
       <c r="G30" s="1"/>
@@ -5289,7 +5484,7 @@
       </c>
       <c r="D38" s="41"/>
       <c r="E38" s="34" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="F38" s="47"/>
       <c r="G38" s="41"/>
@@ -5312,7 +5507,7 @@
       </c>
       <c r="D39" s="41"/>
       <c r="E39" s="64" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="F39" s="47"/>
       <c r="G39" s="41"/>
@@ -5331,7 +5526,7 @@
         <v>228</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="22" t="s">
@@ -5350,10 +5545,10 @@
         <v>37</v>
       </c>
       <c r="J40" s="20" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="K40" s="65" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="50" x14ac:dyDescent="0.35">
@@ -5364,7 +5559,7 @@
         <v>228</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="22" t="s">
@@ -5383,10 +5578,10 @@
         <v>31</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="K41" s="65" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="50" x14ac:dyDescent="0.35">
@@ -5397,7 +5592,7 @@
         <v>228</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="22" t="s">
@@ -5414,10 +5609,10 @@
         <v>39</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
       <c r="K42" s="65" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
@@ -5428,7 +5623,7 @@
         <v>228</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="22" t="s">
@@ -5447,7 +5642,7 @@
         <v>467</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="K43" s="24"/>
     </row>
@@ -5546,7 +5741,7 @@
         <v>228</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="22" t="s">
@@ -5565,10 +5760,10 @@
         <v>389</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="K47" s="66" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
     </row>
     <row r="48" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.35">
@@ -5608,24 +5803,24 @@
         <v>228</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="21" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="H49" s="46"/>
       <c r="I49" s="46" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="K49" s="46"/>
     </row>
@@ -5666,7 +5861,7 @@
         <v>229</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="22" t="s">
@@ -5683,7 +5878,7 @@
         <v>252</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="K51" s="24"/>
     </row>
@@ -5786,17 +5981,17 @@
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="43" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="F55" s="46" t="s">
         <v>13</v>
       </c>
       <c r="G55" s="46" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="H55" s="46"/>
       <c r="I55" s="3" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="J55" s="46" t="s">
         <v>85</v>
@@ -5843,7 +6038,7 @@
         <v>86</v>
       </c>
       <c r="D57" s="41" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E57" s="22" t="s">
         <v>508</v>
@@ -5874,7 +6069,7 @@
         <v>86</v>
       </c>
       <c r="D58" s="41" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E58" s="21" t="s">
         <v>507</v>
@@ -5905,7 +6100,7 @@
         <v>86</v>
       </c>
       <c r="D59" s="41" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E59" s="21" t="s">
         <v>545</v>
@@ -5933,23 +6128,23 @@
         <v>230</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D60" s="41" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E60" s="43" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="F60" s="24" t="s">
         <v>13</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="H60" s="3"/>
       <c r="I60" s="3" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="J60" s="3" t="s">
         <v>85</v>
@@ -5964,13 +6159,13 @@
         <v>230</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D61" s="41" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E61" s="43" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="F61" s="24" t="s">
         <v>380</v>
@@ -5983,10 +6178,10 @@
         <v>382</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="K61" s="66" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
@@ -5997,23 +6192,23 @@
         <v>230</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D62" s="41" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E62" s="21" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="F62" s="24" t="s">
         <v>13</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="H62" s="3"/>
       <c r="I62" s="3" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="J62" s="3" t="s">
         <v>85</v>
@@ -6031,20 +6226,20 @@
         <v>86</v>
       </c>
       <c r="D63" s="41" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E63" s="21" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="F63" s="46" t="s">
         <v>13</v>
       </c>
       <c r="G63" s="46" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
       <c r="H63" s="46"/>
       <c r="I63" s="3" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="J63" s="46" t="s">
         <v>85</v>
@@ -6063,7 +6258,7 @@
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="42" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="46"/>
@@ -6085,10 +6280,10 @@
         <v>224</v>
       </c>
       <c r="D65" s="41" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E65" s="42" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="46"/>
@@ -6107,23 +6302,23 @@
         <v>230</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D66" s="41" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E66" s="63" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="H66" s="3"/>
       <c r="I66" s="3" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="J66" s="3" t="s">
         <v>85</v>
@@ -6167,7 +6362,7 @@
         <v>231</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="22" t="s">
@@ -6187,7 +6382,7 @@
         <v>309</v>
       </c>
       <c r="K68" s="46" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -6210,11 +6405,11 @@
         <v>13</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="H69" s="55"/>
       <c r="I69" s="3" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>85</v>
@@ -6238,14 +6433,14 @@
         <v>508</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="H70" s="1"/>
       <c r="I70" s="1" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>85</v>
@@ -6272,11 +6467,11 @@
         <v>13</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="H71" s="46"/>
       <c r="I71" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="J71" s="3" t="s">
         <v>85</v>
@@ -6303,11 +6498,11 @@
         <v>13</v>
       </c>
       <c r="G72" s="46" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="H72" s="46"/>
       <c r="I72" s="46" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="J72" s="46" t="s">
         <v>85</v>
@@ -6428,7 +6623,7 @@
         <v>232</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="22" t="s">
@@ -6448,7 +6643,7 @@
         <v>310</v>
       </c>
       <c r="K77" s="46" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
     </row>
     <row r="78" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -6793,7 +6988,7 @@
         <v>234</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="22" t="s">
@@ -6810,10 +7005,10 @@
         <v>494</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="K90" s="65" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
     </row>
     <row r="91" spans="1:11" ht="25" x14ac:dyDescent="0.35">
@@ -6853,7 +7048,7 @@
         <v>234</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="22" t="s">
@@ -6873,7 +7068,7 @@
         <v>312</v>
       </c>
       <c r="K92" s="46" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.35">
@@ -7023,7 +7218,7 @@
         <v>235</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="22" t="s">
@@ -7040,10 +7235,10 @@
         <v>60</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="K98" s="65" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.35">
@@ -7575,7 +7770,7 @@
         <v>238</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="22" t="s">
@@ -7595,7 +7790,7 @@
         <v>311</v>
       </c>
       <c r="K118" s="66" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
     </row>
     <row r="119" spans="1:11" ht="50" x14ac:dyDescent="0.35">
@@ -7606,7 +7801,7 @@
         <v>238</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D119" s="1"/>
       <c r="E119" s="22" t="s">
@@ -7623,10 +7818,10 @@
         <v>65</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="K119" s="65" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
     </row>
     <row r="120" spans="1:11" ht="50" x14ac:dyDescent="0.35">
@@ -7637,7 +7832,7 @@
         <v>238</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D120" s="1"/>
       <c r="E120" s="22" t="s">
@@ -7654,10 +7849,10 @@
         <v>67</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="K120" s="65" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.35">
@@ -7718,7 +7913,7 @@
       </c>
       <c r="D123" s="1"/>
       <c r="E123" s="48" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
@@ -8118,7 +8313,7 @@
         <v>80</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D139" s="1"/>
       <c r="E139" s="22" t="s">
@@ -8238,7 +8433,7 @@
       </c>
       <c r="D143" s="1"/>
       <c r="E143" s="34" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="F143" s="1"/>
       <c r="G143" s="46"/>
@@ -9120,7 +9315,7 @@
         <v>347</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D175" s="38"/>
       <c r="E175" s="21" t="s">
@@ -9288,7 +9483,7 @@
         <v>391</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D181" s="24"/>
       <c r="E181" s="21" t="s">
@@ -9514,7 +9709,7 @@
         <v>401</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D189" s="24"/>
       <c r="E189" s="21" t="s">
@@ -9630,7 +9825,7 @@
         <v>414</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D193" s="24"/>
       <c r="E193" s="21" t="s">
@@ -9931,7 +10126,7 @@
         <v>425</v>
       </c>
       <c r="C204" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D204" s="24"/>
       <c r="E204" s="21" t="s">
@@ -10740,7 +10935,7 @@
       </c>
       <c r="D235" s="41"/>
       <c r="E235" s="48" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="F235" s="41"/>
       <c r="G235" s="46"/>
@@ -10817,7 +11012,7 @@
         <v>439</v>
       </c>
       <c r="C238" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D238" s="46"/>
       <c r="E238" s="44" t="s">
@@ -10834,10 +11029,10 @@
         <v>458</v>
       </c>
       <c r="J238" s="3" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="K238" s="46" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
     </row>
     <row r="239" spans="1:11" ht="25" x14ac:dyDescent="0.35">
@@ -10877,7 +11072,7 @@
         <v>439</v>
       </c>
       <c r="C240" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D240" s="46"/>
       <c r="E240" s="44" t="s">
@@ -10894,10 +11089,10 @@
         <v>462</v>
       </c>
       <c r="J240" s="3" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="K240" s="46" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
     </row>
     <row r="241" spans="1:11" ht="25" x14ac:dyDescent="0.35">
@@ -10912,7 +11107,7 @@
       </c>
       <c r="D241" s="46"/>
       <c r="E241" s="44" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="F241" s="41" t="s">
         <v>463</v>
@@ -11640,7 +11835,7 @@
         <v>616</v>
       </c>
       <c r="C267" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D267" s="46"/>
       <c r="E267" s="43" t="s">
@@ -11657,10 +11852,10 @@
         <v>625</v>
       </c>
       <c r="J267" s="3" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="K267" s="66" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
     </row>
     <row r="268" spans="1:11" ht="25" x14ac:dyDescent="0.35">
@@ -11874,7 +12069,7 @@
       </c>
       <c r="D275" s="3"/>
       <c r="E275" s="42" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="F275" s="24"/>
       <c r="G275" s="24"/>
@@ -12063,7 +12258,7 @@
         <v>644</v>
       </c>
       <c r="C282" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D282" s="46"/>
       <c r="E282" s="21" t="s">
@@ -12146,7 +12341,7 @@
         <v>660</v>
       </c>
       <c r="C285" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D285" s="46"/>
       <c r="E285" s="43" t="s">
@@ -12165,7 +12360,7 @@
         <v>674</v>
       </c>
       <c r="J285" s="3" t="s">
-        <v>931</v>
+        <v>1149</v>
       </c>
       <c r="K285" s="24"/>
     </row>
@@ -12642,7 +12837,7 @@
         <v>709</v>
       </c>
       <c r="C303" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D303" s="3"/>
       <c r="E303" s="21" t="s">
@@ -12661,10 +12856,10 @@
         <v>27</v>
       </c>
       <c r="J303" s="1" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="K303" s="65" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
     </row>
     <row r="304" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
@@ -12675,7 +12870,7 @@
         <v>709</v>
       </c>
       <c r="C304" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D304" s="3"/>
       <c r="E304" s="21" t="s">
@@ -12692,7 +12887,7 @@
         <v>326</v>
       </c>
       <c r="J304" s="1" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="K304" s="24"/>
     </row>
@@ -12704,7 +12899,7 @@
         <v>709</v>
       </c>
       <c r="C305" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D305" s="3"/>
       <c r="E305" s="21" t="s">
@@ -12723,10 +12918,10 @@
         <v>15</v>
       </c>
       <c r="J305" s="1" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="K305" s="65" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
     </row>
     <row r="306" spans="1:11" x14ac:dyDescent="0.35">
@@ -12856,7 +13051,7 @@
       </c>
       <c r="D311" s="3"/>
       <c r="E311" s="62" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="F311" s="41"/>
       <c r="G311" s="46"/>
@@ -12904,7 +13099,7 @@
         <v>712</v>
       </c>
       <c r="C313" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D313" s="3"/>
       <c r="E313" s="21" t="s">
@@ -12933,7 +13128,7 @@
         <v>712</v>
       </c>
       <c r="C314" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D314" s="3"/>
       <c r="E314" s="21" t="s">
@@ -12950,10 +13145,10 @@
         <v>719</v>
       </c>
       <c r="J314" s="3" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="K314" s="1" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="315" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
@@ -12993,7 +13188,7 @@
         <v>720</v>
       </c>
       <c r="C316" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D316" s="3"/>
       <c r="E316" s="21" t="s">
@@ -13003,11 +13198,11 @@
         <v>13</v>
       </c>
       <c r="G316" s="3" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="H316" s="3"/>
       <c r="I316" s="3" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="J316" s="3" t="s">
         <v>85</v>
@@ -13022,7 +13217,7 @@
         <v>720</v>
       </c>
       <c r="C317" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D317" s="3" t="s">
         <v>712</v>
@@ -13034,11 +13229,11 @@
         <v>13</v>
       </c>
       <c r="G317" s="3" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="H317" s="55"/>
       <c r="I317" s="46" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="J317" s="46" t="s">
         <v>85</v>
@@ -13053,7 +13248,7 @@
         <v>720</v>
       </c>
       <c r="C318" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D318" s="3" t="s">
         <v>712</v>
@@ -13065,11 +13260,11 @@
         <v>13</v>
       </c>
       <c r="G318" s="3" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="H318" s="55"/>
       <c r="I318" s="3" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="J318" s="46" t="s">
         <v>85</v>
@@ -13144,7 +13339,7 @@
         <v>795</v>
       </c>
       <c r="C321" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D321" s="3"/>
       <c r="E321" s="22" t="s">
@@ -13161,7 +13356,7 @@
         <v>802</v>
       </c>
       <c r="J321" s="1" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="K321" s="24"/>
     </row>
@@ -13231,11 +13426,11 @@
         <v>795</v>
       </c>
       <c r="C324" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D324" s="3"/>
       <c r="E324" s="21" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="F324" s="1" t="s">
         <v>13</v>
@@ -13250,7 +13445,7 @@
         <v>886</v>
       </c>
       <c r="J324" s="3" t="s">
-        <v>887</v>
+        <v>1150</v>
       </c>
       <c r="K324" s="24"/>
     </row>
@@ -13262,32 +13457,32 @@
         <v>795</v>
       </c>
       <c r="C325" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D325" s="3"/>
       <c r="E325" s="21" t="s">
         <v>547</v>
       </c>
       <c r="F325" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="G325" s="3" t="s">
         <v>888</v>
       </c>
-      <c r="G325" s="3" t="s">
+      <c r="H325" s="3" t="s">
         <v>889</v>
       </c>
-      <c r="H325" s="3" t="s">
+      <c r="I325" s="55" t="s">
         <v>890</v>
       </c>
-      <c r="I325" s="55" t="s">
-        <v>891</v>
-      </c>
       <c r="J325" s="3" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="K325" s="66" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="326" spans="1:11" ht="50" x14ac:dyDescent="0.35">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="326" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A326" s="24">
         <v>325</v>
       </c>
@@ -13295,24 +13490,24 @@
         <v>795</v>
       </c>
       <c r="C326" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D326" s="3"/>
       <c r="E326" s="43" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="F326" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G326" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="H326" s="55"/>
       <c r="I326" s="1" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="J326" s="3" t="s">
-        <v>894</v>
+        <v>1151</v>
       </c>
       <c r="K326" s="24"/>
     </row>
@@ -13324,26 +13519,26 @@
         <v>795</v>
       </c>
       <c r="C327" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D327" s="3"/>
       <c r="E327" s="21" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="F327" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="G327" s="3" t="s">
+        <v>894</v>
+      </c>
+      <c r="H327" s="3" t="s">
+        <v>894</v>
+      </c>
+      <c r="I327" s="55" t="s">
         <v>895</v>
       </c>
-      <c r="G327" s="3" t="s">
+      <c r="J327" s="3" t="s">
         <v>896</v>
-      </c>
-      <c r="H327" s="3" t="s">
-        <v>896</v>
-      </c>
-      <c r="I327" s="55" t="s">
-        <v>897</v>
-      </c>
-      <c r="J327" s="3" t="s">
-        <v>898</v>
       </c>
       <c r="K327" s="24"/>
     </row>
@@ -13355,21 +13550,21 @@
         <v>795</v>
       </c>
       <c r="C328" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D328" s="3"/>
       <c r="E328" s="22" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="F328" s="24" t="s">
         <v>13</v>
       </c>
       <c r="G328" s="3" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="H328" s="3"/>
       <c r="I328" s="3" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="J328" s="3" t="s">
         <v>85</v>
@@ -13388,7 +13583,7 @@
       </c>
       <c r="D329" s="3"/>
       <c r="E329" s="31" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="F329" s="1"/>
       <c r="G329" s="55"/>
@@ -13523,7 +13718,7 @@
         <v>831</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D334" s="1"/>
       <c r="E334" s="22" t="s">
@@ -13533,11 +13728,11 @@
         <v>13</v>
       </c>
       <c r="G334" s="61" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="H334" s="61"/>
       <c r="I334" s="61" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="J334" s="61" t="s">
         <v>85</v>
@@ -13668,7 +13863,7 @@
         <v>843</v>
       </c>
       <c r="C339" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D339" s="3"/>
       <c r="E339" s="21" t="s">
@@ -13687,10 +13882,10 @@
         <v>855</v>
       </c>
       <c r="J339" s="3" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="K339" s="67" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
     </row>
     <row r="340" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -13701,7 +13896,7 @@
         <v>843</v>
       </c>
       <c r="C340" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D340" s="3"/>
       <c r="E340" s="21" t="s">
@@ -13720,10 +13915,10 @@
         <v>858</v>
       </c>
       <c r="J340" s="3" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="K340" s="3" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
     </row>
     <row r="341" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -13755,7 +13950,7 @@
         <v>843</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D342" s="1"/>
       <c r="E342" s="22" t="s">
@@ -13765,11 +13960,11 @@
         <v>13</v>
       </c>
       <c r="G342" s="3" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="H342" s="3"/>
       <c r="I342" s="3" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="J342" s="3" t="s">
         <v>85</v>
@@ -13781,24 +13976,24 @@
         <v>342</v>
       </c>
       <c r="B343" s="3" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C343" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D343" s="3"/>
       <c r="E343" s="53" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="F343" s="1" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="G343" s="3" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="H343" s="55"/>
       <c r="I343" s="3" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="J343" s="46" t="s">
         <v>85</v>
@@ -13810,7 +14005,7 @@
         <v>343</v>
       </c>
       <c r="B344" s="3" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C344" s="3" t="s">
         <v>86</v>
@@ -13820,14 +14015,14 @@
         <v>827</v>
       </c>
       <c r="F344" s="1" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="G344" s="3" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="H344" s="55"/>
       <c r="I344" s="3" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="J344" s="46" t="s">
         <v>85</v>
@@ -13839,30 +14034,30 @@
         <v>344</v>
       </c>
       <c r="B345" s="3" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C345" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D345" s="3"/>
       <c r="E345" s="21" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="F345" s="1" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="G345" s="3" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="H345" s="55"/>
       <c r="I345" s="3" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="J345" s="3" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="K345" s="3" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
     </row>
     <row r="346" spans="1:11" ht="50" x14ac:dyDescent="0.35">
@@ -13870,24 +14065,24 @@
         <v>345</v>
       </c>
       <c r="B346" s="3" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="C346" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D346" s="3"/>
       <c r="E346" s="53" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="F346" s="3" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="G346" s="3" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="H346" s="55"/>
       <c r="I346" s="3" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
       <c r="J346" s="3" t="s">
         <v>85</v>
@@ -13899,13 +14094,13 @@
         <v>346</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="C347" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D347" s="3" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E347" s="43" t="s">
         <v>507</v>
@@ -13914,11 +14109,11 @@
         <v>13</v>
       </c>
       <c r="G347" s="3" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="H347" s="55"/>
       <c r="I347" s="3" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="J347" s="3" t="s">
         <v>85</v>
@@ -13930,13 +14125,13 @@
         <v>347</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="C348" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D348" s="3" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E348" s="43" t="s">
         <v>508</v>
@@ -13945,11 +14140,11 @@
         <v>13</v>
       </c>
       <c r="G348" s="3" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="H348" s="55"/>
       <c r="I348" s="3" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="J348" s="3" t="s">
         <v>85</v>
@@ -13961,13 +14156,13 @@
         <v>348</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="C349" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D349" s="3" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E349" s="43" t="s">
         <v>545</v>
@@ -13976,11 +14171,11 @@
         <v>13</v>
       </c>
       <c r="G349" s="3" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="H349" s="55"/>
       <c r="I349" s="3" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="J349" s="3" t="s">
         <v>85</v>
@@ -13992,26 +14187,26 @@
         <v>349</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="C350" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D350" s="3" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E350" s="21" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="F350" s="24" t="s">
         <v>13</v>
       </c>
       <c r="G350" s="3" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="H350" s="3"/>
       <c r="I350" s="3" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="J350" s="3" t="s">
         <v>85</v>
@@ -14023,26 +14218,26 @@
         <v>350</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="C351" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D351" s="3" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E351" s="21" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="F351" s="24" t="s">
         <v>379</v>
       </c>
       <c r="G351" s="3" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="H351" s="3"/>
       <c r="I351" s="3" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
       <c r="J351" s="3" t="s">
         <v>85</v>
@@ -14054,32 +14249,32 @@
         <v>351</v>
       </c>
       <c r="B352" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="C352" s="3" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D352" s="3" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E352" s="21" t="s">
         <v>986</v>
       </c>
-      <c r="C352" s="3" t="s">
-        <v>1049</v>
-      </c>
-      <c r="D352" s="3" t="s">
-        <v>1007</v>
-      </c>
-      <c r="E352" s="21" t="s">
-        <v>989</v>
-      </c>
       <c r="F352" s="24" t="s">
         <v>13</v>
       </c>
       <c r="G352" s="3" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="H352" s="3"/>
       <c r="I352" s="3" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="J352" s="3" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="K352" s="68" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
     </row>
     <row r="353" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
@@ -14087,26 +14282,26 @@
         <v>352</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="C353" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D353" s="3" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E353" s="43" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="F353" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G353" s="3" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="H353" s="3"/>
       <c r="I353" s="3" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="J353" s="3" t="s">
         <v>85</v>
@@ -14118,24 +14313,24 @@
         <v>353</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="C354" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D354" s="3"/>
       <c r="E354" s="43" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="F354" s="46" t="s">
         <v>13</v>
       </c>
       <c r="G354" s="46" t="s">
-        <v>1084</v>
+        <v>1081</v>
       </c>
       <c r="H354" s="46"/>
       <c r="I354" s="3" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="J354" s="46" t="s">
         <v>85</v>
@@ -14147,16 +14342,16 @@
         <v>354</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="C355" s="3" t="s">
         <v>224</v>
       </c>
       <c r="D355" s="3" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E355" s="42" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="F355" s="55"/>
       <c r="G355" s="55"/>
@@ -14172,14 +14367,14 @@
         <v>355</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="C356" s="3" t="s">
         <v>224</v>
       </c>
       <c r="D356" s="3"/>
       <c r="E356" s="42" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="F356" s="55"/>
       <c r="G356" s="55"/>
@@ -14195,24 +14390,24 @@
         <v>356</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="C357" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D357" s="3"/>
       <c r="E357" s="53" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="F357" s="3" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="G357" s="3" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="H357" s="55"/>
       <c r="I357" s="3" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="J357" s="3" t="s">
         <v>85</v>
@@ -14224,7 +14419,7 @@
         <v>357</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="C358" s="3" t="s">
         <v>86</v>
@@ -14239,11 +14434,11 @@
         <v>13</v>
       </c>
       <c r="G358" s="3" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="H358" s="55"/>
       <c r="I358" s="3" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="J358" s="3" t="s">
         <v>85</v>
@@ -14255,7 +14450,7 @@
         <v>358</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="C359" s="3" t="s">
         <v>86</v>
@@ -14270,11 +14465,11 @@
         <v>13</v>
       </c>
       <c r="G359" s="3" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="H359" s="55"/>
       <c r="I359" s="3" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="J359" s="3" t="s">
         <v>85</v>
@@ -14286,7 +14481,7 @@
         <v>359</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="C360" s="3" t="s">
         <v>86</v>
@@ -14301,11 +14496,11 @@
         <v>13</v>
       </c>
       <c r="G360" s="3" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="H360" s="55"/>
       <c r="I360" s="3" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="J360" s="3" t="s">
         <v>85</v>
@@ -14317,7 +14512,7 @@
         <v>360</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="C361" s="3" t="s">
         <v>86</v>
@@ -14332,11 +14527,11 @@
         <v>13</v>
       </c>
       <c r="G361" s="3" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="H361" s="55"/>
       <c r="I361" s="3" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="J361" s="3" t="s">
         <v>85</v>
@@ -14348,7 +14543,7 @@
         <v>361</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="C362" s="3" t="s">
         <v>224</v>
@@ -14373,24 +14568,24 @@
         <v>362</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="C363" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D363" s="3"/>
       <c r="E363" s="53" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="F363" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G363" s="3" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="H363" s="55"/>
       <c r="I363" s="3" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
       <c r="J363" s="3" t="s">
         <v>466</v>
@@ -14402,7 +14597,7 @@
         <v>363</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="C364" s="3" t="s">
         <v>86</v>
@@ -14415,11 +14610,11 @@
         <v>13</v>
       </c>
       <c r="G364" s="3" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="H364" s="55"/>
       <c r="I364" s="3" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="J364" s="3" t="s">
         <v>85</v>
@@ -14431,7 +14626,7 @@
         <v>364</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="C365" s="3" t="s">
         <v>86</v>
@@ -14444,11 +14639,11 @@
         <v>13</v>
       </c>
       <c r="G365" s="3" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="H365" s="55"/>
       <c r="I365" s="3" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="J365" s="3" t="s">
         <v>85</v>
@@ -14460,7 +14655,7 @@
         <v>365</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="C366" s="3" t="s">
         <v>86</v>
@@ -14473,11 +14668,11 @@
         <v>13</v>
       </c>
       <c r="G366" s="3" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="H366" s="55"/>
       <c r="I366" s="3" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="J366" s="3" t="s">
         <v>85</v>
@@ -14489,24 +14684,24 @@
         <v>366</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="C367" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D367" s="3"/>
       <c r="E367" s="21" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="F367" s="24" t="s">
         <v>13</v>
       </c>
       <c r="G367" s="3" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="H367" s="3"/>
       <c r="I367" s="3" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="J367" s="3" t="s">
         <v>85</v>
@@ -14518,24 +14713,24 @@
         <v>367</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="C368" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D368" s="3"/>
       <c r="E368" s="21" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="F368" s="24" t="s">
         <v>13</v>
       </c>
       <c r="G368" s="3" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="H368" s="3"/>
       <c r="I368" s="3" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="J368" s="3" t="s">
         <v>85</v>
@@ -14547,30 +14742,30 @@
         <v>368</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="C369" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D369" s="3"/>
       <c r="E369" s="21" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="F369" s="24" t="s">
         <v>13</v>
       </c>
       <c r="G369" s="3" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="H369" s="3"/>
       <c r="I369" s="3" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="J369" s="3" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="K369" s="68" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
     </row>
     <row r="370" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
@@ -14578,24 +14773,24 @@
         <v>369</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="C370" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D370" s="1"/>
       <c r="E370" s="43" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="F370" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G370" s="3" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="H370" s="3"/>
       <c r="I370" s="3" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="J370" s="3" t="s">
         <v>85</v>
@@ -14607,24 +14802,24 @@
         <v>370</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="C371" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D371" s="1"/>
       <c r="E371" s="43" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="F371" s="46" t="s">
         <v>13</v>
       </c>
       <c r="G371" s="46" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="H371" s="46"/>
       <c r="I371" s="3" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="J371" s="46" t="s">
         <v>85</v>
@@ -14636,14 +14831,14 @@
         <v>371</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="C372" s="3" t="s">
         <v>224</v>
       </c>
       <c r="D372" s="3"/>
       <c r="E372" s="42" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="F372" s="55"/>
       <c r="G372" s="55"/>
@@ -14659,24 +14854,24 @@
         <v>372</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="C373" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D373" s="3"/>
       <c r="E373" s="53" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F373" s="3" t="s">
         <v>1016</v>
       </c>
-      <c r="F373" s="3" t="s">
-        <v>1019</v>
-      </c>
       <c r="G373" s="3" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="H373" s="55"/>
       <c r="I373" s="3" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="J373" s="3" t="s">
         <v>466</v>
@@ -14688,24 +14883,24 @@
         <v>373</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="C374" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D374" s="3"/>
       <c r="E374" s="43" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="F374" s="3" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="G374" s="3" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="H374" s="55"/>
       <c r="I374" s="3" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="J374" s="3" t="s">
         <v>85</v>
@@ -14717,24 +14912,24 @@
         <v>374</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="C375" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D375" s="3"/>
       <c r="E375" s="43" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="F375" s="3" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="G375" s="3" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="H375" s="55"/>
       <c r="I375" s="3" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="J375" s="3" t="s">
         <v>85</v>
@@ -14746,30 +14941,30 @@
         <v>375</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="C376" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D376" s="3"/>
       <c r="E376" s="43" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="F376" s="3" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="G376" s="3" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="H376" s="55"/>
       <c r="I376" s="3" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="J376" s="3" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="K376" s="68" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
     </row>
     <row r="377" spans="1:11" ht="25" x14ac:dyDescent="0.35">
@@ -14777,24 +14972,24 @@
         <v>376</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="C377" s="3" t="s">
         <v>86</v>
       </c>
       <c r="D377" s="3"/>
       <c r="E377" s="44" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="F377" s="46" t="s">
         <v>13</v>
       </c>
       <c r="G377" s="46" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="H377" s="46"/>
       <c r="I377" s="46" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="J377" s="46" t="s">
         <v>85</v>
@@ -14806,14 +15001,14 @@
         <v>377</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="C378" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D378" s="1"/>
       <c r="E378" s="30" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="F378" s="3" t="s">
         <v>12</v>
@@ -14837,7 +15032,7 @@
         <v>378</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="C379" s="3" t="s">
         <v>86</v>
@@ -14850,11 +15045,11 @@
         <v>13</v>
       </c>
       <c r="G379" s="3" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="H379" s="55"/>
       <c r="I379" s="3" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="J379" s="3" t="s">
         <v>85</v>
@@ -14866,10 +15061,10 @@
         <v>379</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="C380" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D380" s="1"/>
       <c r="E380" s="21" t="s">
@@ -14879,14 +15074,14 @@
         <v>13</v>
       </c>
       <c r="G380" s="3" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="H380" s="55"/>
       <c r="I380" s="3" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="J380" s="3" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
       <c r="K380" s="24"/>
     </row>
@@ -14895,24 +15090,24 @@
         <v>380</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="C381" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D381" s="1"/>
       <c r="E381" s="30" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="F381" s="3" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="G381" s="3" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="H381" s="55"/>
       <c r="I381" s="3" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="J381" s="3" t="s">
         <v>466</v>
@@ -14923,7 +15118,7 @@
         <v>381</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="C382" s="3" t="s">
         <v>86</v>
@@ -14938,11 +15133,11 @@
         <v>13</v>
       </c>
       <c r="G382" s="3" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="H382" s="55"/>
       <c r="I382" s="3" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="J382" s="46" t="s">
         <v>85</v>
@@ -14953,7 +15148,7 @@
         <v>382</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="C383" s="3" t="s">
         <v>86</v>
@@ -14968,11 +15163,11 @@
         <v>13</v>
       </c>
       <c r="G383" s="3" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="H383" s="55"/>
       <c r="I383" s="3" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="J383" s="46" t="s">
         <v>85</v>
@@ -14983,7 +15178,7 @@
         <v>383</v>
       </c>
       <c r="B384" s="20" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="C384" s="32" t="s">
         <v>86</v>
@@ -14998,11 +15193,11 @@
         <v>13</v>
       </c>
       <c r="G384" s="32" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
       <c r="H384" s="57"/>
       <c r="I384" s="32" t="s">
-        <v>1094</v>
+        <v>1091</v>
       </c>
       <c r="J384" s="69" t="s">
         <v>85</v>
@@ -15013,7 +15208,7 @@
         <v>384</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="C385" s="3" t="s">
         <v>86</v>
@@ -15028,11 +15223,11 @@
         <v>13</v>
       </c>
       <c r="G385" s="3" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
       <c r="H385" s="55"/>
       <c r="I385" s="3" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
       <c r="J385" s="46" t="s">
         <v>85</v>
@@ -15044,14 +15239,14 @@
         <v>385</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="C386" s="24" t="s">
         <v>224</v>
       </c>
       <c r="D386" s="24"/>
       <c r="E386" s="34" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="F386" s="24"/>
       <c r="G386" s="24"/>
@@ -15067,14 +15262,14 @@
         <v>386</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="C387" s="24" t="s">
         <v>224</v>
       </c>
       <c r="D387" s="24"/>
       <c r="E387" s="34" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="F387" s="24"/>
       <c r="G387" s="24"/>
@@ -15090,7 +15285,7 @@
         <v>387</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="C388" s="24" t="s">
         <v>224</v>
@@ -15115,24 +15310,24 @@
         <v>388</v>
       </c>
       <c r="B389" s="3" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="C389" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D389" s="1"/>
       <c r="E389" s="30" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="F389" s="3" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="G389" s="3" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="H389" s="55"/>
       <c r="I389" s="3" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="J389" s="3" t="s">
         <v>466</v>
@@ -15144,7 +15339,7 @@
         <v>389</v>
       </c>
       <c r="B390" s="3" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="C390" s="3" t="s">
         <v>86</v>
@@ -15157,11 +15352,11 @@
         <v>13</v>
       </c>
       <c r="G390" s="3" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="H390" s="55"/>
       <c r="I390" s="3" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="J390" s="3" t="s">
         <v>85</v>
@@ -15173,29 +15368,29 @@
         <v>390</v>
       </c>
       <c r="B391" s="3" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="C391" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D391" s="24"/>
       <c r="E391" s="21" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="F391" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G391" s="3" t="s">
-        <v>1106</v>
-      </c>
-      <c r="H391" s="55" t="s">
-        <v>1107</v>
+        <v>1103</v>
+      </c>
+      <c r="H391" s="46" t="s">
+        <v>1104</v>
       </c>
       <c r="I391" s="3" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="J391" s="3" t="s">
-        <v>1109</v>
+        <v>1152</v>
       </c>
       <c r="K391" s="1"/>
     </row>
@@ -15204,24 +15399,24 @@
         <v>391</v>
       </c>
       <c r="B392" s="3" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="C392" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D392" s="1"/>
       <c r="E392" s="30" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="F392" s="3" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
       <c r="G392" s="3" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
       <c r="H392" s="55"/>
       <c r="I392" s="3" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
       <c r="J392" s="3" t="s">
         <v>466</v>
@@ -15233,7 +15428,7 @@
         <v>392</v>
       </c>
       <c r="B393" s="3" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="C393" s="3" t="s">
         <v>86</v>
@@ -15248,11 +15443,11 @@
         <v>13</v>
       </c>
       <c r="G393" s="3" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
       <c r="H393" s="55"/>
       <c r="I393" s="1" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
       <c r="J393" s="3" t="s">
         <v>85</v>
@@ -15264,7 +15459,7 @@
         <v>393</v>
       </c>
       <c r="B394" s="3" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="C394" s="3" t="s">
         <v>86</v>
@@ -15279,11 +15474,11 @@
         <v>13</v>
       </c>
       <c r="G394" s="3" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
       <c r="H394" s="55"/>
       <c r="I394" s="3" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="J394" s="3" t="s">
         <v>85</v>
@@ -15295,7 +15490,7 @@
         <v>394</v>
       </c>
       <c r="B395" s="3" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="C395" s="3" t="s">
         <v>86</v>
@@ -15310,11 +15505,11 @@
         <v>13</v>
       </c>
       <c r="G395" s="3" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
       <c r="H395" s="55"/>
       <c r="I395" s="3" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
       <c r="J395" s="3" t="s">
         <v>85</v>
@@ -15326,10 +15521,10 @@
         <v>395</v>
       </c>
       <c r="B396" s="3" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="C396" s="3" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="D396" s="24" t="s">
         <v>192</v>
@@ -15341,17 +15536,17 @@
         <v>13</v>
       </c>
       <c r="G396" s="3" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
       <c r="H396" s="55"/>
       <c r="I396" s="3" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="J396" s="1" t="s">
         <v>308</v>
       </c>
       <c r="K396" s="46" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
     </row>
     <row r="397" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -15359,7 +15554,7 @@
         <v>396</v>
       </c>
       <c r="B397" s="3" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="C397" s="3" t="s">
         <v>86</v>
@@ -15374,11 +15569,11 @@
         <v>13</v>
       </c>
       <c r="G397" s="3" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
       <c r="H397" s="55"/>
       <c r="I397" s="3" t="s">
-        <v>1125</v>
+        <v>1121</v>
       </c>
       <c r="J397" s="3" t="s">
         <v>85</v>
@@ -15390,7 +15585,7 @@
         <v>397</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="C398" s="24" t="s">
         <v>224</v>
@@ -15415,14 +15610,14 @@
         <v>398</v>
       </c>
       <c r="B399" s="3" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="C399" s="24" t="s">
         <v>224</v>
       </c>
       <c r="D399" s="24"/>
       <c r="E399" s="64" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
       <c r="F399" s="24"/>
       <c r="G399" s="24"/>
@@ -15436,24 +15631,24 @@
         <v>399</v>
       </c>
       <c r="B400" s="3" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="C400" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D400" s="1"/>
       <c r="E400" s="30" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="F400" s="3" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="G400" s="3" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="H400" s="55"/>
       <c r="I400" s="3" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="J400" s="3" t="s">
         <v>466</v>
@@ -15465,7 +15660,7 @@
         <v>400</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="C401" s="3" t="s">
         <v>86</v>
@@ -15478,11 +15673,11 @@
         <v>13</v>
       </c>
       <c r="G401" s="3" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="H401" s="55"/>
       <c r="I401" s="3" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="J401" s="3" t="s">
         <v>85</v>
@@ -15494,7 +15689,7 @@
         <v>401</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="C402" s="3" t="s">
         <v>86</v>
@@ -15507,11 +15702,11 @@
         <v>13</v>
       </c>
       <c r="G402" s="3" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
       <c r="H402" s="55"/>
       <c r="I402" s="3" t="s">
-        <v>1147</v>
+        <v>1143</v>
       </c>
       <c r="J402" s="3" t="s">
         <v>85</v>
@@ -15523,7 +15718,7 @@
         <v>402</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="C403" s="3" t="s">
         <v>86</v>
@@ -15536,11 +15731,11 @@
         <v>13</v>
       </c>
       <c r="G403" s="3" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="H403" s="55"/>
       <c r="I403" s="3" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="J403" s="3" t="s">
         <v>85</v>
@@ -15552,14 +15747,14 @@
         <v>403</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="C404" s="3" t="s">
         <v>224</v>
       </c>
       <c r="D404" s="24"/>
       <c r="E404" s="64" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
       <c r="F404" s="55"/>
       <c r="G404" s="55"/>
@@ -15575,14 +15770,14 @@
         <v>404</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="C405" s="3" t="s">
         <v>224</v>
       </c>
       <c r="D405" s="24"/>
       <c r="E405" s="64" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="F405" s="55"/>
       <c r="G405" s="55"/>
@@ -15625,7 +15820,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M73"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
@@ -16533,7 +16728,7 @@
         <v>126</v>
       </c>
       <c r="B39" s="51" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="C39" s="40" t="s">
         <v>547</v>
@@ -16545,13 +16740,13 @@
         <v>13</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>193</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
@@ -16559,7 +16754,7 @@
         <v>126</v>
       </c>
       <c r="B40" s="51" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="C40" s="40" t="s">
         <v>547</v>
@@ -16571,11 +16766,11 @@
         <v>13</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -16583,7 +16778,7 @@
         <v>126</v>
       </c>
       <c r="B41" s="51" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="C41" s="40" t="s">
         <v>547</v>
@@ -16595,11 +16790,11 @@
         <v>13</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -16607,7 +16802,7 @@
         <v>126</v>
       </c>
       <c r="B42" s="51" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="C42" s="40" t="s">
         <v>547</v>
@@ -16619,11 +16814,11 @@
         <v>13</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -16631,7 +16826,7 @@
         <v>126</v>
       </c>
       <c r="B43" s="51" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="C43" s="40" t="s">
         <v>547</v>
@@ -16658,20 +16853,20 @@
         <v>228</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="D44" s="40" t="s">
         <v>13</v>
       </c>
       <c r="E44" s="50" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="G44" s="50"/>
       <c r="H44" s="50" t="s">
-        <v>1132</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
@@ -16682,7 +16877,7 @@
         <v>228</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="D45" s="40" t="s">
         <v>13</v>
@@ -16691,13 +16886,13 @@
         <v>13</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
       <c r="G45" s="50" t="s">
-        <v>1134</v>
+        <v>1130</v>
       </c>
       <c r="H45" s="50" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
@@ -16708,20 +16903,670 @@
         <v>228</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="D46" s="40" t="s">
         <v>13</v>
       </c>
       <c r="E46" s="50" t="s">
-        <v>1136</v>
+        <v>1132</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>1137</v>
+        <v>1133</v>
       </c>
       <c r="G46" s="50"/>
       <c r="H46" s="50" t="s">
-        <v>1138</v>
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="A47" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>660</v>
+      </c>
+      <c r="C47" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="D47" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="50" t="s">
+        <v>1153</v>
+      </c>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="A48" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>660</v>
+      </c>
+      <c r="C48" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="D48" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="50" t="s">
+        <v>1155</v>
+      </c>
+      <c r="G48" s="50"/>
+      <c r="H48" s="50" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="A49" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>660</v>
+      </c>
+      <c r="C49" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="D49" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="50" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G49" s="50"/>
+      <c r="H49" s="50" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="A50" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B50" s="26" t="s">
+        <v>660</v>
+      </c>
+      <c r="C50" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="D50" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" s="50" t="s">
+        <v>1159</v>
+      </c>
+      <c r="G50" s="50"/>
+      <c r="H50" s="50" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="A51" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B51" s="26" t="s">
+        <v>660</v>
+      </c>
+      <c r="C51" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="D51" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="50" t="s">
+        <v>1161</v>
+      </c>
+      <c r="G51" s="50"/>
+      <c r="H51" s="50" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="A52" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B52" s="26" t="s">
+        <v>660</v>
+      </c>
+      <c r="C52" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="D52" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="50" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G52" s="50"/>
+      <c r="H52" s="50" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="A53" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B53" s="26" t="s">
+        <v>660</v>
+      </c>
+      <c r="C53" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="D53" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="50" t="s">
+        <v>1165</v>
+      </c>
+      <c r="G53" s="50"/>
+      <c r="H53" s="50" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="A54" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B54" s="26" t="s">
+        <v>660</v>
+      </c>
+      <c r="C54" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="D54" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="50" t="s">
+        <v>1167</v>
+      </c>
+      <c r="G54" s="50"/>
+      <c r="H54" s="50" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="A55" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>660</v>
+      </c>
+      <c r="C55" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="D55" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="50" t="s">
+        <v>1169</v>
+      </c>
+      <c r="G55" s="50"/>
+      <c r="H55" s="50" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="A56" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B56" s="26" t="s">
+        <v>660</v>
+      </c>
+      <c r="C56" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="D56" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="50" t="s">
+        <v>1171</v>
+      </c>
+      <c r="G56" s="50"/>
+      <c r="H56" s="50" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="A57" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B57" s="26" t="s">
+        <v>660</v>
+      </c>
+      <c r="C57" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="D57" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="50" t="s">
+        <v>1173</v>
+      </c>
+      <c r="G57" s="50"/>
+      <c r="H57" s="50" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="A58" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B58" s="26" t="s">
+        <v>660</v>
+      </c>
+      <c r="C58" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="D58" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="50" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G58" s="50"/>
+      <c r="H58" s="50" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="A59" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>660</v>
+      </c>
+      <c r="C59" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="D59" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" s="50" t="s">
+        <v>1177</v>
+      </c>
+      <c r="G59" s="50"/>
+      <c r="H59" s="50" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="87.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B60" s="75" t="s">
+        <v>795</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>897</v>
+      </c>
+      <c r="D60" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="50" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F60" s="50" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G60" s="50"/>
+      <c r="H60" s="50" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B61" s="75" t="s">
+        <v>795</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>897</v>
+      </c>
+      <c r="D61" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61" s="50" t="s">
+        <v>1182</v>
+      </c>
+      <c r="F61" s="50" t="s">
+        <v>1183</v>
+      </c>
+      <c r="G61" s="50"/>
+      <c r="H61" s="50" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="75" x14ac:dyDescent="0.35">
+      <c r="A62" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B62" s="75" t="s">
+        <v>795</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>897</v>
+      </c>
+      <c r="D62" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" s="50" t="s">
+        <v>1185</v>
+      </c>
+      <c r="F62" s="50" t="s">
+        <v>1186</v>
+      </c>
+      <c r="G62" s="50"/>
+      <c r="H62" s="13" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="75" x14ac:dyDescent="0.35">
+      <c r="A63" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" s="75" t="s">
+        <v>795</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>897</v>
+      </c>
+      <c r="D63" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63" s="50" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F63" s="50" t="s">
+        <v>1189</v>
+      </c>
+      <c r="G63" s="50"/>
+      <c r="H63" s="50" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="A64" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" s="75" t="s">
+        <v>795</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>897</v>
+      </c>
+      <c r="D64" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E64" s="50" t="s">
+        <v>1191</v>
+      </c>
+      <c r="F64" s="50" t="s">
+        <v>1192</v>
+      </c>
+      <c r="G64" s="50"/>
+      <c r="H64" s="50" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B65" s="75" t="s">
+        <v>795</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>897</v>
+      </c>
+      <c r="D65" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65" s="50" t="s">
+        <v>1194</v>
+      </c>
+      <c r="F65" s="50" t="s">
+        <v>1195</v>
+      </c>
+      <c r="G65" s="50"/>
+      <c r="H65" s="50" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A66" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B66" s="75" t="s">
+        <v>795</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>897</v>
+      </c>
+      <c r="D66" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E66" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" s="50" t="s">
+        <v>1197</v>
+      </c>
+      <c r="G66" s="50"/>
+      <c r="H66" s="50" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="A67" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B67" s="75" t="s">
+        <v>795</v>
+      </c>
+      <c r="C67" s="50" t="s">
+        <v>898</v>
+      </c>
+      <c r="D67" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E67" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F67" s="50" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G67" s="50"/>
+      <c r="H67" s="50" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="50" x14ac:dyDescent="0.35">
+      <c r="A68" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B68" s="75" t="s">
+        <v>795</v>
+      </c>
+      <c r="C68" s="50" t="s">
+        <v>898</v>
+      </c>
+      <c r="D68" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E68" s="50" t="s">
+        <v>1201</v>
+      </c>
+      <c r="F68" s="50" t="s">
+        <v>1202</v>
+      </c>
+      <c r="G68" s="50"/>
+      <c r="H68" s="50" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="75" x14ac:dyDescent="0.35">
+      <c r="A69" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B69" s="26" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>897</v>
+      </c>
+      <c r="D69" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E69" s="50" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F69" s="50" t="s">
+        <v>1205</v>
+      </c>
+      <c r="G69" s="50"/>
+      <c r="H69" s="50" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="A70" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B70" s="26" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>897</v>
+      </c>
+      <c r="D70" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70" s="50" t="s">
+        <v>1207</v>
+      </c>
+      <c r="F70" s="50" t="s">
+        <v>1208</v>
+      </c>
+      <c r="G70" s="50" t="s">
+        <v>1209</v>
+      </c>
+      <c r="H70" s="50" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="50" x14ac:dyDescent="0.35">
+      <c r="A71" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B71" s="26" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>897</v>
+      </c>
+      <c r="D71" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E71" s="50" t="s">
+        <v>1211</v>
+      </c>
+      <c r="F71" s="50" t="s">
+        <v>1212</v>
+      </c>
+      <c r="G71" s="50"/>
+      <c r="H71" s="50" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A72" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B72" s="26" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>897</v>
+      </c>
+      <c r="D72" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E72" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F72" s="50" t="s">
+        <v>1214</v>
+      </c>
+      <c r="G72" s="50"/>
+      <c r="H72" s="50" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B73" s="26" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>897</v>
+      </c>
+      <c r="D73" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E73" s="50" t="s">
+        <v>267</v>
+      </c>
+      <c r="F73" s="50" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G73" s="50"/>
+      <c r="H73" s="50" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -16750,15 +17595,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16980,6 +17816,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
   <ds:schemaRefs>
@@ -16999,14 +17844,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17024,4 +17861,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
type to organizationType for both Organization and ResearchOrganization Classes
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3CF2F1-14F7-4A14-B8D3-7A5CB457BD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E860F5EF-0621-4FEA-9B7A-7D5E7AF34A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="10" windowWidth="15270" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="350" yWindow="50" windowWidth="17480" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3088" uniqueCount="1219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3088" uniqueCount="1217">
   <si>
     <t>Preferred Term</t>
   </si>
@@ -3379,12 +3379,6 @@
   </si>
   <si>
     <t>The literal identifier (i.e., distinctive designation) of the research organization.</t>
-  </si>
-  <si>
-    <t>Research Organization Type</t>
-  </si>
-  <si>
-    <t>A characterization or classification of the research organization.</t>
   </si>
   <si>
     <t>Research Organization Label</t>
@@ -5079,7 +5073,7 @@
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="22" t="s">
-        <v>546</v>
+        <v>1210</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>274</v>
@@ -5490,7 +5484,7 @@
       </c>
       <c r="D38" s="41"/>
       <c r="E38" s="34" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="F38" s="47"/>
       <c r="G38" s="41"/>
@@ -5513,7 +5507,7 @@
       </c>
       <c r="D39" s="41"/>
       <c r="E39" s="64" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="F39" s="47"/>
       <c r="G39" s="41"/>
@@ -5819,14 +5813,14 @@
         <v>13</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="H49" s="46"/>
       <c r="I49" s="46" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="K49" s="46"/>
     </row>
@@ -6241,7 +6235,7 @@
         <v>13</v>
       </c>
       <c r="G63" s="46" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="H63" s="46"/>
       <c r="I63" s="3" t="s">
@@ -8537,7 +8531,7 @@
       </c>
       <c r="D147" s="1"/>
       <c r="E147" s="31" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
@@ -11757,14 +11751,14 @@
         <v>263</v>
       </c>
       <c r="B264" s="46" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="C264" s="41" t="s">
         <v>4</v>
       </c>
       <c r="D264" s="41"/>
       <c r="E264" s="45" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="F264" s="1" t="s">
         <v>616</v>
@@ -11788,7 +11782,7 @@
         <v>264</v>
       </c>
       <c r="B265" s="46" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="C265" s="3" t="s">
         <v>1041</v>
@@ -11819,7 +11813,7 @@
         <v>265</v>
       </c>
       <c r="B266" s="46" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="C266" s="46" t="s">
         <v>86</v>
@@ -11848,7 +11842,7 @@
         <v>266</v>
       </c>
       <c r="B267" s="46" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="C267" s="1" t="s">
         <v>86</v>
@@ -11879,7 +11873,7 @@
         <v>267</v>
       </c>
       <c r="B268" s="46" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>86</v>
@@ -11910,7 +11904,7 @@
         <v>268</v>
       </c>
       <c r="B269" s="46" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="C269" s="1" t="s">
         <v>86</v>
@@ -11941,7 +11935,7 @@
         <v>269</v>
       </c>
       <c r="B270" s="46" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>86</v>
@@ -11972,7 +11966,7 @@
         <v>270</v>
       </c>
       <c r="B271" s="46" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="C271" s="3" t="s">
         <v>223</v>
@@ -11995,7 +11989,7 @@
         <v>271</v>
       </c>
       <c r="B272" s="46" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="C272" s="3" t="s">
         <v>223</v>
@@ -12018,7 +12012,7 @@
         <v>272</v>
       </c>
       <c r="B273" s="46" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="C273" s="3" t="s">
         <v>223</v>
@@ -12041,7 +12035,7 @@
         <v>273</v>
       </c>
       <c r="B274" s="46" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="C274" s="3" t="s">
         <v>223</v>
@@ -12231,7 +12225,7 @@
         <v>656</v>
       </c>
       <c r="J280" s="3" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="K280" s="24"/>
     </row>
@@ -12316,7 +12310,7 @@
         <v>671</v>
       </c>
       <c r="J283" s="3" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="K283" s="24"/>
     </row>
@@ -12797,7 +12791,7 @@
       </c>
       <c r="D301" s="3"/>
       <c r="E301" s="21" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="F301" s="1" t="s">
         <v>28</v>
@@ -13072,7 +13066,7 @@
         <v>713</v>
       </c>
       <c r="J311" s="3" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="K311" s="24"/>
     </row>
@@ -13401,7 +13395,7 @@
         <v>882</v>
       </c>
       <c r="J322" s="3" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="K322" s="24"/>
     </row>
@@ -13463,7 +13457,7 @@
         <v>888</v>
       </c>
       <c r="J324" s="3" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="K324" s="24"/>
     </row>
@@ -15037,7 +15031,7 @@
         <v>1031</v>
       </c>
       <c r="J378" s="3" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="K378" s="24"/>
     </row>
@@ -15346,7 +15340,7 @@
         <v>1100</v>
       </c>
       <c r="J389" s="3" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="K389" s="1"/>
     </row>
@@ -15486,17 +15480,17 @@
         <v>192</v>
       </c>
       <c r="E394" s="22" t="s">
-        <v>1212</v>
-      </c>
-      <c r="F394" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G394" s="3" t="s">
-        <v>1113</v>
-      </c>
-      <c r="H394" s="55"/>
-      <c r="I394" s="3" t="s">
-        <v>1114</v>
+        <v>1210</v>
+      </c>
+      <c r="F394" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G394" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H394" s="1"/>
+      <c r="I394" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="J394" s="1" t="s">
         <v>307</v>
@@ -15525,11 +15519,11 @@
         <v>13</v>
       </c>
       <c r="G395" s="3" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="H395" s="55"/>
       <c r="I395" s="3" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="J395" s="3" t="s">
         <v>85</v>
@@ -15573,7 +15567,7 @@
       </c>
       <c r="D397" s="24"/>
       <c r="E397" s="64" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="F397" s="24"/>
       <c r="G397" s="24"/>
@@ -15587,24 +15581,24 @@
         <v>397</v>
       </c>
       <c r="B398" s="3" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="C398" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D398" s="1"/>
       <c r="E398" s="30" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="F398" s="3" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="G398" s="3" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="H398" s="55"/>
       <c r="I398" s="3" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="J398" s="3" t="s">
         <v>465</v>
@@ -15616,7 +15610,7 @@
         <v>398</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="C399" s="3" t="s">
         <v>86</v>
@@ -15629,11 +15623,11 @@
         <v>13</v>
       </c>
       <c r="G399" s="3" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="H399" s="55"/>
       <c r="I399" s="3" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="J399" s="3" t="s">
         <v>85</v>
@@ -15645,7 +15639,7 @@
         <v>399</v>
       </c>
       <c r="B400" s="1" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="C400" s="3" t="s">
         <v>86</v>
@@ -15658,11 +15652,11 @@
         <v>13</v>
       </c>
       <c r="G400" s="3" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="H400" s="55"/>
       <c r="I400" s="3" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="J400" s="3" t="s">
         <v>85</v>
@@ -15674,7 +15668,7 @@
         <v>400</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="C401" s="3" t="s">
         <v>86</v>
@@ -15687,11 +15681,11 @@
         <v>13</v>
       </c>
       <c r="G401" s="3" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="H401" s="55"/>
       <c r="I401" s="3" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="J401" s="3" t="s">
         <v>85</v>
@@ -15703,14 +15697,14 @@
         <v>401</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="C402" s="3" t="s">
         <v>223</v>
       </c>
       <c r="D402" s="24"/>
       <c r="E402" s="64" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="F402" s="55"/>
       <c r="G402" s="55"/>
@@ -16006,7 +16000,7 @@
         <v>192</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>546</v>
+        <v>1210</v>
       </c>
       <c r="D12" s="27" t="s">
         <v>313</v>
@@ -16032,7 +16026,7 @@
         <v>192</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>546</v>
+        <v>1210</v>
       </c>
       <c r="D13" s="27" t="s">
         <v>313</v>
@@ -16056,7 +16050,7 @@
         <v>192</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>546</v>
+        <v>1210</v>
       </c>
       <c r="D14" s="27" t="s">
         <v>313</v>
@@ -16082,7 +16076,7 @@
         <v>192</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>546</v>
+        <v>1210</v>
       </c>
       <c r="D15" s="27" t="s">
         <v>313</v>
@@ -16816,14 +16810,14 @@
         <v>13</v>
       </c>
       <c r="E45" s="50" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="G45" s="50"/>
       <c r="H45" s="50" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
@@ -16843,13 +16837,13 @@
         <v>13</v>
       </c>
       <c r="F46" s="13" t="s">
+        <v>1121</v>
+      </c>
+      <c r="G46" s="50" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H46" s="50" t="s">
         <v>1123</v>
-      </c>
-      <c r="G46" s="50" t="s">
-        <v>1124</v>
-      </c>
-      <c r="H46" s="50" t="s">
-        <v>1125</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
@@ -16866,14 +16860,14 @@
         <v>13</v>
       </c>
       <c r="E47" s="50" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="G47" s="50"/>
       <c r="H47" s="50" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -16893,11 +16887,11 @@
         <v>13</v>
       </c>
       <c r="F48" s="50" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="G48" s="50"/>
       <c r="H48" s="50" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -16917,11 +16911,11 @@
         <v>13</v>
       </c>
       <c r="F49" s="50" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="G49" s="50"/>
       <c r="H49" s="50" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -16941,11 +16935,11 @@
         <v>13</v>
       </c>
       <c r="F50" s="50" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="G50" s="50"/>
       <c r="H50" s="50" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -16965,11 +16959,11 @@
         <v>13</v>
       </c>
       <c r="F51" s="50" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="G51" s="50"/>
       <c r="H51" s="50" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -16989,11 +16983,11 @@
         <v>13</v>
       </c>
       <c r="F52" s="50" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="G52" s="50"/>
       <c r="H52" s="50" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -17013,11 +17007,11 @@
         <v>13</v>
       </c>
       <c r="F53" s="50" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="G53" s="50"/>
       <c r="H53" s="50" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -17037,11 +17031,11 @@
         <v>13</v>
       </c>
       <c r="F54" s="50" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="G54" s="50"/>
       <c r="H54" s="50" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -17061,11 +17055,11 @@
         <v>13</v>
       </c>
       <c r="F55" s="50" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="G55" s="50"/>
       <c r="H55" s="50" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -17085,11 +17079,11 @@
         <v>13</v>
       </c>
       <c r="F56" s="50" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="G56" s="50"/>
       <c r="H56" s="50" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -17109,11 +17103,11 @@
         <v>13</v>
       </c>
       <c r="F57" s="50" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="G57" s="50"/>
       <c r="H57" s="50" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -17133,11 +17127,11 @@
         <v>13</v>
       </c>
       <c r="F58" s="50" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="G58" s="50"/>
       <c r="H58" s="50" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -17157,11 +17151,11 @@
         <v>13</v>
       </c>
       <c r="F59" s="50" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="G59" s="50"/>
       <c r="H59" s="50" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -17181,11 +17175,11 @@
         <v>13</v>
       </c>
       <c r="F60" s="50" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="G60" s="50"/>
       <c r="H60" s="50" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="87.5" x14ac:dyDescent="0.35">
@@ -17202,14 +17196,14 @@
         <v>13</v>
       </c>
       <c r="E61" s="50" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="F61" s="50" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="G61" s="50"/>
       <c r="H61" s="50" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
@@ -17226,14 +17220,14 @@
         <v>13</v>
       </c>
       <c r="E62" s="50" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="F62" s="50" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="G62" s="50"/>
       <c r="H62" s="50" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="75" x14ac:dyDescent="0.35">
@@ -17250,14 +17244,14 @@
         <v>13</v>
       </c>
       <c r="E63" s="50" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="F63" s="50" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="G63" s="50"/>
       <c r="H63" s="13" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="75" x14ac:dyDescent="0.35">
@@ -17274,14 +17268,14 @@
         <v>13</v>
       </c>
       <c r="E64" s="50" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="F64" s="50" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="G64" s="50"/>
       <c r="H64" s="50" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="62.5" x14ac:dyDescent="0.35">
@@ -17298,14 +17292,14 @@
         <v>13</v>
       </c>
       <c r="E65" s="50" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="F65" s="50" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="G65" s="50"/>
       <c r="H65" s="50" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
@@ -17322,14 +17316,14 @@
         <v>13</v>
       </c>
       <c r="E66" s="50" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="F66" s="50" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="G66" s="50"/>
       <c r="H66" s="50" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
@@ -17349,11 +17343,11 @@
         <v>13</v>
       </c>
       <c r="F67" s="50" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="G67" s="50"/>
       <c r="H67" s="50" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -17373,11 +17367,11 @@
         <v>13</v>
       </c>
       <c r="F68" s="50" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="G68" s="50"/>
       <c r="H68" s="50" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="50" x14ac:dyDescent="0.35">
@@ -17394,14 +17388,14 @@
         <v>13</v>
       </c>
       <c r="E69" s="50" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="F69" s="50" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="G69" s="50"/>
       <c r="H69" s="50" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="75" x14ac:dyDescent="0.35">
@@ -17418,14 +17412,14 @@
         <v>13</v>
       </c>
       <c r="E70" s="50" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="F70" s="50" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="G70" s="50"/>
       <c r="H70" s="50" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="25" x14ac:dyDescent="0.35">
@@ -17442,16 +17436,16 @@
         <v>13</v>
       </c>
       <c r="E71" s="50" t="s">
+        <v>1198</v>
+      </c>
+      <c r="F71" s="50" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G71" s="50" t="s">
         <v>1200</v>
       </c>
-      <c r="F71" s="50" t="s">
+      <c r="H71" s="50" t="s">
         <v>1201</v>
-      </c>
-      <c r="G71" s="50" t="s">
-        <v>1202</v>
-      </c>
-      <c r="H71" s="50" t="s">
-        <v>1203</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="50" x14ac:dyDescent="0.35">
@@ -17468,14 +17462,14 @@
         <v>13</v>
       </c>
       <c r="E72" s="50" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="F72" s="50" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="G72" s="50"/>
       <c r="H72" s="50" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
@@ -17495,11 +17489,11 @@
         <v>13</v>
       </c>
       <c r="F73" s="50" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="G73" s="50"/>
       <c r="H73" s="50" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
@@ -17519,7 +17513,7 @@
         <v>266</v>
       </c>
       <c r="F74" s="50" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="G74" s="50"/>
       <c r="H74" s="50" t="s">
@@ -17543,24 +17537,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17782,33 +17758,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17826,4 +17794,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
conditionTarget Fix - QC from Dave
Update relationship name
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32A1BE1-BD6A-4EE7-8201-A4DD9FCF52C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E500421-736D-4283-9A6D-3A48CFDF9E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2470" yWindow="470" windowWidth="16590" windowHeight="9280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="200" yWindow="40" windowWidth="18210" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3209" uniqueCount="1249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3209" uniqueCount="1250">
   <si>
     <t>Preferred Term</t>
   </si>
@@ -3807,6 +3807,9 @@
   </si>
   <si>
     <t>C202579</t>
+  </si>
+  <si>
+    <t>conditionTarget</t>
   </si>
 </sst>
 </file>
@@ -4283,6 +4286,9 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -4297,9 +4303,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5158,7 +5161,7 @@
       </c>
       <c r="K19" s="24"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A20" s="24">
         <v>19</v>
       </c>
@@ -12894,7 +12897,7 @@
       </c>
       <c r="K299" s="24"/>
     </row>
-    <row r="300" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A300" s="24">
         <v>299</v>
       </c>
@@ -16205,7 +16208,7 @@
       <c r="G415" s="1" t="s">
         <v>1202</v>
       </c>
-      <c r="H415" s="76"/>
+      <c r="H415" s="71"/>
       <c r="I415" s="41" t="s">
         <v>1203</v>
       </c>
@@ -16342,7 +16345,7 @@
       </c>
       <c r="D420" s="24"/>
       <c r="E420" s="64" t="s">
-        <v>1087</v>
+        <v>1249</v>
       </c>
       <c r="F420" s="24"/>
       <c r="G420" s="24"/>
@@ -16405,14 +16408,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="72" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
       <c r="I1" s="5"/>
@@ -16422,16 +16425,16 @@
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="74" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
@@ -16439,11 +16442,11 @@
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="72" t="s">
         <v>167</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
       <c r="D3" s="23"/>
       <c r="E3" s="17"/>
       <c r="F3" s="16"/>
@@ -16466,10 +16469,10 @@
       <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:13" s="6" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="B5" s="75"/>
+      <c r="B5" s="76"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
       <c r="E5" s="17"/>
@@ -18175,12 +18178,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18406,18 +18409,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18443,19 +18456,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
remove Criteria relationships from StudyVersion
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6EF849-712A-4495-BB1E-94CF3131766D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838EF15D-70E0-4E2D-8A1D-45FF69673D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="300" windowWidth="18020" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1720" yWindow="1570" windowWidth="17480" windowHeight="9230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
     <sheet name="DDF valid value sets" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DDF Entities&amp;Attributes'!$A$1:$K$449</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DDF Entities&amp;Attributes'!$A$1:$K$448</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DDF valid value sets'!$A$6:$M$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3486" uniqueCount="1404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3481" uniqueCount="1403">
   <si>
     <t>Preferred Term</t>
   </si>
@@ -4208,9 +4208,6 @@
   </si>
   <si>
     <t>A symbol or combination of symbols which is assigned to the comment annotation.</t>
-  </si>
-  <si>
-    <t>A USDM relationship between the StudyVersion and EligibilityCriterion classes which identifies the set of eligibility criteria associated with the study version.</t>
   </si>
   <si>
     <t>notes</t>
@@ -5123,11 +5120,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K449"/>
+  <dimension ref="A1:K448"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F344" sqref="F344"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
@@ -6209,13 +6206,13 @@
       </c>
       <c r="D40" s="41"/>
       <c r="E40" s="64" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F40" s="47"/>
       <c r="G40" s="41"/>
       <c r="H40" s="47"/>
       <c r="I40" s="3" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="J40" s="3" t="s">
         <v>450</v>
@@ -6714,13 +6711,13 @@
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="31" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F57" s="47"/>
       <c r="G57" s="46"/>
       <c r="H57" s="46"/>
       <c r="I57" s="3" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="J57" s="3" t="s">
         <v>450</v>
@@ -7072,13 +7069,13 @@
         <v>968</v>
       </c>
       <c r="E69" s="42" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F69" s="47"/>
       <c r="G69" s="46"/>
       <c r="H69" s="46"/>
       <c r="I69" s="3" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="J69" s="3" t="s">
         <v>450</v>
@@ -7335,13 +7332,13 @@
         <v>526</v>
       </c>
       <c r="E78" s="31" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F78" s="47"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
       <c r="I78" s="3" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="J78" s="3" t="s">
         <v>450</v>
@@ -7602,13 +7599,13 @@
         <v>526</v>
       </c>
       <c r="E87" s="31" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F87" s="47"/>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
       <c r="I87" s="3" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="J87" s="3" t="s">
         <v>450</v>
@@ -7963,13 +7960,13 @@
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="31" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F100" s="47"/>
       <c r="G100" s="46"/>
       <c r="H100" s="46"/>
       <c r="I100" s="3" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="J100" s="3" t="s">
         <v>450</v>
@@ -8185,13 +8182,13 @@
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="31" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F108" s="47"/>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
       <c r="I108" s="3" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="J108" s="3" t="s">
         <v>450</v>
@@ -8314,13 +8311,13 @@
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="31" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F113" s="47"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
       <c r="I113" s="3" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="J113" s="3" t="s">
         <v>450</v>
@@ -8836,7 +8833,7 @@
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
       <c r="I131" s="1" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J131" s="1" t="s">
         <v>450</v>
@@ -8905,13 +8902,13 @@
       </c>
       <c r="D134" s="1"/>
       <c r="E134" s="31" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F134" s="47"/>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
       <c r="I134" s="3" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="J134" s="3" t="s">
         <v>450</v>
@@ -9115,7 +9112,7 @@
       <c r="G142" s="41"/>
       <c r="H142" s="41"/>
       <c r="I142" s="1" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="J142" s="1" t="s">
         <v>450</v>
@@ -9134,13 +9131,13 @@
       </c>
       <c r="D143" s="41"/>
       <c r="E143" s="31" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F143" s="47"/>
       <c r="G143" s="41"/>
       <c r="H143" s="41"/>
       <c r="I143" s="3" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="J143" s="3" t="s">
         <v>84</v>
@@ -9445,13 +9442,13 @@
       </c>
       <c r="D154" s="1"/>
       <c r="E154" s="34" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F154" s="47"/>
       <c r="G154" s="46"/>
       <c r="H154" s="46"/>
       <c r="I154" s="3" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="J154" s="3" t="s">
         <v>450</v>
@@ -9530,7 +9527,7 @@
       <c r="G157" s="1"/>
       <c r="H157" s="1"/>
       <c r="I157" s="1" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="J157" s="1" t="s">
         <v>450</v>
@@ -9599,13 +9596,13 @@
       </c>
       <c r="D160" s="1"/>
       <c r="E160" s="31" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F160" s="47"/>
       <c r="G160" s="1"/>
       <c r="H160" s="1"/>
       <c r="I160" s="3" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="J160" s="3" t="s">
         <v>450</v>
@@ -9885,13 +9882,13 @@
       </c>
       <c r="D170" s="1"/>
       <c r="E170" s="31" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F170" s="47"/>
       <c r="G170" s="46"/>
       <c r="H170" s="46"/>
       <c r="I170" s="3" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="J170" s="3" t="s">
         <v>450</v>
@@ -10055,13 +10052,13 @@
       </c>
       <c r="D176" s="1"/>
       <c r="E176" s="31" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F176" s="47"/>
       <c r="G176" s="46"/>
       <c r="H176" s="46"/>
       <c r="I176" s="3" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="J176" s="3" t="s">
         <v>450</v>
@@ -10590,13 +10587,13 @@
       </c>
       <c r="D195" s="24"/>
       <c r="E195" s="34" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F195" s="47"/>
       <c r="G195" s="24"/>
       <c r="H195" s="24"/>
       <c r="I195" s="3" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="J195" s="3" t="s">
         <v>450</v>
@@ -10814,13 +10811,13 @@
       </c>
       <c r="D203" s="24"/>
       <c r="E203" s="34" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F203" s="47"/>
       <c r="G203" s="24"/>
       <c r="H203" s="24"/>
       <c r="I203" s="3" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="J203" s="3" t="s">
         <v>450</v>
@@ -11106,11 +11103,11 @@
         <v>13</v>
       </c>
       <c r="G213" s="3" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="H213" s="55"/>
       <c r="I213" s="3" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="J213" s="3" t="s">
         <v>450</v>
@@ -11129,13 +11126,13 @@
       </c>
       <c r="D214" s="1"/>
       <c r="E214" s="34" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F214" s="47"/>
       <c r="G214" s="3"/>
       <c r="H214" s="3"/>
       <c r="I214" s="3" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="J214" s="3" t="s">
         <v>450</v>
@@ -11349,13 +11346,13 @@
       </c>
       <c r="D222" s="24"/>
       <c r="E222" s="34" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F222" s="47"/>
       <c r="G222" s="24"/>
       <c r="H222" s="24"/>
       <c r="I222" s="3" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="J222" s="3" t="s">
         <v>450</v>
@@ -13199,13 +13196,13 @@
       </c>
       <c r="D288" s="46"/>
       <c r="E288" s="48" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F288" s="47"/>
       <c r="G288" s="3"/>
       <c r="H288" s="46"/>
       <c r="I288" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J288" s="3" t="s">
         <v>450</v>
@@ -13659,13 +13656,13 @@
         <v>526</v>
       </c>
       <c r="E304" s="42" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F304" s="47"/>
       <c r="G304" s="24"/>
       <c r="H304" s="24"/>
       <c r="I304" s="3" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="J304" s="3" t="s">
         <v>450</v>
@@ -14665,45 +14662,49 @@
       </c>
       <c r="D340" s="3"/>
       <c r="E340" s="34" t="s">
-        <v>941</v>
+        <v>1370</v>
       </c>
       <c r="F340" s="41"/>
       <c r="G340" s="46"/>
       <c r="H340" s="46"/>
       <c r="I340" s="3" t="s">
-        <v>1370</v>
+        <v>1396</v>
       </c>
       <c r="J340" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K340" s="24"/>
     </row>
-    <row r="341" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A341" s="24">
         <v>340</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="C341" s="3" t="s">
-        <v>216</v>
+        <v>4</v>
       </c>
       <c r="D341" s="3"/>
-      <c r="E341" s="34" t="s">
-        <v>1371</v>
-      </c>
-      <c r="F341" s="47"/>
-      <c r="G341" s="46"/>
-      <c r="H341" s="46"/>
-      <c r="I341" s="3" t="s">
-        <v>1397</v>
+      <c r="E341" s="53" t="s">
+        <v>679</v>
+      </c>
+      <c r="F341" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G341" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="H341" s="1"/>
+      <c r="I341" s="1" t="s">
+        <v>681</v>
       </c>
       <c r="J341" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K341" s="24"/>
     </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A342" s="24">
         <v>341</v>
       </c>
@@ -14711,28 +14712,28 @@
         <v>679</v>
       </c>
       <c r="C342" s="3" t="s">
-        <v>4</v>
+        <v>1009</v>
       </c>
       <c r="D342" s="3"/>
-      <c r="E342" s="53" t="s">
-        <v>679</v>
-      </c>
-      <c r="F342" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="G342" s="1" t="s">
-        <v>680</v>
-      </c>
-      <c r="H342" s="1"/>
-      <c r="I342" s="1" t="s">
-        <v>681</v>
+      <c r="E342" s="21" t="s">
+        <v>523</v>
+      </c>
+      <c r="F342" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G342" s="46" t="s">
+        <v>682</v>
+      </c>
+      <c r="H342" s="46"/>
+      <c r="I342" s="46" t="s">
+        <v>683</v>
       </c>
       <c r="J342" s="3" t="s">
-        <v>450</v>
+        <v>1169</v>
       </c>
       <c r="K342" s="24"/>
     </row>
-    <row r="343" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A343" s="24">
         <v>342</v>
       </c>
@@ -14744,53 +14745,53 @@
       </c>
       <c r="D343" s="3"/>
       <c r="E343" s="21" t="s">
-        <v>523</v>
+        <v>235</v>
       </c>
       <c r="F343" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G343" s="46" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="H343" s="46"/>
-      <c r="I343" s="46" t="s">
-        <v>683</v>
+      <c r="I343" s="3" t="s">
+        <v>685</v>
       </c>
       <c r="J343" s="3" t="s">
-        <v>1169</v>
-      </c>
-      <c r="K343" s="24"/>
-    </row>
-    <row r="344" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
+        <v>1015</v>
+      </c>
+      <c r="K343" s="1" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="344" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A344" s="24">
         <v>343</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>679</v>
+        <v>686</v>
       </c>
       <c r="C344" s="3" t="s">
-        <v>1009</v>
+        <v>4</v>
       </c>
       <c r="D344" s="3"/>
-      <c r="E344" s="21" t="s">
-        <v>235</v>
+      <c r="E344" s="53" t="s">
+        <v>686</v>
       </c>
       <c r="F344" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G344" s="46" t="s">
-        <v>684</v>
+        <v>688</v>
+      </c>
+      <c r="G344" s="3" t="s">
+        <v>689</v>
       </c>
       <c r="H344" s="46"/>
       <c r="I344" s="3" t="s">
-        <v>685</v>
+        <v>690</v>
       </c>
       <c r="J344" s="3" t="s">
-        <v>1015</v>
-      </c>
-      <c r="K344" s="1" t="s">
-        <v>1034</v>
-      </c>
+        <v>450</v>
+      </c>
+      <c r="K344" s="24"/>
     </row>
     <row r="345" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A345" s="24">
@@ -14800,24 +14801,24 @@
         <v>686</v>
       </c>
       <c r="C345" s="3" t="s">
-        <v>4</v>
+        <v>1009</v>
       </c>
       <c r="D345" s="3"/>
-      <c r="E345" s="53" t="s">
-        <v>686</v>
+      <c r="E345" s="21" t="s">
+        <v>687</v>
       </c>
       <c r="F345" s="1" t="s">
-        <v>688</v>
+        <v>13</v>
       </c>
       <c r="G345" s="3" t="s">
-        <v>689</v>
-      </c>
-      <c r="H345" s="46"/>
+        <v>1020</v>
+      </c>
+      <c r="H345" s="3"/>
       <c r="I345" s="3" t="s">
-        <v>690</v>
+        <v>1021</v>
       </c>
       <c r="J345" s="3" t="s">
-        <v>450</v>
+        <v>84</v>
       </c>
       <c r="K345" s="24"/>
     </row>
@@ -14831,21 +14832,23 @@
       <c r="C346" s="3" t="s">
         <v>1009</v>
       </c>
-      <c r="D346" s="3"/>
+      <c r="D346" s="3" t="s">
+        <v>679</v>
+      </c>
       <c r="E346" s="21" t="s">
-        <v>687</v>
+        <v>523</v>
       </c>
       <c r="F346" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G346" s="3" t="s">
-        <v>1020</v>
-      </c>
-      <c r="H346" s="3"/>
-      <c r="I346" s="3" t="s">
-        <v>1021</v>
-      </c>
-      <c r="J346" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="H346" s="55"/>
+      <c r="I346" s="46" t="s">
+        <v>890</v>
+      </c>
+      <c r="J346" s="46" t="s">
         <v>84</v>
       </c>
       <c r="K346" s="24"/>
@@ -14864,55 +14867,55 @@
         <v>679</v>
       </c>
       <c r="E347" s="21" t="s">
-        <v>523</v>
+        <v>235</v>
       </c>
       <c r="F347" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G347" s="3" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="H347" s="55"/>
-      <c r="I347" s="46" t="s">
-        <v>890</v>
+      <c r="I347" s="3" t="s">
+        <v>892</v>
       </c>
       <c r="J347" s="46" t="s">
         <v>84</v>
       </c>
       <c r="K347" s="24"/>
     </row>
-    <row r="348" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A348" s="24">
         <v>347</v>
       </c>
-      <c r="B348" s="1" t="s">
-        <v>686</v>
+      <c r="B348" s="24" t="s">
+        <v>760</v>
       </c>
       <c r="C348" s="3" t="s">
-        <v>1009</v>
-      </c>
-      <c r="D348" s="3" t="s">
-        <v>679</v>
-      </c>
-      <c r="E348" s="21" t="s">
-        <v>235</v>
+        <v>4</v>
+      </c>
+      <c r="D348" s="3"/>
+      <c r="E348" s="53" t="s">
+        <v>760</v>
       </c>
       <c r="F348" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G348" s="3" t="s">
-        <v>891</v>
-      </c>
-      <c r="H348" s="55"/>
-      <c r="I348" s="3" t="s">
-        <v>892</v>
-      </c>
-      <c r="J348" s="46" t="s">
-        <v>84</v>
+      <c r="G348" s="24" t="s">
+        <v>761</v>
+      </c>
+      <c r="H348" s="3" t="s">
+        <v>762</v>
+      </c>
+      <c r="I348" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="J348" s="3" t="s">
+        <v>450</v>
       </c>
       <c r="K348" s="24"/>
     </row>
-    <row r="349" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A349" s="24">
         <v>348</v>
       </c>
@@ -14920,30 +14923,28 @@
         <v>760</v>
       </c>
       <c r="C349" s="3" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="D349" s="3"/>
-      <c r="E349" s="53" t="s">
-        <v>760</v>
+      <c r="E349" s="22" t="s">
+        <v>487</v>
       </c>
       <c r="F349" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G349" s="24" t="s">
-        <v>761</v>
-      </c>
-      <c r="H349" s="3" t="s">
-        <v>762</v>
-      </c>
-      <c r="I349" s="1" t="s">
-        <v>763</v>
-      </c>
-      <c r="J349" s="3" t="s">
-        <v>450</v>
+        <v>764</v>
+      </c>
+      <c r="H349" s="24"/>
+      <c r="I349" s="24" t="s">
+        <v>766</v>
+      </c>
+      <c r="J349" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="K349" s="24"/>
     </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A350" s="24">
         <v>349</v>
       </c>
@@ -14951,28 +14952,28 @@
         <v>760</v>
       </c>
       <c r="C350" s="3" t="s">
-        <v>85</v>
+        <v>1009</v>
       </c>
       <c r="D350" s="3"/>
       <c r="E350" s="22" t="s">
-        <v>487</v>
+        <v>211</v>
       </c>
       <c r="F350" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G350" s="24" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="H350" s="24"/>
       <c r="I350" s="24" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="J350" s="1" t="s">
-        <v>84</v>
+        <v>896</v>
       </c>
       <c r="K350" s="24"/>
     </row>
-    <row r="351" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A351" s="24">
         <v>350</v>
       </c>
@@ -14980,28 +14981,28 @@
         <v>760</v>
       </c>
       <c r="C351" s="3" t="s">
-        <v>1009</v>
+        <v>85</v>
       </c>
       <c r="D351" s="3"/>
-      <c r="E351" s="22" t="s">
-        <v>211</v>
+      <c r="E351" s="21" t="s">
+        <v>486</v>
       </c>
       <c r="F351" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G351" s="24" t="s">
-        <v>765</v>
-      </c>
-      <c r="H351" s="24"/>
-      <c r="I351" s="24" t="s">
-        <v>767</v>
-      </c>
-      <c r="J351" s="1" t="s">
-        <v>896</v>
+      <c r="G351" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="H351" s="55"/>
+      <c r="I351" s="3" t="s">
+        <v>846</v>
+      </c>
+      <c r="J351" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="K351" s="24"/>
     </row>
-    <row r="352" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A352" s="24">
         <v>351</v>
       </c>
@@ -15013,24 +15014,24 @@
       </c>
       <c r="D352" s="3"/>
       <c r="E352" s="21" t="s">
-        <v>486</v>
+        <v>521</v>
       </c>
       <c r="F352" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G352" s="1" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="H352" s="55"/>
       <c r="I352" s="3" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="J352" s="3" t="s">
         <v>84</v>
       </c>
       <c r="K352" s="24"/>
     </row>
-    <row r="353" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A353" s="24">
         <v>352</v>
       </c>
@@ -15038,28 +15039,30 @@
         <v>760</v>
       </c>
       <c r="C353" s="3" t="s">
-        <v>85</v>
+        <v>1009</v>
       </c>
       <c r="D353" s="3"/>
       <c r="E353" s="21" t="s">
-        <v>521</v>
+        <v>862</v>
       </c>
       <c r="F353" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G353" s="1" t="s">
-        <v>847</v>
-      </c>
-      <c r="H353" s="55"/>
-      <c r="I353" s="3" t="s">
-        <v>848</v>
+        <v>849</v>
+      </c>
+      <c r="H353" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="I353" s="1" t="s">
+        <v>851</v>
       </c>
       <c r="J353" s="3" t="s">
-        <v>84</v>
+        <v>1098</v>
       </c>
       <c r="K353" s="24"/>
     </row>
-    <row r="354" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:11" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A354" s="24">
         <v>353</v>
       </c>
@@ -15071,26 +15074,28 @@
       </c>
       <c r="D354" s="3"/>
       <c r="E354" s="21" t="s">
-        <v>862</v>
+        <v>523</v>
       </c>
       <c r="F354" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G354" s="1" t="s">
-        <v>849</v>
+        <v>852</v>
+      </c>
+      <c r="G354" s="3" t="s">
+        <v>853</v>
       </c>
       <c r="H354" s="3" t="s">
-        <v>850</v>
-      </c>
-      <c r="I354" s="1" t="s">
-        <v>851</v>
+        <v>854</v>
+      </c>
+      <c r="I354" s="55" t="s">
+        <v>855</v>
       </c>
       <c r="J354" s="3" t="s">
-        <v>1098</v>
-      </c>
-      <c r="K354" s="24"/>
-    </row>
-    <row r="355" spans="1:11" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>929</v>
+      </c>
+      <c r="K354" s="66" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="355" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A355" s="24">
         <v>354</v>
       </c>
@@ -15101,27 +15106,23 @@
         <v>1009</v>
       </c>
       <c r="D355" s="3"/>
-      <c r="E355" s="21" t="s">
-        <v>523</v>
+      <c r="E355" s="43" t="s">
+        <v>863</v>
       </c>
       <c r="F355" s="1" t="s">
-        <v>852</v>
+        <v>13</v>
       </c>
       <c r="G355" s="3" t="s">
-        <v>853</v>
-      </c>
-      <c r="H355" s="3" t="s">
-        <v>854</v>
-      </c>
-      <c r="I355" s="55" t="s">
-        <v>855</v>
+        <v>856</v>
+      </c>
+      <c r="H355" s="55"/>
+      <c r="I355" s="1" t="s">
+        <v>857</v>
       </c>
       <c r="J355" s="3" t="s">
-        <v>929</v>
-      </c>
-      <c r="K355" s="66" t="s">
-        <v>930</v>
-      </c>
+        <v>1099</v>
+      </c>
+      <c r="K355" s="24"/>
     </row>
     <row r="356" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A356" s="24">
@@ -15134,21 +15135,23 @@
         <v>1009</v>
       </c>
       <c r="D356" s="3"/>
-      <c r="E356" s="43" t="s">
-        <v>863</v>
+      <c r="E356" s="21" t="s">
+        <v>864</v>
       </c>
       <c r="F356" s="1" t="s">
-        <v>13</v>
+        <v>858</v>
       </c>
       <c r="G356" s="3" t="s">
-        <v>856</v>
-      </c>
-      <c r="H356" s="55"/>
-      <c r="I356" s="1" t="s">
-        <v>857</v>
+        <v>859</v>
+      </c>
+      <c r="H356" s="3" t="s">
+        <v>859</v>
+      </c>
+      <c r="I356" s="55" t="s">
+        <v>860</v>
       </c>
       <c r="J356" s="3" t="s">
-        <v>1099</v>
+        <v>861</v>
       </c>
       <c r="K356" s="24"/>
     </row>
@@ -15163,23 +15166,21 @@
         <v>1009</v>
       </c>
       <c r="D357" s="3"/>
-      <c r="E357" s="21" t="s">
-        <v>864</v>
-      </c>
-      <c r="F357" s="1" t="s">
-        <v>858</v>
+      <c r="E357" s="22" t="s">
+        <v>865</v>
+      </c>
+      <c r="F357" s="24" t="s">
+        <v>13</v>
       </c>
       <c r="G357" s="3" t="s">
-        <v>859</v>
-      </c>
-      <c r="H357" s="3" t="s">
-        <v>859</v>
-      </c>
-      <c r="I357" s="55" t="s">
-        <v>860</v>
+        <v>1027</v>
+      </c>
+      <c r="H357" s="3"/>
+      <c r="I357" s="3" t="s">
+        <v>1028</v>
       </c>
       <c r="J357" s="3" t="s">
-        <v>861</v>
+        <v>84</v>
       </c>
       <c r="K357" s="24"/>
     </row>
@@ -15191,24 +15192,20 @@
         <v>760</v>
       </c>
       <c r="C358" s="3" t="s">
-        <v>1009</v>
+        <v>216</v>
       </c>
       <c r="D358" s="3"/>
-      <c r="E358" s="22" t="s">
-        <v>865</v>
-      </c>
-      <c r="F358" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G358" s="3" t="s">
-        <v>1027</v>
-      </c>
-      <c r="H358" s="3"/>
-      <c r="I358" s="3" t="s">
-        <v>1028</v>
+      <c r="E358" s="31" t="s">
+        <v>866</v>
+      </c>
+      <c r="F358" s="1"/>
+      <c r="G358" s="55"/>
+      <c r="H358" s="55"/>
+      <c r="I358" s="1" t="s">
+        <v>1342</v>
       </c>
       <c r="J358" s="3" t="s">
-        <v>84</v>
+        <v>450</v>
       </c>
       <c r="K358" s="24"/>
     </row>
@@ -15224,45 +15221,49 @@
       </c>
       <c r="D359" s="3"/>
       <c r="E359" s="31" t="s">
-        <v>866</v>
-      </c>
-      <c r="F359" s="1"/>
+        <v>1370</v>
+      </c>
+      <c r="F359" s="47"/>
       <c r="G359" s="55"/>
       <c r="H359" s="55"/>
-      <c r="I359" s="1" t="s">
-        <v>1342</v>
+      <c r="I359" s="3" t="s">
+        <v>1395</v>
       </c>
       <c r="J359" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K359" s="24"/>
     </row>
-    <row r="360" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:11" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A360" s="24">
         <v>359</v>
       </c>
-      <c r="B360" s="24" t="s">
-        <v>760</v>
+      <c r="B360" s="1" t="s">
+        <v>796</v>
       </c>
       <c r="C360" s="3" t="s">
-        <v>216</v>
+        <v>4</v>
       </c>
       <c r="D360" s="3"/>
-      <c r="E360" s="31" t="s">
-        <v>1371</v>
-      </c>
-      <c r="F360" s="47"/>
-      <c r="G360" s="55"/>
+      <c r="E360" s="53" t="s">
+        <v>796</v>
+      </c>
+      <c r="F360" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="G360" s="3" t="s">
+        <v>806</v>
+      </c>
       <c r="H360" s="55"/>
       <c r="I360" s="3" t="s">
-        <v>1396</v>
+        <v>807</v>
       </c>
       <c r="J360" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K360" s="24"/>
     </row>
-    <row r="361" spans="1:11" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A361" s="24">
         <v>360</v>
       </c>
@@ -15270,24 +15271,24 @@
         <v>796</v>
       </c>
       <c r="C361" s="3" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="D361" s="3"/>
-      <c r="E361" s="53" t="s">
-        <v>796</v>
+      <c r="E361" s="21" t="s">
+        <v>487</v>
       </c>
       <c r="F361" s="1" t="s">
-        <v>805</v>
+        <v>13</v>
       </c>
       <c r="G361" s="3" t="s">
-        <v>806</v>
+        <v>799</v>
       </c>
       <c r="H361" s="55"/>
       <c r="I361" s="3" t="s">
-        <v>807</v>
-      </c>
-      <c r="J361" s="3" t="s">
-        <v>450</v>
+        <v>800</v>
+      </c>
+      <c r="J361" s="46" t="s">
+        <v>84</v>
       </c>
       <c r="K361" s="24"/>
     </row>
@@ -15303,17 +15304,17 @@
       </c>
       <c r="D362" s="3"/>
       <c r="E362" s="21" t="s">
-        <v>487</v>
+        <v>797</v>
       </c>
       <c r="F362" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G362" s="3" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="H362" s="55"/>
       <c r="I362" s="3" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="J362" s="46" t="s">
         <v>84</v>
@@ -15324,86 +15325,86 @@
       <c r="A363" s="24">
         <v>362</v>
       </c>
-      <c r="B363" s="1" t="s">
+      <c r="B363" s="20" t="s">
         <v>796</v>
       </c>
-      <c r="C363" s="3" t="s">
+      <c r="C363" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="D363" s="3"/>
-      <c r="E363" s="21" t="s">
-        <v>797</v>
-      </c>
-      <c r="F363" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G363" s="3" t="s">
-        <v>801</v>
-      </c>
-      <c r="H363" s="55"/>
-      <c r="I363" s="3" t="s">
-        <v>802</v>
+      <c r="D363" s="32"/>
+      <c r="E363" s="56" t="s">
+        <v>798</v>
+      </c>
+      <c r="F363" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G363" s="32" t="s">
+        <v>803</v>
+      </c>
+      <c r="H363" s="57"/>
+      <c r="I363" s="32" t="s">
+        <v>804</v>
       </c>
       <c r="J363" s="46" t="s">
         <v>84</v>
       </c>
       <c r="K363" s="24"/>
     </row>
-    <row r="364" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A364" s="24">
         <v>363</v>
       </c>
-      <c r="B364" s="20" t="s">
+      <c r="B364" s="1" t="s">
         <v>796</v>
       </c>
-      <c r="C364" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="D364" s="32"/>
-      <c r="E364" s="56" t="s">
-        <v>798</v>
-      </c>
-      <c r="F364" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G364" s="32" t="s">
-        <v>803</v>
-      </c>
-      <c r="H364" s="57"/>
-      <c r="I364" s="32" t="s">
-        <v>804</v>
-      </c>
-      <c r="J364" s="46" t="s">
+      <c r="C364" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D364" s="1"/>
+      <c r="E364" s="22" t="s">
+        <v>687</v>
+      </c>
+      <c r="F364" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G364" s="3" t="s">
+        <v>1012</v>
+      </c>
+      <c r="H364" s="3"/>
+      <c r="I364" s="3" t="s">
+        <v>1222</v>
+      </c>
+      <c r="J364" s="61" t="s">
         <v>84</v>
       </c>
       <c r="K364" s="24"/>
     </row>
-    <row r="365" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A365" s="24">
         <v>364</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>796</v>
-      </c>
-      <c r="C365" s="1" t="s">
-        <v>1009</v>
-      </c>
-      <c r="D365" s="1"/>
-      <c r="E365" s="22" t="s">
-        <v>687</v>
-      </c>
-      <c r="F365" s="24" t="s">
-        <v>13</v>
+        <v>808</v>
+      </c>
+      <c r="C365" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D365" s="3"/>
+      <c r="E365" s="53" t="s">
+        <v>808</v>
+      </c>
+      <c r="F365" s="1" t="s">
+        <v>809</v>
       </c>
       <c r="G365" s="3" t="s">
-        <v>1012</v>
-      </c>
-      <c r="H365" s="3"/>
+        <v>810</v>
+      </c>
+      <c r="H365" s="55"/>
       <c r="I365" s="3" t="s">
-        <v>1222</v>
-      </c>
-      <c r="J365" s="61" t="s">
-        <v>84</v>
+        <v>811</v>
+      </c>
+      <c r="J365" s="3" t="s">
+        <v>450</v>
       </c>
       <c r="K365" s="24"/>
     </row>
@@ -15415,24 +15416,24 @@
         <v>808</v>
       </c>
       <c r="C366" s="3" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="D366" s="3"/>
-      <c r="E366" s="53" t="s">
-        <v>808</v>
+      <c r="E366" s="21" t="s">
+        <v>486</v>
       </c>
       <c r="F366" s="1" t="s">
-        <v>809</v>
+        <v>13</v>
       </c>
       <c r="G366" s="3" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="H366" s="55"/>
       <c r="I366" s="3" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="J366" s="3" t="s">
-        <v>450</v>
+        <v>84</v>
       </c>
       <c r="K366" s="24"/>
     </row>
@@ -15448,24 +15449,24 @@
       </c>
       <c r="D367" s="3"/>
       <c r="E367" s="21" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="F367" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G367" s="3" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="H367" s="55"/>
       <c r="I367" s="3" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="J367" s="3" t="s">
         <v>84</v>
       </c>
       <c r="K367" s="24"/>
     </row>
-    <row r="368" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A368" s="24">
         <v>367</v>
       </c>
@@ -15477,24 +15478,24 @@
       </c>
       <c r="D368" s="3"/>
       <c r="E368" s="21" t="s">
-        <v>487</v>
+        <v>521</v>
       </c>
       <c r="F368" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G368" s="3" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="H368" s="55"/>
       <c r="I368" s="3" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="J368" s="3" t="s">
         <v>84</v>
       </c>
       <c r="K368" s="24"/>
     </row>
-    <row r="369" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:11" ht="50" x14ac:dyDescent="0.35">
       <c r="A369" s="24">
         <v>368</v>
       </c>
@@ -15502,28 +15503,32 @@
         <v>808</v>
       </c>
       <c r="C369" s="3" t="s">
-        <v>85</v>
+        <v>1009</v>
       </c>
       <c r="D369" s="3"/>
       <c r="E369" s="21" t="s">
-        <v>521</v>
+        <v>824</v>
       </c>
       <c r="F369" s="1" t="s">
-        <v>13</v>
+        <v>818</v>
       </c>
       <c r="G369" s="3" t="s">
-        <v>816</v>
-      </c>
-      <c r="H369" s="55"/>
-      <c r="I369" s="3" t="s">
-        <v>817</v>
+        <v>819</v>
+      </c>
+      <c r="H369" s="3" t="s">
+        <v>819</v>
+      </c>
+      <c r="I369" s="55" t="s">
+        <v>820</v>
       </c>
       <c r="J369" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K369" s="24"/>
-    </row>
-    <row r="370" spans="1:11" ht="50" x14ac:dyDescent="0.35">
+        <v>931</v>
+      </c>
+      <c r="K369" s="67" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="370" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A370" s="24">
         <v>369</v>
       </c>
@@ -15535,61 +15540,57 @@
       </c>
       <c r="D370" s="3"/>
       <c r="E370" s="21" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="F370" s="1" t="s">
-        <v>818</v>
+        <v>821</v>
       </c>
       <c r="G370" s="3" t="s">
-        <v>819</v>
+        <v>822</v>
       </c>
       <c r="H370" s="3" t="s">
-        <v>819</v>
+        <v>822</v>
       </c>
       <c r="I370" s="55" t="s">
-        <v>820</v>
+        <v>823</v>
       </c>
       <c r="J370" s="3" t="s">
-        <v>931</v>
-      </c>
-      <c r="K370" s="67" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="371" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>933</v>
+      </c>
+      <c r="K370" s="3" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="371" spans="1:11" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A371" s="24">
         <v>370</v>
       </c>
       <c r="B371" s="1" t="s">
         <v>808</v>
       </c>
-      <c r="C371" s="3" t="s">
+      <c r="C371" s="1" t="s">
         <v>1009</v>
       </c>
-      <c r="D371" s="3"/>
-      <c r="E371" s="21" t="s">
-        <v>825</v>
-      </c>
-      <c r="F371" s="1" t="s">
-        <v>821</v>
+      <c r="D371" s="1"/>
+      <c r="E371" s="22" t="s">
+        <v>827</v>
+      </c>
+      <c r="F371" s="24" t="s">
+        <v>13</v>
       </c>
       <c r="G371" s="3" t="s">
-        <v>822</v>
-      </c>
-      <c r="H371" s="3" t="s">
-        <v>822</v>
-      </c>
-      <c r="I371" s="55" t="s">
-        <v>823</v>
+        <v>1013</v>
+      </c>
+      <c r="H371" s="3"/>
+      <c r="I371" s="3" t="s">
+        <v>1014</v>
       </c>
       <c r="J371" s="3" t="s">
-        <v>933</v>
-      </c>
-      <c r="K371" s="3" t="s">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="372" spans="1:11" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+      <c r="K371" s="3"/>
+    </row>
+    <row r="372" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A372" s="24">
         <v>371</v>
       </c>
@@ -15597,24 +15598,20 @@
         <v>808</v>
       </c>
       <c r="C372" s="1" t="s">
-        <v>1009</v>
+        <v>216</v>
       </c>
       <c r="D372" s="1"/>
-      <c r="E372" s="22" t="s">
-        <v>827</v>
-      </c>
-      <c r="F372" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G372" s="3" t="s">
-        <v>1013</v>
-      </c>
+      <c r="E372" s="31" t="s">
+        <v>826</v>
+      </c>
+      <c r="F372" s="1"/>
+      <c r="G372" s="3"/>
       <c r="H372" s="3"/>
-      <c r="I372" s="3" t="s">
-        <v>1014</v>
+      <c r="I372" s="1" t="s">
+        <v>1343</v>
       </c>
       <c r="J372" s="3" t="s">
-        <v>84</v>
+        <v>450</v>
       </c>
       <c r="K372" s="3"/>
     </row>
@@ -15630,45 +15627,49 @@
       </c>
       <c r="D373" s="1"/>
       <c r="E373" s="31" t="s">
-        <v>826</v>
-      </c>
-      <c r="F373" s="1"/>
+        <v>1370</v>
+      </c>
+      <c r="F373" s="47"/>
       <c r="G373" s="3"/>
       <c r="H373" s="3"/>
-      <c r="I373" s="1" t="s">
-        <v>1343</v>
+      <c r="I373" s="3" t="s">
+        <v>1372</v>
       </c>
       <c r="J373" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K373" s="3"/>
     </row>
-    <row r="374" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A374" s="24">
         <v>373</v>
       </c>
-      <c r="B374" s="1" t="s">
-        <v>808</v>
-      </c>
-      <c r="C374" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D374" s="1"/>
-      <c r="E374" s="31" t="s">
-        <v>1371</v>
-      </c>
-      <c r="F374" s="47"/>
-      <c r="G374" s="3"/>
-      <c r="H374" s="3"/>
+      <c r="B374" s="3" t="s">
+        <v>876</v>
+      </c>
+      <c r="C374" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D374" s="3"/>
+      <c r="E374" s="53" t="s">
+        <v>876</v>
+      </c>
+      <c r="F374" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="G374" s="3" t="s">
+        <v>876</v>
+      </c>
+      <c r="H374" s="55"/>
       <c r="I374" s="3" t="s">
-        <v>1373</v>
+        <v>885</v>
       </c>
       <c r="J374" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="K374" s="3"/>
-    </row>
-    <row r="375" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+      <c r="K374" s="24"/>
+    </row>
+    <row r="375" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A375" s="24">
         <v>374</v>
       </c>
@@ -15676,28 +15677,28 @@
         <v>876</v>
       </c>
       <c r="C375" s="3" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="D375" s="3"/>
-      <c r="E375" s="53" t="s">
-        <v>876</v>
+      <c r="E375" s="21" t="s">
+        <v>792</v>
       </c>
       <c r="F375" s="1" t="s">
-        <v>884</v>
+        <v>878</v>
       </c>
       <c r="G375" s="3" t="s">
-        <v>876</v>
+        <v>879</v>
       </c>
       <c r="H375" s="55"/>
       <c r="I375" s="3" t="s">
-        <v>885</v>
-      </c>
-      <c r="J375" s="3" t="s">
-        <v>450</v>
+        <v>880</v>
+      </c>
+      <c r="J375" s="46" t="s">
+        <v>84</v>
       </c>
       <c r="K375" s="24"/>
     </row>
-    <row r="376" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:11" ht="50" x14ac:dyDescent="0.35">
       <c r="A376" s="24">
         <v>375</v>
       </c>
@@ -15705,84 +15706,86 @@
         <v>876</v>
       </c>
       <c r="C376" s="3" t="s">
-        <v>85</v>
+        <v>1009</v>
       </c>
       <c r="D376" s="3"/>
       <c r="E376" s="21" t="s">
-        <v>792</v>
+        <v>877</v>
       </c>
       <c r="F376" s="1" t="s">
-        <v>878</v>
+        <v>881</v>
       </c>
       <c r="G376" s="3" t="s">
-        <v>879</v>
+        <v>882</v>
       </c>
       <c r="H376" s="55"/>
       <c r="I376" s="3" t="s">
-        <v>880</v>
-      </c>
-      <c r="J376" s="46" t="s">
-        <v>84</v>
-      </c>
-      <c r="K376" s="24"/>
+        <v>883</v>
+      </c>
+      <c r="J376" s="3" t="s">
+        <v>935</v>
+      </c>
+      <c r="K376" s="3" t="s">
+        <v>936</v>
+      </c>
     </row>
     <row r="377" spans="1:11" ht="50" x14ac:dyDescent="0.35">
       <c r="A377" s="24">
         <v>376</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>876</v>
+        <v>947</v>
       </c>
       <c r="C377" s="3" t="s">
-        <v>1009</v>
+        <v>4</v>
       </c>
       <c r="D377" s="3"/>
-      <c r="E377" s="21" t="s">
-        <v>877</v>
-      </c>
-      <c r="F377" s="1" t="s">
-        <v>881</v>
+      <c r="E377" s="53" t="s">
+        <v>947</v>
+      </c>
+      <c r="F377" s="3" t="s">
+        <v>944</v>
       </c>
       <c r="G377" s="3" t="s">
-        <v>882</v>
+        <v>945</v>
       </c>
       <c r="H377" s="55"/>
       <c r="I377" s="3" t="s">
-        <v>883</v>
+        <v>946</v>
       </c>
       <c r="J377" s="3" t="s">
-        <v>935</v>
-      </c>
-      <c r="K377" s="3" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="378" spans="1:11" ht="50" x14ac:dyDescent="0.35">
+        <v>450</v>
+      </c>
+      <c r="K377" s="1"/>
+    </row>
+    <row r="378" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A378" s="24">
         <v>377</v>
       </c>
-      <c r="B378" s="3" t="s">
+      <c r="B378" s="1" t="s">
         <v>947</v>
       </c>
       <c r="C378" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D378" s="3"/>
-      <c r="E378" s="53" t="s">
-        <v>947</v>
+        <v>85</v>
+      </c>
+      <c r="D378" s="3" t="s">
+        <v>968</v>
+      </c>
+      <c r="E378" s="43" t="s">
+        <v>486</v>
       </c>
       <c r="F378" s="3" t="s">
-        <v>944</v>
+        <v>13</v>
       </c>
       <c r="G378" s="3" t="s">
-        <v>945</v>
+        <v>951</v>
       </c>
       <c r="H378" s="55"/>
       <c r="I378" s="3" t="s">
-        <v>946</v>
+        <v>952</v>
       </c>
       <c r="J378" s="3" t="s">
-        <v>450</v>
+        <v>84</v>
       </c>
       <c r="K378" s="1"/>
     </row>
@@ -15800,17 +15803,17 @@
         <v>968</v>
       </c>
       <c r="E379" s="43" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="F379" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G379" s="3" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="H379" s="55"/>
       <c r="I379" s="3" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="J379" s="3" t="s">
         <v>84</v>
@@ -15831,24 +15834,24 @@
         <v>968</v>
       </c>
       <c r="E380" s="43" t="s">
-        <v>487</v>
+        <v>521</v>
       </c>
       <c r="F380" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G380" s="3" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="H380" s="55"/>
       <c r="I380" s="3" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="J380" s="3" t="s">
         <v>84</v>
       </c>
       <c r="K380" s="1"/>
     </row>
-    <row r="381" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A381" s="24">
         <v>380</v>
       </c>
@@ -15856,23 +15859,23 @@
         <v>947</v>
       </c>
       <c r="C381" s="3" t="s">
-        <v>85</v>
+        <v>1009</v>
       </c>
       <c r="D381" s="3" t="s">
         <v>968</v>
       </c>
-      <c r="E381" s="43" t="s">
-        <v>521</v>
-      </c>
-      <c r="F381" s="3" t="s">
+      <c r="E381" s="21" t="s">
+        <v>939</v>
+      </c>
+      <c r="F381" s="24" t="s">
         <v>13</v>
       </c>
       <c r="G381" s="3" t="s">
-        <v>955</v>
-      </c>
-      <c r="H381" s="55"/>
+        <v>1029</v>
+      </c>
+      <c r="H381" s="3"/>
       <c r="I381" s="3" t="s">
-        <v>956</v>
+        <v>1030</v>
       </c>
       <c r="J381" s="3" t="s">
         <v>84</v>
@@ -15893,24 +15896,24 @@
         <v>968</v>
       </c>
       <c r="E382" s="21" t="s">
-        <v>939</v>
+        <v>949</v>
       </c>
       <c r="F382" s="24" t="s">
         <v>13</v>
       </c>
       <c r="G382" s="3" t="s">
-        <v>1029</v>
+        <v>1238</v>
       </c>
       <c r="H382" s="3"/>
       <c r="I382" s="3" t="s">
-        <v>1030</v>
+        <v>1239</v>
       </c>
       <c r="J382" s="3" t="s">
         <v>84</v>
       </c>
       <c r="K382" s="1"/>
     </row>
-    <row r="383" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:11" ht="50" x14ac:dyDescent="0.35">
       <c r="A383" s="24">
         <v>382</v>
       </c>
@@ -15924,24 +15927,26 @@
         <v>968</v>
       </c>
       <c r="E383" s="21" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="F383" s="24" t="s">
         <v>13</v>
       </c>
       <c r="G383" s="3" t="s">
-        <v>1238</v>
+        <v>1240</v>
       </c>
       <c r="H383" s="3"/>
       <c r="I383" s="3" t="s">
-        <v>1239</v>
+        <v>1241</v>
       </c>
       <c r="J383" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K383" s="1"/>
-    </row>
-    <row r="384" spans="1:11" ht="50" x14ac:dyDescent="0.35">
+        <v>907</v>
+      </c>
+      <c r="K383" s="68" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="384" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A384" s="24">
         <v>383</v>
       </c>
@@ -15954,25 +15959,23 @@
       <c r="D384" s="3" t="s">
         <v>968</v>
       </c>
-      <c r="E384" s="21" t="s">
-        <v>950</v>
-      </c>
-      <c r="F384" s="24" t="s">
+      <c r="E384" s="43" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F384" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G384" s="3" t="s">
-        <v>1240</v>
+        <v>1031</v>
       </c>
       <c r="H384" s="3"/>
       <c r="I384" s="3" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="J384" s="3" t="s">
-        <v>907</v>
-      </c>
-      <c r="K384" s="68" t="s">
-        <v>908</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="K384" s="1"/>
     </row>
     <row r="385" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A385" s="24">
@@ -15982,25 +15985,25 @@
         <v>947</v>
       </c>
       <c r="C385" s="3" t="s">
-        <v>1009</v>
+        <v>85</v>
       </c>
       <c r="D385" s="3" t="s">
         <v>968</v>
       </c>
       <c r="E385" s="43" t="s">
-        <v>1008</v>
-      </c>
-      <c r="F385" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G385" s="3" t="s">
-        <v>1031</v>
-      </c>
-      <c r="H385" s="3"/>
+        <v>1036</v>
+      </c>
+      <c r="F385" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="G385" s="46" t="s">
+        <v>1037</v>
+      </c>
+      <c r="H385" s="46"/>
       <c r="I385" s="3" t="s">
-        <v>1242</v>
-      </c>
-      <c r="J385" s="3" t="s">
+        <v>1038</v>
+      </c>
+      <c r="J385" s="46" t="s">
         <v>84</v>
       </c>
       <c r="K385" s="1"/>
@@ -16013,26 +16016,22 @@
         <v>947</v>
       </c>
       <c r="C386" s="3" t="s">
-        <v>85</v>
+        <v>216</v>
       </c>
       <c r="D386" s="3" t="s">
         <v>968</v>
       </c>
-      <c r="E386" s="43" t="s">
-        <v>1036</v>
-      </c>
-      <c r="F386" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="G386" s="46" t="s">
-        <v>1037</v>
-      </c>
-      <c r="H386" s="46"/>
-      <c r="I386" s="3" t="s">
-        <v>1038</v>
-      </c>
-      <c r="J386" s="46" t="s">
-        <v>84</v>
+      <c r="E386" s="42" t="s">
+        <v>941</v>
+      </c>
+      <c r="F386" s="55"/>
+      <c r="G386" s="55"/>
+      <c r="H386" s="55"/>
+      <c r="I386" s="1" t="s">
+        <v>1344</v>
+      </c>
+      <c r="J386" s="3" t="s">
+        <v>450</v>
       </c>
       <c r="K386" s="1"/>
     </row>
@@ -16046,17 +16045,15 @@
       <c r="C387" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D387" s="3" t="s">
-        <v>968</v>
-      </c>
+      <c r="D387" s="3"/>
       <c r="E387" s="42" t="s">
-        <v>941</v>
+        <v>948</v>
       </c>
       <c r="F387" s="55"/>
       <c r="G387" s="55"/>
       <c r="H387" s="55"/>
       <c r="I387" s="1" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="J387" s="3" t="s">
         <v>450</v>
@@ -16073,49 +16070,53 @@
       <c r="C388" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D388" s="3"/>
+      <c r="D388" s="3" t="s">
+        <v>968</v>
+      </c>
       <c r="E388" s="42" t="s">
-        <v>948</v>
-      </c>
-      <c r="F388" s="55"/>
+        <v>1370</v>
+      </c>
+      <c r="F388" s="47"/>
       <c r="G388" s="55"/>
       <c r="H388" s="55"/>
-      <c r="I388" s="1" t="s">
-        <v>1345</v>
+      <c r="I388" s="3" t="s">
+        <v>1390</v>
       </c>
       <c r="J388" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K388" s="1"/>
     </row>
-    <row r="389" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A389" s="24">
         <v>388</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>947</v>
+        <v>957</v>
       </c>
       <c r="C389" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D389" s="3" t="s">
-        <v>968</v>
-      </c>
-      <c r="E389" s="42" t="s">
-        <v>1371</v>
-      </c>
-      <c r="F389" s="47"/>
-      <c r="G389" s="55"/>
+        <v>4</v>
+      </c>
+      <c r="D389" s="3"/>
+      <c r="E389" s="53" t="s">
+        <v>957</v>
+      </c>
+      <c r="F389" s="3" t="s">
+        <v>958</v>
+      </c>
+      <c r="G389" s="3" t="s">
+        <v>957</v>
+      </c>
       <c r="H389" s="55"/>
       <c r="I389" s="3" t="s">
-        <v>1391</v>
+        <v>959</v>
       </c>
       <c r="J389" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K389" s="1"/>
     </row>
-    <row r="390" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A390" s="24">
         <v>389</v>
       </c>
@@ -16123,28 +16124,30 @@
         <v>957</v>
       </c>
       <c r="C390" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D390" s="3"/>
-      <c r="E390" s="53" t="s">
-        <v>957</v>
+        <v>85</v>
+      </c>
+      <c r="D390" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="E390" s="43" t="s">
+        <v>486</v>
       </c>
       <c r="F390" s="3" t="s">
-        <v>958</v>
+        <v>13</v>
       </c>
       <c r="G390" s="3" t="s">
-        <v>957</v>
+        <v>960</v>
       </c>
       <c r="H390" s="55"/>
       <c r="I390" s="3" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="J390" s="3" t="s">
-        <v>450</v>
+        <v>84</v>
       </c>
       <c r="K390" s="1"/>
     </row>
-    <row r="391" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A391" s="24">
         <v>390</v>
       </c>
@@ -16158,17 +16161,17 @@
         <v>526</v>
       </c>
       <c r="E391" s="43" t="s">
-        <v>486</v>
+        <v>339</v>
       </c>
       <c r="F391" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G391" s="3" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="H391" s="55"/>
       <c r="I391" s="3" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="J391" s="3" t="s">
         <v>84</v>
@@ -16189,17 +16192,17 @@
         <v>526</v>
       </c>
       <c r="E392" s="43" t="s">
-        <v>339</v>
+        <v>487</v>
       </c>
       <c r="F392" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G392" s="3" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="H392" s="55"/>
       <c r="I392" s="3" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="J392" s="3" t="s">
         <v>84</v>
@@ -16220,24 +16223,24 @@
         <v>526</v>
       </c>
       <c r="E393" s="43" t="s">
-        <v>487</v>
+        <v>521</v>
       </c>
       <c r="F393" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G393" s="3" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="H393" s="55"/>
       <c r="I393" s="3" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="J393" s="3" t="s">
         <v>84</v>
       </c>
       <c r="K393" s="1"/>
     </row>
-    <row r="394" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A394" s="24">
         <v>393</v>
       </c>
@@ -16245,26 +16248,22 @@
         <v>957</v>
       </c>
       <c r="C394" s="3" t="s">
-        <v>85</v>
+        <v>216</v>
       </c>
       <c r="D394" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="E394" s="43" t="s">
-        <v>521</v>
-      </c>
-      <c r="F394" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G394" s="3" t="s">
-        <v>966</v>
-      </c>
+      <c r="E394" s="42" t="s">
+        <v>577</v>
+      </c>
+      <c r="F394" s="55"/>
+      <c r="G394" s="55"/>
       <c r="H394" s="55"/>
-      <c r="I394" s="3" t="s">
-        <v>967</v>
+      <c r="I394" s="1" t="s">
+        <v>1346</v>
       </c>
       <c r="J394" s="3" t="s">
-        <v>84</v>
+        <v>450</v>
       </c>
       <c r="K394" s="1"/>
     </row>
@@ -16281,48 +16280,50 @@
       <c r="D395" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="E395" s="42" t="s">
-        <v>577</v>
-      </c>
-      <c r="F395" s="55"/>
+      <c r="E395" s="31" t="s">
+        <v>1370</v>
+      </c>
+      <c r="F395" s="47"/>
       <c r="G395" s="55"/>
       <c r="H395" s="55"/>
-      <c r="I395" s="1" t="s">
-        <v>1346</v>
+      <c r="I395" s="3" t="s">
+        <v>1378</v>
       </c>
       <c r="J395" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K395" s="1"/>
     </row>
-    <row r="396" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A396" s="24">
         <v>395</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>957</v>
+        <v>968</v>
       </c>
       <c r="C396" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="D396" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="E396" s="31" t="s">
-        <v>1371</v>
-      </c>
-      <c r="F396" s="47"/>
-      <c r="G396" s="55"/>
+        <v>4</v>
+      </c>
+      <c r="D396" s="3"/>
+      <c r="E396" s="53" t="s">
+        <v>968</v>
+      </c>
+      <c r="F396" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G396" s="3" t="s">
+        <v>969</v>
+      </c>
       <c r="H396" s="55"/>
       <c r="I396" s="3" t="s">
-        <v>1379</v>
+        <v>970</v>
       </c>
       <c r="J396" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K396" s="1"/>
     </row>
-    <row r="397" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A397" s="24">
         <v>396</v>
       </c>
@@ -16330,24 +16331,24 @@
         <v>968</v>
       </c>
       <c r="C397" s="3" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="D397" s="3"/>
-      <c r="E397" s="53" t="s">
-        <v>968</v>
+      <c r="E397" s="43" t="s">
+        <v>486</v>
       </c>
       <c r="F397" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G397" s="3" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="H397" s="55"/>
       <c r="I397" s="3" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="J397" s="3" t="s">
-        <v>450</v>
+        <v>84</v>
       </c>
       <c r="K397" s="1"/>
     </row>
@@ -16363,24 +16364,24 @@
       </c>
       <c r="D398" s="3"/>
       <c r="E398" s="43" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="F398" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G398" s="3" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="H398" s="55"/>
       <c r="I398" s="3" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="J398" s="3" t="s">
         <v>84</v>
       </c>
       <c r="K398" s="1"/>
     </row>
-    <row r="399" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A399" s="24">
         <v>398</v>
       </c>
@@ -16392,24 +16393,24 @@
       </c>
       <c r="D399" s="3"/>
       <c r="E399" s="43" t="s">
-        <v>487</v>
+        <v>521</v>
       </c>
       <c r="F399" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G399" s="3" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="H399" s="55"/>
       <c r="I399" s="3" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="J399" s="3" t="s">
         <v>84</v>
       </c>
       <c r="K399" s="1"/>
     </row>
-    <row r="400" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A400" s="24">
         <v>399</v>
       </c>
@@ -16417,21 +16418,21 @@
         <v>968</v>
       </c>
       <c r="C400" s="3" t="s">
-        <v>85</v>
+        <v>1009</v>
       </c>
       <c r="D400" s="3"/>
-      <c r="E400" s="43" t="s">
-        <v>521</v>
-      </c>
-      <c r="F400" s="3" t="s">
+      <c r="E400" s="21" t="s">
+        <v>939</v>
+      </c>
+      <c r="F400" s="24" t="s">
         <v>13</v>
       </c>
       <c r="G400" s="3" t="s">
-        <v>975</v>
-      </c>
-      <c r="H400" s="55"/>
+        <v>1016</v>
+      </c>
+      <c r="H400" s="3"/>
       <c r="I400" s="3" t="s">
-        <v>976</v>
+        <v>1017</v>
       </c>
       <c r="J400" s="3" t="s">
         <v>84</v>
@@ -16450,24 +16451,24 @@
       </c>
       <c r="D401" s="3"/>
       <c r="E401" s="21" t="s">
-        <v>939</v>
+        <v>949</v>
       </c>
       <c r="F401" s="24" t="s">
         <v>13</v>
       </c>
       <c r="G401" s="3" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="H401" s="3"/>
       <c r="I401" s="3" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="J401" s="3" t="s">
         <v>84</v>
       </c>
       <c r="K401" s="1"/>
     </row>
-    <row r="402" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:11" ht="50" x14ac:dyDescent="0.35">
       <c r="A402" s="24">
         <v>401</v>
       </c>
@@ -16479,24 +16480,28 @@
       </c>
       <c r="D402" s="3"/>
       <c r="E402" s="21" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="F402" s="24" t="s">
         <v>13</v>
       </c>
       <c r="G402" s="3" t="s">
-        <v>1018</v>
-      </c>
-      <c r="H402" s="3"/>
+        <v>1032</v>
+      </c>
+      <c r="H402" s="3" t="s">
+        <v>1221</v>
+      </c>
       <c r="I402" s="3" t="s">
-        <v>1019</v>
+        <v>1033</v>
       </c>
       <c r="J402" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K402" s="1"/>
-    </row>
-    <row r="403" spans="1:11" ht="50" x14ac:dyDescent="0.35">
+        <v>907</v>
+      </c>
+      <c r="K402" s="68" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="403" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A403" s="24">
         <v>402</v>
       </c>
@@ -16506,28 +16511,24 @@
       <c r="C403" s="3" t="s">
         <v>1009</v>
       </c>
-      <c r="D403" s="3"/>
-      <c r="E403" s="21" t="s">
-        <v>950</v>
-      </c>
-      <c r="F403" s="24" t="s">
+      <c r="D403" s="1"/>
+      <c r="E403" s="43" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F403" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G403" s="3" t="s">
-        <v>1032</v>
-      </c>
-      <c r="H403" s="3" t="s">
-        <v>1221</v>
-      </c>
+        <v>1010</v>
+      </c>
+      <c r="H403" s="3"/>
       <c r="I403" s="3" t="s">
-        <v>1033</v>
+        <v>1011</v>
       </c>
       <c r="J403" s="3" t="s">
-        <v>907</v>
-      </c>
-      <c r="K403" s="68" t="s">
-        <v>908</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="K403" s="1"/>
     </row>
     <row r="404" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A404" s="24">
@@ -16537,23 +16538,23 @@
         <v>968</v>
       </c>
       <c r="C404" s="3" t="s">
-        <v>1009</v>
+        <v>85</v>
       </c>
       <c r="D404" s="1"/>
       <c r="E404" s="43" t="s">
-        <v>1008</v>
-      </c>
-      <c r="F404" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G404" s="3" t="s">
-        <v>1010</v>
-      </c>
-      <c r="H404" s="3"/>
+        <v>1036</v>
+      </c>
+      <c r="F404" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="G404" s="46" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H404" s="46"/>
       <c r="I404" s="3" t="s">
-        <v>1011</v>
-      </c>
-      <c r="J404" s="3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="J404" s="46" t="s">
         <v>84</v>
       </c>
       <c r="K404" s="1"/>
@@ -16566,24 +16567,20 @@
         <v>968</v>
       </c>
       <c r="C405" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D405" s="1"/>
-      <c r="E405" s="43" t="s">
-        <v>1036</v>
-      </c>
-      <c r="F405" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="G405" s="46" t="s">
-        <v>1059</v>
-      </c>
-      <c r="H405" s="46"/>
-      <c r="I405" s="3" t="s">
-        <v>1060</v>
-      </c>
-      <c r="J405" s="46" t="s">
-        <v>84</v>
+        <v>216</v>
+      </c>
+      <c r="D405" s="3"/>
+      <c r="E405" s="42" t="s">
+        <v>941</v>
+      </c>
+      <c r="F405" s="55"/>
+      <c r="G405" s="55"/>
+      <c r="H405" s="55"/>
+      <c r="I405" s="1" t="s">
+        <v>1347</v>
+      </c>
+      <c r="J405" s="3" t="s">
+        <v>450</v>
       </c>
       <c r="K405" s="1"/>
     </row>
@@ -16599,45 +16596,49 @@
       </c>
       <c r="D406" s="3"/>
       <c r="E406" s="42" t="s">
-        <v>941</v>
-      </c>
-      <c r="F406" s="55"/>
+        <v>1370</v>
+      </c>
+      <c r="F406" s="47"/>
       <c r="G406" s="55"/>
       <c r="H406" s="55"/>
-      <c r="I406" s="1" t="s">
-        <v>1347</v>
+      <c r="I406" s="3" t="s">
+        <v>1387</v>
       </c>
       <c r="J406" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K406" s="1"/>
     </row>
-    <row r="407" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A407" s="24">
         <v>406</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>968</v>
+        <v>977</v>
       </c>
       <c r="C407" s="3" t="s">
-        <v>216</v>
+        <v>4</v>
       </c>
       <c r="D407" s="3"/>
-      <c r="E407" s="42" t="s">
-        <v>1371</v>
-      </c>
-      <c r="F407" s="47"/>
-      <c r="G407" s="55"/>
+      <c r="E407" s="53" t="s">
+        <v>977</v>
+      </c>
+      <c r="F407" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="G407" s="3" t="s">
+        <v>977</v>
+      </c>
       <c r="H407" s="55"/>
       <c r="I407" s="3" t="s">
-        <v>1388</v>
+        <v>981</v>
       </c>
       <c r="J407" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K407" s="1"/>
     </row>
-    <row r="408" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A408" s="24">
         <v>407</v>
       </c>
@@ -16645,24 +16646,24 @@
         <v>977</v>
       </c>
       <c r="C408" s="3" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="D408" s="3"/>
-      <c r="E408" s="53" t="s">
-        <v>977</v>
+      <c r="E408" s="43" t="s">
+        <v>978</v>
       </c>
       <c r="F408" s="3" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="G408" s="3" t="s">
-        <v>977</v>
+        <v>983</v>
       </c>
       <c r="H408" s="55"/>
       <c r="I408" s="3" t="s">
-        <v>981</v>
+        <v>984</v>
       </c>
       <c r="J408" s="3" t="s">
-        <v>450</v>
+        <v>84</v>
       </c>
       <c r="K408" s="1"/>
     </row>
@@ -16678,24 +16679,24 @@
       </c>
       <c r="D409" s="3"/>
       <c r="E409" s="43" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="F409" s="3" t="s">
-        <v>982</v>
+        <v>985</v>
       </c>
       <c r="G409" s="3" t="s">
-        <v>983</v>
+        <v>986</v>
       </c>
       <c r="H409" s="55"/>
       <c r="I409" s="3" t="s">
-        <v>984</v>
+        <v>987</v>
       </c>
       <c r="J409" s="3" t="s">
         <v>84</v>
       </c>
       <c r="K409" s="1"/>
     </row>
-    <row r="410" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:11" ht="50" x14ac:dyDescent="0.35">
       <c r="A410" s="24">
         <v>409</v>
       </c>
@@ -16703,28 +16704,30 @@
         <v>977</v>
       </c>
       <c r="C410" s="3" t="s">
-        <v>85</v>
+        <v>1009</v>
       </c>
       <c r="D410" s="3"/>
       <c r="E410" s="43" t="s">
-        <v>979</v>
+        <v>877</v>
       </c>
       <c r="F410" s="3" t="s">
-        <v>985</v>
+        <v>988</v>
       </c>
       <c r="G410" s="3" t="s">
-        <v>986</v>
+        <v>989</v>
       </c>
       <c r="H410" s="55"/>
       <c r="I410" s="3" t="s">
-        <v>987</v>
+        <v>990</v>
       </c>
       <c r="J410" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K410" s="1"/>
-    </row>
-    <row r="411" spans="1:11" ht="50" x14ac:dyDescent="0.35">
+        <v>935</v>
+      </c>
+      <c r="K410" s="68" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="411" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A411" s="24">
         <v>410</v>
       </c>
@@ -16732,90 +16735,88 @@
         <v>977</v>
       </c>
       <c r="C411" s="3" t="s">
-        <v>1009</v>
+        <v>85</v>
       </c>
       <c r="D411" s="3"/>
-      <c r="E411" s="43" t="s">
-        <v>877</v>
-      </c>
-      <c r="F411" s="3" t="s">
-        <v>988</v>
-      </c>
-      <c r="G411" s="3" t="s">
-        <v>989</v>
-      </c>
-      <c r="H411" s="55"/>
-      <c r="I411" s="3" t="s">
-        <v>990</v>
-      </c>
-      <c r="J411" s="3" t="s">
-        <v>935</v>
-      </c>
-      <c r="K411" s="68" t="s">
-        <v>936</v>
-      </c>
+      <c r="E411" s="44" t="s">
+        <v>991</v>
+      </c>
+      <c r="F411" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="G411" s="46" t="s">
+        <v>992</v>
+      </c>
+      <c r="H411" s="46"/>
+      <c r="I411" s="46" t="s">
+        <v>993</v>
+      </c>
+      <c r="J411" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="K411" s="1"/>
     </row>
     <row r="412" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A412" s="24">
         <v>411</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>977</v>
-      </c>
-      <c r="C412" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D412" s="3"/>
-      <c r="E412" s="44" t="s">
-        <v>991</v>
-      </c>
-      <c r="F412" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="G412" s="46" t="s">
-        <v>992</v>
-      </c>
-      <c r="H412" s="46"/>
-      <c r="I412" s="46" t="s">
-        <v>993</v>
-      </c>
-      <c r="J412" s="46" t="s">
-        <v>84</v>
-      </c>
-      <c r="K412" s="1"/>
-    </row>
-    <row r="413" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+        <v>995</v>
+      </c>
+      <c r="C412" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D412" s="1"/>
+      <c r="E412" s="30" t="s">
+        <v>995</v>
+      </c>
+      <c r="F412" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G412" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H412" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I412" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J412" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="K412" s="24"/>
+    </row>
+    <row r="413" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A413" s="24">
         <v>412</v>
       </c>
       <c r="B413" s="1" t="s">
         <v>995</v>
       </c>
-      <c r="C413" s="1" t="s">
-        <v>4</v>
+      <c r="C413" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="D413" s="1"/>
-      <c r="E413" s="30" t="s">
-        <v>995</v>
+      <c r="E413" s="21" t="s">
+        <v>339</v>
       </c>
       <c r="F413" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G413" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H413" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I413" s="1" t="s">
-        <v>11</v>
+        <v>996</v>
+      </c>
+      <c r="H413" s="55"/>
+      <c r="I413" s="3" t="s">
+        <v>997</v>
       </c>
       <c r="J413" s="3" t="s">
-        <v>450</v>
+        <v>84</v>
       </c>
       <c r="K413" s="24"/>
     </row>
-    <row r="414" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A414" s="24">
         <v>413</v>
       </c>
@@ -16823,55 +16824,54 @@
         <v>995</v>
       </c>
       <c r="C414" s="3" t="s">
-        <v>85</v>
+        <v>1009</v>
       </c>
       <c r="D414" s="1"/>
       <c r="E414" s="21" t="s">
-        <v>339</v>
+        <v>523</v>
       </c>
       <c r="F414" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G414" s="3" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="H414" s="55"/>
       <c r="I414" s="3" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="J414" s="3" t="s">
-        <v>84</v>
+        <v>1166</v>
       </c>
       <c r="K414" s="24"/>
     </row>
-    <row r="415" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A415" s="24">
         <v>414</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>995</v>
-      </c>
-      <c r="C415" s="3" t="s">
-        <v>1009</v>
+        <v>1039</v>
+      </c>
+      <c r="C415" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D415" s="1"/>
-      <c r="E415" s="21" t="s">
-        <v>523</v>
+      <c r="E415" s="30" t="s">
+        <v>1039</v>
       </c>
       <c r="F415" s="3" t="s">
-        <v>13</v>
+        <v>1040</v>
       </c>
       <c r="G415" s="3" t="s">
-        <v>998</v>
+        <v>1039</v>
       </c>
       <c r="H415" s="55"/>
       <c r="I415" s="3" t="s">
-        <v>999</v>
+        <v>1041</v>
       </c>
       <c r="J415" s="3" t="s">
-        <v>1166</v>
-      </c>
-      <c r="K415" s="24"/>
+        <v>450</v>
+      </c>
     </row>
     <row r="416" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A416" s="24">
@@ -16880,25 +16880,27 @@
       <c r="B416" s="1" t="s">
         <v>1039</v>
       </c>
-      <c r="C416" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D416" s="1"/>
-      <c r="E416" s="30" t="s">
-        <v>1039</v>
+      <c r="C416" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D416" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="E416" s="21" t="s">
+        <v>486</v>
       </c>
       <c r="F416" s="3" t="s">
-        <v>1040</v>
+        <v>13</v>
       </c>
       <c r="G416" s="3" t="s">
-        <v>1039</v>
+        <v>1042</v>
       </c>
       <c r="H416" s="55"/>
       <c r="I416" s="3" t="s">
-        <v>1041</v>
-      </c>
-      <c r="J416" s="3" t="s">
-        <v>450</v>
+        <v>1043</v>
+      </c>
+      <c r="J416" s="46" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="417" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -16915,17 +16917,17 @@
         <v>526</v>
       </c>
       <c r="E417" s="21" t="s">
-        <v>486</v>
+        <v>339</v>
       </c>
       <c r="F417" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G417" s="3" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="H417" s="55"/>
       <c r="I417" s="3" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="J417" s="46" t="s">
         <v>84</v>
@@ -16935,29 +16937,29 @@
       <c r="A418" s="24">
         <v>417</v>
       </c>
-      <c r="B418" s="1" t="s">
+      <c r="B418" s="20" t="s">
         <v>1039</v>
       </c>
-      <c r="C418" s="3" t="s">
+      <c r="C418" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="D418" s="3" t="s">
+      <c r="D418" s="32" t="s">
         <v>526</v>
       </c>
-      <c r="E418" s="21" t="s">
-        <v>339</v>
-      </c>
-      <c r="F418" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G418" s="3" t="s">
-        <v>1044</v>
-      </c>
-      <c r="H418" s="55"/>
-      <c r="I418" s="3" t="s">
-        <v>1045</v>
-      </c>
-      <c r="J418" s="46" t="s">
+      <c r="E418" s="56" t="s">
+        <v>487</v>
+      </c>
+      <c r="F418" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G418" s="32" t="s">
+        <v>1046</v>
+      </c>
+      <c r="H418" s="57"/>
+      <c r="I418" s="32" t="s">
+        <v>1047</v>
+      </c>
+      <c r="J418" s="69" t="s">
         <v>84</v>
       </c>
     </row>
@@ -16965,64 +16967,59 @@
       <c r="A419" s="24">
         <v>418</v>
       </c>
-      <c r="B419" s="20" t="s">
+      <c r="B419" s="1" t="s">
         <v>1039</v>
       </c>
-      <c r="C419" s="32" t="s">
+      <c r="C419" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D419" s="32" t="s">
+      <c r="D419" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="E419" s="56" t="s">
-        <v>487</v>
-      </c>
-      <c r="F419" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="G419" s="32" t="s">
-        <v>1046</v>
-      </c>
-      <c r="H419" s="57"/>
-      <c r="I419" s="32" t="s">
-        <v>1047</v>
-      </c>
-      <c r="J419" s="69" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="420" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="E419" s="21" t="s">
+        <v>521</v>
+      </c>
+      <c r="F419" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G419" s="3" t="s">
+        <v>1048</v>
+      </c>
+      <c r="H419" s="55"/>
+      <c r="I419" s="3" t="s">
+        <v>1049</v>
+      </c>
+      <c r="J419" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="K419" s="1"/>
+    </row>
+    <row r="420" spans="1:11" ht="50" x14ac:dyDescent="0.35">
       <c r="A420" s="24">
         <v>419</v>
       </c>
       <c r="B420" s="1" t="s">
         <v>1039</v>
       </c>
-      <c r="C420" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D420" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="E420" s="21" t="s">
-        <v>521</v>
-      </c>
-      <c r="F420" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G420" s="3" t="s">
-        <v>1048</v>
-      </c>
-      <c r="H420" s="55"/>
-      <c r="I420" s="3" t="s">
-        <v>1049</v>
-      </c>
-      <c r="J420" s="46" t="s">
-        <v>84</v>
+      <c r="C420" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="D420" s="24"/>
+      <c r="E420" s="34" t="s">
+        <v>943</v>
+      </c>
+      <c r="F420" s="24"/>
+      <c r="G420" s="24"/>
+      <c r="H420" s="24"/>
+      <c r="I420" s="1" t="s">
+        <v>1348</v>
+      </c>
+      <c r="J420" s="3" t="s">
+        <v>450</v>
       </c>
       <c r="K420" s="1"/>
     </row>
-    <row r="421" spans="1:11" ht="50" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:11" ht="75" x14ac:dyDescent="0.35">
       <c r="A421" s="24">
         <v>420</v>
       </c>
@@ -17034,20 +17031,20 @@
       </c>
       <c r="D421" s="24"/>
       <c r="E421" s="34" t="s">
-        <v>943</v>
+        <v>1050</v>
       </c>
       <c r="F421" s="24"/>
       <c r="G421" s="24"/>
       <c r="H421" s="24"/>
       <c r="I421" s="1" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="J421" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K421" s="1"/>
     </row>
-    <row r="422" spans="1:11" ht="75" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A422" s="24">
         <v>421</v>
       </c>
@@ -17057,15 +17054,17 @@
       <c r="C422" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="D422" s="24"/>
+      <c r="D422" s="3" t="s">
+        <v>526</v>
+      </c>
       <c r="E422" s="34" t="s">
-        <v>1050</v>
+        <v>577</v>
       </c>
       <c r="F422" s="24"/>
       <c r="G422" s="24"/>
       <c r="H422" s="24"/>
       <c r="I422" s="1" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="J422" s="3" t="s">
         <v>450</v>
@@ -17086,76 +17085,78 @@
         <v>526</v>
       </c>
       <c r="E423" s="34" t="s">
-        <v>577</v>
-      </c>
-      <c r="F423" s="24"/>
+        <v>1370</v>
+      </c>
+      <c r="F423" s="47"/>
       <c r="G423" s="24"/>
       <c r="H423" s="24"/>
-      <c r="I423" s="1" t="s">
-        <v>1350</v>
+      <c r="I423" s="3" t="s">
+        <v>1379</v>
       </c>
       <c r="J423" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K423" s="1"/>
     </row>
-    <row r="424" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:11" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A424" s="24">
         <v>423</v>
       </c>
-      <c r="B424" s="1" t="s">
-        <v>1039</v>
-      </c>
-      <c r="C424" s="24" t="s">
-        <v>216</v>
-      </c>
-      <c r="D424" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="E424" s="34" t="s">
-        <v>1371</v>
-      </c>
-      <c r="F424" s="47"/>
-      <c r="G424" s="24"/>
-      <c r="H424" s="24"/>
+      <c r="B424" s="3" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C424" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D424" s="1"/>
+      <c r="E424" s="30" t="s">
+        <v>1052</v>
+      </c>
+      <c r="F424" s="3" t="s">
+        <v>1053</v>
+      </c>
+      <c r="G424" s="3" t="s">
+        <v>1052</v>
+      </c>
+      <c r="H424" s="55"/>
       <c r="I424" s="3" t="s">
-        <v>1380</v>
+        <v>1231</v>
       </c>
       <c r="J424" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K424" s="1"/>
     </row>
-    <row r="425" spans="1:11" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A425" s="24">
         <v>424</v>
       </c>
       <c r="B425" s="3" t="s">
         <v>1052</v>
       </c>
-      <c r="C425" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D425" s="1"/>
-      <c r="E425" s="30" t="s">
-        <v>1052</v>
+      <c r="C425" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D425" s="24"/>
+      <c r="E425" s="21" t="s">
+        <v>487</v>
       </c>
       <c r="F425" s="3" t="s">
-        <v>1053</v>
+        <v>13</v>
       </c>
       <c r="G425" s="3" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="H425" s="55"/>
       <c r="I425" s="3" t="s">
-        <v>1231</v>
+        <v>1055</v>
       </c>
       <c r="J425" s="3" t="s">
-        <v>450</v>
+        <v>84</v>
       </c>
       <c r="K425" s="1"/>
     </row>
-    <row r="426" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A426" s="24">
         <v>425</v>
       </c>
@@ -17163,84 +17164,86 @@
         <v>1052</v>
       </c>
       <c r="C426" s="3" t="s">
-        <v>85</v>
+        <v>1009</v>
       </c>
       <c r="D426" s="24"/>
       <c r="E426" s="21" t="s">
-        <v>487</v>
+        <v>862</v>
       </c>
       <c r="F426" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G426" s="3" t="s">
-        <v>1054</v>
-      </c>
-      <c r="H426" s="55"/>
+        <v>1056</v>
+      </c>
+      <c r="H426" s="46" t="s">
+        <v>1057</v>
+      </c>
       <c r="I426" s="3" t="s">
-        <v>1055</v>
+        <v>1058</v>
       </c>
       <c r="J426" s="3" t="s">
-        <v>84</v>
+        <v>1100</v>
       </c>
       <c r="K426" s="1"/>
     </row>
-    <row r="427" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:11" ht="50" x14ac:dyDescent="0.35">
       <c r="A427" s="24">
         <v>426</v>
       </c>
       <c r="B427" s="3" t="s">
-        <v>1052</v>
-      </c>
-      <c r="C427" s="3" t="s">
-        <v>1009</v>
-      </c>
-      <c r="D427" s="24"/>
-      <c r="E427" s="21" t="s">
-        <v>862</v>
+        <v>1061</v>
+      </c>
+      <c r="C427" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D427" s="1"/>
+      <c r="E427" s="30" t="s">
+        <v>1061</v>
       </c>
       <c r="F427" s="3" t="s">
-        <v>13</v>
+        <v>1062</v>
       </c>
       <c r="G427" s="3" t="s">
-        <v>1056</v>
-      </c>
-      <c r="H427" s="46" t="s">
-        <v>1057</v>
-      </c>
+        <v>1063</v>
+      </c>
+      <c r="H427" s="55"/>
       <c r="I427" s="3" t="s">
-        <v>1058</v>
+        <v>1064</v>
       </c>
       <c r="J427" s="3" t="s">
-        <v>1100</v>
-      </c>
-      <c r="K427" s="1"/>
-    </row>
-    <row r="428" spans="1:11" ht="50" x14ac:dyDescent="0.35">
+        <v>450</v>
+      </c>
+      <c r="K427" s="46"/>
+    </row>
+    <row r="428" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A428" s="24">
         <v>427</v>
       </c>
       <c r="B428" s="3" t="s">
         <v>1061</v>
       </c>
-      <c r="C428" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D428" s="1"/>
-      <c r="E428" s="30" t="s">
-        <v>1061</v>
+      <c r="C428" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D428" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="E428" s="22" t="s">
+        <v>769</v>
       </c>
       <c r="F428" s="3" t="s">
-        <v>1062</v>
+        <v>13</v>
       </c>
       <c r="G428" s="3" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="H428" s="55"/>
-      <c r="I428" s="3" t="s">
-        <v>1064</v>
+      <c r="I428" s="1" t="s">
+        <v>1066</v>
       </c>
       <c r="J428" s="3" t="s">
-        <v>450</v>
+        <v>84</v>
       </c>
       <c r="K428" s="46"/>
     </row>
@@ -17258,17 +17261,17 @@
         <v>186</v>
       </c>
       <c r="E429" s="22" t="s">
-        <v>769</v>
+        <v>592</v>
       </c>
       <c r="F429" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G429" s="3" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="H429" s="55"/>
-      <c r="I429" s="1" t="s">
-        <v>1066</v>
+      <c r="I429" s="3" t="s">
+        <v>1068</v>
       </c>
       <c r="J429" s="3" t="s">
         <v>84</v>
@@ -17289,24 +17292,24 @@
         <v>186</v>
       </c>
       <c r="E430" s="22" t="s">
-        <v>592</v>
+        <v>486</v>
       </c>
       <c r="F430" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G430" s="3" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="H430" s="55"/>
       <c r="I430" s="3" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="J430" s="3" t="s">
         <v>84</v>
       </c>
       <c r="K430" s="46"/>
     </row>
-    <row r="431" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="431" spans="1:11" ht="50" x14ac:dyDescent="0.35">
       <c r="A431" s="24">
         <v>430</v>
       </c>
@@ -17314,30 +17317,32 @@
         <v>1061</v>
       </c>
       <c r="C431" s="3" t="s">
-        <v>85</v>
+        <v>1009</v>
       </c>
       <c r="D431" s="24" t="s">
         <v>186</v>
       </c>
       <c r="E431" s="22" t="s">
-        <v>486</v>
-      </c>
-      <c r="F431" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G431" s="3" t="s">
-        <v>1069</v>
-      </c>
-      <c r="H431" s="55"/>
-      <c r="I431" s="3" t="s">
-        <v>1070</v>
-      </c>
-      <c r="J431" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K431" s="46"/>
-    </row>
-    <row r="432" spans="1:11" ht="50" x14ac:dyDescent="0.35">
+        <v>1163</v>
+      </c>
+      <c r="F431" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G431" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H431" s="1"/>
+      <c r="I431" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="J431" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="K431" s="46" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="432" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A432" s="24">
         <v>431</v>
       </c>
@@ -17345,61 +17350,55 @@
         <v>1061</v>
       </c>
       <c r="C432" s="3" t="s">
-        <v>1009</v>
+        <v>85</v>
       </c>
       <c r="D432" s="24" t="s">
         <v>186</v>
       </c>
       <c r="E432" s="22" t="s">
-        <v>1163</v>
-      </c>
-      <c r="F432" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="G432" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="H432" s="1"/>
-      <c r="I432" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="J432" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="K432" s="46" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="433" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+        <v>521</v>
+      </c>
+      <c r="F432" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G432" s="3" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H432" s="55"/>
+      <c r="I432" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="J432" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K432" s="46"/>
+    </row>
+    <row r="433" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A433" s="24">
         <v>432</v>
       </c>
       <c r="B433" s="3" t="s">
         <v>1061</v>
       </c>
-      <c r="C433" s="3" t="s">
-        <v>85</v>
+      <c r="C433" s="24" t="s">
+        <v>216</v>
       </c>
       <c r="D433" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E433" s="22" t="s">
-        <v>521</v>
-      </c>
-      <c r="F433" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G433" s="3" t="s">
-        <v>1071</v>
-      </c>
-      <c r="H433" s="55"/>
-      <c r="I433" s="3" t="s">
-        <v>1072</v>
-      </c>
-      <c r="J433" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K433" s="46"/>
+      <c r="E433" s="31" t="s">
+        <v>770</v>
+      </c>
+      <c r="F433" s="24"/>
+      <c r="G433" s="24"/>
+      <c r="H433" s="24"/>
+      <c r="I433" s="1" t="s">
+        <v>1351</v>
+      </c>
+      <c r="J433" s="24" t="s">
+        <v>450</v>
+      </c>
+      <c r="K433" s="1"/>
     </row>
     <row r="434" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A434" s="24">
@@ -17411,74 +17410,76 @@
       <c r="C434" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="D434" s="24" t="s">
-        <v>186</v>
-      </c>
-      <c r="E434" s="31" t="s">
-        <v>770</v>
+      <c r="D434" s="24"/>
+      <c r="E434" s="64" t="s">
+        <v>1087</v>
       </c>
       <c r="F434" s="24"/>
       <c r="G434" s="24"/>
       <c r="H434" s="24"/>
       <c r="I434" s="1" t="s">
-        <v>1351</v>
-      </c>
-      <c r="J434" s="24" t="s">
+        <v>1352</v>
+      </c>
+      <c r="J434" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K434" s="1"/>
     </row>
-    <row r="435" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A435" s="24">
         <v>434</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>1061</v>
-      </c>
-      <c r="C435" s="24" t="s">
-        <v>216</v>
-      </c>
-      <c r="D435" s="24"/>
-      <c r="E435" s="64" t="s">
-        <v>1087</v>
-      </c>
-      <c r="F435" s="24"/>
-      <c r="G435" s="24"/>
-      <c r="H435" s="24"/>
-      <c r="I435" s="1" t="s">
-        <v>1352</v>
+        <v>1085</v>
+      </c>
+      <c r="C435" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D435" s="1"/>
+      <c r="E435" s="30" t="s">
+        <v>1085</v>
+      </c>
+      <c r="F435" s="3" t="s">
+        <v>1094</v>
+      </c>
+      <c r="G435" s="3" t="s">
+        <v>1095</v>
+      </c>
+      <c r="H435" s="55"/>
+      <c r="I435" s="3" t="s">
+        <v>1096</v>
       </c>
       <c r="J435" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K435" s="1"/>
     </row>
-    <row r="436" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="436" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A436" s="24">
         <v>435</v>
       </c>
-      <c r="B436" s="3" t="s">
+      <c r="B436" s="1" t="s">
         <v>1085</v>
       </c>
-      <c r="C436" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D436" s="1"/>
-      <c r="E436" s="30" t="s">
-        <v>1085</v>
+      <c r="C436" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D436" s="24"/>
+      <c r="E436" s="21" t="s">
+        <v>486</v>
       </c>
       <c r="F436" s="3" t="s">
-        <v>1094</v>
+        <v>13</v>
       </c>
       <c r="G436" s="3" t="s">
-        <v>1095</v>
+        <v>1088</v>
       </c>
       <c r="H436" s="55"/>
       <c r="I436" s="3" t="s">
-        <v>1096</v>
+        <v>1089</v>
       </c>
       <c r="J436" s="3" t="s">
-        <v>450</v>
+        <v>84</v>
       </c>
       <c r="K436" s="1"/>
     </row>
@@ -17494,17 +17495,17 @@
       </c>
       <c r="D437" s="24"/>
       <c r="E437" s="21" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="F437" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G437" s="3" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
       <c r="H437" s="55"/>
       <c r="I437" s="3" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
       <c r="J437" s="3" t="s">
         <v>84</v>
@@ -17523,24 +17524,24 @@
       </c>
       <c r="D438" s="24"/>
       <c r="E438" s="21" t="s">
-        <v>487</v>
+        <v>521</v>
       </c>
       <c r="F438" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G438" s="3" t="s">
-        <v>1090</v>
+        <v>1092</v>
       </c>
       <c r="H438" s="55"/>
       <c r="I438" s="3" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="J438" s="3" t="s">
         <v>84</v>
       </c>
       <c r="K438" s="1"/>
     </row>
-    <row r="439" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A439" s="24">
         <v>438</v>
       </c>
@@ -17548,82 +17549,82 @@
         <v>1085</v>
       </c>
       <c r="C439" s="3" t="s">
-        <v>85</v>
+        <v>216</v>
       </c>
       <c r="D439" s="24"/>
-      <c r="E439" s="21" t="s">
-        <v>521</v>
-      </c>
-      <c r="F439" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G439" s="3" t="s">
-        <v>1092</v>
-      </c>
+      <c r="E439" s="64" t="s">
+        <v>1086</v>
+      </c>
+      <c r="F439" s="55"/>
+      <c r="G439" s="55"/>
       <c r="H439" s="55"/>
-      <c r="I439" s="3" t="s">
-        <v>1093</v>
+      <c r="I439" s="1" t="s">
+        <v>1353</v>
       </c>
       <c r="J439" s="3" t="s">
-        <v>84</v>
+        <v>450</v>
       </c>
       <c r="K439" s="1"/>
     </row>
-    <row r="440" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="440" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A440" s="24">
         <v>439</v>
       </c>
-      <c r="B440" s="1" t="s">
-        <v>1085</v>
-      </c>
-      <c r="C440" s="3" t="s">
-        <v>216</v>
+      <c r="B440" s="24" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C440" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D440" s="24"/>
-      <c r="E440" s="64" t="s">
-        <v>1086</v>
-      </c>
-      <c r="F440" s="55"/>
-      <c r="G440" s="55"/>
-      <c r="H440" s="55"/>
-      <c r="I440" s="1" t="s">
-        <v>1353</v>
+      <c r="E440" s="45" t="s">
+        <v>1195</v>
+      </c>
+      <c r="F440" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G440" s="1" t="s">
+        <v>1201</v>
+      </c>
+      <c r="H440" s="71"/>
+      <c r="I440" s="41" t="s">
+        <v>1202</v>
       </c>
       <c r="J440" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K440" s="1"/>
     </row>
-    <row r="441" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="441" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A441" s="24">
         <v>440</v>
       </c>
       <c r="B441" s="24" t="s">
         <v>1195</v>
       </c>
-      <c r="C441" s="1" t="s">
-        <v>4</v>
+      <c r="C441" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="D441" s="24"/>
-      <c r="E441" s="45" t="s">
-        <v>1195</v>
+      <c r="E441" s="22" t="s">
+        <v>1196</v>
       </c>
       <c r="F441" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G441" s="1" t="s">
-        <v>1201</v>
-      </c>
-      <c r="H441" s="71"/>
-      <c r="I441" s="41" t="s">
-        <v>1202</v>
-      </c>
-      <c r="J441" s="3" t="s">
-        <v>450</v>
+        <v>1197</v>
+      </c>
+      <c r="H441" s="1"/>
+      <c r="I441" s="1" t="s">
+        <v>1198</v>
+      </c>
+      <c r="J441" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="K441" s="1"/>
     </row>
-    <row r="442" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="442" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A442" s="24">
         <v>441</v>
       </c>
@@ -17635,49 +17636,49 @@
       </c>
       <c r="D442" s="24"/>
       <c r="E442" s="22" t="s">
-        <v>1196</v>
+        <v>751</v>
       </c>
       <c r="F442" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G442" s="1" t="s">
-        <v>1197</v>
+        <v>1199</v>
       </c>
       <c r="H442" s="1"/>
       <c r="I442" s="1" t="s">
-        <v>1198</v>
+        <v>1200</v>
       </c>
       <c r="J442" s="1" t="s">
         <v>84</v>
       </c>
       <c r="K442" s="1"/>
     </row>
-    <row r="443" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="443" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A443" s="24">
         <v>442</v>
       </c>
       <c r="B443" s="24" t="s">
-        <v>1195</v>
-      </c>
-      <c r="C443" s="3" t="s">
-        <v>85</v>
+        <v>1203</v>
+      </c>
+      <c r="C443" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D443" s="24"/>
-      <c r="E443" s="22" t="s">
-        <v>751</v>
-      </c>
-      <c r="F443" s="1" t="s">
-        <v>13</v>
+      <c r="E443" s="45" t="s">
+        <v>1203</v>
+      </c>
+      <c r="F443" s="54" t="s">
+        <v>734</v>
       </c>
       <c r="G443" s="1" t="s">
-        <v>1199</v>
+        <v>1208</v>
       </c>
       <c r="H443" s="1"/>
       <c r="I443" s="1" t="s">
-        <v>1200</v>
-      </c>
-      <c r="J443" s="1" t="s">
-        <v>84</v>
+        <v>1209</v>
+      </c>
+      <c r="J443" s="3" t="s">
+        <v>450</v>
       </c>
       <c r="K443" s="1"/>
     </row>
@@ -17688,29 +17689,29 @@
       <c r="B444" s="24" t="s">
         <v>1203</v>
       </c>
-      <c r="C444" s="1" t="s">
-        <v>4</v>
+      <c r="C444" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="D444" s="24"/>
-      <c r="E444" s="45" t="s">
-        <v>1203</v>
-      </c>
-      <c r="F444" s="54" t="s">
-        <v>734</v>
+      <c r="E444" s="22" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F444" s="1" t="s">
+        <v>1205</v>
       </c>
       <c r="G444" s="1" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="H444" s="1"/>
       <c r="I444" s="1" t="s">
-        <v>1209</v>
-      </c>
-      <c r="J444" s="3" t="s">
-        <v>450</v>
+        <v>1207</v>
+      </c>
+      <c r="J444" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="K444" s="1"/>
     </row>
-    <row r="445" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="445" spans="1:11" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A445" s="24">
         <v>444</v>
       </c>
@@ -17718,78 +17719,78 @@
         <v>1203</v>
       </c>
       <c r="C445" s="3" t="s">
-        <v>85</v>
+        <v>216</v>
       </c>
       <c r="D445" s="24"/>
-      <c r="E445" s="22" t="s">
-        <v>1204</v>
-      </c>
-      <c r="F445" s="1" t="s">
-        <v>1205</v>
-      </c>
-      <c r="G445" s="1" t="s">
-        <v>1206</v>
-      </c>
-      <c r="H445" s="1"/>
-      <c r="I445" s="1" t="s">
-        <v>1207</v>
+      <c r="E445" s="64" t="s">
+        <v>1248</v>
+      </c>
+      <c r="F445" s="24"/>
+      <c r="G445" s="24"/>
+      <c r="H445" s="24"/>
+      <c r="I445" s="3" t="s">
+        <v>1354</v>
       </c>
       <c r="J445" s="1" t="s">
-        <v>84</v>
+        <v>450</v>
       </c>
       <c r="K445" s="1"/>
     </row>
-    <row r="446" spans="1:11" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="446" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A446" s="24">
         <v>445</v>
       </c>
-      <c r="B446" s="24" t="s">
-        <v>1203</v>
-      </c>
-      <c r="C446" s="3" t="s">
-        <v>216</v>
+      <c r="B446" s="1" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C446" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D446" s="24"/>
-      <c r="E446" s="64" t="s">
-        <v>1248</v>
-      </c>
-      <c r="F446" s="24"/>
-      <c r="G446" s="24"/>
-      <c r="H446" s="24"/>
+      <c r="E446" s="53" t="s">
+        <v>1362</v>
+      </c>
+      <c r="F446" s="3" t="s">
+        <v>1363</v>
+      </c>
+      <c r="G446" s="3" t="s">
+        <v>1364</v>
+      </c>
+      <c r="H446" s="3"/>
       <c r="I446" s="3" t="s">
-        <v>1354</v>
-      </c>
-      <c r="J446" s="1" t="s">
+        <v>1365</v>
+      </c>
+      <c r="J446" s="3" t="s">
         <v>450</v>
       </c>
       <c r="K446" s="1"/>
     </row>
-    <row r="447" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="447" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A447" s="24">
         <v>446</v>
       </c>
       <c r="B447" s="1" t="s">
         <v>1362</v>
       </c>
-      <c r="C447" s="1" t="s">
-        <v>4</v>
+      <c r="C447" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="D447" s="24"/>
-      <c r="E447" s="53" t="s">
-        <v>1362</v>
+      <c r="E447" s="21" t="s">
+        <v>339</v>
       </c>
       <c r="F447" s="3" t="s">
-        <v>1363</v>
+        <v>13</v>
       </c>
       <c r="G447" s="3" t="s">
-        <v>1364</v>
+        <v>1366</v>
       </c>
       <c r="H447" s="3"/>
       <c r="I447" s="3" t="s">
-        <v>1365</v>
+        <v>1367</v>
       </c>
       <c r="J447" s="3" t="s">
-        <v>450</v>
+        <v>84</v>
       </c>
       <c r="K447" s="1"/>
     </row>
@@ -17805,55 +17806,26 @@
       </c>
       <c r="D448" s="24"/>
       <c r="E448" s="21" t="s">
-        <v>339</v>
+        <v>211</v>
       </c>
       <c r="F448" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G448" s="3" t="s">
-        <v>1366</v>
+        <v>1368</v>
       </c>
       <c r="H448" s="3"/>
-      <c r="I448" s="3" t="s">
-        <v>1367</v>
+      <c r="I448" s="1" t="s">
+        <v>1369</v>
       </c>
       <c r="J448" s="3" t="s">
         <v>84</v>
       </c>
       <c r="K448" s="1"/>
     </row>
-    <row r="449" spans="1:11" ht="25" x14ac:dyDescent="0.35">
-      <c r="A449" s="24">
-        <v>448</v>
-      </c>
-      <c r="B449" s="1" t="s">
-        <v>1362</v>
-      </c>
-      <c r="C449" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D449" s="24"/>
-      <c r="E449" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="F449" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G449" s="3" t="s">
-        <v>1368</v>
-      </c>
-      <c r="H449" s="3"/>
-      <c r="I449" s="1" t="s">
-        <v>1369</v>
-      </c>
-      <c r="J449" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K449" s="1"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:K449" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="G342">
+  <autoFilter ref="A1:K448" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="G341">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
@@ -17870,11 +17842,11 @@
     <hyperlink ref="K295" r:id="rId11" xr:uid="{3AB94896-41CC-43F9-96AA-23E28EB90807}"/>
     <hyperlink ref="K331" r:id="rId12" xr:uid="{5A4ED305-DAB1-4AB2-9821-67E85648C298}"/>
     <hyperlink ref="K333" r:id="rId13" xr:uid="{4C709FBD-08C2-4341-A1B8-9E6314E092CD}"/>
-    <hyperlink ref="K355" r:id="rId14" xr:uid="{A5546FE9-D80B-4535-B6AC-978D1E0D7964}"/>
-    <hyperlink ref="K370" r:id="rId15" xr:uid="{9390E52B-52E6-4CB8-8ADF-0E1102C02629}"/>
-    <hyperlink ref="K384" r:id="rId16" xr:uid="{0C9C0ED7-816D-40BE-8D70-35A4ABA9D43A}"/>
-    <hyperlink ref="K403" r:id="rId17" xr:uid="{69A12BC5-7D82-4136-A0E7-F5E7EC34F8B0}"/>
-    <hyperlink ref="K411" r:id="rId18" xr:uid="{9442A440-660A-4576-B105-2AC531645C93}"/>
+    <hyperlink ref="K354" r:id="rId14" xr:uid="{A5546FE9-D80B-4535-B6AC-978D1E0D7964}"/>
+    <hyperlink ref="K369" r:id="rId15" xr:uid="{9390E52B-52E6-4CB8-8ADF-0E1102C02629}"/>
+    <hyperlink ref="K383" r:id="rId16" xr:uid="{0C9C0ED7-816D-40BE-8D70-35A4ABA9D43A}"/>
+    <hyperlink ref="K402" r:id="rId17" xr:uid="{69A12BC5-7D82-4136-A0E7-F5E7EC34F8B0}"/>
+    <hyperlink ref="K410" r:id="rId18" xr:uid="{9442A440-660A-4576-B105-2AC531645C93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>
@@ -19673,6 +19645,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -19894,25 +19884,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19930,30 +19928,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixes from Berber 406
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED73BC78-4821-4604-BB94-7EA89325D916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070B7272-9CDE-4B8D-8E0C-9A42575C7542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="130" windowWidth="18800" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="220" windowWidth="15090" windowHeight="9980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3622" uniqueCount="1611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3627" uniqueCount="1612">
   <si>
     <t>Synonym(s)</t>
   </si>
@@ -4382,12 +4382,6 @@
     <t>documentVersions</t>
   </si>
   <si>
-    <t>A USDM relationship between the StudyVersion and StudyDefinitionDocumentVersion classes which identifies the version of the study protocol document associated with the study version.</t>
-  </si>
-  <si>
-    <t>A USDM relationship between the Study and StudyDefinitionDocument classes signifying that the study is documented in a study protocol document.</t>
-  </si>
-  <si>
     <t>C207413</t>
   </si>
   <si>
@@ -4932,6 +4926,15 @@
   </si>
   <si>
     <t>C202496</t>
+  </si>
+  <si>
+    <t>A USDM relationship between the StudyDefinitionDocumentVersion and GovernanceDate classes which provides the set of governance dates associated with the study definition document version.</t>
+  </si>
+  <si>
+    <t>A USDM relationship between the Study and StudyDefinitionDocument classes signifying that the study is documented in a study definition document.</t>
+  </si>
+  <si>
+    <t>A USDM relationship between the StudyVersion and StudyDefinitionDocumentVersion classes which identifies the version of the study definition document associated with the study version.</t>
   </si>
 </sst>
 </file>
@@ -5215,7 +5218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -5454,6 +5457,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -5468,21 +5477,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5922,7 +5916,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K458"/>
+  <dimension ref="A1:K459"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6080,7 +6074,7 @@
         <v>512</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>651</v>
@@ -6112,7 +6106,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="72" t="s">
-        <v>1428</v>
+        <v>1610</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>441</v>
@@ -6389,7 +6383,7 @@
         <v>512</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
       <c r="G16" s="46" t="s">
         <v>535</v>
@@ -7120,7 +7114,7 @@
         <v>512</v>
       </c>
       <c r="F43" s="74" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="G43" s="46" t="s">
         <v>536</v>
@@ -7149,7 +7143,7 @@
         <v>925</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>1051</v>
@@ -7265,7 +7259,7 @@
         <v>477</v>
       </c>
       <c r="F48" s="74" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>1190</v>
@@ -7294,7 +7288,7 @@
         <v>512</v>
       </c>
       <c r="F49" s="74" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
       <c r="G49" s="46" t="s">
         <v>1186</v>
@@ -7323,7 +7317,7 @@
         <v>1028</v>
       </c>
       <c r="F50" s="74" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
       <c r="G50" s="46" t="s">
         <v>1192</v>
@@ -7439,7 +7433,7 @@
         <v>477</v>
       </c>
       <c r="F54" s="74" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>507</v>
@@ -7470,7 +7464,7 @@
         <v>512</v>
       </c>
       <c r="F55" s="74" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="G55" s="46" t="s">
         <v>537</v>
@@ -7500,8 +7494,8 @@
       <c r="E56" s="43" t="s">
         <v>926</v>
       </c>
-      <c r="F56" s="85" t="s">
-        <v>1501</v>
+      <c r="F56" s="80" t="s">
+        <v>1499</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>999</v>
@@ -7532,7 +7526,7 @@
         <v>927</v>
       </c>
       <c r="F57" s="74" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>1206</v>
@@ -7564,8 +7558,8 @@
       <c r="E58" s="21" t="s">
         <v>916</v>
       </c>
-      <c r="F58" s="85" t="s">
-        <v>1503</v>
+      <c r="F58" s="80" t="s">
+        <v>1501</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>1001</v>
@@ -7596,7 +7590,7 @@
         <v>1013</v>
       </c>
       <c r="F59" s="74" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="G59" s="46" t="s">
         <v>1208</v>
@@ -7627,7 +7621,7 @@
         <v>985</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>1003</v>
@@ -7797,7 +7791,7 @@
         <v>330</v>
       </c>
       <c r="F66" s="74" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>844</v>
@@ -7859,7 +7853,7 @@
         <v>477</v>
       </c>
       <c r="F68" s="74" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>849</v>
@@ -7890,7 +7884,7 @@
         <v>512</v>
       </c>
       <c r="F69" s="74" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
       <c r="G69" s="46" t="s">
         <v>851</v>
@@ -8089,7 +8083,7 @@
         <v>330</v>
       </c>
       <c r="F76" s="74" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="G76" s="3" t="s">
         <v>813</v>
@@ -8151,7 +8145,7 @@
         <v>477</v>
       </c>
       <c r="F78" s="74" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="G78" s="3" t="s">
         <v>818</v>
@@ -8182,7 +8176,7 @@
         <v>512</v>
       </c>
       <c r="F79" s="74" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="G79" s="3" t="s">
         <v>820</v>
@@ -8546,8 +8540,8 @@
       <c r="E92" s="22" t="s">
         <v>512</v>
       </c>
-      <c r="F92" s="86" t="s">
-        <v>1512</v>
+      <c r="F92" s="81" t="s">
+        <v>1510</v>
       </c>
       <c r="G92" s="46" t="s">
         <v>538</v>
@@ -8744,7 +8738,7 @@
         <v>512</v>
       </c>
       <c r="F99" s="74" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="G99" s="46" t="s">
         <v>539</v>
@@ -9035,7 +9029,7 @@
         <v>512</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="G110" s="46" t="s">
         <v>540</v>
@@ -9122,7 +9116,7 @@
         <v>477</v>
       </c>
       <c r="F113" s="74" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="G113" s="3" t="s">
         <v>587</v>
@@ -9151,7 +9145,7 @@
         <v>512</v>
       </c>
       <c r="F114" s="74" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="G114" s="3" t="s">
         <v>589</v>
@@ -9180,7 +9174,7 @@
         <v>330</v>
       </c>
       <c r="F115" s="74" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
       <c r="G115" s="3" t="s">
         <v>591</v>
@@ -9296,7 +9290,7 @@
         <v>512</v>
       </c>
       <c r="F119" s="74" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="G119" s="46" t="s">
         <v>541</v>
@@ -9880,7 +9874,7 @@
         <v>512</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="G141" s="46" t="s">
         <v>542</v>
@@ -10054,7 +10048,7 @@
         <v>512</v>
       </c>
       <c r="F147" s="74" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="G147" s="46" t="s">
         <v>543</v>
@@ -10315,7 +10309,7 @@
       <c r="E157" s="22" t="s">
         <v>477</v>
       </c>
-      <c r="F157" s="87" t="s">
+      <c r="F157" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G157" s="3" t="s">
@@ -10344,7 +10338,7 @@
       <c r="E158" s="21" t="s">
         <v>478</v>
       </c>
-      <c r="F158" s="87" t="s">
+      <c r="F158" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G158" s="3" t="s">
@@ -10373,7 +10367,7 @@
       <c r="E159" s="21" t="s">
         <v>512</v>
       </c>
-      <c r="F159" s="87" t="s">
+      <c r="F159" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G159" s="3" t="s">
@@ -10461,7 +10455,7 @@
         <v>477</v>
       </c>
       <c r="F162" s="79" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="G162" s="3" t="s">
         <v>593</v>
@@ -10490,7 +10484,7 @@
         <v>512</v>
       </c>
       <c r="F163" s="74" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
       <c r="G163" s="3" t="s">
         <v>595</v>
@@ -10519,7 +10513,7 @@
         <v>330</v>
       </c>
       <c r="F164" s="74" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
       <c r="G164" s="46" t="s">
         <v>597</v>
@@ -10689,7 +10683,7 @@
         <v>512</v>
       </c>
       <c r="F170" s="74" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="G170" s="46" t="s">
         <v>544</v>
@@ -11365,7 +11359,7 @@
         <v>227</v>
       </c>
       <c r="F194" s="74" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="G194" s="3" t="s">
         <v>377</v>
@@ -11394,7 +11388,7 @@
         <v>512</v>
       </c>
       <c r="F195" s="74" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="G195" s="46" t="s">
         <v>545</v>
@@ -11423,7 +11417,7 @@
         <v>379</v>
       </c>
       <c r="F196" s="1" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
       <c r="G196" s="3" t="s">
         <v>380</v>
@@ -11501,8 +11495,8 @@
       <c r="E199" s="21" t="s">
         <v>477</v>
       </c>
-      <c r="F199" s="88" t="s">
-        <v>1608</v>
+      <c r="F199" s="1" t="s">
+        <v>1606</v>
       </c>
       <c r="G199" s="3" t="s">
         <v>382</v>
@@ -11530,8 +11524,8 @@
       <c r="E200" s="21" t="s">
         <v>732</v>
       </c>
-      <c r="F200" s="88" t="s">
-        <v>1609</v>
+      <c r="F200" s="1" t="s">
+        <v>1607</v>
       </c>
       <c r="G200" s="3" t="s">
         <v>384</v>
@@ -11559,8 +11553,8 @@
       <c r="E201" s="21" t="s">
         <v>733</v>
       </c>
-      <c r="F201" s="88" t="s">
-        <v>1610</v>
+      <c r="F201" s="1" t="s">
+        <v>1608</v>
       </c>
       <c r="G201" s="3" t="s">
         <v>386</v>
@@ -11647,7 +11641,7 @@
         <v>512</v>
       </c>
       <c r="F204" s="74" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="G204" s="46" t="s">
         <v>546</v>
@@ -11763,7 +11757,7 @@
         <v>402</v>
       </c>
       <c r="F208" s="74" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="G208" s="3" t="s">
         <v>1368</v>
@@ -11817,7 +11811,7 @@
         <v>477</v>
       </c>
       <c r="F210" s="74" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="G210" s="3" t="s">
         <v>397</v>
@@ -11904,7 +11898,7 @@
         <v>512</v>
       </c>
       <c r="F213" s="74" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="G213" s="46" t="s">
         <v>547</v>
@@ -12124,7 +12118,7 @@
         <v>512</v>
       </c>
       <c r="F221" s="74" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="G221" s="46" t="s">
         <v>548</v>
@@ -12184,7 +12178,7 @@
         <v>477</v>
       </c>
       <c r="F223" s="74" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="G223" s="1" t="s">
         <v>1144</v>
@@ -12215,7 +12209,7 @@
         <v>478</v>
       </c>
       <c r="F224" s="74" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="G224" s="1" t="s">
         <v>1146</v>
@@ -12246,7 +12240,7 @@
         <v>512</v>
       </c>
       <c r="F225" s="74" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="G225" s="1" t="s">
         <v>1148</v>
@@ -12460,7 +12454,7 @@
         <v>477</v>
       </c>
       <c r="F233" s="74" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
       <c r="G233" s="1" t="s">
         <v>1150</v>
@@ -12491,7 +12485,7 @@
         <v>478</v>
       </c>
       <c r="F234" s="74" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
       <c r="G234" s="1" t="s">
         <v>1152</v>
@@ -12522,7 +12516,7 @@
         <v>512</v>
       </c>
       <c r="F235" s="74" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="G235" s="1" t="s">
         <v>1154</v>
@@ -12659,7 +12653,7 @@
         <v>477</v>
       </c>
       <c r="F240" s="24" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="G240" s="1" t="s">
         <v>1156</v>
@@ -12688,7 +12682,7 @@
         <v>478</v>
       </c>
       <c r="F241" s="24" t="s">
-        <v>1529</v>
+        <v>1527</v>
       </c>
       <c r="G241" s="1" t="s">
         <v>1158</v>
@@ -12717,7 +12711,7 @@
         <v>512</v>
       </c>
       <c r="F242" s="24" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
       <c r="G242" s="1" t="s">
         <v>1160</v>
@@ -12941,7 +12935,7 @@
         <v>512</v>
       </c>
       <c r="F250" s="74" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
       <c r="G250" s="46" t="s">
         <v>549</v>
@@ -13219,7 +13213,7 @@
         <v>1217</v>
       </c>
       <c r="F260" s="74" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
       <c r="G260" s="41" t="s">
         <v>1218</v>
@@ -13335,7 +13329,7 @@
         <v>512</v>
       </c>
       <c r="F264" s="74" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
       <c r="G264" s="3" t="s">
         <v>509</v>
@@ -13364,7 +13358,7 @@
         <v>477</v>
       </c>
       <c r="F265" s="74" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
       <c r="G265" s="3" t="s">
         <v>510</v>
@@ -13393,7 +13387,7 @@
         <v>1165</v>
       </c>
       <c r="F266" s="74" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
       <c r="G266" s="41" t="s">
         <v>1166</v>
@@ -13472,7 +13466,7 @@
         <v>570</v>
       </c>
       <c r="F269" s="74" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="G269" s="3" t="s">
         <v>571</v>
@@ -13501,7 +13495,7 @@
         <v>501</v>
       </c>
       <c r="F270" s="74" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="G270" s="3" t="s">
         <v>503</v>
@@ -13530,7 +13524,7 @@
         <v>502</v>
       </c>
       <c r="F271" s="74" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
       <c r="G271" s="3" t="s">
         <v>505</v>
@@ -13559,7 +13553,7 @@
         <v>477</v>
       </c>
       <c r="F272" s="74" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
       <c r="G272" s="3" t="s">
         <v>573</v>
@@ -13587,7 +13581,7 @@
       <c r="E273" s="21" t="s">
         <v>1384</v>
       </c>
-      <c r="F273" s="87" t="s">
+      <c r="F273" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G273" s="3" t="s">
@@ -13616,7 +13610,7 @@
       <c r="E274" s="21" t="s">
         <v>1385</v>
       </c>
-      <c r="F274" s="87" t="s">
+      <c r="F274" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G274" s="3" t="s">
@@ -13746,7 +13740,7 @@
         <v>517</v>
       </c>
       <c r="F279" s="74" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="G279" s="3" t="s">
         <v>518</v>
@@ -13775,7 +13769,7 @@
         <v>477</v>
       </c>
       <c r="F280" s="74" t="s">
-        <v>1539</v>
+        <v>1537</v>
       </c>
       <c r="G280" s="3" t="s">
         <v>520</v>
@@ -13804,7 +13798,7 @@
         <v>330</v>
       </c>
       <c r="F281" s="74" t="s">
-        <v>1542</v>
+        <v>1540</v>
       </c>
       <c r="G281" s="3" t="s">
         <v>522</v>
@@ -13833,7 +13827,7 @@
         <v>478</v>
       </c>
       <c r="F282" s="74" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
       <c r="G282" s="46" t="s">
         <v>524</v>
@@ -13862,7 +13856,7 @@
         <v>512</v>
       </c>
       <c r="F283" s="74" t="s">
-        <v>1540</v>
+        <v>1538</v>
       </c>
       <c r="G283" s="46" t="s">
         <v>526</v>
@@ -13941,7 +13935,7 @@
         <v>527</v>
       </c>
       <c r="F286" s="74" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="G286" s="3" t="s">
         <v>528</v>
@@ -13970,7 +13964,7 @@
         <v>477</v>
       </c>
       <c r="F287" s="74" t="s">
-        <v>1543</v>
+        <v>1541</v>
       </c>
       <c r="G287" s="3" t="s">
         <v>530</v>
@@ -13999,7 +13993,7 @@
         <v>478</v>
       </c>
       <c r="F288" s="74" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
       <c r="G288" s="3" t="s">
         <v>532</v>
@@ -14028,7 +14022,7 @@
         <v>512</v>
       </c>
       <c r="F289" s="74" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
       <c r="G289" s="3" t="s">
         <v>534</v>
@@ -14144,7 +14138,7 @@
         <v>581</v>
       </c>
       <c r="F293" s="74" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
       <c r="G293" s="3" t="s">
         <v>585</v>
@@ -14175,7 +14169,7 @@
         <v>330</v>
       </c>
       <c r="F294" s="74" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
       <c r="G294" s="3" t="s">
         <v>805</v>
@@ -14206,7 +14200,7 @@
         <v>478</v>
       </c>
       <c r="F295" s="74" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="G295" s="46" t="s">
         <v>809</v>
@@ -14237,7 +14231,7 @@
         <v>477</v>
       </c>
       <c r="F296" s="74" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="G296" s="46" t="s">
         <v>807</v>
@@ -14268,7 +14262,7 @@
         <v>512</v>
       </c>
       <c r="F297" s="74" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
       <c r="G297" s="46" t="s">
         <v>811</v>
@@ -14401,7 +14395,7 @@
         <v>602</v>
       </c>
       <c r="F302" s="74" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
       <c r="G302" s="41" t="s">
         <v>605</v>
@@ -14430,7 +14424,7 @@
         <v>477</v>
       </c>
       <c r="F303" s="74" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="G303" s="3" t="s">
         <v>607</v>
@@ -14459,7 +14453,7 @@
         <v>478</v>
       </c>
       <c r="F304" s="74" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="G304" s="3" t="s">
         <v>609</v>
@@ -14488,7 +14482,7 @@
         <v>512</v>
       </c>
       <c r="F305" s="74" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="G305" s="3" t="s">
         <v>611</v>
@@ -14517,7 +14511,7 @@
         <v>603</v>
       </c>
       <c r="F306" s="74" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
       <c r="G306" s="3" t="s">
         <v>613</v>
@@ -14546,7 +14540,7 @@
         <v>514</v>
       </c>
       <c r="F307" s="74" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
       <c r="G307" s="3" t="s">
         <v>615</v>
@@ -14600,7 +14594,7 @@
         <v>617</v>
       </c>
       <c r="F309" s="24" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="G309" s="3" t="s">
         <v>627</v>
@@ -14631,7 +14625,7 @@
         <v>227</v>
       </c>
       <c r="F310" s="74" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
       <c r="G310" s="3" t="s">
         <v>630</v>
@@ -14662,7 +14656,7 @@
         <v>618</v>
       </c>
       <c r="F311" s="74" t="s">
-        <v>1557</v>
+        <v>1555</v>
       </c>
       <c r="G311" s="3" t="s">
         <v>632</v>
@@ -14691,7 +14685,7 @@
         <v>619</v>
       </c>
       <c r="F312" s="74" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
       <c r="G312" s="3" t="s">
         <v>634</v>
@@ -14720,7 +14714,7 @@
         <v>620</v>
       </c>
       <c r="F313" s="74" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
       <c r="G313" s="3" t="s">
         <v>636</v>
@@ -14751,7 +14745,7 @@
         <v>621</v>
       </c>
       <c r="F314" s="74" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
       <c r="G314" s="3" t="s">
         <v>639</v>
@@ -14780,7 +14774,7 @@
         <v>622</v>
       </c>
       <c r="F315" s="74" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
       <c r="G315" s="3" t="s">
         <v>641</v>
@@ -14938,7 +14932,7 @@
         <v>766</v>
       </c>
       <c r="F321" s="74" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
       <c r="G321" s="1" t="s">
         <v>767</v>
@@ -15029,7 +15023,7 @@
         <v>306</v>
       </c>
       <c r="F324" s="1" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
       <c r="G324" s="1" t="s">
         <v>307</v>
@@ -15144,7 +15138,7 @@
       <c r="G328" s="46"/>
       <c r="H328" s="46"/>
       <c r="I328" s="1" t="s">
-        <v>1427</v>
+        <v>1611</v>
       </c>
       <c r="J328" s="3" t="s">
         <v>441</v>
@@ -15266,7 +15260,7 @@
         <v>657</v>
       </c>
       <c r="F333" s="74" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="G333" s="1" t="s">
         <v>658</v>
@@ -15295,7 +15289,7 @@
         <v>514</v>
       </c>
       <c r="F334" s="74" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="G334" s="46" t="s">
         <v>660</v>
@@ -15324,7 +15318,7 @@
         <v>227</v>
       </c>
       <c r="F335" s="74" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="G335" s="46" t="s">
         <v>662</v>
@@ -15384,7 +15378,7 @@
         <v>665</v>
       </c>
       <c r="F337" s="74" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
       <c r="G337" s="3" t="s">
         <v>997</v>
@@ -15415,7 +15409,7 @@
         <v>514</v>
       </c>
       <c r="F338" s="74" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="G338" s="3" t="s">
         <v>866</v>
@@ -15446,7 +15440,7 @@
         <v>227</v>
       </c>
       <c r="F339" s="74" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
       <c r="G339" s="3" t="s">
         <v>868</v>
@@ -15475,7 +15469,7 @@
         <v>738</v>
       </c>
       <c r="F340" s="1" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
       <c r="G340" s="24" t="s">
         <v>739</v>
@@ -15506,7 +15500,7 @@
         <v>478</v>
       </c>
       <c r="F341" s="1" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="G341" s="24" t="s">
         <v>741</v>
@@ -15535,7 +15529,7 @@
         <v>203</v>
       </c>
       <c r="F342" s="1" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="G342" s="24" t="s">
         <v>742</v>
@@ -15564,7 +15558,7 @@
         <v>477</v>
       </c>
       <c r="F343" s="74" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="G343" s="1" t="s">
         <v>822</v>
@@ -15593,7 +15587,7 @@
         <v>512</v>
       </c>
       <c r="F344" s="74" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="G344" s="1" t="s">
         <v>824</v>
@@ -15622,7 +15616,7 @@
         <v>839</v>
       </c>
       <c r="F345" s="74" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="G345" s="1" t="s">
         <v>826</v>
@@ -15686,7 +15680,7 @@
         <v>840</v>
       </c>
       <c r="F347" s="74" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="G347" s="3" t="s">
         <v>833</v>
@@ -15746,7 +15740,7 @@
         <v>842</v>
       </c>
       <c r="F349" s="74" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="G349" s="3" t="s">
         <v>1004</v>
@@ -15854,7 +15848,7 @@
         <v>478</v>
       </c>
       <c r="F353" s="74" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
       <c r="G353" s="3" t="s">
         <v>776</v>
@@ -15883,7 +15877,7 @@
         <v>774</v>
       </c>
       <c r="F354" s="74" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="G354" s="3" t="s">
         <v>778</v>
@@ -15912,7 +15906,7 @@
         <v>775</v>
       </c>
       <c r="F355" s="74" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
       <c r="G355" s="32" t="s">
         <v>780</v>
@@ -15941,7 +15935,7 @@
         <v>665</v>
       </c>
       <c r="F356" s="74" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="G356" s="3" t="s">
         <v>989</v>
@@ -15999,7 +15993,7 @@
         <v>477</v>
       </c>
       <c r="F358" s="74" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="G358" s="3" t="s">
         <v>789</v>
@@ -16028,7 +16022,7 @@
         <v>478</v>
       </c>
       <c r="F359" s="74" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="G359" s="3" t="s">
         <v>791</v>
@@ -16057,7 +16051,7 @@
         <v>512</v>
       </c>
       <c r="F360" s="74" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="G360" s="3" t="s">
         <v>793</v>
@@ -16152,7 +16146,7 @@
         <v>804</v>
       </c>
       <c r="F363" s="24" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="G363" s="3" t="s">
         <v>990</v>
@@ -16351,7 +16345,7 @@
         <v>477</v>
       </c>
       <c r="F370" s="74" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="G370" s="3" t="s">
         <v>928</v>
@@ -16382,7 +16376,7 @@
         <v>478</v>
       </c>
       <c r="F371" s="74" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="G371" s="3" t="s">
         <v>930</v>
@@ -16413,7 +16407,7 @@
         <v>512</v>
       </c>
       <c r="F372" s="74" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="G372" s="3" t="s">
         <v>932</v>
@@ -16444,7 +16438,7 @@
         <v>916</v>
       </c>
       <c r="F373" s="74" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="G373" s="3" t="s">
         <v>1006</v>
@@ -16474,7 +16468,7 @@
       <c r="E374" s="21" t="s">
         <v>926</v>
       </c>
-      <c r="F374" s="89" t="s">
+      <c r="F374" s="24" t="s">
         <v>9</v>
       </c>
       <c r="G374" s="3" t="s">
@@ -16505,7 +16499,7 @@
       <c r="E375" s="21" t="s">
         <v>927</v>
       </c>
-      <c r="F375" s="89" t="s">
+      <c r="F375" s="24" t="s">
         <v>9</v>
       </c>
       <c r="G375" s="3" t="s">
@@ -16539,7 +16533,7 @@
         <v>985</v>
       </c>
       <c r="F376" s="74" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="G376" s="3" t="s">
         <v>1008</v>
@@ -16570,7 +16564,7 @@
         <v>1013</v>
       </c>
       <c r="F377" s="74" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="G377" s="46" t="s">
         <v>1014</v>
@@ -16709,7 +16703,7 @@
         <v>477</v>
       </c>
       <c r="F382" s="74" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="G382" s="3" t="s">
         <v>937</v>
@@ -16740,7 +16734,7 @@
         <v>330</v>
       </c>
       <c r="F383" s="74" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="G383" s="3" t="s">
         <v>939</v>
@@ -16771,7 +16765,7 @@
         <v>478</v>
       </c>
       <c r="F384" s="74" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="G384" s="3" t="s">
         <v>941</v>
@@ -16802,7 +16796,7 @@
         <v>512</v>
       </c>
       <c r="F385" s="74" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="G385" s="3" t="s">
         <v>943</v>
@@ -16885,7 +16879,7 @@
         <v>945</v>
       </c>
       <c r="F388" s="74" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
       <c r="G388" s="3" t="s">
         <v>946</v>
@@ -16914,7 +16908,7 @@
         <v>477</v>
       </c>
       <c r="F389" s="74" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="G389" s="3" t="s">
         <v>948</v>
@@ -16943,7 +16937,7 @@
         <v>478</v>
       </c>
       <c r="F390" s="74" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="G390" s="3" t="s">
         <v>950</v>
@@ -16972,7 +16966,7 @@
         <v>512</v>
       </c>
       <c r="F391" s="74" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="G391" s="3" t="s">
         <v>952</v>
@@ -17001,7 +16995,7 @@
         <v>916</v>
       </c>
       <c r="F392" s="74" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="G392" s="3" t="s">
         <v>993</v>
@@ -17030,7 +17024,7 @@
         <v>926</v>
       </c>
       <c r="F393" s="74" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="G393" s="3" t="s">
         <v>995</v>
@@ -17059,7 +17053,7 @@
         <v>927</v>
       </c>
       <c r="F394" s="74" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
       <c r="G394" s="3" t="s">
         <v>1009</v>
@@ -17091,7 +17085,7 @@
       <c r="E395" s="43" t="s">
         <v>985</v>
       </c>
-      <c r="F395" s="87" t="s">
+      <c r="F395" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G395" s="3" t="s">
@@ -17121,7 +17115,7 @@
         <v>1013</v>
       </c>
       <c r="F396" s="74" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="G396" s="46" t="s">
         <v>1036</v>
@@ -17318,7 +17312,7 @@
         <v>968</v>
       </c>
       <c r="F403" s="74" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
       <c r="G403" s="46" t="s">
         <v>969</v>
@@ -17378,7 +17372,7 @@
         <v>330</v>
       </c>
       <c r="F405" s="74" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="G405" s="3" t="s">
         <v>973</v>
@@ -17407,7 +17401,7 @@
         <v>514</v>
       </c>
       <c r="F406" s="74" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
       <c r="G406" s="3" t="s">
         <v>975</v>
@@ -17466,7 +17460,7 @@
         <v>477</v>
       </c>
       <c r="F408" s="74" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
       <c r="G408" s="3" t="s">
         <v>1019</v>
@@ -17496,7 +17490,7 @@
         <v>330</v>
       </c>
       <c r="F409" s="74" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
       <c r="G409" s="3" t="s">
         <v>1021</v>
@@ -17526,7 +17520,7 @@
         <v>478</v>
       </c>
       <c r="F410" s="74" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
       <c r="G410" s="32" t="s">
         <v>1023</v>
@@ -17556,7 +17550,7 @@
         <v>512</v>
       </c>
       <c r="F411" s="74" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
       <c r="G411" s="3" t="s">
         <v>1025</v>
@@ -17718,7 +17712,7 @@
         <v>478</v>
       </c>
       <c r="F417" s="74" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
       <c r="G417" s="3" t="s">
         <v>1031</v>
@@ -17747,7 +17741,7 @@
         <v>839</v>
       </c>
       <c r="F418" s="74" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
       <c r="G418" s="3" t="s">
         <v>1033</v>
@@ -17809,7 +17803,7 @@
         <v>746</v>
       </c>
       <c r="F420" s="74" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="G420" s="3" t="s">
         <v>1042</v>
@@ -17840,7 +17834,7 @@
         <v>581</v>
       </c>
       <c r="F421" s="74" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="G421" s="3" t="s">
         <v>1044</v>
@@ -17871,7 +17865,7 @@
         <v>477</v>
       </c>
       <c r="F422" s="74" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="G422" s="3" t="s">
         <v>1046</v>
@@ -17918,7 +17912,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="424" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A424" s="24">
         <v>423</v>
       </c>
@@ -17935,7 +17929,7 @@
         <v>512</v>
       </c>
       <c r="F424" s="74" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
       <c r="G424" s="3" t="s">
         <v>1048</v>
@@ -18045,7 +18039,7 @@
         <v>477</v>
       </c>
       <c r="F428" s="74" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="G428" s="3" t="s">
         <v>1062</v>
@@ -18074,7 +18068,7 @@
         <v>478</v>
       </c>
       <c r="F429" s="74" t="s">
-        <v>1604</v>
+        <v>1602</v>
       </c>
       <c r="G429" s="3" t="s">
         <v>1064</v>
@@ -18103,7 +18097,7 @@
         <v>512</v>
       </c>
       <c r="F430" s="74" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
       <c r="G430" s="3" t="s">
         <v>1066</v>
@@ -18157,7 +18151,7 @@
         <v>1169</v>
       </c>
       <c r="F432" s="24" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="G432" s="1" t="s">
         <v>1175</v>
@@ -18186,7 +18180,7 @@
         <v>1170</v>
       </c>
       <c r="F433" s="74" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
       <c r="G433" s="1" t="s">
         <v>1171</v>
@@ -18215,7 +18209,7 @@
         <v>729</v>
       </c>
       <c r="F434" s="74" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
       <c r="G434" s="1" t="s">
         <v>1173</v>
@@ -18355,7 +18349,7 @@
       <c r="E439" s="21" t="s">
         <v>330</v>
       </c>
-      <c r="F439" s="87" t="s">
+      <c r="F439" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G439" s="3" t="s">
@@ -18384,7 +18378,7 @@
       <c r="E440" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="F440" s="87" t="s">
+      <c r="F440" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G440" s="3" t="s">
@@ -18903,13 +18897,38 @@
       </c>
       <c r="K458" s="55"/>
     </row>
+    <row r="459" spans="1:11" ht="50" x14ac:dyDescent="0.35">
+      <c r="A459" s="24">
+        <v>459</v>
+      </c>
+      <c r="B459" s="1" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C459" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D459" s="24"/>
+      <c r="E459" s="34" t="s">
+        <v>643</v>
+      </c>
+      <c r="F459" s="3"/>
+      <c r="G459" s="3"/>
+      <c r="H459" s="3"/>
+      <c r="I459" s="1" t="s">
+        <v>1609</v>
+      </c>
+      <c r="J459" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="K459" s="55"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K458" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="F383">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G333">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F383">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="K35" r:id="rId1" xr:uid="{AAAD5805-A040-471F-BED3-41A48DF55291}"/>
@@ -18959,15 +18978,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="J1" s="5"/>
@@ -18977,17 +18996,17 @@
       <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="84" t="s">
         <v>159</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
@@ -18995,11 +19014,11 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="82" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
       <c r="F3" s="17"/>
@@ -19024,10 +19043,10 @@
       <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:14" s="6" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="85" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="84"/>
+      <c r="B5" s="86"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
@@ -19209,7 +19228,7 @@
         <v>514</v>
       </c>
       <c r="D11" s="76" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="E11" s="77" t="s">
         <v>1373</v>
@@ -19241,7 +19260,7 @@
         <v>514</v>
       </c>
       <c r="D12" s="76" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="E12" s="77" t="s">
         <v>1373</v>
@@ -19273,7 +19292,7 @@
         <v>514</v>
       </c>
       <c r="D13" s="76" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="E13" s="77" t="s">
         <v>1373</v>
@@ -19305,13 +19324,13 @@
         <v>514</v>
       </c>
       <c r="D14" s="77" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="E14" s="76" t="s">
         <v>1374</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="G14" s="13" t="s">
         <v>672</v>
@@ -19337,7 +19356,7 @@
         <v>514</v>
       </c>
       <c r="D15" s="77" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="E15" s="76" t="s">
         <v>1374</v>
@@ -19369,7 +19388,7 @@
         <v>839</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="E16" s="40" t="s">
         <v>1374</v>
@@ -19403,7 +19422,7 @@
         <v>839</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="E17" s="40" t="s">
         <v>1374</v>
@@ -19435,13 +19454,13 @@
         <v>839</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="E18" s="40" t="s">
         <v>1374</v>
       </c>
       <c r="F18" s="75" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="G18" s="50" t="s">
         <v>1132</v>
@@ -19467,7 +19486,7 @@
         <v>839</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="E19" s="40" t="s">
         <v>1374</v>
@@ -19499,7 +19518,7 @@
         <v>839</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="E20" s="40" t="s">
         <v>1374</v>
@@ -19750,13 +19769,13 @@
         <v>227</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="E28" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F28" s="75" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="G28" s="50" t="s">
         <v>1089</v>
@@ -19782,13 +19801,13 @@
         <v>227</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="E29" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F29" s="75" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="G29" s="50" t="s">
         <v>1087</v>
@@ -19814,13 +19833,13 @@
         <v>227</v>
       </c>
       <c r="D30" s="40" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="E30" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F30" s="75" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="G30" s="50" t="s">
         <v>1085</v>
@@ -19846,13 +19865,13 @@
         <v>227</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="E31" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F31" s="75" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="G31" s="50" t="s">
         <v>1096</v>
@@ -19878,13 +19897,13 @@
         <v>227</v>
       </c>
       <c r="D32" s="40" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="E32" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F32" s="75" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="G32" s="50" t="s">
         <v>1093</v>
@@ -19910,13 +19929,13 @@
         <v>227</v>
       </c>
       <c r="D33" s="40" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="E33" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F33" s="75" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="G33" s="50" t="s">
         <v>1079</v>
@@ -19942,13 +19961,13 @@
         <v>227</v>
       </c>
       <c r="D34" s="40" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="E34" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F34" s="75" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="G34" s="50" t="s">
         <v>1083</v>
@@ -19974,13 +19993,13 @@
         <v>227</v>
       </c>
       <c r="D35" s="40" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="E35" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F35" s="75" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="G35" s="50" t="s">
         <v>1091</v>
@@ -20001,13 +20020,13 @@
         <v>227</v>
       </c>
       <c r="D36" s="40" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="E36" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F36" s="75" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="G36" s="50" t="s">
         <v>1077</v>
@@ -20028,13 +20047,13 @@
         <v>227</v>
       </c>
       <c r="D37" s="40" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="E37" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F37" s="75" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="G37" s="50" t="s">
         <v>1081</v>
@@ -20055,13 +20074,13 @@
         <v>227</v>
       </c>
       <c r="D38" s="40" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="E38" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F38" s="75" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="G38" s="50" t="s">
         <v>1098</v>
@@ -20082,13 +20101,13 @@
         <v>227</v>
       </c>
       <c r="D39" s="40" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="E39" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F39" s="75" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="G39" s="50" t="s">
         <v>1095</v>
@@ -20109,13 +20128,13 @@
         <v>227</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="E40" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F40" s="75" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="G40" s="50" t="s">
         <v>1075</v>
@@ -20485,7 +20504,7 @@
         <v>925</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="E52" s="40" t="s">
         <v>1374</v>
@@ -20494,7 +20513,7 @@
         <v>1057</v>
       </c>
       <c r="G52" s="78" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="H52" s="50"/>
       <c r="I52" s="50" t="s">
@@ -20512,16 +20531,16 @@
         <v>925</v>
       </c>
       <c r="D53" s="40" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="E53" s="40" t="s">
         <v>1374</v>
       </c>
       <c r="F53" s="75" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="G53" s="78" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="H53" s="50" t="s">
         <v>1055</v>
@@ -20541,7 +20560,7 @@
         <v>925</v>
       </c>
       <c r="D54" s="40" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="E54" s="40" t="s">
         <v>1374</v>
@@ -20550,7 +20569,7 @@
         <v>1053</v>
       </c>
       <c r="G54" s="78" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="H54" s="50"/>
       <c r="I54" s="50" t="s">
@@ -20568,7 +20587,7 @@
         <v>840</v>
       </c>
       <c r="D55" s="40" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="E55" s="50" t="s">
         <v>1373</v>
@@ -20595,7 +20614,7 @@
         <v>840</v>
       </c>
       <c r="D56" s="40" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="E56" s="50" t="s">
         <v>1373</v>
@@ -20622,13 +20641,13 @@
         <v>839</v>
       </c>
       <c r="D57" s="40" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="E57" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F57" s="75" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="G57" s="50" t="s">
         <v>1118</v>
@@ -20649,7 +20668,7 @@
         <v>839</v>
       </c>
       <c r="D58" s="40" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="E58" s="50" t="s">
         <v>1373</v>
@@ -20676,7 +20695,7 @@
         <v>839</v>
       </c>
       <c r="D59" s="40" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="E59" s="50" t="s">
         <v>1373</v>
@@ -20703,7 +20722,7 @@
         <v>839</v>
       </c>
       <c r="D60" s="40" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="E60" s="50" t="s">
         <v>1373</v>
@@ -20730,7 +20749,7 @@
         <v>839</v>
       </c>
       <c r="D61" s="40" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="E61" s="50" t="s">
         <v>1373</v>
@@ -20757,7 +20776,7 @@
         <v>839</v>
       </c>
       <c r="D62" s="40" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="E62" s="50" t="s">
         <v>1373</v>
@@ -20784,7 +20803,7 @@
         <v>839</v>
       </c>
       <c r="D63" s="40" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="E63" s="50" t="s">
         <v>1373</v>
@@ -20811,13 +20830,13 @@
         <v>514</v>
       </c>
       <c r="D64" s="40" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="E64" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F64" s="75" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="G64" s="13" t="s">
         <v>977</v>
@@ -20840,13 +20859,13 @@
         <v>514</v>
       </c>
       <c r="D65" s="40" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="E65" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F65" s="75" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="G65" s="13" t="s">
         <v>979</v>
@@ -20867,13 +20886,13 @@
         <v>514</v>
       </c>
       <c r="D66" s="40" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="E66" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F66" s="75" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>981</v>
@@ -20894,13 +20913,13 @@
         <v>514</v>
       </c>
       <c r="D67" s="40" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="E67" s="50" t="s">
         <v>1373</v>
       </c>
       <c r="F67" s="75" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>983</v>
@@ -20921,7 +20940,7 @@
         <v>514</v>
       </c>
       <c r="D68" s="40" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="E68" s="50" t="s">
         <v>1373</v>
@@ -21174,7 +21193,7 @@
     <mergeCell ref="A5:B5"/>
   </mergeCells>
   <conditionalFormatting sqref="G18">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -21182,24 +21201,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -21421,33 +21422,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21465,4 +21458,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates to Abbreviation Class
based on DIH QA
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DE89ED-232A-4C9D-BD94-5BAC9E56BF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EDBB58-1E4A-4A8E-9124-0DE0CF8C9E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="950" yWindow="410" windowWidth="17870" windowHeight="9880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2370" yWindow="0" windowWidth="15260" windowHeight="9860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3667" uniqueCount="1633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3665" uniqueCount="1631">
   <si>
     <t>Synonym(s)</t>
   </si>
@@ -4943,12 +4943,6 @@
     <t>A USDM relationship between the StudyDefinitionDocument and StudyDefinitionDocumentVersion classes which identifies the set of versions associated with the study definition document.</t>
   </si>
   <si>
-    <t>abbreviation</t>
-  </si>
-  <si>
-    <t>longName</t>
-  </si>
-  <si>
     <t>Abbreviation</t>
   </si>
   <si>
@@ -4958,12 +4952,6 @@
     <t>A set of letters that are drawn from a word or from a sequence of words and that are used for brevity in place of the full word or phrase. (CDISC Glossary)</t>
   </si>
   <si>
-    <t>Y (Point to CDISC Glossary)</t>
-  </si>
-  <si>
-    <t>https://www.cdisc.org/standards/glossary#standard__versions</t>
-  </si>
-  <si>
     <t>Abbreviation Long Name</t>
   </si>
   <si>
@@ -4977,6 +4965,12 @@
   </si>
   <si>
     <t>A USDM relationship between the StudyVersion and Abbreviation classes which provides the set of abbreviations associated with the study version.</t>
+  </si>
+  <si>
+    <t>abbreviatedText</t>
+  </si>
+  <si>
+    <t>expandedText</t>
   </si>
 </sst>
 </file>
@@ -5508,6 +5502,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -5522,9 +5519,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -15319,13 +15313,13 @@
       </c>
       <c r="D333" s="3"/>
       <c r="E333" s="34" t="s">
-        <v>1631</v>
+        <v>1627</v>
       </c>
       <c r="F333" s="41"/>
       <c r="G333" s="46"/>
       <c r="H333" s="46"/>
       <c r="I333" s="3" t="s">
-        <v>1632</v>
+        <v>1628</v>
       </c>
       <c r="J333" s="3" t="s">
         <v>426</v>
@@ -19014,24 +19008,24 @@
         <v>461</v>
       </c>
       <c r="B461" s="24" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
       <c r="C461" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D461" s="24"/>
-      <c r="E461" s="88" t="s">
-        <v>1623</v>
+      <c r="E461" s="83" t="s">
+        <v>1621</v>
       </c>
       <c r="F461" s="3" t="s">
-        <v>1624</v>
+        <v>1622</v>
       </c>
       <c r="G461" s="3" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
       <c r="H461" s="3"/>
       <c r="I461" s="3" t="s">
-        <v>1625</v>
+        <v>1623</v>
       </c>
       <c r="J461" s="3" t="s">
         <v>426</v>
@@ -19043,69 +19037,65 @@
         <v>462</v>
       </c>
       <c r="B462" s="24" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
       <c r="C462" s="3" t="s">
         <v>939</v>
       </c>
       <c r="D462" s="24"/>
       <c r="E462" s="21" t="s">
+        <v>1629</v>
+      </c>
+      <c r="F462" s="3" t="s">
+        <v>1622</v>
+      </c>
+      <c r="G462" s="3" t="s">
         <v>1621</v>
-      </c>
-      <c r="F462" s="3" t="s">
-        <v>1624</v>
-      </c>
-      <c r="G462" s="3" t="s">
-        <v>1623</v>
       </c>
       <c r="H462" s="3"/>
       <c r="I462" s="3" t="s">
-        <v>1625</v>
+        <v>1623</v>
       </c>
       <c r="J462" s="3" t="s">
-        <v>1626</v>
-      </c>
-      <c r="K462" s="46" t="s">
-        <v>1627</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="K462" s="46"/>
     </row>
     <row r="463" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A463" s="24">
         <v>463</v>
       </c>
       <c r="B463" s="24" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
       <c r="C463" s="3" t="s">
         <v>939</v>
       </c>
       <c r="D463" s="24"/>
       <c r="E463" s="21" t="s">
-        <v>1622</v>
+        <v>1630</v>
       </c>
       <c r="F463" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G463" s="3" t="s">
-        <v>1628</v>
+        <v>1624</v>
       </c>
       <c r="H463" s="3"/>
       <c r="I463" s="3" t="s">
-        <v>1629</v>
+        <v>1625</v>
       </c>
       <c r="J463" s="3" t="s">
-        <v>1626</v>
-      </c>
-      <c r="K463" s="46" t="s">
-        <v>1627</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="K463" s="46"/>
     </row>
     <row r="464" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A464" s="24">
         <v>464</v>
       </c>
       <c r="B464" s="24" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
       <c r="C464" s="3" t="s">
         <v>195</v>
@@ -19118,7 +19108,7 @@
       <c r="G464" s="3"/>
       <c r="H464" s="3"/>
       <c r="I464" s="3" t="s">
-        <v>1630</v>
+        <v>1626</v>
       </c>
       <c r="J464" s="3" t="s">
         <v>426</v>
@@ -19181,15 +19171,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="84" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="J1" s="5"/>
@@ -19199,17 +19189,17 @@
       <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
@@ -19217,11 +19207,11 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="84" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
       <c r="F3" s="17"/>
@@ -19246,10 +19236,10 @@
       <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:14" s="6" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="86" t="s">
+      <c r="A5" s="87" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="87"/>
+      <c r="B5" s="88"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
@@ -21404,24 +21394,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -21643,10 +21615,40 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -21670,21 +21672,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ticket 420 additional edits
change relationship name identifierScope to scope
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E365F160-2398-47D3-BA4A-5B79E6513228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C113B1-4341-4C4C-AEB0-0F401ABD287D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="16840" windowHeight="10070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="16840" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -4964,9 +4964,6 @@
     <t>expandedText</t>
   </si>
   <si>
-    <t>identifierScope</t>
-  </si>
-  <si>
     <t>Identifier</t>
   </si>
   <si>
@@ -5043,6 +5040,9 @@
   </si>
   <si>
     <t>A document that describes the collection of clinical studies that are to be performed in sequence, or in parallel, with a particular active substance, device, procedure, or treatment strategy, typically with the intention of submitting them as part of an application for a marketing authorization. (CDISC Glossary)</t>
+  </si>
+  <si>
+    <t>scope</t>
   </si>
 </sst>
 </file>
@@ -5577,6 +5577,12 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -5591,12 +5597,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6298,7 +6298,7 @@
         <v>74</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>313</v>
@@ -6307,11 +6307,11 @@
         <v>9</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>73</v>
@@ -6329,16 +6329,16 @@
         <v>193</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>1628</v>
+        <v>1654</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>424</v>
@@ -15420,13 +15420,13 @@
       </c>
       <c r="D334" s="3"/>
       <c r="E334" s="42" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="F334" s="41"/>
       <c r="G334" s="46"/>
       <c r="H334" s="46"/>
       <c r="I334" s="3" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="J334" s="3" t="s">
         <v>424</v>
@@ -19227,24 +19227,24 @@
         <v>466</v>
       </c>
       <c r="B466" s="24" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="C466" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D466" s="24"/>
       <c r="E466" s="83" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="F466" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G466" s="3" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="H466" s="3"/>
       <c r="I466" s="1" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="J466" s="3" t="s">
         <v>424</v>
@@ -19255,7 +19255,7 @@
         <v>467</v>
       </c>
       <c r="B467" s="24" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="C467" s="3" t="s">
         <v>937</v>
@@ -19268,11 +19268,11 @@
         <v>9</v>
       </c>
       <c r="G467" s="3" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="H467" s="3"/>
       <c r="I467" s="3" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="J467" s="3" t="s">
         <v>1357</v>
@@ -19283,13 +19283,13 @@
         <v>468</v>
       </c>
       <c r="B468" s="24" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="C468" s="24" t="s">
         <v>74</v>
       </c>
       <c r="D468" s="3" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="E468" s="21" t="s">
         <v>313</v>
@@ -19298,11 +19298,11 @@
         <v>9</v>
       </c>
       <c r="G468" s="3" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="H468" s="3"/>
       <c r="I468" s="3" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="J468" s="3" t="s">
         <v>73</v>
@@ -19313,24 +19313,24 @@
         <v>469</v>
       </c>
       <c r="B469" s="24" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="C469" s="3" t="s">
         <v>193</v>
       </c>
       <c r="D469" s="3" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="E469" s="31" t="s">
-        <v>1628</v>
+        <v>1654</v>
       </c>
       <c r="F469" s="24"/>
       <c r="G469" s="24"/>
       <c r="H469" s="24"/>
       <c r="I469" s="3" t="s">
-        <v>1641</v>
-      </c>
-      <c r="J469" s="89" t="s">
+        <v>1640</v>
+      </c>
+      <c r="J469" s="84" t="s">
         <v>424</v>
       </c>
     </row>
@@ -19339,24 +19339,24 @@
         <v>470</v>
       </c>
       <c r="B470" s="24" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="C470" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D470" s="24"/>
       <c r="E470" s="83" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="F470" s="3" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="G470" s="3" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="H470" s="3"/>
       <c r="I470" s="3" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="J470" s="3" t="s">
         <v>424</v>
@@ -19367,24 +19367,24 @@
         <v>471</v>
       </c>
       <c r="B471" s="24" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="C471" s="24" t="s">
         <v>74</v>
       </c>
       <c r="D471" s="24"/>
-      <c r="E471" s="90" t="s">
+      <c r="E471" s="85" t="s">
         <v>313</v>
       </c>
       <c r="F471" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G471" s="3" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="H471" s="3"/>
       <c r="I471" s="3" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="J471" s="3" t="s">
         <v>73</v>
@@ -19395,20 +19395,20 @@
         <v>472</v>
       </c>
       <c r="B472" s="24" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="C472" s="3" t="s">
         <v>193</v>
       </c>
       <c r="D472" s="24"/>
       <c r="E472" s="31" t="s">
-        <v>1628</v>
+        <v>1654</v>
       </c>
       <c r="F472" s="3"/>
       <c r="G472" s="3"/>
       <c r="H472" s="3"/>
       <c r="I472" s="3" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="J472" s="3" t="s">
         <v>73</v>
@@ -19470,15 +19470,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="86" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="J1" s="5"/>
@@ -19488,17 +19488,17 @@
       <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
@@ -19506,11 +19506,11 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" s="6" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="86" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
       <c r="F3" s="17"/>
@@ -19535,10 +19535,10 @@
       <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:14" s="6" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="89" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="88"/>
+      <c r="B5" s="90"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
@@ -21677,7 +21677,7 @@
         <v>108</v>
       </c>
       <c r="B76" s="51" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="C76" s="13" t="s">
         <v>488</v>
@@ -21692,13 +21692,13 @@
         <v>9</v>
       </c>
       <c r="G76" s="13" t="s">
+        <v>1647</v>
+      </c>
+      <c r="H76" s="13" t="s">
         <v>1648</v>
       </c>
-      <c r="H76" s="13" t="s">
+      <c r="I76" s="13" t="s">
         <v>1649</v>
-      </c>
-      <c r="I76" s="13" t="s">
-        <v>1650</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="62.5" x14ac:dyDescent="0.35">
@@ -21706,7 +21706,7 @@
         <v>108</v>
       </c>
       <c r="B77" s="51" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="C77" s="13" t="s">
         <v>488</v>
@@ -21718,16 +21718,16 @@
         <v>1323</v>
       </c>
       <c r="F77" s="13" t="s">
+        <v>1650</v>
+      </c>
+      <c r="G77" s="13" t="s">
         <v>1651</v>
       </c>
-      <c r="G77" s="13" t="s">
+      <c r="H77" s="13" t="s">
         <v>1652</v>
       </c>
-      <c r="H77" s="13" t="s">
+      <c r="I77" s="13" t="s">
         <v>1653</v>
-      </c>
-      <c r="I77" s="13" t="s">
-        <v>1654</v>
       </c>
     </row>
   </sheetData>
@@ -21751,24 +21751,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -21990,10 +21972,40 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -22017,21 +22029,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Richard Marshall QC fixes
ticket 444
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F7797B-176E-4A5E-BC5B-B0A5A991554F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8646F4B0-CDEB-4260-83BB-715BA22E775E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1350" yWindow="40" windowWidth="16440" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2050" yWindow="0" windowWidth="14710" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3964" uniqueCount="1736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3965" uniqueCount="1736">
   <si>
     <t>Synonym(s)</t>
   </si>
@@ -19275,7 +19275,7 @@
     </row>
     <row r="459" spans="1:11" ht="50" x14ac:dyDescent="0.35">
       <c r="A459" s="24">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B459" s="1" t="s">
         <v>1337</v>
@@ -19300,7 +19300,7 @@
     </row>
     <row r="460" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A460" s="24">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B460" s="1" t="s">
         <v>1337</v>
@@ -19325,7 +19325,7 @@
     </row>
     <row r="461" spans="1:11" ht="50" x14ac:dyDescent="0.35">
       <c r="A461" s="24">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B461" s="1" t="s">
         <v>1337</v>
@@ -19350,7 +19350,7 @@
     </row>
     <row r="462" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A462" s="24">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B462" s="24" t="s">
         <v>1593</v>
@@ -19379,7 +19379,7 @@
     </row>
     <row r="463" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A463" s="24">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B463" s="24" t="s">
         <v>1593</v>
@@ -19408,7 +19408,7 @@
     </row>
     <row r="464" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A464" s="24">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B464" s="24" t="s">
         <v>1593</v>
@@ -19437,7 +19437,7 @@
     </row>
     <row r="465" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A465" s="24">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B465" s="24" t="s">
         <v>1593</v>
@@ -19462,7 +19462,7 @@
     </row>
     <row r="466" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A466" s="24">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B466" s="24" t="s">
         <v>1608</v>
@@ -19491,7 +19491,7 @@
     </row>
     <row r="467" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A467" s="24">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B467" s="24" t="s">
         <v>1608</v>
@@ -19520,7 +19520,7 @@
     </row>
     <row r="468" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A468" s="24">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B468" s="24" t="s">
         <v>1608</v>
@@ -19551,7 +19551,7 @@
     </row>
     <row r="469" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A469" s="24">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B469" s="24" t="s">
         <v>1608</v>
@@ -19578,7 +19578,7 @@
     </row>
     <row r="470" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A470" s="24">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B470" s="24" t="s">
         <v>1603</v>
@@ -19607,7 +19607,7 @@
     </row>
     <row r="471" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A471" s="24">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B471" s="24" t="s">
         <v>1603</v>
@@ -19636,7 +19636,7 @@
     </row>
     <row r="472" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A472" s="24">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B472" s="24" t="s">
         <v>1603</v>
@@ -19661,7 +19661,7 @@
     </row>
     <row r="473" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A473" s="24">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B473" s="46" t="s">
         <v>1631</v>
@@ -19690,7 +19690,7 @@
     </row>
     <row r="474" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A474" s="24">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B474" s="46" t="s">
         <v>1631</v>
@@ -19719,7 +19719,7 @@
     </row>
     <row r="475" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A475" s="24">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B475" s="46" t="s">
         <v>1631</v>
@@ -19748,7 +19748,7 @@
     </row>
     <row r="476" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A476" s="24">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B476" s="46" t="s">
         <v>1631</v>
@@ -19777,7 +19777,7 @@
     </row>
     <row r="477" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A477" s="24">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B477" s="46" t="s">
         <v>1631</v>
@@ -19808,7 +19808,7 @@
     </row>
     <row r="478" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A478" s="24">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B478" s="46" t="s">
         <v>1631</v>
@@ -19839,7 +19839,7 @@
     </row>
     <row r="479" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A479" s="24">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B479" s="46" t="s">
         <v>1631</v>
@@ -19864,7 +19864,7 @@
     </row>
     <row r="480" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A480" s="24">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B480" s="46" t="s">
         <v>1631</v>
@@ -19889,7 +19889,7 @@
     </row>
     <row r="481" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A481" s="24">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B481" s="46" t="s">
         <v>1631</v>
@@ -19914,7 +19914,7 @@
     </row>
     <row r="482" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A482" s="24">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B482" s="46" t="s">
         <v>1631</v>
@@ -19939,7 +19939,7 @@
     </row>
     <row r="483" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A483" s="24">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B483" s="46" t="s">
         <v>1632</v>
@@ -19968,7 +19968,7 @@
     </row>
     <row r="484" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A484" s="24">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B484" s="46" t="s">
         <v>1632</v>
@@ -19999,7 +19999,7 @@
     </row>
     <row r="485" spans="1:11" ht="50" x14ac:dyDescent="0.35">
       <c r="A485" s="24">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B485" s="3" t="s">
         <v>1632</v>
@@ -20026,7 +20026,7 @@
     </row>
     <row r="486" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A486" s="24">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B486" s="46" t="s">
         <v>1658</v>
@@ -20055,7 +20055,7 @@
     </row>
     <row r="487" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A487" s="24">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B487" s="46" t="s">
         <v>1658</v>
@@ -20084,7 +20084,7 @@
     </row>
     <row r="488" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A488" s="24">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B488" s="46" t="s">
         <v>1658</v>
@@ -20113,7 +20113,7 @@
     </row>
     <row r="489" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A489" s="24">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B489" s="46" t="s">
         <v>1658</v>
@@ -20142,7 +20142,7 @@
     </row>
     <row r="490" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A490" s="24">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B490" s="46" t="s">
         <v>1658</v>
@@ -20171,7 +20171,7 @@
     </row>
     <row r="491" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A491" s="24">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B491" s="46" t="s">
         <v>1669</v>
@@ -20200,7 +20200,7 @@
     </row>
     <row r="492" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A492" s="24">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B492" s="46" t="s">
         <v>1669</v>
@@ -20229,7 +20229,7 @@
     </row>
     <row r="493" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A493" s="24">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B493" s="46" t="s">
         <v>1669</v>
@@ -20258,7 +20258,7 @@
     </row>
     <row r="494" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A494" s="24">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B494" s="46" t="s">
         <v>1669</v>
@@ -20287,7 +20287,7 @@
     </row>
     <row r="495" spans="1:11" ht="62.5" x14ac:dyDescent="0.35">
       <c r="A495" s="24">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B495" s="46" t="s">
         <v>1669</v>
@@ -20316,7 +20316,7 @@
     </row>
     <row r="496" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A496" s="24">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B496" s="46" t="s">
         <v>1669</v>
@@ -20341,7 +20341,7 @@
     </row>
     <row r="497" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A497" s="24">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B497" s="46" t="s">
         <v>1669</v>
@@ -20366,7 +20366,7 @@
     </row>
     <row r="498" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A498" s="24">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B498" s="3" t="s">
         <v>1670</v>
@@ -20395,7 +20395,7 @@
     </row>
     <row r="499" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A499" s="24">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B499" s="3" t="s">
         <v>1670</v>
@@ -20424,7 +20424,7 @@
     </row>
     <row r="500" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A500" s="24">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B500" s="3" t="s">
         <v>1670</v>
@@ -20453,7 +20453,7 @@
     </row>
     <row r="501" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A501" s="24">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B501" s="3" t="s">
         <v>1670</v>
@@ -20482,7 +20482,7 @@
     </row>
     <row r="502" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A502" s="24">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B502" s="3" t="s">
         <v>1670</v>
@@ -20507,7 +20507,7 @@
     </row>
     <row r="503" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A503" s="24">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B503" s="3" t="s">
         <v>1670</v>
@@ -20532,7 +20532,7 @@
     </row>
     <row r="504" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A504" s="24">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B504" s="46" t="s">
         <v>1671</v>
@@ -20561,7 +20561,7 @@
     </row>
     <row r="505" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A505" s="24">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B505" s="46" t="s">
         <v>1671</v>
@@ -20592,7 +20592,7 @@
     </row>
     <row r="506" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A506" s="24">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B506" s="46" t="s">
         <v>1671</v>
@@ -20610,7 +20610,9 @@
       <c r="I506" s="3" t="s">
         <v>1704</v>
       </c>
-      <c r="J506" s="46"/>
+      <c r="J506" s="3" t="s">
+        <v>424</v>
+      </c>
       <c r="K506" s="46"/>
     </row>
   </sheetData>
@@ -22977,15 +22979,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -23207,6 +23200,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -23217,24 +23219,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23254,6 +23238,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
updated codelist info for C66726
Added 'SDTM Terminology Codelist' in front of the codelist c-code in Has Value List column. Also updated in the changes file.
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC02AB8E-1F25-492B-A36D-03791CE7FD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794EE37E-F9E3-445C-92A0-58CF11CA34F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2050" yWindow="0" windowWidth="14710" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5021,9 +5021,6 @@
     <t>The physical form in which active and/or inert ingredient(s) are presented.</t>
   </si>
   <si>
-    <t>Y (C66726)</t>
-  </si>
-  <si>
     <t>A USDM relationship between the AdministrableProductn and CommentAnnotation classes which provides the set of notes related to the administrable product.</t>
   </si>
   <si>
@@ -5283,6 +5280,9 @@
   </si>
   <si>
     <t>A characterization or classification of the study governance date.</t>
+  </si>
+  <si>
+    <t>Y (SDTM Terminology Codelist C66726)</t>
   </si>
 </sst>
 </file>
@@ -7514,7 +7514,7 @@
         <v>989</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="K44" s="46"/>
     </row>
@@ -14918,14 +14918,14 @@
         <v>1474</v>
       </c>
       <c r="G307" s="3" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="H307" s="46"/>
       <c r="I307" s="3" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="J307" s="3" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="K307" s="24"/>
     </row>
@@ -15012,7 +15012,7 @@
         <v>595</v>
       </c>
       <c r="J310" s="3" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="K310" s="24"/>
     </row>
@@ -15724,7 +15724,7 @@
         <v>619</v>
       </c>
       <c r="J336" s="3" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="K336" s="24"/>
     </row>
@@ -16053,7 +16053,7 @@
         <v>769</v>
       </c>
       <c r="J347" s="3" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="K347" s="24"/>
     </row>
@@ -16115,7 +16115,7 @@
         <v>775</v>
       </c>
       <c r="J349" s="3" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="K349" s="24"/>
     </row>
@@ -16348,24 +16348,24 @@
         <v>357</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="C358" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D358" s="3"/>
       <c r="E358" s="53" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="F358" s="1" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="G358" s="3" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="H358" s="46"/>
       <c r="I358" s="3" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="J358" s="3" t="s">
         <v>424</v>
@@ -16377,7 +16377,7 @@
         <v>358</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="C359" s="3" t="s">
         <v>74</v>
@@ -16390,11 +16390,11 @@
         <v>1388</v>
       </c>
       <c r="G359" s="3" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="H359" s="46"/>
       <c r="I359" s="3" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="J359" s="3" t="s">
         <v>73</v>
@@ -16406,7 +16406,7 @@
         <v>359</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="C360" s="3" t="s">
         <v>74</v>
@@ -16419,11 +16419,11 @@
         <v>1389</v>
       </c>
       <c r="G360" s="3" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="H360" s="46"/>
       <c r="I360" s="3" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="J360" s="3" t="s">
         <v>73</v>
@@ -16435,7 +16435,7 @@
         <v>360</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="C361" s="3" t="s">
         <v>74</v>
@@ -16448,11 +16448,11 @@
         <v>1390</v>
       </c>
       <c r="G361" s="3" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="H361" s="46"/>
       <c r="I361" s="3" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="J361" s="3" t="s">
         <v>73</v>
@@ -16464,7 +16464,7 @@
         <v>361</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="C362" s="3" t="s">
         <v>924</v>
@@ -16497,7 +16497,7 @@
         <v>362</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="C363" s="3" t="s">
         <v>924</v>
@@ -16530,7 +16530,7 @@
         <v>363</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="C364" s="1" t="s">
         <v>924</v>
@@ -16543,7 +16543,7 @@
         <v>1391</v>
       </c>
       <c r="G364" s="3" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="H364" s="3"/>
       <c r="I364" s="3" t="s">
@@ -16559,7 +16559,7 @@
         <v>364</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="C365" s="1" t="s">
         <v>193</v>
@@ -16572,7 +16572,7 @@
       <c r="G365" s="3"/>
       <c r="H365" s="3"/>
       <c r="I365" s="1" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="J365" s="3" t="s">
         <v>424</v>
@@ -16584,7 +16584,7 @@
         <v>365</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="C366" s="1" t="s">
         <v>193</v>
@@ -16597,7 +16597,7 @@
       <c r="G366" s="3"/>
       <c r="H366" s="3"/>
       <c r="I366" s="3" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="J366" s="3" t="s">
         <v>424</v>
@@ -16609,7 +16609,7 @@
         <v>366</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="C367" s="1" t="s">
         <v>193</v>
@@ -16622,7 +16622,7 @@
       <c r="G367" s="46"/>
       <c r="H367" s="3"/>
       <c r="I367" s="3" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="J367" s="3" t="s">
         <v>424</v>
@@ -17830,7 +17830,7 @@
         <v>914</v>
       </c>
       <c r="J408" s="3" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="K408" s="24"/>
     </row>
@@ -18176,7 +18176,7 @@
         <v>972</v>
       </c>
       <c r="J420" s="3" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="K420" s="1"/>
     </row>
@@ -19102,7 +19102,7 @@
         <v>1332</v>
       </c>
       <c r="J452" s="3" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="K452" s="46"/>
     </row>
@@ -19511,7 +19511,7 @@
         <v>1612</v>
       </c>
       <c r="J467" s="3" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="K467" s="1"/>
     </row>
@@ -19799,7 +19799,7 @@
         <v>1646</v>
       </c>
       <c r="J477" s="3" t="s">
-        <v>1647</v>
+        <v>1734</v>
       </c>
       <c r="K477" s="1"/>
     </row>
@@ -19830,7 +19830,7 @@
         <v>778</v>
       </c>
       <c r="J478" s="3" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="K478" s="1"/>
     </row>
@@ -19852,7 +19852,7 @@
       <c r="G479" s="3"/>
       <c r="H479" s="3"/>
       <c r="I479" s="3" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="J479" s="3" t="s">
         <v>424</v>
@@ -19877,7 +19877,7 @@
       <c r="G480" s="3"/>
       <c r="H480" s="3"/>
       <c r="I480" s="3" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="J480" s="3" t="s">
         <v>424</v>
@@ -19902,7 +19902,7 @@
       <c r="G481" s="3"/>
       <c r="H481" s="3"/>
       <c r="I481" s="3" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="J481" s="3" t="s">
         <v>424</v>
@@ -19927,7 +19927,7 @@
       <c r="G482" s="3"/>
       <c r="H482" s="3"/>
       <c r="I482" s="3" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="J482" s="3" t="s">
         <v>424</v>
@@ -19952,11 +19952,11 @@
         <v>9</v>
       </c>
       <c r="G483" s="3" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="H483" s="3"/>
       <c r="I483" s="1" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="J483" s="3" t="s">
         <v>424</v>
@@ -19983,11 +19983,11 @@
         <v>9</v>
       </c>
       <c r="G484" s="3" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="H484" s="3"/>
       <c r="I484" s="3" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="J484" s="3" t="s">
         <v>73</v>
@@ -20014,7 +20014,7 @@
       <c r="G485" s="3"/>
       <c r="H485" s="3"/>
       <c r="I485" s="3" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="J485" s="3" t="s">
         <v>424</v>
@@ -20026,24 +20026,24 @@
         <v>485</v>
       </c>
       <c r="B486" s="46" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="C486" s="46" t="s">
         <v>3</v>
       </c>
       <c r="D486" s="24"/>
       <c r="E486" s="83" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="F486" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G486" s="3" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="H486" s="3"/>
       <c r="I486" s="3" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="J486" s="3" t="s">
         <v>424</v>
@@ -20055,7 +20055,7 @@
         <v>486</v>
       </c>
       <c r="B487" s="46" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="C487" s="46" t="s">
         <v>74</v>
@@ -20068,11 +20068,11 @@
         <v>9</v>
       </c>
       <c r="G487" s="3" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="H487" s="3"/>
       <c r="I487" s="3" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="J487" s="3" t="s">
         <v>73</v>
@@ -20084,7 +20084,7 @@
         <v>487</v>
       </c>
       <c r="B488" s="46" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="C488" s="46" t="s">
         <v>74</v>
@@ -20097,11 +20097,11 @@
         <v>9</v>
       </c>
       <c r="G488" s="3" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="H488" s="3"/>
       <c r="I488" s="3" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="J488" s="3" t="s">
         <v>73</v>
@@ -20113,7 +20113,7 @@
         <v>488</v>
       </c>
       <c r="B489" s="46" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="C489" s="3" t="s">
         <v>924</v>
@@ -20126,11 +20126,11 @@
         <v>9</v>
       </c>
       <c r="G489" s="3" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="H489" s="3"/>
       <c r="I489" s="3" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="J489" s="3" t="s">
         <v>73</v>
@@ -20142,7 +20142,7 @@
         <v>489</v>
       </c>
       <c r="B490" s="46" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="C490" s="3" t="s">
         <v>924</v>
@@ -20155,14 +20155,14 @@
         <v>9</v>
       </c>
       <c r="G490" s="3" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="H490" s="3"/>
       <c r="I490" s="1" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="J490" s="3" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="K490" s="46"/>
     </row>
@@ -20171,24 +20171,24 @@
         <v>490</v>
       </c>
       <c r="B491" s="46" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="C491" s="46" t="s">
         <v>3</v>
       </c>
       <c r="D491" s="24"/>
       <c r="E491" s="83" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="F491" s="3" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="G491" s="3" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="H491" s="3"/>
       <c r="I491" s="3" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="J491" s="3" t="s">
         <v>424</v>
@@ -20200,7 +20200,7 @@
         <v>491</v>
       </c>
       <c r="B492" s="46" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="C492" s="46" t="s">
         <v>74</v>
@@ -20213,11 +20213,11 @@
         <v>9</v>
       </c>
       <c r="G492" s="3" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="H492" s="3"/>
       <c r="I492" s="3" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="J492" s="3" t="s">
         <v>73</v>
@@ -20229,7 +20229,7 @@
         <v>492</v>
       </c>
       <c r="B493" s="46" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="C493" s="46" t="s">
         <v>74</v>
@@ -20242,11 +20242,11 @@
         <v>9</v>
       </c>
       <c r="G493" s="3" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="H493" s="3"/>
       <c r="I493" s="3" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="J493" s="3" t="s">
         <v>73</v>
@@ -20258,7 +20258,7 @@
         <v>493</v>
       </c>
       <c r="B494" s="46" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="C494" s="46" t="s">
         <v>74</v>
@@ -20271,11 +20271,11 @@
         <v>9</v>
       </c>
       <c r="G494" s="3" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="H494" s="3"/>
       <c r="I494" s="46" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="J494" s="3" t="s">
         <v>73</v>
@@ -20287,7 +20287,7 @@
         <v>494</v>
       </c>
       <c r="B495" s="46" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="C495" s="3" t="s">
         <v>924</v>
@@ -20300,11 +20300,11 @@
         <v>9</v>
       </c>
       <c r="G495" s="3" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="H495" s="3"/>
       <c r="I495" s="3" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="J495" s="3" t="s">
         <v>813</v>
@@ -20316,20 +20316,20 @@
         <v>495</v>
       </c>
       <c r="B496" s="46" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="C496" s="3" t="s">
         <v>193</v>
       </c>
       <c r="D496" s="24"/>
       <c r="E496" s="34" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="F496" s="3"/>
       <c r="G496" s="3"/>
       <c r="H496" s="3"/>
       <c r="I496" s="3" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="J496" s="3" t="s">
         <v>424</v>
@@ -20341,20 +20341,20 @@
         <v>496</v>
       </c>
       <c r="B497" s="46" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="C497" s="3" t="s">
         <v>193</v>
       </c>
       <c r="D497" s="24"/>
       <c r="E497" s="34" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="F497" s="3"/>
       <c r="G497" s="3"/>
       <c r="H497" s="3"/>
       <c r="I497" s="3" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="J497" s="3" t="s">
         <v>424</v>
@@ -20366,24 +20366,24 @@
         <v>497</v>
       </c>
       <c r="B498" s="3" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="C498" s="46" t="s">
         <v>3</v>
       </c>
       <c r="D498" s="24"/>
       <c r="E498" s="83" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="F498" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G498" s="3" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="H498" s="3"/>
       <c r="I498" s="3" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="J498" s="3" t="s">
         <v>424</v>
@@ -20395,7 +20395,7 @@
         <v>498</v>
       </c>
       <c r="B499" s="3" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="C499" s="46" t="s">
         <v>74</v>
@@ -20408,11 +20408,11 @@
         <v>9</v>
       </c>
       <c r="G499" s="3" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="H499" s="3"/>
       <c r="I499" s="3" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="J499" s="3" t="s">
         <v>73</v>
@@ -20424,7 +20424,7 @@
         <v>499</v>
       </c>
       <c r="B500" s="3" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="C500" s="46" t="s">
         <v>74</v>
@@ -20437,11 +20437,11 @@
         <v>9</v>
       </c>
       <c r="G500" s="3" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="H500" s="3"/>
       <c r="I500" s="3" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="J500" s="3" t="s">
         <v>73</v>
@@ -20453,7 +20453,7 @@
         <v>500</v>
       </c>
       <c r="B501" s="3" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="C501" s="46" t="s">
         <v>74</v>
@@ -20466,11 +20466,11 @@
         <v>9</v>
       </c>
       <c r="G501" s="3" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="H501" s="3"/>
       <c r="I501" s="46" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="J501" s="3" t="s">
         <v>73</v>
@@ -20482,20 +20482,20 @@
         <v>501</v>
       </c>
       <c r="B502" s="3" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="C502" s="3" t="s">
         <v>193</v>
       </c>
       <c r="D502" s="24"/>
       <c r="E502" s="34" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="F502" s="3"/>
       <c r="G502" s="3"/>
       <c r="H502" s="3"/>
       <c r="I502" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="J502" s="3" t="s">
         <v>424</v>
@@ -20507,20 +20507,20 @@
         <v>502</v>
       </c>
       <c r="B503" s="3" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="C503" s="3" t="s">
         <v>193</v>
       </c>
       <c r="D503" s="24"/>
       <c r="E503" s="34" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="F503" s="3"/>
       <c r="G503" s="3"/>
       <c r="H503" s="3"/>
       <c r="I503" s="3" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="J503" s="3" t="s">
         <v>424</v>
@@ -20532,24 +20532,24 @@
         <v>503</v>
       </c>
       <c r="B504" s="46" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="C504" s="46" t="s">
         <v>3</v>
       </c>
       <c r="D504" s="24"/>
       <c r="E504" s="83" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="F504" s="3" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="G504" s="3" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="H504" s="3"/>
       <c r="I504" s="3" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="J504" s="3" t="s">
         <v>424</v>
@@ -20561,7 +20561,7 @@
         <v>504</v>
       </c>
       <c r="B505" s="46" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="C505" s="3" t="s">
         <v>924</v>
@@ -20574,17 +20574,17 @@
         <v>9</v>
       </c>
       <c r="G505" s="3" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="H505" s="3"/>
       <c r="I505" s="3" t="s">
+        <v>1699</v>
+      </c>
+      <c r="J505" s="3" t="s">
         <v>1700</v>
       </c>
-      <c r="J505" s="3" t="s">
+      <c r="K505" s="46" t="s">
         <v>1701</v>
-      </c>
-      <c r="K505" s="46" t="s">
-        <v>1702</v>
       </c>
     </row>
     <row r="506" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
@@ -20592,20 +20592,20 @@
         <v>505</v>
       </c>
       <c r="B506" s="46" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="C506" s="3" t="s">
         <v>193</v>
       </c>
       <c r="D506" s="24"/>
       <c r="E506" s="34" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="F506" s="3"/>
       <c r="G506" s="3"/>
       <c r="H506" s="3"/>
       <c r="I506" s="3" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="J506" s="3" t="s">
         <v>424</v>
@@ -22945,14 +22945,14 @@
         <v>1299</v>
       </c>
       <c r="F78" s="13" t="s">
+        <v>1705</v>
+      </c>
+      <c r="G78" s="13" t="s">
         <v>1706</v>
-      </c>
-      <c r="G78" s="13" t="s">
-        <v>1707</v>
       </c>
       <c r="H78" s="13"/>
       <c r="I78" s="13" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
     </row>
   </sheetData>
@@ -22976,15 +22976,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -23206,6 +23197,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -23216,24 +23216,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23253,6 +23235,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Added Data Robustness definition
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F433CA20-A032-45E5-849D-847D46A53CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4430053-032B-4F61-AC04-6AE34F4545F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="180" windowWidth="13430" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="15490" windowHeight="10010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4297" uniqueCount="1836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4298" uniqueCount="1837">
   <si>
     <t>Synonym(s)</t>
   </si>
@@ -5586,6 +5586,9 @@
   </si>
   <si>
     <t>The value representing the number of individuals enrolled in a study.</t>
+  </si>
+  <si>
+    <t>The data's ability to remain accurate and relevant despite changes or disruptions to the data environment.</t>
   </si>
 </sst>
 </file>
@@ -24616,7 +24619,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A100" s="37" t="s">
         <v>107</v>
       </c>
@@ -24639,7 +24642,9 @@
         <v>1788</v>
       </c>
       <c r="H100" s="13"/>
-      <c r="I100" s="13"/>
+      <c r="I100" s="13" t="s">
+        <v>1836</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A6:N74" xr:uid="{00000000-0001-0000-0100-000000000000}">
@@ -24671,15 +24676,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -24901,6 +24897,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
   <ds:schemaRefs>
@@ -24920,14 +24925,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24945,4 +24942,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixes from RichardMarshall in 595
Fixes from RichardMarshall in 595
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C83DE8-0BF8-4E30-8C54-A619C89F92AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98BA56A-404A-4815-98C4-8678B2816A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="220" windowWidth="19020" windowHeight="9180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="240" windowWidth="18820" windowHeight="9690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -6467,9 +6467,6 @@
     <t>NA; Not Applicable</t>
   </si>
   <si>
-    <t>Determination of a value is not relevant in the current context.</t>
-  </si>
-  <si>
     <t>Not Applicable</t>
   </si>
   <si>
@@ -6486,6 +6483,9 @@
   </si>
   <si>
     <t>Alternative combinations of symbols used to represent aliases or alternatives to the standard code.</t>
+  </si>
+  <si>
+    <t>Determination of a value is not relevant in the current context. (NCI)</t>
   </si>
 </sst>
 </file>
@@ -8743,7 +8743,7 @@
       <c r="G32" s="41"/>
       <c r="H32" s="47"/>
       <c r="I32" s="1" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>413</v>
@@ -13012,14 +13012,14 @@
         <v>9</v>
       </c>
       <c r="G181" s="3" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
       <c r="H181" s="3"/>
       <c r="I181" s="3" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="J181" s="1" t="s">
-        <v>413</v>
+        <v>72</v>
       </c>
       <c r="K181" s="24"/>
     </row>
@@ -13041,14 +13041,14 @@
         <v>9</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>2133</v>
+        <v>2132</v>
       </c>
       <c r="H182" s="3"/>
       <c r="I182" s="3" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
       <c r="J182" s="1" t="s">
-        <v>413</v>
+        <v>72</v>
       </c>
       <c r="K182" s="24"/>
     </row>
@@ -27298,13 +27298,13 @@
         <v>2127</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
       <c r="H43" s="50" t="s">
         <v>2128</v>
       </c>
       <c r="I43" s="13" t="s">
-        <v>2129</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.35">
@@ -29671,6 +29671,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -29892,15 +29901,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
   <ds:schemaRefs>
@@ -29910,6 +29910,24 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -29927,22 +29945,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
QC fixes from Berber
removed additional non-readable character in study epoch name definition
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EADDB1E-5719-483B-A08F-4DA7FAC6F525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14391108-94BC-4D1B-9F00-4C68388BF210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="150" windowWidth="18850" windowHeight="9180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="18580" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -6501,10 +6501,10 @@
     <t>A named time period defined in the protocol, wherein a study activity is specified and unchanging throughout the interval, to support a study-specific purpose.</t>
   </si>
   <si>
-    <t>The literal identifier (i.e., distinctive designation) of the study epoch, i.e., the named time period defined in the protocol, wherein a study activity is specified and unchanging throughout the interval, to support a study-specific purpose.</t>
-  </si>
-  <si>
     <t>A characterization or classification of the study epoch, i.e., the named time period defined in the protocol, wherein a study activity is specified and unchanging throughout the interval, to support a study-specific purpose.</t>
+  </si>
+  <si>
+    <t>The literal identifier (i.e., distinctive designation) of the study epoch, i.e., the named time period defined in the protocol, wherein a study activity is specified and unchanging throughout the interval, to support a study-specific purpose.</t>
   </si>
 </sst>
 </file>
@@ -11222,7 +11222,7 @@
       </c>
       <c r="H96" s="1"/>
       <c r="I96" s="3" t="s">
-        <v>2140</v>
+        <v>2141</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>68</v>
@@ -11280,7 +11280,7 @@
       </c>
       <c r="H98" s="1"/>
       <c r="I98" s="1" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="J98" s="1" t="s">
         <v>784</v>
@@ -30264,6 +30264,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -30485,15 +30494,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
   <ds:schemaRefs>
@@ -30513,6 +30513,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30530,12 +30538,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixes on QuantityRange class
Fixes on QuantityRange class
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741F2FA3-EE7D-4928-B465-55BBC8856C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBAC94B-49F4-407F-BC27-339F550DFAA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="100" windowWidth="16600" windowHeight="9880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="920" windowWidth="16600" windowHeight="9880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5419" uniqueCount="2375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5405" uniqueCount="2374">
   <si>
     <t>Synonym(s)</t>
   </si>
@@ -6954,9 +6954,6 @@
   </si>
   <si>
     <t>QuantityRange</t>
-  </si>
-  <si>
-    <t>range</t>
   </si>
   <si>
     <t>Quantity or Range</t>
@@ -12960,7 +12957,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K647"/>
+  <dimension ref="A1:K645"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -13886,13 +13883,13 @@
       </c>
       <c r="D34" s="41"/>
       <c r="E34" s="34" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="F34" s="47"/>
       <c r="G34" s="41"/>
       <c r="H34" s="47"/>
       <c r="I34" s="1" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>407</v>
@@ -14637,13 +14634,13 @@
         <v>812</v>
       </c>
       <c r="E59" s="21" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
       <c r="F59" s="3" t="s">
+        <v>2304</v>
+      </c>
+      <c r="G59" s="3" t="s">
         <v>2305</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>2306</v>
       </c>
       <c r="H59" s="3"/>
       <c r="I59" s="3" t="s">
@@ -14668,13 +14665,13 @@
         <v>812</v>
       </c>
       <c r="E60" s="21" t="s">
-        <v>2296</v>
+        <v>2295</v>
       </c>
       <c r="F60" s="3" t="s">
+        <v>2306</v>
+      </c>
+      <c r="G60" s="3" t="s">
         <v>2307</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>2308</v>
       </c>
       <c r="H60" s="3"/>
       <c r="I60" s="3" t="s">
@@ -20203,17 +20200,17 @@
       </c>
       <c r="D255" s="46"/>
       <c r="E255" s="21" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="F255" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G255" s="3" t="s">
-        <v>2374</v>
+        <v>2373</v>
       </c>
       <c r="H255" s="3"/>
       <c r="I255" s="3" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="J255" s="46" t="s">
         <v>68</v>
@@ -23505,14 +23502,14 @@
         <v>714</v>
       </c>
       <c r="F372" s="1" t="s">
+        <v>2362</v>
+      </c>
+      <c r="G372" s="3" t="s">
         <v>2363</v>
-      </c>
-      <c r="G372" s="3" t="s">
-        <v>2364</v>
       </c>
       <c r="H372" s="3"/>
       <c r="I372" s="1" t="s">
-        <v>2365</v>
+        <v>2364</v>
       </c>
       <c r="J372" s="3" t="s">
         <v>68</v>
@@ -23949,13 +23946,13 @@
         <v>812</v>
       </c>
       <c r="E387" s="21" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
       <c r="F387" s="3" t="s">
+        <v>2300</v>
+      </c>
+      <c r="G387" s="3" t="s">
         <v>2301</v>
-      </c>
-      <c r="G387" s="3" t="s">
-        <v>2302</v>
       </c>
       <c r="H387" s="3"/>
       <c r="I387" s="3" t="s">
@@ -23980,13 +23977,13 @@
         <v>812</v>
       </c>
       <c r="E388" s="21" t="s">
-        <v>2296</v>
+        <v>2295</v>
       </c>
       <c r="F388" s="3" t="s">
+        <v>2302</v>
+      </c>
+      <c r="G388" s="3" t="s">
         <v>2303</v>
-      </c>
-      <c r="G388" s="3" t="s">
-        <v>2304</v>
       </c>
       <c r="H388" s="3"/>
       <c r="I388" s="3" t="s">
@@ -24504,13 +24501,13 @@
       </c>
       <c r="D406" s="1"/>
       <c r="E406" s="21" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
       <c r="F406" s="3" t="s">
+        <v>2296</v>
+      </c>
+      <c r="G406" s="3" t="s">
         <v>2297</v>
-      </c>
-      <c r="G406" s="3" t="s">
-        <v>2298</v>
       </c>
       <c r="H406" s="3"/>
       <c r="I406" s="3" t="s">
@@ -24533,13 +24530,13 @@
       </c>
       <c r="D407" s="1"/>
       <c r="E407" s="21" t="s">
-        <v>2296</v>
+        <v>2295</v>
       </c>
       <c r="F407" s="3" t="s">
+        <v>2298</v>
+      </c>
+      <c r="G407" s="3" t="s">
         <v>2299</v>
-      </c>
-      <c r="G407" s="3" t="s">
-        <v>2300</v>
       </c>
       <c r="H407" s="3"/>
       <c r="I407" s="3" t="s">
@@ -25923,7 +25920,7 @@
       <c r="G455" s="24"/>
       <c r="H455" s="24"/>
       <c r="I455" s="1" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="J455" s="3" t="s">
         <v>407</v>
@@ -26149,7 +26146,7 @@
       </c>
       <c r="H463" s="3"/>
       <c r="I463" s="3" t="s">
-        <v>2362</v>
+        <v>2361</v>
       </c>
       <c r="J463" s="3" t="s">
         <v>68</v>
@@ -27596,19 +27593,19 @@
       </c>
       <c r="D514" s="81"/>
       <c r="E514" s="43" t="s">
-        <v>2366</v>
+        <v>2365</v>
       </c>
       <c r="F514" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G514" s="3" t="s">
+        <v>2366</v>
+      </c>
+      <c r="H514" s="3" t="s">
         <v>2367</v>
       </c>
-      <c r="H514" s="3" t="s">
+      <c r="I514" s="3" t="s">
         <v>2368</v>
-      </c>
-      <c r="I514" s="3" t="s">
-        <v>2369</v>
       </c>
       <c r="J514" s="3" t="s">
         <v>68</v>
@@ -27774,11 +27771,11 @@
         <v>9</v>
       </c>
       <c r="G520" s="3" t="s">
-        <v>2359</v>
+        <v>2358</v>
       </c>
       <c r="H520" s="3"/>
       <c r="I520" s="3" t="s">
-        <v>2360</v>
+        <v>2359</v>
       </c>
       <c r="J520" s="3" t="s">
         <v>68</v>
@@ -29797,13 +29794,13 @@
         <v>185</v>
       </c>
       <c r="E591" s="34" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="F591" s="24"/>
       <c r="G591" s="24"/>
       <c r="H591" s="24"/>
       <c r="I591" s="1" t="s">
-        <v>2370</v>
+        <v>2369</v>
       </c>
       <c r="J591" s="46" t="s">
         <v>407</v>
@@ -30638,13 +30635,13 @@
         <v>185</v>
       </c>
       <c r="E620" s="34" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="F620" s="1"/>
       <c r="G620" s="1"/>
       <c r="H620" s="3"/>
       <c r="I620" s="1" t="s">
-        <v>2371</v>
+        <v>2370</v>
       </c>
       <c r="J620" s="46" t="s">
         <v>407</v>
@@ -31058,103 +31055,107 @@
         <v>9</v>
       </c>
       <c r="G634" s="3" t="s">
-        <v>2293</v>
+        <v>2292</v>
       </c>
       <c r="H634" s="3"/>
       <c r="I634" s="3" t="s">
-        <v>2294</v>
+        <v>2293</v>
       </c>
       <c r="J634" s="3" t="s">
         <v>407</v>
       </c>
       <c r="K634" s="1"/>
     </row>
-    <row r="635" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="635" spans="1:11" ht="50" x14ac:dyDescent="0.35">
       <c r="A635" s="24">
         <v>634</v>
       </c>
-      <c r="B635" s="96" t="s">
-        <v>2291</v>
+      <c r="B635" s="25" t="s">
+        <v>2308</v>
       </c>
       <c r="C635" s="3" t="s">
-        <v>849</v>
+        <v>3</v>
       </c>
       <c r="D635" s="24"/>
-      <c r="E635" s="43" t="s">
-        <v>601</v>
+      <c r="E635" s="52" t="s">
+        <v>2308</v>
       </c>
       <c r="F635" s="3" t="s">
-        <v>759</v>
+        <v>2313</v>
       </c>
       <c r="G635" s="3" t="s">
-        <v>751</v>
-      </c>
-      <c r="H635" s="3"/>
+        <v>2314</v>
+      </c>
+      <c r="H635" s="3" t="s">
+        <v>2315</v>
+      </c>
       <c r="I635" s="3" t="s">
-        <v>760</v>
+        <v>2316</v>
       </c>
       <c r="J635" s="3" t="s">
-        <v>68</v>
+        <v>407</v>
       </c>
       <c r="K635" s="1"/>
     </row>
-    <row r="636" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="636" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A636" s="24">
         <v>635</v>
       </c>
-      <c r="B636" s="96" t="s">
-        <v>2291</v>
+      <c r="B636" s="78" t="s">
+        <v>2308</v>
       </c>
       <c r="C636" s="3" t="s">
-        <v>849</v>
+        <v>69</v>
       </c>
       <c r="D636" s="24"/>
       <c r="E636" s="43" t="s">
-        <v>2292</v>
+        <v>298</v>
       </c>
       <c r="F636" s="3" t="s">
-        <v>824</v>
+        <v>9</v>
       </c>
       <c r="G636" s="3" t="s">
-        <v>821</v>
-      </c>
-      <c r="H636" s="3"/>
-      <c r="I636" s="46" t="s">
-        <v>2280</v>
+        <v>2317</v>
+      </c>
+      <c r="H636" s="3" t="s">
+        <v>2318</v>
+      </c>
+      <c r="I636" s="3" t="s">
+        <v>2319</v>
       </c>
       <c r="J636" s="3" t="s">
         <v>68</v>
       </c>
       <c r="K636" s="1"/>
     </row>
-    <row r="637" spans="1:11" ht="50" x14ac:dyDescent="0.35">
+    <row r="637" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A637" s="24">
         <v>636</v>
       </c>
-      <c r="B637" s="25" t="s">
+      <c r="B637" s="78" t="s">
+        <v>2308</v>
+      </c>
+      <c r="C637" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D637" s="24"/>
+      <c r="E637" s="21" t="s">
         <v>2309</v>
       </c>
-      <c r="C637" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D637" s="24"/>
-      <c r="E637" s="52" t="s">
-        <v>2309</v>
-      </c>
       <c r="F637" s="3" t="s">
-        <v>2314</v>
+        <v>2320</v>
       </c>
       <c r="G637" s="3" t="s">
-        <v>2315</v>
+        <v>2321</v>
       </c>
       <c r="H637" s="3" t="s">
-        <v>2316</v>
+        <v>2322</v>
       </c>
       <c r="I637" s="3" t="s">
-        <v>2317</v>
+        <v>2323</v>
       </c>
       <c r="J637" s="3" t="s">
-        <v>407</v>
+        <v>68</v>
       </c>
       <c r="K637" s="1"/>
     </row>
@@ -31163,26 +31164,24 @@
         <v>637</v>
       </c>
       <c r="B638" s="78" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="C638" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D638" s="24"/>
-      <c r="E638" s="43" t="s">
-        <v>298</v>
+      <c r="E638" s="21" t="s">
+        <v>2310</v>
       </c>
       <c r="F638" s="3" t="s">
-        <v>9</v>
+        <v>2324</v>
       </c>
       <c r="G638" s="3" t="s">
-        <v>2318</v>
-      </c>
-      <c r="H638" s="3" t="s">
-        <v>2319</v>
-      </c>
+        <v>2325</v>
+      </c>
+      <c r="H638" s="3"/>
       <c r="I638" s="3" t="s">
-        <v>2320</v>
+        <v>2326</v>
       </c>
       <c r="J638" s="3" t="s">
         <v>68</v>
@@ -31194,145 +31193,143 @@
         <v>638</v>
       </c>
       <c r="B639" s="78" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="C639" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D639" s="24"/>
       <c r="E639" s="21" t="s">
-        <v>2310</v>
+        <v>2311</v>
       </c>
       <c r="F639" s="3" t="s">
-        <v>2321</v>
+        <v>9</v>
       </c>
       <c r="G639" s="3" t="s">
-        <v>2322</v>
-      </c>
-      <c r="H639" s="3" t="s">
-        <v>2323</v>
-      </c>
+        <v>2327</v>
+      </c>
+      <c r="H639" s="3"/>
       <c r="I639" s="3" t="s">
-        <v>2324</v>
+        <v>2328</v>
       </c>
       <c r="J639" s="3" t="s">
         <v>68</v>
       </c>
       <c r="K639" s="1"/>
     </row>
-    <row r="640" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="640" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A640" s="24">
         <v>639</v>
       </c>
       <c r="B640" s="78" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="C640" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D640" s="24"/>
       <c r="E640" s="21" t="s">
-        <v>2311</v>
+        <v>2312</v>
       </c>
       <c r="F640" s="3" t="s">
-        <v>2325</v>
+        <v>9</v>
       </c>
       <c r="G640" s="3" t="s">
-        <v>2326</v>
+        <v>2329</v>
       </c>
       <c r="H640" s="3"/>
       <c r="I640" s="3" t="s">
-        <v>2327</v>
+        <v>2330</v>
       </c>
       <c r="J640" s="3" t="s">
         <v>68</v>
       </c>
       <c r="K640" s="1"/>
     </row>
-    <row r="641" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="641" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A641" s="24">
         <v>640</v>
       </c>
-      <c r="B641" s="78" t="s">
-        <v>2309</v>
+      <c r="B641" s="38" t="s">
+        <v>2347</v>
       </c>
       <c r="C641" s="3" t="s">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="D641" s="24"/>
-      <c r="E641" s="21" t="s">
-        <v>2312</v>
-      </c>
-      <c r="F641" s="3" t="s">
-        <v>9</v>
+      <c r="E641" s="52" t="s">
+        <v>2347</v>
+      </c>
+      <c r="F641" s="1" t="s">
+        <v>2348</v>
       </c>
       <c r="G641" s="3" t="s">
-        <v>2328</v>
-      </c>
-      <c r="H641" s="3"/>
+        <v>2347</v>
+      </c>
+      <c r="H641" s="46"/>
       <c r="I641" s="3" t="s">
-        <v>2329</v>
+        <v>2349</v>
       </c>
       <c r="J641" s="3" t="s">
-        <v>68</v>
+        <v>407</v>
       </c>
       <c r="K641" s="1"/>
     </row>
-    <row r="642" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="642" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A642" s="24">
         <v>641</v>
       </c>
-      <c r="B642" s="78" t="s">
-        <v>2309</v>
+      <c r="B642" s="38" t="s">
+        <v>2347</v>
       </c>
       <c r="C642" s="3" t="s">
         <v>69</v>
       </c>
       <c r="D642" s="24"/>
       <c r="E642" s="21" t="s">
-        <v>2313</v>
-      </c>
-      <c r="F642" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="F642" s="70" t="s">
         <v>9</v>
       </c>
       <c r="G642" s="3" t="s">
-        <v>2330</v>
-      </c>
-      <c r="H642" s="3"/>
+        <v>2350</v>
+      </c>
+      <c r="H642" s="46"/>
       <c r="I642" s="3" t="s">
-        <v>2331</v>
-      </c>
-      <c r="J642" s="3" t="s">
+        <v>2351</v>
+      </c>
+      <c r="J642" s="46" t="s">
         <v>68</v>
       </c>
       <c r="K642" s="1"/>
     </row>
-    <row r="643" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="643" spans="1:11" ht="25" x14ac:dyDescent="0.35">
       <c r="A643" s="24">
         <v>642</v>
       </c>
       <c r="B643" s="38" t="s">
-        <v>2348</v>
+        <v>2347</v>
       </c>
       <c r="C643" s="3" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="D643" s="24"/>
-      <c r="E643" s="52" t="s">
-        <v>2348</v>
-      </c>
-      <c r="F643" s="1" t="s">
-        <v>2349</v>
+      <c r="E643" s="21" t="s">
+        <v>704</v>
+      </c>
+      <c r="F643" s="70" t="s">
+        <v>9</v>
       </c>
       <c r="G643" s="3" t="s">
-        <v>2348</v>
+        <v>2352</v>
       </c>
       <c r="H643" s="46"/>
       <c r="I643" s="3" t="s">
-        <v>2350</v>
-      </c>
-      <c r="J643" s="3" t="s">
-        <v>407</v>
+        <v>2353</v>
+      </c>
+      <c r="J643" s="46" t="s">
+        <v>68</v>
       </c>
       <c r="K643" s="1"/>
     </row>
@@ -31341,116 +31338,58 @@
         <v>643</v>
       </c>
       <c r="B644" s="38" t="s">
-        <v>2348</v>
-      </c>
-      <c r="C644" s="3" t="s">
+        <v>2347</v>
+      </c>
+      <c r="C644" s="32" t="s">
         <v>69</v>
       </c>
       <c r="D644" s="24"/>
-      <c r="E644" s="21" t="s">
-        <v>298</v>
+      <c r="E644" s="54" t="s">
+        <v>705</v>
       </c>
       <c r="F644" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="G644" s="3" t="s">
-        <v>2351</v>
-      </c>
-      <c r="H644" s="46"/>
-      <c r="I644" s="3" t="s">
-        <v>2352</v>
+      <c r="G644" s="32" t="s">
+        <v>2354</v>
+      </c>
+      <c r="H644" s="65"/>
+      <c r="I644" s="32" t="s">
+        <v>2355</v>
       </c>
       <c r="J644" s="46" t="s">
         <v>68</v>
       </c>
       <c r="K644" s="1"/>
     </row>
-    <row r="645" spans="1:11" ht="25" x14ac:dyDescent="0.35">
+    <row r="645" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A645" s="24">
         <v>644</v>
       </c>
       <c r="B645" s="38" t="s">
-        <v>2348</v>
-      </c>
-      <c r="C645" s="3" t="s">
-        <v>69</v>
+        <v>2347</v>
+      </c>
+      <c r="C645" s="1" t="s">
+        <v>849</v>
       </c>
       <c r="D645" s="24"/>
-      <c r="E645" s="21" t="s">
-        <v>704</v>
+      <c r="E645" s="22" t="s">
+        <v>601</v>
       </c>
       <c r="F645" s="70" t="s">
         <v>9</v>
       </c>
       <c r="G645" s="3" t="s">
-        <v>2353</v>
-      </c>
-      <c r="H645" s="46"/>
+        <v>2356</v>
+      </c>
+      <c r="H645" s="3"/>
       <c r="I645" s="3" t="s">
-        <v>2354</v>
-      </c>
-      <c r="J645" s="46" t="s">
+        <v>2357</v>
+      </c>
+      <c r="J645" s="3" t="s">
         <v>68</v>
       </c>
       <c r="K645" s="1"/>
-    </row>
-    <row r="646" spans="1:11" ht="25" x14ac:dyDescent="0.35">
-      <c r="A646" s="24">
-        <v>645</v>
-      </c>
-      <c r="B646" s="38" t="s">
-        <v>2348</v>
-      </c>
-      <c r="C646" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="D646" s="24"/>
-      <c r="E646" s="54" t="s">
-        <v>705</v>
-      </c>
-      <c r="F646" s="70" t="s">
-        <v>9</v>
-      </c>
-      <c r="G646" s="32" t="s">
-        <v>2355</v>
-      </c>
-      <c r="H646" s="65"/>
-      <c r="I646" s="32" t="s">
-        <v>2356</v>
-      </c>
-      <c r="J646" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="K646" s="1"/>
-    </row>
-    <row r="647" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="A647" s="24">
-        <v>646</v>
-      </c>
-      <c r="B647" s="38" t="s">
-        <v>2348</v>
-      </c>
-      <c r="C647" s="1" t="s">
-        <v>849</v>
-      </c>
-      <c r="D647" s="24"/>
-      <c r="E647" s="22" t="s">
-        <v>601</v>
-      </c>
-      <c r="F647" s="70" t="s">
-        <v>9</v>
-      </c>
-      <c r="G647" s="3" t="s">
-        <v>2357</v>
-      </c>
-      <c r="H647" s="3"/>
-      <c r="I647" s="3" t="s">
-        <v>2358</v>
-      </c>
-      <c r="J647" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="K647" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K633" xr:uid="{00000000-0001-0000-0000-000000000000}">
@@ -33203,11 +33142,11 @@
         <v>9</v>
       </c>
       <c r="G57" s="50" t="s">
-        <v>2332</v>
+        <v>2331</v>
       </c>
       <c r="H57" s="50"/>
       <c r="I57" s="50" t="s">
-        <v>2333</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="25" x14ac:dyDescent="0.35">
@@ -33230,11 +33169,11 @@
         <v>9</v>
       </c>
       <c r="G58" s="50" t="s">
-        <v>2334</v>
+        <v>2333</v>
       </c>
       <c r="H58" s="50"/>
       <c r="I58" s="50" t="s">
-        <v>2335</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.35">
@@ -33257,11 +33196,11 @@
         <v>9</v>
       </c>
       <c r="G59" s="50" t="s">
-        <v>2336</v>
+        <v>2335</v>
       </c>
       <c r="H59" s="13"/>
       <c r="I59" s="50" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.35">
@@ -33284,11 +33223,11 @@
         <v>9</v>
       </c>
       <c r="G60" s="50" t="s">
-        <v>2338</v>
+        <v>2337</v>
       </c>
       <c r="H60" s="13"/>
       <c r="I60" s="50" t="s">
-        <v>2339</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="25" x14ac:dyDescent="0.35">
@@ -33308,14 +33247,14 @@
         <v>1139</v>
       </c>
       <c r="F61" s="50" t="s">
+        <v>2339</v>
+      </c>
+      <c r="G61" s="50" t="s">
         <v>2340</v>
-      </c>
-      <c r="G61" s="50" t="s">
-        <v>2341</v>
       </c>
       <c r="H61" s="50"/>
       <c r="I61" s="50" t="s">
-        <v>2342</v>
+        <v>2341</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="50" x14ac:dyDescent="0.35">
@@ -33335,14 +33274,14 @@
         <v>1139</v>
       </c>
       <c r="F62" s="13" t="s">
+        <v>2342</v>
+      </c>
+      <c r="G62" s="13" t="s">
         <v>2343</v>
-      </c>
-      <c r="G62" s="13" t="s">
-        <v>2344</v>
       </c>
       <c r="H62" s="50"/>
       <c r="I62" s="13" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="25" x14ac:dyDescent="0.35">
@@ -35313,15 +35252,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -35543,6 +35473,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -35553,24 +35492,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -35590,6 +35511,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="de0c653c-2bd3-43b1-95fa-012c57f61cfe"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="848a8810-16a6-4d79-96d3-e3dfb86099b7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fix to Multicentre definition
shorten definition
</commit_message>
<xml_diff>
--- a/Deliverables/CT/USDM_CT.xlsx
+++ b/Deliverables/CT/USDM_CT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muhlbradtee\Documents\GitHub\DDF-RA\Deliverables\CT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC3B3E1-F999-40A4-A29C-6541F1ECFFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B0CE2C-B408-4FE8-80C5-B57C14BAD083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="430" windowWidth="15470" windowHeight="9880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2910" yWindow="460" windowWidth="15470" windowHeight="9880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DDF Entities&amp;Attributes" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5417" uniqueCount="2415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5417" uniqueCount="2414">
   <si>
     <t>Synonym(s)</t>
   </si>
@@ -7050,9 +7050,6 @@
   </si>
   <si>
     <t>Multicentre</t>
-  </si>
-  <si>
-    <t>A clinical trial conducted according to a single protocol but at more than one site, and therefore, carried out by more than one investigator. (ICH E6 1.40)</t>
   </si>
   <si>
     <t>Single Country</t>
@@ -15374,13 +15371,13 @@
       </c>
       <c r="D34" s="41"/>
       <c r="E34" s="34" t="s">
-        <v>2335</v>
+        <v>2334</v>
       </c>
       <c r="F34" s="47"/>
       <c r="G34" s="41"/>
       <c r="H34" s="47"/>
       <c r="I34" s="1" t="s">
-        <v>2336</v>
+        <v>2335</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>406</v>
@@ -20392,7 +20389,7 @@
         <v>199</v>
       </c>
       <c r="F209" s="1" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="G209" s="1" t="s">
         <v>2073</v>
@@ -20421,7 +20418,7 @@
         <v>441</v>
       </c>
       <c r="F210" s="3" t="s">
-        <v>2364</v>
+        <v>2363</v>
       </c>
       <c r="G210" s="3" t="s">
         <v>2277</v>
@@ -20450,7 +20447,7 @@
         <v>467</v>
       </c>
       <c r="F211" s="3" t="s">
-        <v>2365</v>
+        <v>2364</v>
       </c>
       <c r="G211" s="3" t="s">
         <v>2279</v>
@@ -21691,17 +21688,17 @@
       </c>
       <c r="D255" s="46"/>
       <c r="E255" s="21" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="F255" s="3" t="s">
-        <v>2366</v>
+        <v>2365</v>
       </c>
       <c r="G255" s="3" t="s">
-        <v>2363</v>
+        <v>2362</v>
       </c>
       <c r="H255" s="3"/>
       <c r="I255" s="3" t="s">
-        <v>2362</v>
+        <v>2361</v>
       </c>
       <c r="J255" s="46" t="s">
         <v>67</v>
@@ -23514,7 +23511,7 @@
         <v>441</v>
       </c>
       <c r="F319" s="70" t="s">
-        <v>2367</v>
+        <v>2366</v>
       </c>
       <c r="G319" s="3" t="s">
         <v>2271</v>
@@ -23543,7 +23540,7 @@
         <v>442</v>
       </c>
       <c r="F320" s="70" t="s">
-        <v>2368</v>
+        <v>2367</v>
       </c>
       <c r="G320" s="3" t="s">
         <v>2273</v>
@@ -23572,7 +23569,7 @@
         <v>467</v>
       </c>
       <c r="F321" s="3" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
       <c r="G321" s="3" t="s">
         <v>2275</v>
@@ -24993,14 +24990,14 @@
         <v>713</v>
       </c>
       <c r="F372" s="1" t="s">
+        <v>2351</v>
+      </c>
+      <c r="G372" s="3" t="s">
         <v>2352</v>
-      </c>
-      <c r="G372" s="3" t="s">
-        <v>2353</v>
       </c>
       <c r="H372" s="3"/>
       <c r="I372" s="1" t="s">
-        <v>2354</v>
+        <v>2353</v>
       </c>
       <c r="J372" s="3" t="s">
         <v>67</v>
@@ -27335,10 +27332,10 @@
         <v>1171</v>
       </c>
       <c r="J452" s="3" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="K452" s="91" t="s">
-        <v>2404</v>
+        <v>2403</v>
       </c>
     </row>
     <row r="453" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
@@ -27413,7 +27410,7 @@
       <c r="G455" s="24"/>
       <c r="H455" s="24"/>
       <c r="I455" s="1" t="s">
-        <v>2350</v>
+        <v>2349</v>
       </c>
       <c r="J455" s="3" t="s">
         <v>406</v>
@@ -27639,7 +27636,7 @@
       </c>
       <c r="H463" s="3"/>
       <c r="I463" s="3" t="s">
-        <v>2351</v>
+        <v>2350</v>
       </c>
       <c r="J463" s="3" t="s">
         <v>67</v>
@@ -27758,10 +27755,10 @@
         <v>1418</v>
       </c>
       <c r="J467" s="3" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K467" s="91" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="468" spans="1:11" ht="25" x14ac:dyDescent="0.35">
@@ -28106,10 +28103,10 @@
         <v>1775</v>
       </c>
       <c r="J479" s="3" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="K479" s="91" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="480" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
@@ -28475,10 +28472,10 @@
         <v>1468</v>
       </c>
       <c r="J492" s="3" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
       <c r="K492" s="91" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="493" spans="1:11" ht="25" x14ac:dyDescent="0.35">
@@ -29092,19 +29089,19 @@
       </c>
       <c r="D514" s="81"/>
       <c r="E514" s="43" t="s">
+        <v>2354</v>
+      </c>
+      <c r="F514" s="3" t="s">
+        <v>2369</v>
+      </c>
+      <c r="G514" s="3" t="s">
         <v>2355</v>
       </c>
-      <c r="F514" s="3" t="s">
-        <v>2370</v>
-      </c>
-      <c r="G514" s="3" t="s">
+      <c r="H514" s="3" t="s">
         <v>2356</v>
       </c>
-      <c r="H514" s="3" t="s">
+      <c r="I514" s="3" t="s">
         <v>2357</v>
-      </c>
-      <c r="I514" s="3" t="s">
-        <v>2358</v>
       </c>
       <c r="J514" s="3" t="s">
         <v>67</v>
@@ -29267,14 +29264,14 @@
         <v>1128</v>
       </c>
       <c r="F520" s="70" t="s">
-        <v>2371</v>
+        <v>2370</v>
       </c>
       <c r="G520" s="3" t="s">
-        <v>2348</v>
+        <v>2347</v>
       </c>
       <c r="H520" s="3"/>
       <c r="I520" s="3" t="s">
-        <v>2349</v>
+        <v>2348</v>
       </c>
       <c r="J520" s="3" t="s">
         <v>67</v>
@@ -29406,10 +29403,10 @@
         <v>1562</v>
       </c>
       <c r="J525" s="3" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
       <c r="K525" s="91" t="s">
-        <v>2408</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="526" spans="1:11" x14ac:dyDescent="0.35">
@@ -29835,10 +29832,10 @@
         <v>1685</v>
       </c>
       <c r="J540" s="3" t="s">
-        <v>2400</v>
+        <v>2399</v>
       </c>
       <c r="K540" s="91" t="s">
-        <v>2409</v>
+        <v>2408</v>
       </c>
     </row>
     <row r="541" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
@@ -30148,10 +30145,10 @@
         <v>1771</v>
       </c>
       <c r="J551" s="32" t="s">
-        <v>2401</v>
+        <v>2400</v>
       </c>
       <c r="K551" s="91" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
     </row>
     <row r="552" spans="1:11" ht="25" x14ac:dyDescent="0.35">
@@ -30239,10 +30236,10 @@
         <v>1784</v>
       </c>
       <c r="J554" s="3" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="K554" s="91" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="555" spans="1:11" ht="37.5" x14ac:dyDescent="0.35">
@@ -30413,10 +30410,10 @@
         <v>1795</v>
       </c>
       <c r="J560" s="3" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="K560" s="91" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
     </row>
     <row r="561" spans="1:11" ht="50" x14ac:dyDescent="0.35">
@@ -31305,13 +31302,13 @@
         <v>184</v>
       </c>
       <c r="E591" s="34" t="s">
-        <v>2335</v>
+        <v>2334</v>
       </c>
       <c r="F591" s="24"/>
       <c r="G591" s="24"/>
       <c r="H591" s="24"/>
       <c r="I591" s="1" t="s">
-        <v>2359</v>
+        <v>2358</v>
       </c>
       <c r="J591" s="46" t="s">
         <v>406</v>
@@ -31467,10 +31464,10 @@
         <v>1882</v>
       </c>
       <c r="J596" s="3" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="K596" s="91" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
     </row>
     <row r="597" spans="1:11" ht="25" x14ac:dyDescent="0.35">
@@ -32150,13 +32147,13 @@
         <v>184</v>
       </c>
       <c r="E620" s="34" t="s">
-        <v>2335</v>
+        <v>2334</v>
       </c>
       <c r="F620" s="1"/>
       <c r="G620" s="1"/>
       <c r="H620" s="3"/>
       <c r="I620" s="1" t="s">
-        <v>2360</v>
+        <v>2359</v>
       </c>
       <c r="J620" s="46" t="s">
         <v>406</v>
@@ -32567,7 +32564,7 @@
         <v>2281</v>
       </c>
       <c r="F634" s="3" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="G634" s="3" t="s">
         <v>2282</v>
@@ -32627,7 +32624,7 @@
         <v>297</v>
       </c>
       <c r="F636" s="3" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="G636" s="3" t="s">
         <v>2307</v>
@@ -32718,7 +32715,7 @@
         <v>2301</v>
       </c>
       <c r="F639" s="3" t="s">
-        <v>2374</v>
+        <v>2373</v>
       </c>
       <c r="G639" s="3" t="s">
         <v>2317</v>
@@ -32747,7 +32744,7 @@
         <v>2302</v>
       </c>
       <c r="F640" s="3" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
       <c r="G640" s="3" t="s">
         <v>2319</v>
@@ -32766,24 +32763,24 @@
         <v>640</v>
       </c>
       <c r="B641" s="38" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="C641" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D641" s="24"/>
       <c r="E641" s="52" t="s">
+        <v>2336</v>
+      </c>
+      <c r="F641" s="1" t="s">
         <v>2337</v>
       </c>
-      <c r="F641" s="1" t="s">
-        <v>2338</v>
-      </c>
       <c r="G641" s="3" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="H641" s="46"/>
       <c r="I641" s="3" t="s">
-        <v>2339</v>
+        <v>2338</v>
       </c>
       <c r="J641" s="3" t="s">
         <v>406</v>
@@ -32795,7 +32792,7 @@
         <v>641</v>
       </c>
       <c r="B642" s="38" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="C642" s="3" t="s">
         <v>68</v>
@@ -32805,14 +32802,14 @@
         <v>297</v>
       </c>
       <c r="F642" s="70" t="s">
-        <v>2376</v>
+        <v>2375</v>
       </c>
       <c r="G642" s="3" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="H642" s="46"/>
       <c r="I642" s="3" t="s">
-        <v>2341</v>
+        <v>2340</v>
       </c>
       <c r="J642" s="46" t="s">
         <v>67</v>
@@ -32824,7 +32821,7 @@
         <v>642</v>
       </c>
       <c r="B643" s="38" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="C643" s="3" t="s">
         <v>68</v>
@@ -32834,14 +32831,14 @@
         <v>703</v>
       </c>
       <c r="F643" s="70" t="s">
-        <v>2377</v>
+        <v>2376</v>
       </c>
       <c r="G643" s="3" t="s">
-        <v>2342</v>
+        <v>2341</v>
       </c>
       <c r="H643" s="46"/>
       <c r="I643" s="3" t="s">
-        <v>2343</v>
+        <v>2342</v>
       </c>
       <c r="J643" s="46" t="s">
         <v>67</v>
@@ -32853,7 +32850,7 @@
         <v>643</v>
       </c>
       <c r="B644" s="38" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="C644" s="32" t="s">
         <v>68</v>
@@ -32863,14 +32860,14 @@
         <v>704</v>
       </c>
       <c r="F644" s="70" t="s">
-        <v>2378</v>
+        <v>2377</v>
       </c>
       <c r="G644" s="32" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="H644" s="65"/>
       <c r="I644" s="32" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="J644" s="46" t="s">
         <v>67</v>
@@ -32882,7 +32879,7 @@
         <v>644</v>
       </c>
       <c r="B645" s="38" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="C645" s="1" t="s">
         <v>848</v>
@@ -32892,14 +32889,14 @@
         <v>600</v>
       </c>
       <c r="F645" s="70" t="s">
-        <v>2379</v>
+        <v>2378</v>
       </c>
       <c r="G645" s="3" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="H645" s="3"/>
       <c r="I645" s="3" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
       <c r="J645" s="3" t="s">
         <v>67</v>
@@ -32983,7 +32980,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+      <selection pane="bottomLeft" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
@@ -34390,7 +34387,7 @@
         <v>469</v>
       </c>
       <c r="D48" s="40" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="E48" s="40" t="s">
         <v>1138</v>
@@ -34668,7 +34665,7 @@
         <v>1138</v>
       </c>
       <c r="F57" s="40" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
       <c r="G57" s="50" t="s">
         <v>2321</v>
@@ -34678,7 +34675,7 @@
         <v>2322</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="25" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" s="50" t="s">
         <v>101</v>
       </c>
@@ -34695,14 +34692,14 @@
         <v>1138</v>
       </c>
       <c r="F58" s="40" t="s">
-        <v>2381</v>
+        <v>2380</v>
       </c>
       <c r="G58" s="50" t="s">
         <v>2323</v>
       </c>
       <c r="H58" s="50"/>
-      <c r="I58" s="50" t="s">
-        <v>2324</v>
+      <c r="I58" s="41" t="s">
+        <v>2322</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.35">
@@ -34722,14 +34719,14 @@
         <v>1138</v>
       </c>
       <c r="F59" s="40" t="s">
-        <v>2382</v>
+        <v>2381</v>
       </c>
       <c r="G59" s="50" t="s">
-        <v>2325</v>
+        <v>2324</v>
       </c>
       <c r="H59" s="13"/>
       <c r="I59" s="50" t="s">
-        <v>2326</v>
+        <v>2325</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.35">
@@ -34749,14 +34746,14 @@
         <v>1138</v>
       </c>
       <c r="F60" s="50" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
       <c r="G60" s="50" t="s">
-        <v>2327</v>
+        <v>2326</v>
       </c>
       <c r="H60" s="13"/>
       <c r="I60" s="50" t="s">
-        <v>2328</v>
+        <v>2327</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="25" x14ac:dyDescent="0.35">
@@ -34776,14 +34773,14 @@
         <v>1138</v>
       </c>
       <c r="F61" s="50" t="s">
+        <v>2328</v>
+      </c>
+      <c r="G61" s="50" t="s">
         <v>2329</v>
-      </c>
-      <c r="G61" s="50" t="s">
-        <v>2330</v>
       </c>
       <c r="H61" s="50"/>
       <c r="I61" s="50" t="s">
-        <v>2331</v>
+        <v>2330</v>
       </c>
     </row>
     <row r="62" spans="1:14" ht="50" x14ac:dyDescent="0.35">
@@ -34803,14 +34800,14 @@
         <v>1138</v>
       </c>
       <c r="F62" s="13" t="s">
+        <v>2331</v>
+      </c>
+      <c r="G62" s="13" t="s">
         <v>2332</v>
-      </c>
-      <c r="G62" s="13" t="s">
-        <v>2333</v>
       </c>
       <c r="H62" s="50"/>
       <c r="I62" s="13" t="s">
-        <v>2334</v>
+        <v>2333</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="25" hidden="1" x14ac:dyDescent="0.35">
@@ -35457,7 +35454,7 @@
         <v>469</v>
       </c>
       <c r="D85" s="40" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
       <c r="E85" s="40" t="s">
         <v>1138</v>
@@ -35486,7 +35483,7 @@
         <v>469</v>
       </c>
       <c r="D86" s="40" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
       <c r="E86" s="40" t="s">
         <v>1138</v>
@@ -35515,7 +35512,7 @@
         <v>469</v>
       </c>
       <c r="D87" s="40" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
       <c r="E87" s="40" t="s">
         <v>1138</v>
@@ -35542,7 +35539,7 @@
         <v>199</v>
       </c>
       <c r="D88" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E88" s="40" t="s">
         <v>1138</v>
@@ -35571,7 +35568,7 @@
         <v>199</v>
       </c>
       <c r="D89" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E89" s="40" t="s">
         <v>1138</v>
@@ -35598,7 +35595,7 @@
         <v>199</v>
       </c>
       <c r="D90" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E90" s="40" t="s">
         <v>1138</v>
@@ -35625,7 +35622,7 @@
         <v>199</v>
       </c>
       <c r="D91" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E91" s="40" t="s">
         <v>1138</v>
@@ -35652,7 +35649,7 @@
         <v>199</v>
       </c>
       <c r="D92" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E92" s="40" t="s">
         <v>1138</v>
@@ -35679,7 +35676,7 @@
         <v>199</v>
       </c>
       <c r="D93" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E93" s="40" t="s">
         <v>1138</v>
@@ -35706,7 +35703,7 @@
         <v>199</v>
       </c>
       <c r="D94" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E94" s="40" t="s">
         <v>1138</v>
@@ -35733,7 +35730,7 @@
         <v>199</v>
       </c>
       <c r="D95" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E95" s="40" t="s">
         <v>1138</v>
@@ -35760,7 +35757,7 @@
         <v>199</v>
       </c>
       <c r="D96" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E96" s="40" t="s">
         <v>1138</v>
@@ -35787,7 +35784,7 @@
         <v>199</v>
       </c>
       <c r="D97" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E97" s="40" t="s">
         <v>1138</v>
@@ -35814,7 +35811,7 @@
         <v>199</v>
       </c>
       <c r="D98" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E98" s="40" t="s">
         <v>1138</v>
@@ -35841,7 +35838,7 @@
         <v>199</v>
       </c>
       <c r="D99" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E99" s="40" t="s">
         <v>1138</v>
@@ -35868,7 +35865,7 @@
         <v>199</v>
       </c>
       <c r="D100" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E100" s="40" t="s">
         <v>1138</v>
@@ -35895,7 +35892,7 @@
         <v>199</v>
       </c>
       <c r="D101" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E101" s="40" t="s">
         <v>1138</v>
@@ -35922,7 +35919,7 @@
         <v>199</v>
       </c>
       <c r="D102" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E102" s="40" t="s">
         <v>1138</v>
@@ -35949,7 +35946,7 @@
         <v>199</v>
       </c>
       <c r="D103" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E103" s="40" t="s">
         <v>1138</v>
@@ -35978,7 +35975,7 @@
         <v>199</v>
       </c>
       <c r="D104" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E104" s="40" t="s">
         <v>1138</v>
@@ -36007,7 +36004,7 @@
         <v>199</v>
       </c>
       <c r="D105" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E105" s="40" t="s">
         <v>1138</v>
@@ -36034,7 +36031,7 @@
         <v>199</v>
       </c>
       <c r="D106" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E106" s="40" t="s">
         <v>1138</v>
@@ -36061,7 +36058,7 @@
         <v>199</v>
       </c>
       <c r="D107" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E107" s="40" t="s">
         <v>1138</v>
@@ -36088,7 +36085,7 @@
         <v>199</v>
       </c>
       <c r="D108" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E108" s="40" t="s">
         <v>1138</v>
@@ -36115,7 +36112,7 @@
         <v>199</v>
       </c>
       <c r="D109" s="40" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E109" s="40" t="s">
         <v>1138</v>
@@ -36142,7 +36139,7 @@
         <v>469</v>
       </c>
       <c r="D110" s="40" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
       <c r="E110" s="40" t="s">
         <v>1138</v>
@@ -36171,7 +36168,7 @@
         <v>469</v>
       </c>
       <c r="D111" s="40" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
       <c r="E111" s="40" t="s">
         <v>1138</v>
@@ -36200,7 +36197,7 @@
         <v>469</v>
       </c>
       <c r="D112" s="40" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
       <c r="E112" s="40" t="s">
         <v>1138</v>
@@ -36227,7 +36224,7 @@
         <v>469</v>
       </c>
       <c r="D113" s="40" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
       <c r="E113" s="40" t="s">
         <v>1138</v>
@@ -36254,7 +36251,7 @@
         <v>1730</v>
       </c>
       <c r="D114" s="40" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
       <c r="E114" s="40" t="s">
         <v>1138</v>
@@ -36281,7 +36278,7 @@
         <v>1730</v>
       </c>
       <c r="D115" s="40" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
       <c r="E115" s="40" t="s">
         <v>1138</v>
@@ -36308,7 +36305,7 @@
         <v>1730</v>
       </c>
       <c r="D116" s="40" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
       <c r="E116" s="40" t="s">
         <v>1138</v>
@@ -36335,7 +36332,7 @@
         <v>1730</v>
       </c>
       <c r="D117" s="40" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
       <c r="E117" s="40" t="s">
         <v>1138</v>
@@ -36362,7 +36359,7 @@
         <v>469</v>
       </c>
       <c r="D118" s="40" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="E118" s="40" t="s">
         <v>1138</v>
@@ -36391,7 +36388,7 @@
         <v>469</v>
       </c>
       <c r="D119" s="40" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="E119" s="40" t="s">
         <v>1138</v>
@@ -36420,7 +36417,7 @@
         <v>469</v>
       </c>
       <c r="D120" s="40" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="E120" s="40" t="s">
         <v>1138</v>
@@ -36449,7 +36446,7 @@
         <v>469</v>
       </c>
       <c r="D121" s="40" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="E121" s="40" t="s">
         <v>1138</v>
@@ -36478,7 +36475,7 @@
         <v>199</v>
       </c>
       <c r="D122" s="40" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="E122" s="40" t="s">
         <v>1138</v>
@@ -36507,7 +36504,7 @@
         <v>199</v>
       </c>
       <c r="D123" s="40" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="E123" s="40" t="s">
         <v>1138</v>
@@ -36534,7 +36531,7 @@
         <v>1807</v>
       </c>
       <c r="D124" s="40" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="E124" s="40" t="s">
         <v>1138</v>
@@ -36561,7 +36558,7 @@
         <v>1807</v>
       </c>
       <c r="D125" s="40" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="E125" s="40" t="s">
         <v>1138</v>
@@ -36588,7 +36585,7 @@
         <v>1807</v>
       </c>
       <c r="D126" s="40" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="E126" s="40" t="s">
         <v>1138</v>
@@ -36615,7 +36612,7 @@
         <v>1807</v>
       </c>
       <c r="D127" s="40" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="E127" s="40" t="s">
         <v>1138</v>
@@ -36642,7 +36639,7 @@
         <v>1807</v>
       </c>
       <c r="D128" s="40" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="E128" s="40" t="s">
         <v>1138</v>
@@ -36669,7 +36666,7 @@
         <v>1807</v>
       </c>
       <c r="D129" s="40" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="E129" s="40" t="s">
         <v>1138</v>
@@ -36696,7 +36693,7 @@
         <v>1807</v>
       </c>
       <c r="D130" s="40" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="E130" s="40" t="s">
         <v>1138</v>
@@ -36723,7 +36720,7 @@
         <v>1807</v>
       </c>
       <c r="D131" s="40" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="E131" s="40" t="s">
         <v>1138</v>
@@ -36795,6 +36792,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D9A8E34D4601248B4650C3759D604D8" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c234dc030e1d129322a3d56f76335218">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de0c653c-2bd3-43b1-95fa-012c57f61cfe" xmlns:ns3="848a8810-16a6-4d79-96d3-e3dfb86099b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a56d1a68c4d05b5a1e5a3c0b3fb5b1a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -37016,15 +37022,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6744B0D-B7F9-4CA7-A5DC-23D611E8ED20}">
   <ds:schemaRefs>
@@ -37044,6 +37041,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19245E31-480A-4933-AB52-6FC5778D0ABF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -37061,12 +37066,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B4CE896-D144-40A9-85D3-0684E5DFDA36}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>